<commit_message>
finished CB_AGD, determined flow structure
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413797F1-5923-4300-9FBF-47E124E06EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ADB921-E577-4A36-85B5-FA1F204D2DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10959,8 +10959,8 @@
   <dimension ref="A1:S263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>

<commit_message>
added CB shift, starting CB_new
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ADB921-E577-4A36-85B5-FA1F204D2DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F5B753-6C92-4436-B26A-61D3EDCFDB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
CB_AGD and shift sim OKgit add .
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F5B753-6C92-4436-B26A-61D3EDCFDB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F09C6-B98B-4803-8339-EE19C515F0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="2175" windowWidth="16200" windowHeight="9397" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
220423-v1 added PE_array, not sim
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA8C5FB-CEDD-4B21-83A9-8F0DC780D4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D4EF3-2F61-40CA-A3C6-C8D00C07562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1617,6 +1617,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1630,9 +1633,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2582,10 +2582,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -3365,12 +3365,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="100"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -10962,8 +10962,8 @@
   <dimension ref="A1:S263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12865,7 +12865,7 @@
       <c r="B74" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="C74" s="104" t="s">
+      <c r="C74" s="99" t="s">
         <v>70</v>
       </c>
       <c r="D74" s="25"/>
@@ -13231,11 +13231,11 @@
     </row>
     <row r="87" spans="1:19" ht="14.25" thickBot="1">
       <c r="A87" s="7"/>
-      <c r="B87" s="102" t="s">
+      <c r="B87" s="103" t="s">
         <v>217</v>
       </c>
-      <c r="C87" s="103"/>
-      <c r="D87" s="103"/>
+      <c r="C87" s="104"/>
+      <c r="D87" s="104"/>
       <c r="E87" s="90" t="s">
         <v>218</v>
       </c>

</xml_diff>

<commit_message>
modified data stream, sort out a way!
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D4EF3-2F61-40CA-A3C6-C8D00C07562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF165326-5D6A-4035-A680-1F7701ECB3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="228">
   <si>
     <t>步骤</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>5+1+5+1+3+2n+2</t>
-  </si>
-  <si>
-    <t>转置</t>
   </si>
   <si>
     <t>S_inv</t>
@@ -768,6 +765,34 @@
   </si>
   <si>
     <t>C</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_5转置</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_6</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_7</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1323,7 +1348,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1635,6 +1660,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1657,11 +1685,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1724025" cy="438150"/>
+    <xdr:ext cx="1538288" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="attachment-1647339354594-b5bf4ceb288e0530" descr="attachment-1647339354594-b5bf4ceb288e0530">
@@ -1682,8 +1710,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="12963525"/>
-          <a:ext cx="1724025" cy="438150"/>
+          <a:off x="295276" y="14135099"/>
+          <a:ext cx="1538288" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1891,9 +1919,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1495425" cy="352425"/>
     <xdr:pic>
@@ -1916,7 +1944,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="323850" y="13882688"/>
+          <a:off x="342900" y="15163800"/>
           <a:ext cx="1495425" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1930,9 +1958,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="638175" cy="419100"/>
     <xdr:pic>
@@ -1955,7 +1983,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="733425" y="13096875"/>
           <a:ext cx="638175" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2413,53 +2441,53 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -2520,7 +2548,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="1"/>
@@ -2618,7 +2646,7 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="8">
         <v>0</v>
@@ -2655,7 +2683,7 @@
     </row>
     <row r="7" spans="1:31" ht="15">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -2666,10 +2694,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2689,7 +2717,7 @@
         <v>4</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -2706,7 +2734,7 @@
     </row>
     <row r="8" spans="1:31" ht="15">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8">
         <v>1</v>
@@ -2714,13 +2742,13 @@
       <c r="C8" s="8"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2757,7 +2785,7 @@
     </row>
     <row r="9" spans="1:31" ht="15">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
@@ -2765,13 +2793,13 @@
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2808,20 +2836,20 @@
     </row>
     <row r="10" spans="1:31" ht="20.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -2863,25 +2891,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="G11" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2912,21 +2940,21 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2957,25 +2985,25 @@
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -3006,21 +3034,21 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -3051,25 +3079,25 @@
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -3100,25 +3128,25 @@
         <v>3</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -3145,31 +3173,31 @@
     </row>
     <row r="17" spans="1:31" ht="15">
       <c r="A17" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -3196,31 +3224,31 @@
     </row>
     <row r="18" spans="1:31">
       <c r="A18" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="I18" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -3251,21 +3279,21 @@
         <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -3298,15 +3326,15 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -3366,7 +3394,7 @@
     </row>
     <row r="22" spans="1:31">
       <c r="A22" s="102" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="101"/>
       <c r="C22" s="101"/>
@@ -3401,7 +3429,7 @@
     </row>
     <row r="23" spans="1:31">
       <c r="A23" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3436,7 +3464,7 @@
     </row>
     <row r="24" spans="1:31">
       <c r="A24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3471,7 +3499,7 @@
     </row>
     <row r="25" spans="1:31">
       <c r="A25" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -3479,10 +3507,10 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -3522,14 +3550,14 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -3571,10 +3599,10 @@
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -3608,14 +3636,14 @@
         <v>2</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -3645,25 +3673,25 @@
     </row>
     <row r="29" spans="1:31">
       <c r="A29" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="3" t="s">
         <v>61</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3694,19 +3722,19 @@
         <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3733,31 +3761,31 @@
     </row>
     <row r="31" spans="1:31">
       <c r="A31" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B31" s="3">
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="H31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3788,21 +3816,21 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3829,7 +3857,7 @@
     </row>
     <row r="33" spans="1:31">
       <c r="A33" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3864,31 +3892,31 @@
     </row>
     <row r="34" spans="1:31" ht="15.75" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="3">
         <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3898,7 +3926,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
@@ -3924,22 +3952,22 @@
         <v>65</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>66</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3966,7 +3994,7 @@
     </row>
     <row r="36" spans="1:31">
       <c r="A36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B36" s="3">
         <v>5</v>
@@ -3981,16 +4009,16 @@
         <v>66</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -4025,17 +4053,17 @@
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -4066,25 +4094,25 @@
         <v>7</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="H38" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -4111,26 +4139,26 @@
     </row>
     <row r="39" spans="1:31">
       <c r="A39" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B39" s="3">
         <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I39" s="7">
         <v>1</v>
@@ -4164,14 +4192,14 @@
         <v>9</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="7">
         <v>5.9</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -4234,7 +4262,7 @@
     </row>
     <row r="42" spans="1:31">
       <c r="A42" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -4273,21 +4301,21 @@
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="G43" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -4318,21 +4346,21 @@
         <v>2</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="7">
@@ -4367,25 +4395,25 @@
         <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="G45" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="H45" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -4418,15 +4446,15 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="7">
@@ -4467,15 +4495,15 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -4508,25 +4536,25 @@
         <v>2</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="H48" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -4557,21 +4585,21 @@
         <v>3</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -4602,25 +4630,25 @@
         <v>3</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -4651,25 +4679,25 @@
         <v>4</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4729,7 +4757,7 @@
     </row>
     <row r="53" spans="1:31">
       <c r="A53" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -4768,25 +4796,25 @@
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="F54" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="7"/>
@@ -4817,25 +4845,25 @@
         <v>2</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E55" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="7"/>
@@ -4866,25 +4894,25 @@
         <v>3</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="H56" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="7"/>
@@ -4915,21 +4943,21 @@
         <v>2</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="7"/>
@@ -4960,25 +4988,25 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="7"/>
@@ -5009,25 +5037,25 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="F59" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G59" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H59" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="I59" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -5058,25 +5086,25 @@
         <v>4</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -10962,8 +10990,8 @@
   <dimension ref="A1:S263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -11031,7 +11059,7 @@
     </row>
     <row r="3" spans="1:19" ht="20.25" customHeight="1">
       <c r="A3" s="72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -11054,7 +11082,7 @@
     </row>
     <row r="4" spans="1:19" ht="20.25" customHeight="1">
       <c r="A4" s="71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -11284,7 +11312,7 @@
     </row>
     <row r="14" spans="1:19" ht="15">
       <c r="A14" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -11336,7 +11364,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="58" t="s">
@@ -11387,14 +11415,14 @@
     <row r="18" spans="1:19" ht="11.25" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>199</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>200</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
@@ -11420,10 +11448,10 @@
         <v>24</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -11472,16 +11500,16 @@
     <row r="21" spans="1:19" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>200</v>
-      </c>
       <c r="D21" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>199</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>200</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="4"/>
@@ -11557,14 +11585,14 @@
     <row r="24" spans="1:19">
       <c r="A24" s="3"/>
       <c r="B24" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>29</v>
@@ -11748,7 +11776,7 @@
         <v>36</v>
       </c>
       <c r="C32" s="61" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="73" t="s">
@@ -11799,14 +11827,14 @@
     <row r="34" spans="1:19">
       <c r="A34" s="4"/>
       <c r="B34" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="4"/>
@@ -11880,14 +11908,14 @@
     <row r="37" spans="1:19">
       <c r="A37" s="4"/>
       <c r="B37" s="53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>43</v>
@@ -11916,7 +11944,7 @@
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="63" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -11963,14 +11991,14 @@
     <row r="40" spans="1:19">
       <c r="A40" s="4"/>
       <c r="B40" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -12044,14 +12072,14 @@
     <row r="43" spans="1:19">
       <c r="A43" s="4"/>
       <c r="B43" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="4"/>
@@ -12080,7 +12108,7 @@
         <v>45</v>
       </c>
       <c r="E44" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -12129,16 +12157,16 @@
     <row r="46" spans="1:19">
       <c r="A46" s="4"/>
       <c r="B46" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C46" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C46" s="29" t="s">
-        <v>200</v>
-      </c>
       <c r="D46" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F46" s="7">
         <v>8</v>
@@ -12365,16 +12393,18 @@
       <c r="S55" s="4"/>
     </row>
     <row r="56" spans="1:19">
-      <c r="A56" s="40"/>
+      <c r="A56" s="17" t="s">
+        <v>221</v>
+      </c>
       <c r="B56" s="76" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C56" s="85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F56" s="39"/>
       <c r="G56" s="41"/>
@@ -12394,14 +12424,14 @@
     <row r="57" spans="1:19">
       <c r="A57" s="40"/>
       <c r="B57" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F57" s="39"/>
       <c r="G57" s="41"/>
@@ -12421,14 +12451,14 @@
     <row r="58" spans="1:19">
       <c r="A58" s="40"/>
       <c r="B58" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F58" s="39"/>
       <c r="G58" s="41"/>
@@ -12446,16 +12476,18 @@
       <c r="S58" s="41"/>
     </row>
     <row r="59" spans="1:19">
-      <c r="A59" s="40"/>
+      <c r="A59" s="17" t="s">
+        <v>222</v>
+      </c>
       <c r="B59" s="68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C59" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D59" s="42"/>
       <c r="E59" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F59" s="39"/>
       <c r="G59" s="41"/>
@@ -12475,14 +12507,14 @@
     <row r="60" spans="1:19">
       <c r="A60" s="40"/>
       <c r="B60" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F60" s="39"/>
       <c r="G60" s="41"/>
@@ -12502,17 +12534,17 @@
     <row r="61" spans="1:19">
       <c r="A61" s="40"/>
       <c r="B61" s="50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C61" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D61" s="44"/>
       <c r="E61" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F61" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G61" s="41"/>
       <c r="H61" s="41"/>
@@ -12529,16 +12561,18 @@
       <c r="S61" s="41"/>
     </row>
     <row r="62" spans="1:19">
-      <c r="A62" s="3"/>
+      <c r="A62" s="17" t="s">
+        <v>223</v>
+      </c>
       <c r="B62" s="77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C62" s="84" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D62" s="24"/>
       <c r="E62" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -12558,14 +12592,14 @@
     <row r="63" spans="1:19">
       <c r="A63" s="3"/>
       <c r="B63" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D63" s="17"/>
       <c r="E63" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="4"/>
@@ -12585,14 +12619,14 @@
     <row r="64" spans="1:19">
       <c r="A64" s="3"/>
       <c r="B64" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C64" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D64" s="17"/>
       <c r="E64" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="4"/>
@@ -12612,17 +12646,17 @@
     <row r="65" spans="1:19">
       <c r="A65" s="3"/>
       <c r="B65" s="67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C65" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D65" s="48"/>
       <c r="E65" s="69" t="s">
         <v>62</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G65" s="41"/>
       <c r="H65" s="41"/>
@@ -12641,10 +12675,10 @@
     <row r="66" spans="1:19">
       <c r="A66" s="3"/>
       <c r="B66" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D66" s="24"/>
       <c r="E66" s="46" t="s">
@@ -12668,14 +12702,14 @@
     <row r="67" spans="1:19">
       <c r="A67" s="3"/>
       <c r="B67" s="43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C67" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D67" s="44"/>
       <c r="E67" s="45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="41"/>
@@ -12693,7 +12727,9 @@
       <c r="S67" s="41"/>
     </row>
     <row r="68" spans="1:19">
-      <c r="A68" s="3"/>
+      <c r="A68" s="17" t="s">
+        <v>224</v>
+      </c>
       <c r="B68" s="64" t="s">
         <v>65</v>
       </c>
@@ -12755,16 +12791,16 @@
     <row r="70" spans="1:19">
       <c r="A70" s="3"/>
       <c r="B70" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C70" s="17" t="s">
-        <v>200</v>
-      </c>
       <c r="D70" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E70" s="27" t="s">
         <v>199</v>
-      </c>
-      <c r="E70" s="27" t="s">
-        <v>200</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>52</v>
@@ -12784,8 +12820,8 @@
       <c r="S70" s="4"/>
     </row>
     <row r="71" spans="1:19">
-      <c r="A71" s="3" t="s">
-        <v>69</v>
+      <c r="A71" s="17" t="s">
+        <v>225</v>
       </c>
       <c r="B71" s="62" t="s">
         <v>66</v>
@@ -12793,7 +12829,7 @@
       <c r="C71" s="25"/>
       <c r="D71" s="25"/>
       <c r="E71" s="63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="4"/>
@@ -12838,12 +12874,12 @@
     <row r="73" spans="1:19">
       <c r="A73" s="40"/>
       <c r="B73" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73" s="17"/>
       <c r="D73" s="17"/>
       <c r="E73" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F73" s="39"/>
       <c r="G73" s="41"/>
@@ -12861,16 +12897,18 @@
       <c r="S73" s="41"/>
     </row>
     <row r="74" spans="1:19">
-      <c r="A74" s="3"/>
+      <c r="A74" s="17" t="s">
+        <v>226</v>
+      </c>
       <c r="B74" s="62" t="s">
         <v>62</v>
       </c>
       <c r="C74" s="99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D74" s="25"/>
       <c r="E74" s="63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -12917,17 +12955,17 @@
     <row r="76" spans="1:19">
       <c r="A76" s="3"/>
       <c r="B76" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C76" s="17" t="s">
         <v>199</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>200</v>
       </c>
       <c r="D76" s="17"/>
       <c r="E76" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
@@ -12946,16 +12984,16 @@
     <row r="77" spans="1:19">
       <c r="A77" s="3"/>
       <c r="B77" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C77" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="25" t="s">
-        <v>74</v>
-      </c>
       <c r="E77" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -12978,13 +13016,13 @@
         <v>64</v>
       </c>
       <c r="C78" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="E78" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="4"/>
@@ -13016,7 +13054,7 @@
         <v>25</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -13035,16 +13073,16 @@
     <row r="80" spans="1:19">
       <c r="A80" s="3"/>
       <c r="B80" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C80" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D80" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D80" s="47" t="s">
-        <v>79</v>
-      </c>
       <c r="E80" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="4"/>
@@ -13067,13 +13105,13 @@
         <v>64</v>
       </c>
       <c r="C81" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D81" s="17" t="s">
-        <v>81</v>
-      </c>
       <c r="E81" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="4"/>
@@ -13105,7 +13143,7 @@
         <v>23</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -13122,18 +13160,20 @@
       <c r="S82" s="4"/>
     </row>
     <row r="83" spans="1:19">
-      <c r="A83" s="4"/>
+      <c r="A83" s="105" t="s">
+        <v>227</v>
+      </c>
       <c r="B83" s="62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C83" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D83" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="D83" s="75" t="s">
-        <v>79</v>
-      </c>
       <c r="E83" s="73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="4"/>
@@ -13153,16 +13193,16 @@
     <row r="84" spans="1:19">
       <c r="A84" s="4"/>
       <c r="B84" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="D84" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D84" s="17" t="s">
-        <v>85</v>
-      </c>
       <c r="E84" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="4"/>
@@ -13182,16 +13222,16 @@
     <row r="85" spans="1:19">
       <c r="A85" s="4"/>
       <c r="B85" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C85" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="D85" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="E85" s="30" t="s">
         <v>201</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>202</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="4"/>
@@ -13232,12 +13272,12 @@
     <row r="87" spans="1:19" ht="14.25" thickBot="1">
       <c r="A87" s="7"/>
       <c r="B87" s="103" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C87" s="104"/>
       <c r="D87" s="104"/>
       <c r="E87" s="90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
@@ -13254,16 +13294,16 @@
     <row r="88" spans="1:19" ht="14.25" thickBot="1">
       <c r="A88" s="39"/>
       <c r="B88" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" s="95" t="s">
         <v>219</v>
       </c>
-      <c r="C88" s="95" t="s">
+      <c r="D88" s="95" t="s">
+        <v>192</v>
+      </c>
+      <c r="E88" s="95" t="s">
         <v>220</v>
-      </c>
-      <c r="D88" s="95" t="s">
-        <v>193</v>
-      </c>
-      <c r="E88" s="95" t="s">
-        <v>221</v>
       </c>
       <c r="I88" s="41"/>
       <c r="J88" s="41"/>
@@ -13279,19 +13319,19 @@
     </row>
     <row r="89" spans="1:19">
       <c r="A89" s="97" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B89" s="87" t="s">
+        <v>198</v>
+      </c>
+      <c r="C89" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="C89" s="91" t="s">
-        <v>200</v>
-      </c>
       <c r="D89" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="E89" s="91" t="s">
         <v>199</v>
-      </c>
-      <c r="E89" s="91" t="s">
-        <v>200</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -13309,15 +13349,15 @@
     </row>
     <row r="90" spans="1:19">
       <c r="A90" s="98" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B90" s="88"/>
       <c r="C90" s="92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D90" s="92"/>
       <c r="E90" s="92" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G90" s="41"/>
       <c r="H90" s="41"/>
@@ -13335,22 +13375,22 @@
     </row>
     <row r="91" spans="1:19">
       <c r="A91" s="97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B91" s="88" t="s">
+        <v>200</v>
+      </c>
+      <c r="C91" s="92" t="s">
+        <v>200</v>
+      </c>
+      <c r="D91" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E91" s="92" t="s">
         <v>201</v>
       </c>
-      <c r="C91" s="92" t="s">
-        <v>201</v>
-      </c>
-      <c r="D91" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E91" s="92" t="s">
-        <v>202</v>
-      </c>
       <c r="G91" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
@@ -13367,18 +13407,18 @@
     </row>
     <row r="92" spans="1:19" ht="14.25" thickBot="1">
       <c r="A92" s="97" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B92" s="89"/>
       <c r="C92" s="96"/>
       <c r="D92" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E92" s="93" t="s">
+        <v>209</v>
+      </c>
+      <c r="G92" s="86" t="s">
         <v>210</v>
-      </c>
-      <c r="G92" s="86" t="s">
-        <v>211</v>
       </c>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>

</xml_diff>

<commit_message>
the same, add revise on excels
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF165326-5D6A-4035-A680-1F7701ECB3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23909509-C102-4914-B54D-95683814DB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1645,6 +1645,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1659,9 +1662,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2610,10 +2610,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -3393,12 +3393,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="102" t="s">
+      <c r="A22" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -10990,8 +10990,8 @@
   <dimension ref="A1:S263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -13160,7 +13160,7 @@
       <c r="S82" s="4"/>
     </row>
     <row r="83" spans="1:19">
-      <c r="A83" s="105" t="s">
+      <c r="A83" s="100" t="s">
         <v>227</v>
       </c>
       <c r="B83" s="62" t="s">
@@ -13271,11 +13271,11 @@
     </row>
     <row r="87" spans="1:19" ht="14.25" thickBot="1">
       <c r="A87" s="7"/>
-      <c r="B87" s="103" t="s">
+      <c r="B87" s="104" t="s">
         <v>216</v>
       </c>
-      <c r="C87" s="104"/>
-      <c r="D87" s="104"/>
+      <c r="C87" s="105"/>
+      <c r="D87" s="105"/>
       <c r="E87" s="90" t="s">
         <v>217</v>
       </c>

</xml_diff>

<commit_message>
220430-v1-night cplt TB-A TB-B, not simed
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23909509-C102-4914-B54D-95683814DB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C249E9-C51E-47C3-89C1-2EC47F190CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="235">
   <si>
     <t>步骤</t>
   </si>
@@ -793,6 +793,34 @@
   </si>
   <si>
     <t>UPD_7</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>cov</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_cov</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>CB</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>(3*3)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_cov_l</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2*3+2n)</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -10990,8 +11018,8 @@
   <dimension ref="A1:S263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -13476,8 +13504,12 @@
     </row>
     <row r="95" spans="1:19">
       <c r="A95" s="4"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
+      <c r="B95" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>229</v>
+      </c>
       <c r="D95" s="18"/>
       <c r="E95" s="18"/>
       <c r="F95" s="7"/>
@@ -13497,8 +13529,12 @@
     </row>
     <row r="96" spans="1:19">
       <c r="A96" s="4"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
+      <c r="B96" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="C96" s="55" t="s">
+        <v>232</v>
+      </c>
       <c r="D96" s="18"/>
       <c r="E96" s="18"/>
       <c r="F96" s="7"/>
@@ -13518,8 +13554,12 @@
     </row>
     <row r="97" spans="1:19">
       <c r="A97" s="4"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
+      <c r="B97" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>231</v>
+      </c>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
       <c r="F97" s="7"/>
@@ -13539,8 +13579,12 @@
     </row>
     <row r="98" spans="1:19">
       <c r="A98" s="4"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
+      <c r="B98" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>233</v>
+      </c>
       <c r="D98" s="18"/>
       <c r="E98" s="18"/>
       <c r="F98" s="7"/>
@@ -13560,8 +13604,12 @@
     </row>
     <row r="99" spans="1:19">
       <c r="A99" s="4"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="18"/>
+      <c r="B99" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>234</v>
+      </c>
       <c r="D99" s="18"/>
       <c r="E99" s="18"/>
       <c r="F99" s="7"/>
@@ -13581,8 +13629,12 @@
     </row>
     <row r="100" spans="1:19">
       <c r="A100" s="4"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="18"/>
+      <c r="B100" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>231</v>
+      </c>
       <c r="D100" s="18"/>
       <c r="E100" s="18"/>
       <c r="F100" s="7"/>

</xml_diff>

<commit_message>
add NEW full config
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C249E9-C51E-47C3-89C1-2EC47F190CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FA6851-F11F-4B93-8A2C-C70A21871092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="239">
   <si>
     <t>步骤</t>
   </si>
@@ -821,6 +821,22 @@
   </si>
   <si>
     <t>(2*3+2n)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>POS</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-POS/1-NEG</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-NEG/1-POS</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEW</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -968,7 +984,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1180,48 +1196,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1370,13 +1344,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1486,9 +1484,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1502,13 +1497,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1520,13 +1509,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1568,16 +1557,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1599,9 +1582,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1628,11 +1608,23 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1640,28 +1632,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1676,6 +1653,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1685,10 +1668,37 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1714,7 +1724,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1538288" cy="333375"/>
@@ -1753,7 +1763,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1657350" cy="533400"/>
@@ -1792,7 +1802,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1866900" cy="333375"/>
@@ -1831,7 +1841,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="533400" cy="371475"/>
@@ -1909,7 +1919,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1285875</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="695325" cy="409575"/>
@@ -1948,7 +1958,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1495425" cy="352425"/>
@@ -1987,7 +1997,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="638175" cy="419100"/>
@@ -2026,7 +2036,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1266825" cy="428625"/>
@@ -2065,7 +2075,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1971675" cy="381000"/>
@@ -2104,7 +2114,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>42862</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1914525" cy="309563"/>
@@ -2638,10 +2648,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="102"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -3421,12 +3431,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -11015,18 +11025,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S263"/>
+  <dimension ref="A1:S274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="29.73046875" customWidth="1"/>
-    <col min="2" max="2" width="11" style="55" customWidth="1"/>
-    <col min="3" max="5" width="13" style="55" customWidth="1"/>
+    <col min="2" max="2" width="11" style="52" customWidth="1"/>
+    <col min="3" max="5" width="13" style="52" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="19" width="14" customWidth="1"/>
   </cols>
@@ -11086,7 +11096,7 @@
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="67" t="s">
         <v>187</v>
       </c>
       <c r="B3" s="13"/>
@@ -11109,7 +11119,7 @@
       <c r="S3" s="4"/>
     </row>
     <row r="4" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="66" t="s">
         <v>204</v>
       </c>
       <c r="B4" s="13"/>
@@ -11244,28 +11254,28 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:19" s="81" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:19" s="75" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A10" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="80"/>
-      <c r="S10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
     </row>
     <row r="11" spans="1:19" ht="15">
       <c r="A11" s="2" t="s">
@@ -11388,14 +11398,14 @@
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="54" t="s">
         <v>191</v>
       </c>
       <c r="D16" s="19"/>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="55" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="3"/>
@@ -11467,52 +11477,50 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="38.25" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="59" t="s">
+    <row r="19" spans="1:19" ht="11.25" customHeight="1">
+      <c r="A19" s="95"/>
+      <c r="B19" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="F19" s="95"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+    </row>
+    <row r="20" spans="1:19" ht="38.25" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C20" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="D20" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="E19" s="57" t="s">
+      <c r="E20" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>21</v>
-      </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -11527,19 +11535,19 @@
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
-      <c r="B21" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="F21" s="7"/>
+      <c r="B21" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -11554,207 +11562,225 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" ht="39.75" customHeight="1">
-      <c r="A22" s="31" t="s">
+    <row r="22" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A23" s="95"/>
+      <c r="B23" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="94"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+    </row>
+    <row r="24" spans="1:19" ht="39.75" customHeight="1">
+      <c r="A24" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B24" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C24" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="73" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="3"/>
-      <c r="B23" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="3"/>
-      <c r="B24" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="3"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
+      <c r="B25" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="3"/>
+      <c r="B27" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-    </row>
-    <row r="27" spans="1:19" s="81" customFormat="1">
-      <c r="A27" s="52" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+    </row>
+    <row r="29" spans="1:19" s="75" customFormat="1">
+      <c r="A29" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="80"/>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="80"/>
-      <c r="S27" s="80"/>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -11775,9 +11801,9 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" ht="33" customHeight="1">
+    <row r="31" spans="1:19">
       <c r="A31" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -11798,21 +11824,17 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" ht="33" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="61" t="s">
-        <v>191</v>
-      </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+    <row r="32" spans="1:19">
+      <c r="A32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -11825,18 +11847,14 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19">
-      <c r="A33" s="4"/>
-      <c r="B33" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>39</v>
-      </c>
+    <row r="33" spans="1:19" ht="33" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="17"/>
-      <c r="E33" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="E33" s="17"/>
       <c r="F33" s="7"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -11852,21 +11870,21 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" ht="33" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="27" t="s">
-        <v>201</v>
+      <c r="B34" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="25"/>
+      <c r="E34" s="68" t="s">
+        <v>37</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -11881,19 +11899,19 @@
     </row>
     <row r="35" spans="1:19">
       <c r="A35" s="4"/>
-      <c r="B35" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="B35" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -11909,18 +11927,18 @@
     <row r="36" spans="1:19">
       <c r="A36" s="4"/>
       <c r="B36" s="26" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="18"/>
+        <v>199</v>
+      </c>
+      <c r="D36" s="17"/>
       <c r="E36" s="27" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -11934,45 +11952,43 @@
       <c r="S36" s="4"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="4"/>
-      <c r="B37" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="54" t="s">
-        <v>201</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" s="95"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+      <c r="Q37" s="40"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" s="4"/>
-      <c r="B38" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="63" t="s">
-        <v>193</v>
+      <c r="B38" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="36"/>
+      <c r="E38" s="68" t="s">
+        <v>40</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -11994,12 +12010,12 @@
       <c r="B39" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="17"/>
+      <c r="C39" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="18"/>
       <c r="E39" s="27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -12018,17 +12034,19 @@
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="4"/>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="C40" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F40" s="3"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
@@ -12044,47 +12062,47 @@
       <c r="S40" s="4"/>
     </row>
     <row r="41" spans="1:19">
-      <c r="A41" s="4"/>
-      <c r="B41" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="95"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="4"/>
-      <c r="B42" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="B42" s="105" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="41"/>
+      <c r="E42" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -12099,19 +12117,19 @@
     </row>
     <row r="43" spans="1:19">
       <c r="A43" s="4"/>
-      <c r="B43" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="B43" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="24"/>
+      <c r="E43" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -12126,17 +12144,15 @@
     </row>
     <row r="44" spans="1:19">
       <c r="A44" s="4"/>
-      <c r="B44" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="73" t="s">
-        <v>188</v>
+      <c r="B44" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="43" t="s">
+        <v>199</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -12154,53 +12170,47 @@
       <c r="S44" s="4"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="4"/>
-      <c r="B45" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" s="42"/>
+      <c r="E45" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="F45" s="95"/>
+      <c r="G45" s="95"/>
+      <c r="H45" s="95"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="40"/>
+      <c r="O45" s="40"/>
+      <c r="P45" s="40"/>
+      <c r="Q45" s="40"/>
+      <c r="R45" s="40"/>
+      <c r="S45" s="40"/>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" s="4"/>
-      <c r="B46" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E46" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="F46" s="7">
-        <v>8</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+      <c r="B46" s="101" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="102" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="41"/>
+      <c r="E46" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -12215,13 +12225,17 @@
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="4"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="B47" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="24"/>
+      <c r="E47" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="7"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -12236,63 +12250,77 @@
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" spans="1:19" s="81" customFormat="1">
-      <c r="A48" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="82"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="80"/>
-      <c r="K48" s="80"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
-      <c r="P48" s="80"/>
-      <c r="Q48" s="80"/>
-      <c r="R48" s="80"/>
-      <c r="S48" s="80"/>
+    <row r="48" spans="1:19">
+      <c r="A48" s="4"/>
+      <c r="B48" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
     </row>
     <row r="49" spans="1:19">
-      <c r="A49" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="F49" s="94"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="40"/>
+      <c r="N49" s="40"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="40"/>
+      <c r="R49" s="40"/>
+      <c r="S49" s="40"/>
     </row>
     <row r="50" spans="1:19">
-      <c r="A50" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="106" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="104" t="s">
+        <v>188</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -12306,13 +12334,19 @@
       <c r="S50" s="4"/>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>47</v>
+      </c>
       <c r="F51" s="7"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -12329,14 +12363,22 @@
       <c r="S51" s="4"/>
     </row>
     <row r="52" spans="1:19">
-      <c r="A52" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="7"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="F52" s="7">
+        <v>8</v>
+      </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -12352,37 +12394,43 @@
       <c r="S52" s="4"/>
     </row>
     <row r="53" spans="1:19">
-      <c r="A53" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C53" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="E53" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="F53" s="94"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="40"/>
+      <c r="L53" s="40"/>
+      <c r="M53" s="40"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="40"/>
+      <c r="R53" s="40"/>
+      <c r="S53" s="40"/>
     </row>
     <row r="54" spans="1:19">
-      <c r="A54" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="A54" s="4"/>
       <c r="B54" s="17"/>
-      <c r="C54" s="38"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
-      <c r="F54" s="7"/>
+      <c r="F54" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -12397,214 +12445,178 @@
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:19">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:19" s="75" customFormat="1">
+      <c r="A55" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="76"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="74"/>
+      <c r="L55" s="74"/>
+      <c r="M55" s="74"/>
+      <c r="N55" s="74"/>
+      <c r="O55" s="74"/>
+      <c r="P55" s="74"/>
+      <c r="Q55" s="74"/>
+      <c r="R55" s="74"/>
+      <c r="S55" s="74"/>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="A57" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="A58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+    </row>
+    <row r="59" spans="1:19">
+      <c r="A59" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="17"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="A60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="17"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+    </row>
+    <row r="61" spans="1:19">
+      <c r="A61" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="17"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="1:19">
+      <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="A56" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B56" s="76" t="s">
-        <v>185</v>
-      </c>
-      <c r="C56" s="85" t="s">
-        <v>207</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="F56" s="39"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="41"/>
-      <c r="L56" s="41"/>
-      <c r="M56" s="41"/>
-      <c r="N56" s="41"/>
-      <c r="O56" s="41"/>
-      <c r="P56" s="41"/>
-      <c r="Q56" s="41"/>
-      <c r="R56" s="41"/>
-      <c r="S56" s="41"/>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="A57" s="40"/>
-      <c r="B57" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="F57" s="39"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="41"/>
-      <c r="L57" s="41"/>
-      <c r="M57" s="41"/>
-      <c r="N57" s="41"/>
-      <c r="O57" s="41"/>
-      <c r="P57" s="41"/>
-      <c r="Q57" s="41"/>
-      <c r="R57" s="41"/>
-      <c r="S57" s="41"/>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="A58" s="40"/>
-      <c r="B58" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F58" s="39"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="41"/>
-      <c r="L58" s="41"/>
-      <c r="M58" s="41"/>
-      <c r="N58" s="41"/>
-      <c r="O58" s="41"/>
-      <c r="P58" s="41"/>
-      <c r="Q58" s="41"/>
-      <c r="R58" s="41"/>
-      <c r="S58" s="41"/>
-    </row>
-    <row r="59" spans="1:19">
-      <c r="A59" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B59" s="68" t="s">
-        <v>191</v>
-      </c>
-      <c r="C59" s="83" t="s">
-        <v>182</v>
-      </c>
-      <c r="D59" s="42"/>
-      <c r="E59" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="F59" s="39"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="41"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="41"/>
-      <c r="L59" s="41"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="41"/>
-      <c r="O59" s="41"/>
-      <c r="P59" s="41"/>
-      <c r="Q59" s="41"/>
-      <c r="R59" s="41"/>
-      <c r="S59" s="41"/>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="A60" s="40"/>
-      <c r="B60" s="49" t="s">
-        <v>197</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="F60" s="39"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
-      <c r="R60" s="41"/>
-      <c r="S60" s="41"/>
-    </row>
-    <row r="61" spans="1:19">
-      <c r="A61" s="40"/>
-      <c r="B61" s="50" t="s">
-        <v>198</v>
-      </c>
-      <c r="C61" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="D61" s="44"/>
-      <c r="E61" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="F61" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="41"/>
-      <c r="L61" s="41"/>
-      <c r="M61" s="41"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
-      <c r="P61" s="41"/>
-      <c r="Q61" s="41"/>
-      <c r="R61" s="41"/>
-      <c r="S61" s="41"/>
-    </row>
-    <row r="62" spans="1:19">
-      <c r="A62" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="B62" s="77" t="s">
-        <v>195</v>
-      </c>
-      <c r="C62" s="84" t="s">
-        <v>182</v>
-      </c>
-      <c r="D62" s="24"/>
-      <c r="E62" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -12618,192 +12630,190 @@
       <c r="S62" s="4"/>
     </row>
     <row r="63" spans="1:19">
-      <c r="A63" s="3"/>
-      <c r="B63" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="17" t="s">
+      <c r="A63" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B63" s="105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="107" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="41"/>
+      <c r="E63" s="108" t="s">
+        <v>185</v>
+      </c>
+      <c r="F63" s="38"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
+      <c r="J63" s="40"/>
+      <c r="K63" s="40"/>
+      <c r="L63" s="40"/>
+      <c r="M63" s="40"/>
+      <c r="N63" s="40"/>
+      <c r="O63" s="40"/>
+      <c r="P63" s="40"/>
+      <c r="Q63" s="40"/>
+      <c r="R63" s="40"/>
+      <c r="S63" s="40"/>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="A64" s="39"/>
+      <c r="B64" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D64" s="24"/>
+      <c r="E64" s="109" t="s">
+        <v>186</v>
+      </c>
+      <c r="F64" s="38"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
+      <c r="J64" s="40"/>
+      <c r="K64" s="40"/>
+      <c r="L64" s="40"/>
+      <c r="M64" s="40"/>
+      <c r="N64" s="40"/>
+      <c r="O64" s="40"/>
+      <c r="P64" s="40"/>
+      <c r="Q64" s="40"/>
+      <c r="R64" s="40"/>
+      <c r="S64" s="40"/>
+    </row>
+    <row r="65" spans="1:19">
+      <c r="A65" s="39"/>
+      <c r="B65" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="42"/>
+      <c r="E65" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="F65" s="38"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40"/>
+      <c r="L65" s="40"/>
+      <c r="M65" s="40"/>
+      <c r="N65" s="40"/>
+      <c r="O65" s="40"/>
+      <c r="P65" s="40"/>
+      <c r="Q65" s="40"/>
+      <c r="R65" s="40"/>
+      <c r="S65" s="40"/>
+    </row>
+    <row r="66" spans="1:19">
+      <c r="A66" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="D66" s="41"/>
+      <c r="E66" s="64" t="s">
+        <v>194</v>
+      </c>
+      <c r="F66" s="38"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
+      <c r="I66" s="40"/>
+      <c r="J66" s="40"/>
+      <c r="K66" s="40"/>
+      <c r="L66" s="40"/>
+      <c r="M66" s="40"/>
+      <c r="N66" s="40"/>
+      <c r="O66" s="40"/>
+      <c r="P66" s="40"/>
+      <c r="Q66" s="40"/>
+      <c r="R66" s="40"/>
+      <c r="S66" s="40"/>
+    </row>
+    <row r="67" spans="1:19">
+      <c r="A67" s="39"/>
+      <c r="B67" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="F63" s="7"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-    </row>
-    <row r="64" spans="1:19">
-      <c r="A64" s="3"/>
-      <c r="B64" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="C64" s="44" t="s">
+      <c r="D67" s="24"/>
+      <c r="E67" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F67" s="38"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="40"/>
+      <c r="J67" s="40"/>
+      <c r="K67" s="40"/>
+      <c r="L67" s="40"/>
+      <c r="M67" s="40"/>
+      <c r="N67" s="40"/>
+      <c r="O67" s="40"/>
+      <c r="P67" s="40"/>
+      <c r="Q67" s="40"/>
+      <c r="R67" s="40"/>
+      <c r="S67" s="40"/>
+    </row>
+    <row r="68" spans="1:19">
+      <c r="A68" s="39"/>
+      <c r="B68" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="27" t="s">
+      <c r="D68" s="42"/>
+      <c r="E68" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="F64" s="3"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-      <c r="S64" s="4"/>
-    </row>
-    <row r="65" spans="1:19">
-      <c r="A65" s="3"/>
-      <c r="B65" s="67" t="s">
-        <v>185</v>
-      </c>
-      <c r="C65" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="D65" s="48"/>
-      <c r="E65" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G65" s="41"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="41"/>
-      <c r="J65" s="41"/>
-      <c r="K65" s="41"/>
-      <c r="L65" s="41"/>
-      <c r="M65" s="41"/>
-      <c r="N65" s="41"/>
-      <c r="O65" s="41"/>
-      <c r="P65" s="41"/>
-      <c r="Q65" s="41"/>
-      <c r="R65" s="41"/>
-      <c r="S65" s="41"/>
-    </row>
-    <row r="66" spans="1:19">
-      <c r="A66" s="3"/>
-      <c r="B66" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="D66" s="24"/>
-      <c r="E66" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F66" s="3"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="41"/>
-      <c r="L66" s="41"/>
-      <c r="M66" s="41"/>
-      <c r="N66" s="41"/>
-      <c r="O66" s="41"/>
-      <c r="P66" s="41"/>
-      <c r="Q66" s="41"/>
-      <c r="R66" s="41"/>
-      <c r="S66" s="41"/>
-    </row>
-    <row r="67" spans="1:19">
-      <c r="A67" s="3"/>
-      <c r="B67" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="C67" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="D67" s="44"/>
-      <c r="E67" s="45" t="s">
-        <v>199</v>
-      </c>
-      <c r="F67" s="3"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="41"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="41"/>
-      <c r="L67" s="41"/>
-      <c r="M67" s="41"/>
-      <c r="N67" s="41"/>
-      <c r="O67" s="41"/>
-      <c r="P67" s="41"/>
-      <c r="Q67" s="41"/>
-      <c r="R67" s="41"/>
-      <c r="S67" s="41"/>
-    </row>
-    <row r="68" spans="1:19">
-      <c r="A68" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="B68" s="64" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="D68" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="E68" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
+      <c r="F68" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="G68" s="40"/>
+      <c r="H68" s="40"/>
+      <c r="I68" s="40"/>
+      <c r="J68" s="40"/>
+      <c r="K68" s="40"/>
+      <c r="L68" s="40"/>
+      <c r="M68" s="40"/>
+      <c r="N68" s="40"/>
+      <c r="O68" s="40"/>
+      <c r="P68" s="40"/>
+      <c r="Q68" s="40"/>
+      <c r="R68" s="40"/>
+      <c r="S68" s="40"/>
     </row>
     <row r="69" spans="1:19">
-      <c r="A69" s="3"/>
-      <c r="B69" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E69" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
+      <c r="A69" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B69" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="D69" s="24"/>
+      <c r="E69" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
@@ -12819,20 +12829,16 @@
     <row r="70" spans="1:19">
       <c r="A70" s="3"/>
       <c r="B70" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>198</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="D70" s="17"/>
       <c r="E70" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="F70" s="7"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -12848,18 +12854,18 @@
       <c r="S70" s="4"/>
     </row>
     <row r="71" spans="1:19">
-      <c r="A71" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="B71" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="F71" s="7"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="17"/>
+      <c r="E71" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -12876,127 +12882,133 @@
     </row>
     <row r="72" spans="1:19">
       <c r="A72" s="3"/>
-      <c r="B72" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F72" s="7"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
-      <c r="Q72" s="4"/>
-      <c r="R72" s="4"/>
-      <c r="S72" s="4"/>
+      <c r="B72" s="101" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" s="45"/>
+      <c r="E72" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G72" s="40"/>
+      <c r="H72" s="40"/>
+      <c r="I72" s="40"/>
+      <c r="J72" s="40"/>
+      <c r="K72" s="40"/>
+      <c r="L72" s="40"/>
+      <c r="M72" s="40"/>
+      <c r="N72" s="40"/>
+      <c r="O72" s="40"/>
+      <c r="P72" s="40"/>
+      <c r="Q72" s="40"/>
+      <c r="R72" s="40"/>
+      <c r="S72" s="40"/>
     </row>
     <row r="73" spans="1:19">
-      <c r="A73" s="40"/>
-      <c r="B73" s="26" t="s">
+      <c r="A73" s="3"/>
+      <c r="B73" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="E73" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="G73" s="40"/>
+      <c r="H73" s="40"/>
+      <c r="I73" s="40"/>
+      <c r="J73" s="40"/>
+      <c r="K73" s="40"/>
+      <c r="L73" s="40"/>
+      <c r="M73" s="40"/>
+      <c r="N73" s="40"/>
+      <c r="O73" s="40"/>
+      <c r="P73" s="40"/>
+      <c r="Q73" s="40"/>
+      <c r="R73" s="40"/>
+      <c r="S73" s="40"/>
+    </row>
+    <row r="74" spans="1:19">
+      <c r="A74" s="3"/>
+      <c r="B74" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="27" t="s">
+      <c r="C74" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D74" s="24"/>
+      <c r="E74" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="F73" s="39"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="41"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="41"/>
-      <c r="L73" s="41"/>
-      <c r="M73" s="41"/>
-      <c r="N73" s="41"/>
-      <c r="O73" s="41"/>
-      <c r="P73" s="41"/>
-      <c r="Q73" s="41"/>
-      <c r="R73" s="41"/>
-      <c r="S73" s="41"/>
-    </row>
-    <row r="74" spans="1:19">
-      <c r="A74" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="B74" s="62" t="s">
+      <c r="F74" s="3"/>
+      <c r="G74" s="40"/>
+      <c r="H74" s="40"/>
+      <c r="I74" s="40"/>
+      <c r="J74" s="40"/>
+      <c r="K74" s="40"/>
+      <c r="L74" s="40"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="40"/>
+      <c r="O74" s="40"/>
+      <c r="P74" s="40"/>
+      <c r="Q74" s="40"/>
+      <c r="R74" s="40"/>
+      <c r="S74" s="40"/>
+    </row>
+    <row r="75" spans="1:19">
+      <c r="A75" s="95"/>
+      <c r="B75" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D75" s="42"/>
+      <c r="E75" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="F75" s="95"/>
+      <c r="G75" s="40"/>
+      <c r="H75" s="40"/>
+      <c r="I75" s="40"/>
+      <c r="J75" s="40"/>
+      <c r="K75" s="40"/>
+      <c r="L75" s="40"/>
+      <c r="M75" s="40"/>
+      <c r="N75" s="40"/>
+      <c r="O75" s="40"/>
+      <c r="P75" s="40"/>
+      <c r="Q75" s="40"/>
+      <c r="R75" s="40"/>
+      <c r="S75" s="40"/>
+    </row>
+    <row r="76" spans="1:19">
+      <c r="A76" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="C74" s="99" t="s">
-        <v>69</v>
-      </c>
-      <c r="D74" s="25"/>
-      <c r="E74" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
-      <c r="Q74" s="4"/>
-      <c r="R74" s="4"/>
-      <c r="S74" s="4"/>
-    </row>
-    <row r="75" spans="1:19">
-      <c r="A75" s="3"/>
-      <c r="B75" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-      <c r="Q75" s="4"/>
-      <c r="R75" s="4"/>
-      <c r="S75" s="4"/>
-    </row>
-    <row r="76" spans="1:19">
-      <c r="A76" s="3"/>
-      <c r="B76" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="D76" s="17"/>
-      <c r="E76" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
+      <c r="D76" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
@@ -13011,21 +13023,23 @@
     </row>
     <row r="77" spans="1:19">
       <c r="A77" s="3"/>
-      <c r="B77" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D77" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E77" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
+      <c r="B77" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
@@ -13041,18 +13055,20 @@
     <row r="78" spans="1:19">
       <c r="A78" s="3"/>
       <c r="B78" s="26" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>74</v>
+        <v>199</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F78" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
@@ -13068,49 +13084,45 @@
       <c r="S78" s="4"/>
     </row>
     <row r="79" spans="1:19">
-      <c r="A79" s="3"/>
+      <c r="A79" s="95"/>
       <c r="B79" s="26" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>22</v>
+        <v>235</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>23</v>
+        <v>235</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
-      <c r="S79" s="4"/>
+        <v>235</v>
+      </c>
+      <c r="F79" s="95"/>
+      <c r="G79" s="40"/>
+      <c r="H79" s="40"/>
+      <c r="I79" s="40"/>
+      <c r="J79" s="40"/>
+      <c r="K79" s="40"/>
+      <c r="L79" s="40"/>
+      <c r="M79" s="40"/>
+      <c r="N79" s="40"/>
+      <c r="O79" s="40"/>
+      <c r="P79" s="40"/>
+      <c r="Q79" s="40"/>
+      <c r="R79" s="40"/>
+      <c r="S79" s="40"/>
     </row>
     <row r="80" spans="1:19">
-      <c r="A80" s="3"/>
-      <c r="B80" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D80" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>78</v>
+      <c r="A80" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B80" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="60" t="s">
+        <v>69</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="4"/>
@@ -13130,16 +13142,12 @@
     <row r="81" spans="1:19">
       <c r="A81" s="3"/>
       <c r="B81" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C81" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>80</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
       <c r="E81" s="27" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="4"/>
@@ -13157,55 +13165,47 @@
       <c r="S81" s="4"/>
     </row>
     <row r="82" spans="1:19">
-      <c r="A82" s="4"/>
-      <c r="B82" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C82" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
-      <c r="Q82" s="4"/>
-      <c r="R82" s="4"/>
-      <c r="S82" s="4"/>
+      <c r="A82" s="39"/>
+      <c r="B82" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" s="17"/>
+      <c r="D82" s="17"/>
+      <c r="E82" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F82" s="38"/>
+      <c r="G82" s="40"/>
+      <c r="H82" s="40"/>
+      <c r="I82" s="40"/>
+      <c r="J82" s="40"/>
+      <c r="K82" s="40"/>
+      <c r="L82" s="40"/>
+      <c r="M82" s="40"/>
+      <c r="N82" s="40"/>
+      <c r="O82" s="40"/>
+      <c r="P82" s="40"/>
+      <c r="Q82" s="40"/>
+      <c r="R82" s="40"/>
+      <c r="S82" s="40"/>
     </row>
     <row r="83" spans="1:19">
-      <c r="A83" s="100" t="s">
-        <v>227</v>
-      </c>
-      <c r="B83" s="62" t="s">
+      <c r="A83" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B83" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" s="25"/>
+      <c r="E83" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="C83" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="D83" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="E83" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="F83" s="7"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
@@ -13219,18 +13219,16 @@
       <c r="S83" s="4"/>
     </row>
     <row r="84" spans="1:19">
-      <c r="A84" s="4"/>
+      <c r="A84" s="3"/>
       <c r="B84" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C84" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>84</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="17"/>
       <c r="E84" s="27" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="4"/>
@@ -13248,20 +13246,20 @@
       <c r="S84" s="4"/>
     </row>
     <row r="85" spans="1:19">
-      <c r="A85" s="4"/>
-      <c r="B85" s="28" t="s">
+      <c r="A85" s="3"/>
+      <c r="B85" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C85" s="37" t="s">
+      <c r="C85" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="D85" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="F85" s="7"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
@@ -13276,37 +13274,50 @@
       <c r="R85" s="4"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" spans="1:19" ht="14.25" thickBot="1">
-      <c r="A86" s="7"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-    </row>
-    <row r="87" spans="1:19" ht="14.25" thickBot="1">
-      <c r="A87" s="7"/>
-      <c r="B87" s="104" t="s">
-        <v>216</v>
-      </c>
-      <c r="C87" s="105"/>
-      <c r="D87" s="105"/>
-      <c r="E87" s="90" t="s">
-        <v>217</v>
-      </c>
+    <row r="86" spans="1:19">
+      <c r="A86" s="95"/>
+      <c r="B86" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D86" s="17"/>
+      <c r="E86" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F86" s="95"/>
+      <c r="G86" s="40"/>
+      <c r="H86" s="40"/>
+      <c r="I86" s="40"/>
+      <c r="J86" s="40"/>
+      <c r="K86" s="40"/>
+      <c r="L86" s="40"/>
+      <c r="M86" s="40"/>
+      <c r="N86" s="40"/>
+      <c r="O86" s="40"/>
+      <c r="P86" s="40"/>
+      <c r="Q86" s="40"/>
+      <c r="R86" s="40"/>
+      <c r="S86" s="40"/>
+    </row>
+    <row r="87" spans="1:19">
+      <c r="A87" s="3"/>
+      <c r="B87" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C87" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
@@ -13319,76 +13330,83 @@
       <c r="R87" s="4"/>
       <c r="S87" s="4"/>
     </row>
-    <row r="88" spans="1:19" ht="14.25" thickBot="1">
-      <c r="A88" s="39"/>
-      <c r="B88" s="94" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="D88" s="95" t="s">
-        <v>192</v>
-      </c>
-      <c r="E88" s="95" t="s">
-        <v>220</v>
-      </c>
-      <c r="I88" s="41"/>
-      <c r="J88" s="41"/>
-      <c r="K88" s="41"/>
-      <c r="L88" s="41"/>
-      <c r="M88" s="41"/>
-      <c r="N88" s="41"/>
-      <c r="O88" s="41"/>
-      <c r="P88" s="41"/>
-      <c r="Q88" s="41"/>
-      <c r="R88" s="41"/>
-      <c r="S88" s="41"/>
+    <row r="88" spans="1:19">
+      <c r="A88" s="3"/>
+      <c r="B88" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
     </row>
     <row r="89" spans="1:19">
-      <c r="A89" s="97" t="s">
-        <v>211</v>
-      </c>
-      <c r="B89" s="87" t="s">
-        <v>198</v>
-      </c>
-      <c r="C89" s="91" t="s">
-        <v>199</v>
-      </c>
-      <c r="D89" s="91" t="s">
-        <v>198</v>
-      </c>
-      <c r="E89" s="91" t="s">
-        <v>199</v>
+      <c r="A89" s="3"/>
+      <c r="B89" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
-      <c r="I89" s="41"/>
-      <c r="J89" s="41"/>
-      <c r="K89" s="41"/>
-      <c r="L89" s="41"/>
-      <c r="M89" s="41"/>
-      <c r="N89" s="41"/>
-      <c r="O89" s="41"/>
-      <c r="P89" s="41"/>
-      <c r="Q89" s="41"/>
-      <c r="R89" s="41"/>
-      <c r="S89" s="41"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
     </row>
     <row r="90" spans="1:19">
-      <c r="A90" s="98" t="s">
-        <v>212</v>
-      </c>
-      <c r="B90" s="88"/>
-      <c r="C90" s="92" t="s">
-        <v>206</v>
-      </c>
-      <c r="D90" s="92"/>
-      <c r="E90" s="92" t="s">
-        <v>214</v>
-      </c>
-      <c r="G90" s="41"/>
-      <c r="H90" s="41"/>
+      <c r="A90" s="3"/>
+      <c r="B90" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D90" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F90" s="7"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
@@ -13402,24 +13420,21 @@
       <c r="S90" s="4"/>
     </row>
     <row r="91" spans="1:19">
-      <c r="A91" s="97" t="s">
-        <v>213</v>
-      </c>
-      <c r="B91" s="88" t="s">
-        <v>200</v>
-      </c>
-      <c r="C91" s="92" t="s">
-        <v>200</v>
-      </c>
-      <c r="D91" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="E91" s="92" t="s">
-        <v>201</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>205</v>
-      </c>
+      <c r="A91" s="3"/>
+      <c r="B91" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
@@ -13433,21 +13448,25 @@
       <c r="R91" s="4"/>
       <c r="S91" s="4"/>
     </row>
-    <row r="92" spans="1:19" ht="14.25" thickBot="1">
-      <c r="A92" s="97" t="s">
-        <v>215</v>
-      </c>
-      <c r="B92" s="89"/>
-      <c r="C92" s="96"/>
-      <c r="D92" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="E92" s="93" t="s">
-        <v>209</v>
-      </c>
-      <c r="G92" s="86" t="s">
-        <v>210</v>
-      </c>
+    <row r="92" spans="1:19">
+      <c r="A92" s="4"/>
+      <c r="B92" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
@@ -13461,11 +13480,21 @@
       <c r="S92" s="4"/>
     </row>
     <row r="93" spans="1:19">
-      <c r="A93" s="4"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
+      <c r="A93" s="93" t="s">
+        <v>227</v>
+      </c>
+      <c r="B93" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="D93" s="103" t="s">
+        <v>78</v>
+      </c>
+      <c r="E93" s="104" t="s">
+        <v>78</v>
+      </c>
       <c r="F93" s="7"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -13483,10 +13512,18 @@
     </row>
     <row r="94" spans="1:19">
       <c r="A94" s="4"/>
-      <c r="B94" s="18"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
+      <c r="B94" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E94" s="43" t="s">
+        <v>84</v>
+      </c>
       <c r="F94" s="7"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -13504,14 +13541,18 @@
     </row>
     <row r="95" spans="1:19">
       <c r="A95" s="4"/>
-      <c r="B95" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="C95" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
+      <c r="B95" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D95" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="E95" s="43" t="s">
+        <v>201</v>
+      </c>
       <c r="F95" s="7"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
@@ -13528,38 +13569,34 @@
       <c r="S95" s="4"/>
     </row>
     <row r="96" spans="1:19">
-      <c r="A96" s="4"/>
-      <c r="B96" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="C96" s="55" t="s">
-        <v>232</v>
-      </c>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
-      <c r="K96" s="4"/>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
-      <c r="N96" s="4"/>
-      <c r="O96" s="4"/>
-      <c r="P96" s="4"/>
-      <c r="Q96" s="4"/>
-      <c r="R96" s="4"/>
-      <c r="S96" s="4"/>
-    </row>
-    <row r="97" spans="1:19">
-      <c r="A97" s="4"/>
-      <c r="B97" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>231</v>
-      </c>
+      <c r="A96" s="40"/>
+      <c r="B96" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D96" s="42"/>
+      <c r="E96" s="48"/>
+      <c r="F96" s="94"/>
+      <c r="G96" s="40"/>
+      <c r="H96" s="40"/>
+      <c r="I96" s="40"/>
+      <c r="J96" s="40"/>
+      <c r="K96" s="40"/>
+      <c r="L96" s="40"/>
+      <c r="M96" s="40"/>
+      <c r="N96" s="40"/>
+      <c r="O96" s="40"/>
+      <c r="P96" s="40"/>
+      <c r="Q96" s="40"/>
+      <c r="R96" s="40"/>
+      <c r="S96" s="40"/>
+    </row>
+    <row r="97" spans="1:19" ht="14.25" thickBot="1">
+      <c r="A97" s="7"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
       <c r="F97" s="7"/>
@@ -13577,19 +13614,16 @@
       <c r="R97" s="4"/>
       <c r="S97" s="4"/>
     </row>
-    <row r="98" spans="1:19">
-      <c r="A98" s="4"/>
-      <c r="B98" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C98" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+    <row r="98" spans="1:19" ht="14.25" thickBot="1">
+      <c r="A98" s="7"/>
+      <c r="B98" s="99" t="s">
+        <v>216</v>
+      </c>
+      <c r="C98" s="100"/>
+      <c r="D98" s="100"/>
+      <c r="E98" s="83" t="s">
+        <v>217</v>
+      </c>
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
@@ -13602,65 +13636,76 @@
       <c r="R98" s="4"/>
       <c r="S98" s="4"/>
     </row>
-    <row r="99" spans="1:19">
-      <c r="A99" s="4"/>
-      <c r="B99" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="4"/>
+    <row r="99" spans="1:19" ht="14.25" thickBot="1">
+      <c r="A99" s="38"/>
+      <c r="B99" s="87" t="s">
+        <v>218</v>
+      </c>
+      <c r="C99" s="88" t="s">
+        <v>219</v>
+      </c>
+      <c r="D99" s="88" t="s">
+        <v>192</v>
+      </c>
+      <c r="E99" s="88" t="s">
+        <v>220</v>
+      </c>
+      <c r="I99" s="40"/>
+      <c r="J99" s="40"/>
+      <c r="K99" s="40"/>
+      <c r="L99" s="40"/>
+      <c r="M99" s="40"/>
+      <c r="N99" s="40"/>
+      <c r="O99" s="40"/>
+      <c r="P99" s="40"/>
+      <c r="Q99" s="40"/>
+      <c r="R99" s="40"/>
+      <c r="S99" s="40"/>
     </row>
     <row r="100" spans="1:19">
-      <c r="A100" s="4"/>
-      <c r="B100" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="C100" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="D100" s="18"/>
-      <c r="E100" s="18"/>
-      <c r="F100" s="7"/>
+      <c r="A100" s="90" t="s">
+        <v>211</v>
+      </c>
+      <c r="B100" s="80" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" s="84" t="s">
+        <v>199</v>
+      </c>
+      <c r="D100" s="84" t="s">
+        <v>198</v>
+      </c>
+      <c r="E100" s="84" t="s">
+        <v>199</v>
+      </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
-      <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
-      <c r="K100" s="4"/>
-      <c r="L100" s="4"/>
-      <c r="M100" s="4"/>
-      <c r="N100" s="4"/>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
-      <c r="Q100" s="4"/>
-      <c r="R100" s="4"/>
-      <c r="S100" s="4"/>
+      <c r="I100" s="40"/>
+      <c r="J100" s="40"/>
+      <c r="K100" s="40"/>
+      <c r="L100" s="40"/>
+      <c r="M100" s="40"/>
+      <c r="N100" s="40"/>
+      <c r="O100" s="40"/>
+      <c r="P100" s="40"/>
+      <c r="Q100" s="40"/>
+      <c r="R100" s="40"/>
+      <c r="S100" s="40"/>
     </row>
     <row r="101" spans="1:19">
-      <c r="A101" s="4"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
-      <c r="E101" s="18"/>
-      <c r="F101" s="7"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
+      <c r="A101" s="91" t="s">
+        <v>212</v>
+      </c>
+      <c r="B101" s="81"/>
+      <c r="C101" s="85" t="s">
+        <v>206</v>
+      </c>
+      <c r="D101" s="85"/>
+      <c r="E101" s="85" t="s">
+        <v>214</v>
+      </c>
+      <c r="G101" s="40"/>
+      <c r="H101" s="40"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
@@ -13674,13 +13719,24 @@
       <c r="S101" s="4"/>
     </row>
     <row r="102" spans="1:19">
-      <c r="A102" s="4"/>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="4"/>
+      <c r="A102" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="B102" s="81" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" s="85" t="s">
+        <v>200</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E102" s="85" t="s">
+        <v>201</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
@@ -13694,15 +13750,21 @@
       <c r="R102" s="4"/>
       <c r="S102" s="4"/>
     </row>
-    <row r="103" spans="1:19">
-      <c r="A103" s="4"/>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
+    <row r="103" spans="1:19" ht="14.25" thickBot="1">
+      <c r="A103" s="90" t="s">
+        <v>215</v>
+      </c>
+      <c r="B103" s="82"/>
+      <c r="C103" s="89"/>
+      <c r="D103" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E103" s="86" t="s">
+        <v>209</v>
+      </c>
+      <c r="G103" s="79" t="s">
+        <v>210</v>
+      </c>
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
@@ -13759,8 +13821,12 @@
     </row>
     <row r="106" spans="1:19">
       <c r="A106" s="4"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
+      <c r="B106" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>229</v>
+      </c>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
       <c r="F106" s="7"/>
@@ -13780,8 +13846,12 @@
     </row>
     <row r="107" spans="1:19">
       <c r="A107" s="4"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="18"/>
+      <c r="B107" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" s="52" t="s">
+        <v>232</v>
+      </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
       <c r="F107" s="7"/>
@@ -13801,8 +13871,12 @@
     </row>
     <row r="108" spans="1:19">
       <c r="A108" s="4"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="18"/>
+      <c r="B108" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>231</v>
+      </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
       <c r="F108" s="7"/>
@@ -13822,8 +13896,12 @@
     </row>
     <row r="109" spans="1:19">
       <c r="A109" s="4"/>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
+      <c r="B109" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>233</v>
+      </c>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
       <c r="F109" s="7"/>
@@ -13843,8 +13921,12 @@
     </row>
     <row r="110" spans="1:19">
       <c r="A110" s="4"/>
-      <c r="B110" s="18"/>
-      <c r="C110" s="18"/>
+      <c r="B110" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>234</v>
+      </c>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
       <c r="F110" s="7"/>
@@ -13864,8 +13946,12 @@
     </row>
     <row r="111" spans="1:19">
       <c r="A111" s="4"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="18"/>
+      <c r="B111" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>231</v>
+      </c>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
       <c r="F111" s="7"/>
@@ -16657,6 +16743,12 @@
     </row>
     <row r="244" spans="1:19">
       <c r="A244" s="4"/>
+      <c r="B244" s="18"/>
+      <c r="C244" s="18"/>
+      <c r="D244" s="18"/>
+      <c r="E244" s="18"/>
+      <c r="F244" s="7"/>
+      <c r="G244" s="4"/>
       <c r="H244" s="4"/>
       <c r="I244" s="4"/>
       <c r="J244" s="4"/>
@@ -16672,6 +16764,12 @@
     </row>
     <row r="245" spans="1:19">
       <c r="A245" s="4"/>
+      <c r="B245" s="18"/>
+      <c r="C245" s="18"/>
+      <c r="D245" s="18"/>
+      <c r="E245" s="18"/>
+      <c r="F245" s="7"/>
+      <c r="G245" s="4"/>
       <c r="H245" s="4"/>
       <c r="I245" s="4"/>
       <c r="J245" s="4"/>
@@ -16687,6 +16785,12 @@
     </row>
     <row r="246" spans="1:19">
       <c r="A246" s="4"/>
+      <c r="B246" s="18"/>
+      <c r="C246" s="18"/>
+      <c r="D246" s="18"/>
+      <c r="E246" s="18"/>
+      <c r="F246" s="7"/>
+      <c r="G246" s="4"/>
       <c r="H246" s="4"/>
       <c r="I246" s="4"/>
       <c r="J246" s="4"/>
@@ -16702,6 +16806,12 @@
     </row>
     <row r="247" spans="1:19">
       <c r="A247" s="4"/>
+      <c r="B247" s="18"/>
+      <c r="C247" s="18"/>
+      <c r="D247" s="18"/>
+      <c r="E247" s="18"/>
+      <c r="F247" s="7"/>
+      <c r="G247" s="4"/>
       <c r="H247" s="4"/>
       <c r="I247" s="4"/>
       <c r="J247" s="4"/>
@@ -16717,6 +16827,12 @@
     </row>
     <row r="248" spans="1:19">
       <c r="A248" s="4"/>
+      <c r="B248" s="18"/>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="18"/>
+      <c r="F248" s="7"/>
+      <c r="G248" s="4"/>
       <c r="H248" s="4"/>
       <c r="I248" s="4"/>
       <c r="J248" s="4"/>
@@ -16732,6 +16848,12 @@
     </row>
     <row r="249" spans="1:19">
       <c r="A249" s="4"/>
+      <c r="B249" s="18"/>
+      <c r="C249" s="18"/>
+      <c r="D249" s="18"/>
+      <c r="E249" s="18"/>
+      <c r="F249" s="7"/>
+      <c r="G249" s="4"/>
       <c r="H249" s="4"/>
       <c r="I249" s="4"/>
       <c r="J249" s="4"/>
@@ -16747,6 +16869,12 @@
     </row>
     <row r="250" spans="1:19">
       <c r="A250" s="4"/>
+      <c r="B250" s="18"/>
+      <c r="C250" s="18"/>
+      <c r="D250" s="18"/>
+      <c r="E250" s="18"/>
+      <c r="F250" s="7"/>
+      <c r="G250" s="4"/>
       <c r="H250" s="4"/>
       <c r="I250" s="4"/>
       <c r="J250" s="4"/>
@@ -16762,6 +16890,12 @@
     </row>
     <row r="251" spans="1:19">
       <c r="A251" s="4"/>
+      <c r="B251" s="18"/>
+      <c r="C251" s="18"/>
+      <c r="D251" s="18"/>
+      <c r="E251" s="18"/>
+      <c r="F251" s="7"/>
+      <c r="G251" s="4"/>
       <c r="H251" s="4"/>
       <c r="I251" s="4"/>
       <c r="J251" s="4"/>
@@ -16777,6 +16911,12 @@
     </row>
     <row r="252" spans="1:19">
       <c r="A252" s="4"/>
+      <c r="B252" s="18"/>
+      <c r="C252" s="18"/>
+      <c r="D252" s="18"/>
+      <c r="E252" s="18"/>
+      <c r="F252" s="7"/>
+      <c r="G252" s="4"/>
       <c r="H252" s="4"/>
       <c r="I252" s="4"/>
       <c r="J252" s="4"/>
@@ -16792,6 +16932,12 @@
     </row>
     <row r="253" spans="1:19">
       <c r="A253" s="4"/>
+      <c r="B253" s="18"/>
+      <c r="C253" s="18"/>
+      <c r="D253" s="18"/>
+      <c r="E253" s="18"/>
+      <c r="F253" s="7"/>
+      <c r="G253" s="4"/>
       <c r="H253" s="4"/>
       <c r="I253" s="4"/>
       <c r="J253" s="4"/>
@@ -16807,6 +16953,12 @@
     </row>
     <row r="254" spans="1:19">
       <c r="A254" s="4"/>
+      <c r="B254" s="18"/>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
+      <c r="E254" s="18"/>
+      <c r="F254" s="7"/>
+      <c r="G254" s="4"/>
       <c r="H254" s="4"/>
       <c r="I254" s="4"/>
       <c r="J254" s="4"/>
@@ -16955,9 +17107,174 @@
       <c r="R263" s="4"/>
       <c r="S263" s="4"/>
     </row>
+    <row r="264" spans="1:19">
+      <c r="A264" s="4"/>
+      <c r="H264" s="4"/>
+      <c r="I264" s="4"/>
+      <c r="J264" s="4"/>
+      <c r="K264" s="4"/>
+      <c r="L264" s="4"/>
+      <c r="M264" s="4"/>
+      <c r="N264" s="4"/>
+      <c r="O264" s="4"/>
+      <c r="P264" s="4"/>
+      <c r="Q264" s="4"/>
+      <c r="R264" s="4"/>
+      <c r="S264" s="4"/>
+    </row>
+    <row r="265" spans="1:19">
+      <c r="A265" s="4"/>
+      <c r="H265" s="4"/>
+      <c r="I265" s="4"/>
+      <c r="J265" s="4"/>
+      <c r="K265" s="4"/>
+      <c r="L265" s="4"/>
+      <c r="M265" s="4"/>
+      <c r="N265" s="4"/>
+      <c r="O265" s="4"/>
+      <c r="P265" s="4"/>
+      <c r="Q265" s="4"/>
+      <c r="R265" s="4"/>
+      <c r="S265" s="4"/>
+    </row>
+    <row r="266" spans="1:19">
+      <c r="A266" s="4"/>
+      <c r="H266" s="4"/>
+      <c r="I266" s="4"/>
+      <c r="J266" s="4"/>
+      <c r="K266" s="4"/>
+      <c r="L266" s="4"/>
+      <c r="M266" s="4"/>
+      <c r="N266" s="4"/>
+      <c r="O266" s="4"/>
+      <c r="P266" s="4"/>
+      <c r="Q266" s="4"/>
+      <c r="R266" s="4"/>
+      <c r="S266" s="4"/>
+    </row>
+    <row r="267" spans="1:19">
+      <c r="A267" s="4"/>
+      <c r="H267" s="4"/>
+      <c r="I267" s="4"/>
+      <c r="J267" s="4"/>
+      <c r="K267" s="4"/>
+      <c r="L267" s="4"/>
+      <c r="M267" s="4"/>
+      <c r="N267" s="4"/>
+      <c r="O267" s="4"/>
+      <c r="P267" s="4"/>
+      <c r="Q267" s="4"/>
+      <c r="R267" s="4"/>
+      <c r="S267" s="4"/>
+    </row>
+    <row r="268" spans="1:19">
+      <c r="A268" s="4"/>
+      <c r="H268" s="4"/>
+      <c r="I268" s="4"/>
+      <c r="J268" s="4"/>
+      <c r="K268" s="4"/>
+      <c r="L268" s="4"/>
+      <c r="M268" s="4"/>
+      <c r="N268" s="4"/>
+      <c r="O268" s="4"/>
+      <c r="P268" s="4"/>
+      <c r="Q268" s="4"/>
+      <c r="R268" s="4"/>
+      <c r="S268" s="4"/>
+    </row>
+    <row r="269" spans="1:19">
+      <c r="A269" s="4"/>
+      <c r="H269" s="4"/>
+      <c r="I269" s="4"/>
+      <c r="J269" s="4"/>
+      <c r="K269" s="4"/>
+      <c r="L269" s="4"/>
+      <c r="M269" s="4"/>
+      <c r="N269" s="4"/>
+      <c r="O269" s="4"/>
+      <c r="P269" s="4"/>
+      <c r="Q269" s="4"/>
+      <c r="R269" s="4"/>
+      <c r="S269" s="4"/>
+    </row>
+    <row r="270" spans="1:19">
+      <c r="A270" s="4"/>
+      <c r="H270" s="4"/>
+      <c r="I270" s="4"/>
+      <c r="J270" s="4"/>
+      <c r="K270" s="4"/>
+      <c r="L270" s="4"/>
+      <c r="M270" s="4"/>
+      <c r="N270" s="4"/>
+      <c r="O270" s="4"/>
+      <c r="P270" s="4"/>
+      <c r="Q270" s="4"/>
+      <c r="R270" s="4"/>
+      <c r="S270" s="4"/>
+    </row>
+    <row r="271" spans="1:19">
+      <c r="A271" s="4"/>
+      <c r="H271" s="4"/>
+      <c r="I271" s="4"/>
+      <c r="J271" s="4"/>
+      <c r="K271" s="4"/>
+      <c r="L271" s="4"/>
+      <c r="M271" s="4"/>
+      <c r="N271" s="4"/>
+      <c r="O271" s="4"/>
+      <c r="P271" s="4"/>
+      <c r="Q271" s="4"/>
+      <c r="R271" s="4"/>
+      <c r="S271" s="4"/>
+    </row>
+    <row r="272" spans="1:19">
+      <c r="A272" s="4"/>
+      <c r="H272" s="4"/>
+      <c r="I272" s="4"/>
+      <c r="J272" s="4"/>
+      <c r="K272" s="4"/>
+      <c r="L272" s="4"/>
+      <c r="M272" s="4"/>
+      <c r="N272" s="4"/>
+      <c r="O272" s="4"/>
+      <c r="P272" s="4"/>
+      <c r="Q272" s="4"/>
+      <c r="R272" s="4"/>
+      <c r="S272" s="4"/>
+    </row>
+    <row r="273" spans="1:19">
+      <c r="A273" s="4"/>
+      <c r="H273" s="4"/>
+      <c r="I273" s="4"/>
+      <c r="J273" s="4"/>
+      <c r="K273" s="4"/>
+      <c r="L273" s="4"/>
+      <c r="M273" s="4"/>
+      <c r="N273" s="4"/>
+      <c r="O273" s="4"/>
+      <c r="P273" s="4"/>
+      <c r="Q273" s="4"/>
+      <c r="R273" s="4"/>
+      <c r="S273" s="4"/>
+    </row>
+    <row r="274" spans="1:19">
+      <c r="A274" s="4"/>
+      <c r="H274" s="4"/>
+      <c r="I274" s="4"/>
+      <c r="J274" s="4"/>
+      <c r="K274" s="4"/>
+      <c r="L274" s="4"/>
+      <c r="M274" s="4"/>
+      <c r="N274" s="4"/>
+      <c r="O274" s="4"/>
+      <c r="P274" s="4"/>
+      <c r="Q274" s="4"/>
+      <c r="R274" s="4"/>
+      <c r="S274" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B98:D98"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
220502-v2 OK to start sim, not verified
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FA6851-F11F-4B93-8A2C-C70A21871092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5E2EE-4D40-48E5-943A-14C0F783B5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="5970" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -1659,21 +1659,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1699,6 +1684,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2648,10 +2648,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="97"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -3431,12 +3431,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="98" t="s">
+      <c r="A22" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="97"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -11028,8 +11028,8 @@
   <dimension ref="A1:S274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12090,10 +12090,10 @@
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="4"/>
-      <c r="B42" s="105" t="s">
+      <c r="B42" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="102" t="s">
+      <c r="C42" s="97" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="41"/>
@@ -12198,10 +12198,10 @@
     </row>
     <row r="46" spans="1:19">
       <c r="A46" s="4"/>
-      <c r="B46" s="101" t="s">
+      <c r="B46" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="102" t="s">
+      <c r="C46" s="97" t="s">
         <v>49</v>
       </c>
       <c r="D46" s="41"/>
@@ -12306,16 +12306,16 @@
     </row>
     <row r="50" spans="1:19">
       <c r="A50" s="4"/>
-      <c r="B50" s="101" t="s">
+      <c r="B50" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="106" t="s">
+      <c r="C50" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="102" t="s">
+      <c r="D50" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="104" t="s">
+      <c r="E50" s="99" t="s">
         <v>188</v>
       </c>
       <c r="F50" s="3"/>
@@ -12633,14 +12633,14 @@
       <c r="A63" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B63" s="105" t="s">
+      <c r="B63" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="107" t="s">
+      <c r="C63" s="102" t="s">
         <v>207</v>
       </c>
       <c r="D63" s="41"/>
-      <c r="E63" s="108" t="s">
+      <c r="E63" s="103" t="s">
         <v>185</v>
       </c>
       <c r="F63" s="38"/>
@@ -12667,7 +12667,7 @@
         <v>208</v>
       </c>
       <c r="D64" s="24"/>
-      <c r="E64" s="109" t="s">
+      <c r="E64" s="104" t="s">
         <v>186</v>
       </c>
       <c r="F64" s="38"/>
@@ -12882,7 +12882,7 @@
     </row>
     <row r="72" spans="1:19">
       <c r="A72" s="3"/>
-      <c r="B72" s="101" t="s">
+      <c r="B72" s="96" t="s">
         <v>185</v>
       </c>
       <c r="C72" s="77" t="s">
@@ -13483,16 +13483,16 @@
       <c r="A93" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="B93" s="101" t="s">
+      <c r="B93" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="C93" s="102" t="s">
+      <c r="C93" s="97" t="s">
         <v>77</v>
       </c>
-      <c r="D93" s="103" t="s">
+      <c r="D93" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="E93" s="104" t="s">
+      <c r="E93" s="99" t="s">
         <v>78</v>
       </c>
       <c r="F93" s="7"/>
@@ -13616,11 +13616,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="99" t="s">
+      <c r="B98" s="108" t="s">
         <v>216</v>
       </c>
-      <c r="C98" s="100"/>
-      <c r="D98" s="100"/>
+      <c r="C98" s="109"/>
+      <c r="D98" s="109"/>
       <c r="E98" s="83" t="s">
         <v>217</v>
       </c>

</xml_diff>

<commit_message>
220503-v5 simed dataflow OK!
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABDF411-D015-4D51-A05F-5616CC06FDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98F9985-CA55-4BF5-BC7F-5A8DB8485BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1042" yWindow="1042" windowWidth="16200" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="487">
   <si>
     <t>步骤</t>
   </si>
@@ -2825,30 +2825,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2910,6 +2886,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3859,10 +3859,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="153" t="s">
+      <c r="A5" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="154"/>
+      <c r="B5" s="175"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4642,12 +4642,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="155" t="s">
+      <c r="A22" s="176" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="154"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="154"/>
+      <c r="B22" s="175"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="175"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -12238,7 +12238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S274"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
@@ -12612,7 +12612,7 @@
       <c r="B16" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="180" t="s">
+      <c r="C16" s="172" t="s">
         <v>486</v>
       </c>
       <c r="D16" s="19"/>
@@ -12726,7 +12726,7 @@
       <c r="D20" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="E20" s="180" t="s">
+      <c r="E20" s="172" t="s">
         <v>486</v>
       </c>
       <c r="F20" s="3"/>
@@ -13086,7 +13086,7 @@
       <c r="B34" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="180" t="s">
+      <c r="C34" s="172" t="s">
         <v>486</v>
       </c>
       <c r="D34" s="25"/>
@@ -13927,7 +13927,7 @@
       <c r="A66" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B66" s="181" t="s">
+      <c r="B66" s="173" t="s">
         <v>486</v>
       </c>
       <c r="C66" s="75" t="s">
@@ -14827,11 +14827,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="156" t="s">
+      <c r="B98" s="177" t="s">
         <v>212</v>
       </c>
-      <c r="C98" s="157"/>
-      <c r="D98" s="157"/>
+      <c r="C98" s="178"/>
+      <c r="D98" s="178"/>
       <c r="E98" s="81" t="s">
         <v>213</v>
       </c>
@@ -18546,11 +18546,11 @@
       <c r="B4" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="178" t="s">
+      <c r="C4" s="170" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="179" t="s">
+      <c r="D4" s="170"/>
+      <c r="E4" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18582,11 +18582,11 @@
       <c r="B7" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="178" t="s">
+      <c r="C7" s="170" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="178"/>
-      <c r="E7" s="179" t="s">
+      <c r="D7" s="170"/>
+      <c r="E7" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18618,11 +18618,11 @@
       <c r="B10" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="178" t="s">
+      <c r="C10" s="170" t="s">
         <v>196</v>
       </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="179" t="s">
+      <c r="D10" s="170"/>
+      <c r="E10" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18654,11 +18654,11 @@
       <c r="B13" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C13" s="178" t="s">
+      <c r="C13" s="170" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="124"/>
-      <c r="E13" s="179" t="s">
+      <c r="E13" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18694,13 +18694,13 @@
       <c r="B16" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="178" t="s">
+      <c r="C16" s="170" t="s">
         <v>195</v>
       </c>
       <c r="D16" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="E16" s="179" t="s">
+      <c r="E16" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18736,13 +18736,13 @@
       <c r="B19" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="170" t="s">
         <v>195</v>
       </c>
       <c r="D19" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="179" t="s">
+      <c r="E19" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -18785,13 +18785,13 @@
       <c r="B22" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="C22" s="178" t="s">
+      <c r="C22" s="170" t="s">
         <v>195</v>
       </c>
       <c r="D22" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="E22" s="179" t="s">
+      <c r="E22" s="171" t="s">
         <v>195</v>
       </c>
     </row>
@@ -19254,67 +19254,67 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="158" t="s">
+      <c r="B6" s="179" t="s">
         <v>310</v>
       </c>
-      <c r="C6" s="159"/>
-      <c r="D6" s="160"/>
-      <c r="E6" s="158" t="s">
+      <c r="C6" s="180"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="179" t="s">
         <v>311</v>
       </c>
-      <c r="F6" s="159"/>
-      <c r="G6" s="160"/>
+      <c r="F6" s="180"/>
+      <c r="G6" s="181"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="179" t="s">
         <v>312</v>
       </c>
-      <c r="C7" s="159"/>
-      <c r="D7" s="159"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="159"/>
-      <c r="L7" s="159"/>
-      <c r="M7" s="159"/>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
-      <c r="P7" s="160"/>
-      <c r="Q7" s="158" t="s">
+      <c r="C7" s="180"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="180"/>
+      <c r="F7" s="180"/>
+      <c r="G7" s="180"/>
+      <c r="H7" s="180"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="180"/>
+      <c r="K7" s="180"/>
+      <c r="L7" s="180"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="180"/>
+      <c r="O7" s="180"/>
+      <c r="P7" s="181"/>
+      <c r="Q7" s="179" t="s">
         <v>313</v>
       </c>
-      <c r="R7" s="159"/>
-      <c r="S7" s="159"/>
-      <c r="T7" s="159"/>
-      <c r="U7" s="159"/>
-      <c r="V7" s="159"/>
-      <c r="W7" s="159"/>
-      <c r="X7" s="159"/>
-      <c r="Y7" s="159"/>
-      <c r="Z7" s="159"/>
-      <c r="AA7" s="160"/>
-      <c r="AB7" s="158" t="s">
+      <c r="R7" s="180"/>
+      <c r="S7" s="180"/>
+      <c r="T7" s="180"/>
+      <c r="U7" s="180"/>
+      <c r="V7" s="180"/>
+      <c r="W7" s="180"/>
+      <c r="X7" s="180"/>
+      <c r="Y7" s="180"/>
+      <c r="Z7" s="180"/>
+      <c r="AA7" s="181"/>
+      <c r="AB7" s="179" t="s">
         <v>314</v>
       </c>
-      <c r="AC7" s="159"/>
-      <c r="AD7" s="159"/>
-      <c r="AE7" s="159"/>
-      <c r="AF7" s="159"/>
-      <c r="AG7" s="159"/>
-      <c r="AH7" s="159"/>
-      <c r="AI7" s="159"/>
-      <c r="AJ7" s="159"/>
-      <c r="AK7" s="159"/>
-      <c r="AL7" s="159"/>
-      <c r="AM7" s="159"/>
-      <c r="AN7" s="159"/>
-      <c r="AO7" s="159"/>
-      <c r="AP7" s="159"/>
-      <c r="AQ7" s="159"/>
-      <c r="AR7" s="160"/>
+      <c r="AC7" s="180"/>
+      <c r="AD7" s="180"/>
+      <c r="AE7" s="180"/>
+      <c r="AF7" s="180"/>
+      <c r="AG7" s="180"/>
+      <c r="AH7" s="180"/>
+      <c r="AI7" s="180"/>
+      <c r="AJ7" s="180"/>
+      <c r="AK7" s="180"/>
+      <c r="AL7" s="180"/>
+      <c r="AM7" s="180"/>
+      <c r="AN7" s="180"/>
+      <c r="AO7" s="180"/>
+      <c r="AP7" s="180"/>
+      <c r="AQ7" s="180"/>
+      <c r="AR7" s="181"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="52"/>
@@ -21178,10 +21178,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -21189,7 +21189,7 @@
     <col min="1" max="16384" width="9.06640625" style="152"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" thickBot="1">
+    <row r="1" spans="1:10" ht="14.25" thickBot="1">
       <c r="A1" s="152" t="s">
         <v>459</v>
       </c>
@@ -21205,214 +21205,362 @@
       <c r="E1" s="152" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="152" t="s">
+        <v>460</v>
+      </c>
+      <c r="H1" s="152" t="s">
+        <v>461</v>
+      </c>
+      <c r="I1" s="152" t="s">
+        <v>462</v>
+      </c>
+      <c r="J1" s="152" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="152">
         <v>0</v>
       </c>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="153" t="s">
         <v>319</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="154" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="162" t="s">
+      <c r="D2" s="154" t="s">
         <v>324</v>
       </c>
-      <c r="E2" s="163"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="155"/>
+      <c r="G2" s="153">
+        <v>0</v>
+      </c>
+      <c r="H2" s="154">
+        <v>0</v>
+      </c>
+      <c r="I2" s="154">
+        <v>0</v>
+      </c>
+      <c r="J2" s="155"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="152">
         <v>1</v>
       </c>
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="156" t="s">
         <v>320</v>
       </c>
-      <c r="C3" s="165" t="s">
+      <c r="C3" s="157" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="165" t="s">
+      <c r="D3" s="157" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="166"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="158"/>
+      <c r="G3" s="156">
+        <v>1</v>
+      </c>
+      <c r="H3" s="157">
+        <v>0</v>
+      </c>
+      <c r="I3" s="157">
+        <v>0</v>
+      </c>
+      <c r="J3" s="158"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="152">
         <v>2</v>
       </c>
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="159" t="s">
         <v>464</v>
       </c>
-      <c r="C4" s="165" t="s">
+      <c r="C4" s="157" t="s">
         <v>398</v>
       </c>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="157" t="s">
         <v>399</v>
       </c>
-      <c r="E4" s="168"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.25" thickBot="1">
+      <c r="E4" s="160"/>
+      <c r="G4" s="159">
+        <v>0</v>
+      </c>
+      <c r="H4" s="157">
+        <v>1</v>
+      </c>
+      <c r="I4" s="157">
+        <v>0</v>
+      </c>
+      <c r="J4" s="160"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.25" thickBot="1">
       <c r="A5" s="152">
         <v>3</v>
       </c>
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="161" t="s">
         <v>465</v>
       </c>
-      <c r="C5" s="170" t="s">
+      <c r="C5" s="162" t="s">
         <v>466</v>
       </c>
-      <c r="D5" s="170" t="s">
+      <c r="D5" s="162" t="s">
         <v>400</v>
       </c>
-      <c r="E5" s="171"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="163"/>
+      <c r="G5" s="161">
+        <v>0</v>
+      </c>
+      <c r="H5" s="162">
+        <v>0</v>
+      </c>
+      <c r="I5" s="162">
+        <v>1</v>
+      </c>
+      <c r="J5" s="163"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="152">
         <v>4</v>
       </c>
-      <c r="B6" s="161" t="s">
+      <c r="B6" s="153" t="s">
         <v>467</v>
       </c>
-      <c r="C6" s="162" t="s">
+      <c r="C6" s="154" t="s">
         <v>474</v>
       </c>
-      <c r="D6" s="162" t="s">
+      <c r="D6" s="154" t="s">
         <v>475</v>
       </c>
-      <c r="E6" s="172" t="s">
+      <c r="E6" s="164" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="153">
+        <v>0</v>
+      </c>
+      <c r="H6" s="153">
+        <v>0</v>
+      </c>
+      <c r="I6" s="153">
+        <v>0</v>
+      </c>
+      <c r="J6" s="153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="152">
         <v>5</v>
       </c>
-      <c r="B7" s="164" t="s">
+      <c r="B7" s="156" t="s">
         <v>329</v>
       </c>
-      <c r="C7" s="165" t="s">
+      <c r="C7" s="157" t="s">
         <v>334</v>
       </c>
-      <c r="D7" s="165" t="s">
+      <c r="D7" s="157" t="s">
         <v>340</v>
       </c>
-      <c r="E7" s="173" t="s">
+      <c r="E7" s="165" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="156">
+        <v>1</v>
+      </c>
+      <c r="H7" s="156">
+        <v>1</v>
+      </c>
+      <c r="I7" s="156">
+        <v>1</v>
+      </c>
+      <c r="J7" s="156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="152">
         <v>6</v>
       </c>
-      <c r="B8" s="167" t="s">
+      <c r="B8" s="159" t="s">
         <v>468</v>
       </c>
-      <c r="C8" s="165" t="s">
+      <c r="C8" s="157" t="s">
         <v>470</v>
       </c>
-      <c r="D8" s="165" t="s">
+      <c r="D8" s="157" t="s">
         <v>472</v>
       </c>
-      <c r="E8" s="173" t="s">
+      <c r="E8" s="165" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="159">
+        <v>2</v>
+      </c>
+      <c r="H8" s="159">
+        <v>2</v>
+      </c>
+      <c r="I8" s="159">
+        <v>2</v>
+      </c>
+      <c r="J8" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.25" thickBot="1">
       <c r="A9" s="152">
         <v>7</v>
       </c>
-      <c r="B9" s="175" t="s">
+      <c r="B9" s="167" t="s">
         <v>469</v>
       </c>
-      <c r="C9" s="176" t="s">
+      <c r="C9" s="168" t="s">
         <v>471</v>
       </c>
-      <c r="D9" s="176" t="s">
+      <c r="D9" s="168" t="s">
         <v>473</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="169" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="167">
+        <v>3</v>
+      </c>
+      <c r="H9" s="167">
+        <v>3</v>
+      </c>
+      <c r="I9" s="167">
+        <v>3</v>
+      </c>
+      <c r="J9" s="167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="152">
         <v>8</v>
       </c>
-      <c r="B10" s="164" t="s">
+      <c r="B10" s="156" t="s">
         <v>332</v>
       </c>
-      <c r="C10" s="165" t="s">
+      <c r="C10" s="157" t="s">
         <v>337</v>
       </c>
-      <c r="D10" s="165" t="s">
+      <c r="D10" s="157" t="s">
         <v>343</v>
       </c>
-      <c r="E10" s="173" t="s">
+      <c r="E10" s="165" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="153">
+        <v>4</v>
+      </c>
+      <c r="H10" s="153">
+        <v>4</v>
+      </c>
+      <c r="I10" s="153">
+        <v>4</v>
+      </c>
+      <c r="J10" s="153">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="152">
         <v>9</v>
       </c>
-      <c r="B11" s="167" t="s">
+      <c r="B11" s="159" t="s">
         <v>477</v>
       </c>
-      <c r="C11" s="165" t="s">
+      <c r="C11" s="157" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="165" t="s">
+      <c r="D11" s="157" t="s">
         <v>344</v>
       </c>
-      <c r="E11" s="173" t="s">
+      <c r="E11" s="165" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="156">
+        <v>5</v>
+      </c>
+      <c r="H11" s="156">
+        <v>5</v>
+      </c>
+      <c r="I11" s="156">
+        <v>5</v>
+      </c>
+      <c r="J11" s="156">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="152">
         <v>10</v>
       </c>
-      <c r="B12" s="164" t="s">
+      <c r="B12" s="156" t="s">
         <v>478</v>
       </c>
-      <c r="C12" s="165" t="s">
+      <c r="C12" s="157" t="s">
         <v>479</v>
       </c>
-      <c r="D12" s="165" t="s">
+      <c r="D12" s="157" t="s">
         <v>345</v>
       </c>
-      <c r="E12" s="173" t="s">
+      <c r="E12" s="165" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" thickBot="1">
+      <c r="G12" s="159">
+        <v>6</v>
+      </c>
+      <c r="H12" s="159">
+        <v>6</v>
+      </c>
+      <c r="I12" s="159">
+        <v>6</v>
+      </c>
+      <c r="J12" s="159">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.25" thickBot="1">
       <c r="A13" s="152">
         <v>11</v>
       </c>
-      <c r="B13" s="169" t="s">
+      <c r="B13" s="161" t="s">
         <v>480</v>
       </c>
-      <c r="C13" s="170" t="s">
+      <c r="C13" s="162" t="s">
         <v>481</v>
       </c>
-      <c r="D13" s="170" t="s">
+      <c r="D13" s="162" t="s">
         <v>482</v>
       </c>
-      <c r="E13" s="174" t="s">
+      <c r="E13" s="166" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" s="167">
+        <v>7</v>
+      </c>
+      <c r="H13" s="167">
+        <v>7</v>
+      </c>
+      <c r="I13" s="167">
+        <v>7</v>
+      </c>
+      <c r="J13" s="167">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="152">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:10">
       <c r="A15" s="152">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:10">
       <c r="A16" s="152">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
220504-v1 sim data flow OK !!!
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98F9985-CA55-4BF5-BC7F-5A8DB8485BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334740E2-DB8C-4A3B-8206-DAF67BC3E9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="489">
   <si>
     <t>步骤</t>
   </si>
@@ -928,10 +928,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>Q</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>没有+Q，</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -960,14 +956,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>G_xi(偶)</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>G_z(奇)</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
     <t>G_z_Q</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -1689,6 +1677,26 @@
   <si>
     <t>cov_vv</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>H_xi -2</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>H_z 2</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>G_xi(偶) 1</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>G_z(奇) 3</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -12613,7 +12621,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="172" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="54" t="s">
@@ -12727,7 +12735,7 @@
         <v>189</v>
       </c>
       <c r="E20" s="172" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -13087,7 +13095,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="172" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="66" t="s">
@@ -13928,7 +13936,7 @@
         <v>218</v>
       </c>
       <c r="B66" s="173" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C66" s="75" t="s">
         <v>180</v>
@@ -18523,7 +18531,7 @@
         <v>243</v>
       </c>
       <c r="C2" s="135" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D2" s="135"/>
       <c r="E2" s="136" t="s">
@@ -18751,7 +18759,7 @@
         <v>258</v>
       </c>
       <c r="C20" s="135" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D20" s="135" t="s">
         <v>255</v>
@@ -18760,7 +18768,7 @@
         <v>259</v>
       </c>
       <c r="F20" s="104" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G20" s="104"/>
     </row>
@@ -18769,7 +18777,7 @@
         <v>250</v>
       </c>
       <c r="C21" s="140" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D21" s="140" t="s">
         <v>250</v>
@@ -18778,7 +18786,7 @@
         <v>250</v>
       </c>
       <c r="F21" s="103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="14.25" thickBot="1">
@@ -18805,8 +18813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -18954,14 +18962,14 @@
     </row>
     <row r="2" spans="1:47">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" s="105">
         <v>1</v>
       </c>
       <c r="C2" s="106"/>
       <c r="D2" s="107" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E2" s="105">
         <v>1</v>
@@ -18969,96 +18977,106 @@
       <c r="F2" s="106"/>
       <c r="G2" s="106"/>
       <c r="H2" s="108" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I2" s="109"/>
       <c r="J2" s="110"/>
       <c r="K2" s="109" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L2" s="109"/>
       <c r="M2" s="109"/>
       <c r="N2" s="108" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O2" s="109"/>
       <c r="P2" s="109"/>
       <c r="Q2" s="108" t="s">
-        <v>268</v>
+        <v>487</v>
       </c>
       <c r="R2" s="109"/>
-      <c r="S2" s="111"/>
+      <c r="S2" s="111">
+        <v>5</v>
+      </c>
       <c r="T2" s="112" t="s">
-        <v>269</v>
-      </c>
-      <c r="U2" s="111"/>
+        <v>488</v>
+      </c>
+      <c r="U2" s="111">
+        <v>4</v>
+      </c>
       <c r="V2" s="108" t="s">
-        <v>260</v>
+        <v>484</v>
       </c>
       <c r="W2" s="110"/>
       <c r="X2" s="108" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Y2" s="110"/>
       <c r="Z2" s="113" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="AA2" s="110"/>
       <c r="AB2" s="114" t="s">
-        <v>243</v>
-      </c>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="109"/>
+        <v>485</v>
+      </c>
+      <c r="AC2" s="115">
+        <v>-3</v>
+      </c>
+      <c r="AD2" s="109">
+        <v>0</v>
+      </c>
       <c r="AE2" s="114" t="s">
-        <v>251</v>
-      </c>
-      <c r="AF2" s="115"/>
+        <v>486</v>
+      </c>
+      <c r="AF2" s="115">
+        <v>3</v>
+      </c>
       <c r="AG2" s="108" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="AH2" s="110"/>
       <c r="AI2" s="108" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="AJ2" s="109"/>
       <c r="AK2" s="109"/>
       <c r="AL2" s="109"/>
       <c r="AM2" s="109"/>
       <c r="AN2" s="114" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO2" s="116" t="s">
+        <v>272</v>
+      </c>
+      <c r="AP2" s="108" t="s">
+        <v>273</v>
+      </c>
+      <c r="AQ2" s="110" t="s">
         <v>274</v>
       </c>
-      <c r="AO2" s="116" t="s">
+      <c r="AR2" s="108" t="s">
         <v>275</v>
       </c>
-      <c r="AP2" s="108" t="s">
+      <c r="AS2" s="110" t="s">
         <v>276</v>
       </c>
-      <c r="AQ2" s="110" t="s">
+      <c r="AT2" s="108" t="s">
         <v>277</v>
       </c>
-      <c r="AR2" s="108" t="s">
+      <c r="AU2" s="110" t="s">
         <v>278</v>
-      </c>
-      <c r="AS2" s="110" t="s">
-        <v>279</v>
-      </c>
-      <c r="AT2" s="108" t="s">
-        <v>280</v>
-      </c>
-      <c r="AU2" s="110" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:47" ht="14.25" thickBot="1">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B3" s="117"/>
       <c r="C3" s="118">
         <v>1</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E3" s="120"/>
       <c r="F3" s="118">
@@ -19079,21 +19097,41 @@
       </c>
       <c r="P3" s="122"/>
       <c r="Q3" s="123"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="125"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="125"/>
+      <c r="R3" s="124">
+        <v>1</v>
+      </c>
+      <c r="S3" s="125">
+        <v>6</v>
+      </c>
+      <c r="T3" s="126">
+        <v>5</v>
+      </c>
+      <c r="U3" s="125">
+        <v>6</v>
+      </c>
       <c r="V3" s="123"/>
-      <c r="W3" s="127"/>
+      <c r="W3" s="127">
+        <v>1</v>
+      </c>
       <c r="X3" s="123"/>
       <c r="Y3" s="127"/>
       <c r="Z3" s="123"/>
       <c r="AA3" s="127"/>
-      <c r="AB3" s="128"/>
-      <c r="AC3" s="129"/>
-      <c r="AD3" s="124"/>
-      <c r="AE3" s="128"/>
-      <c r="AF3" s="129"/>
+      <c r="AB3" s="128">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="129">
+        <v>-5</v>
+      </c>
+      <c r="AD3" s="124">
+        <v>-1</v>
+      </c>
+      <c r="AE3" s="128">
+        <v>-4</v>
+      </c>
+      <c r="AF3" s="129">
+        <v>5</v>
+      </c>
       <c r="AG3" s="123"/>
       <c r="AH3" s="127"/>
       <c r="AI3" s="123"/>
@@ -19102,33 +19140,33 @@
       <c r="AL3" s="124"/>
       <c r="AM3" s="124"/>
       <c r="AN3" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO3" s="122" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP3" s="120" t="s">
+        <v>283</v>
+      </c>
+      <c r="AQ3" s="122" t="s">
         <v>284</v>
       </c>
-      <c r="AO3" s="122" t="s">
+      <c r="AR3" s="120" t="s">
         <v>285</v>
       </c>
-      <c r="AP3" s="120" t="s">
+      <c r="AS3" s="122" t="s">
         <v>286</v>
       </c>
-      <c r="AQ3" s="122" t="s">
+      <c r="AT3" s="120" t="s">
         <v>287</v>
       </c>
-      <c r="AR3" s="120" t="s">
+      <c r="AU3" s="122" t="s">
         <v>288</v>
-      </c>
-      <c r="AS3" s="122" t="s">
-        <v>289</v>
-      </c>
-      <c r="AT3" s="120" t="s">
-        <v>290</v>
-      </c>
-      <c r="AU3" s="122" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:47" ht="14.25" thickBot="1">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B4" s="130"/>
       <c r="C4" s="131"/>
@@ -19136,10 +19174,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="107" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F4" s="119" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G4" s="131">
         <v>1</v>
@@ -19176,33 +19214,33 @@
       <c r="AG4" s="132"/>
       <c r="AH4" s="132"/>
       <c r="AN4" s="120" t="s">
+        <v>290</v>
+      </c>
+      <c r="AO4" s="122" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP4" s="120" t="s">
+        <v>292</v>
+      </c>
+      <c r="AQ4" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="AO4" s="122" t="s">
+      <c r="AR4" s="120" t="s">
         <v>294</v>
       </c>
-      <c r="AP4" s="120" t="s">
+      <c r="AS4" s="122" t="s">
         <v>295</v>
       </c>
-      <c r="AQ4" s="122" t="s">
+      <c r="AT4" s="120" t="s">
         <v>296</v>
       </c>
-      <c r="AR4" s="120" t="s">
+      <c r="AU4" s="122" t="s">
         <v>297</v>
-      </c>
-      <c r="AS4" s="122" t="s">
-        <v>298</v>
-      </c>
-      <c r="AT4" s="120" t="s">
-        <v>299</v>
-      </c>
-      <c r="AU4" s="122" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="14.25" thickBot="1">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E5" s="130"/>
       <c r="F5" s="131"/>
@@ -19229,45 +19267,45 @@
       <c r="AG5" s="132"/>
       <c r="AH5" s="132"/>
       <c r="AN5" s="123" t="s">
+        <v>299</v>
+      </c>
+      <c r="AO5" s="127" t="s">
+        <v>300</v>
+      </c>
+      <c r="AP5" s="123" t="s">
+        <v>301</v>
+      </c>
+      <c r="AQ5" s="127" t="s">
         <v>302</v>
       </c>
-      <c r="AO5" s="127" t="s">
+      <c r="AR5" s="123" t="s">
         <v>303</v>
       </c>
-      <c r="AP5" s="123" t="s">
+      <c r="AS5" s="127" t="s">
         <v>304</v>
       </c>
-      <c r="AQ5" s="127" t="s">
+      <c r="AT5" s="123" t="s">
         <v>305</v>
       </c>
-      <c r="AR5" s="123" t="s">
+      <c r="AU5" s="127" t="s">
         <v>306</v>
-      </c>
-      <c r="AS5" s="127" t="s">
-        <v>307</v>
-      </c>
-      <c r="AT5" s="123" t="s">
-        <v>308</v>
-      </c>
-      <c r="AU5" s="127" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
       <c r="B6" s="179" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C6" s="180"/>
       <c r="D6" s="181"/>
       <c r="E6" s="179" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F6" s="180"/>
       <c r="G6" s="181"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
       <c r="B7" s="179" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C7" s="180"/>
       <c r="D7" s="180"/>
@@ -19284,7 +19322,7 @@
       <c r="O7" s="180"/>
       <c r="P7" s="181"/>
       <c r="Q7" s="179" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="R7" s="180"/>
       <c r="S7" s="180"/>
@@ -19297,7 +19335,7 @@
       <c r="Z7" s="180"/>
       <c r="AA7" s="181"/>
       <c r="AB7" s="179" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AC7" s="180"/>
       <c r="AD7" s="180"/>
@@ -19321,10 +19359,10 @@
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="AM9" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -19332,7 +19370,7 @@
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
       <c r="H10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -19342,7 +19380,7 @@
     </row>
     <row r="15" spans="1:47">
       <c r="AB15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -19393,10 +19431,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="138" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C2" s="139" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D2" s="140"/>
       <c r="E2" s="140"/>
@@ -19414,13 +19452,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="138" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C3" s="139" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D3" s="139" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E3" s="140"/>
       <c r="F3" s="140"/>
@@ -19437,16 +19475,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="138" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="139" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="139" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="139" t="s">
         <v>324</v>
-      </c>
-      <c r="C4" s="139" t="s">
-        <v>325</v>
-      </c>
-      <c r="D4" s="139" t="s">
-        <v>326</v>
-      </c>
-      <c r="E4" s="139" t="s">
-        <v>327</v>
       </c>
       <c r="F4" s="140"/>
       <c r="G4" s="140"/>
@@ -19462,19 +19500,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="138" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="139" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" s="139" t="s">
+        <v>327</v>
+      </c>
+      <c r="E5" s="139" t="s">
         <v>328</v>
       </c>
-      <c r="C5" s="139" t="s">
+      <c r="F5" s="139" t="s">
         <v>329</v>
-      </c>
-      <c r="D5" s="139" t="s">
-        <v>330</v>
-      </c>
-      <c r="E5" s="139" t="s">
-        <v>331</v>
-      </c>
-      <c r="F5" s="139" t="s">
-        <v>332</v>
       </c>
       <c r="G5" s="140"/>
       <c r="H5" s="140"/>
@@ -19489,22 +19527,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="138" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6" s="139" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" s="139" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" s="139" t="s">
         <v>333</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="F6" s="139" t="s">
         <v>334</v>
       </c>
-      <c r="D6" s="139" t="s">
+      <c r="G6" s="139" t="s">
         <v>335</v>
-      </c>
-      <c r="E6" s="139" t="s">
-        <v>336</v>
-      </c>
-      <c r="F6" s="139" t="s">
-        <v>337</v>
-      </c>
-      <c r="G6" s="139" t="s">
-        <v>338</v>
       </c>
       <c r="H6" s="140"/>
       <c r="I6" s="140"/>
@@ -19518,25 +19556,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="138" t="s">
+        <v>336</v>
+      </c>
+      <c r="C7" s="139" t="s">
+        <v>337</v>
+      </c>
+      <c r="D7" s="139" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="139" t="s">
         <v>339</v>
       </c>
-      <c r="C7" s="139" t="s">
+      <c r="F7" s="139" t="s">
         <v>340</v>
       </c>
-      <c r="D7" s="139" t="s">
+      <c r="G7" s="139" t="s">
         <v>341</v>
       </c>
-      <c r="E7" s="139" t="s">
+      <c r="H7" s="139" t="s">
         <v>342</v>
-      </c>
-      <c r="F7" s="139" t="s">
-        <v>343</v>
-      </c>
-      <c r="G7" s="139" t="s">
-        <v>344</v>
-      </c>
-      <c r="H7" s="139" t="s">
-        <v>345</v>
       </c>
       <c r="I7" s="140"/>
       <c r="J7" s="140"/>
@@ -19549,28 +19587,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="138" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="139" t="s">
+        <v>344</v>
+      </c>
+      <c r="D8" s="139" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8" s="139" t="s">
         <v>346</v>
       </c>
-      <c r="C8" s="139" t="s">
+      <c r="F8" s="139" t="s">
         <v>347</v>
       </c>
-      <c r="D8" s="139" t="s">
+      <c r="G8" s="139" t="s">
         <v>348</v>
       </c>
-      <c r="E8" s="139" t="s">
+      <c r="H8" s="139" t="s">
         <v>349</v>
       </c>
-      <c r="F8" s="139" t="s">
+      <c r="I8" s="139" t="s">
         <v>350</v>
-      </c>
-      <c r="G8" s="139" t="s">
-        <v>351</v>
-      </c>
-      <c r="H8" s="139" t="s">
-        <v>352</v>
-      </c>
-      <c r="I8" s="139" t="s">
-        <v>353</v>
       </c>
       <c r="J8" s="140"/>
       <c r="K8" s="140"/>
@@ -19582,31 +19620,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="138" t="s">
+        <v>351</v>
+      </c>
+      <c r="C9" s="139" t="s">
+        <v>352</v>
+      </c>
+      <c r="D9" s="139" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9" s="139" t="s">
         <v>354</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="F9" s="139" t="s">
         <v>355</v>
       </c>
-      <c r="D9" s="139" t="s">
+      <c r="G9" s="139" t="s">
         <v>356</v>
       </c>
-      <c r="E9" s="139" t="s">
+      <c r="H9" s="139" t="s">
         <v>357</v>
       </c>
-      <c r="F9" s="139" t="s">
+      <c r="I9" s="139" t="s">
         <v>358</v>
       </c>
-      <c r="G9" s="139" t="s">
+      <c r="J9" s="139" t="s">
         <v>359</v>
-      </c>
-      <c r="H9" s="139" t="s">
-        <v>360</v>
-      </c>
-      <c r="I9" s="139" t="s">
-        <v>361</v>
-      </c>
-      <c r="J9" s="139" t="s">
-        <v>362</v>
       </c>
       <c r="K9" s="140"/>
       <c r="L9" s="140"/>
@@ -19617,34 +19655,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="138" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="139" t="s">
+        <v>361</v>
+      </c>
+      <c r="D10" s="139" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" s="139" t="s">
         <v>363</v>
       </c>
-      <c r="C10" s="139" t="s">
+      <c r="F10" s="139" t="s">
         <v>364</v>
       </c>
-      <c r="D10" s="139" t="s">
+      <c r="G10" s="139" t="s">
         <v>365</v>
       </c>
-      <c r="E10" s="139" t="s">
+      <c r="H10" s="139" t="s">
         <v>366</v>
       </c>
-      <c r="F10" s="139" t="s">
+      <c r="I10" s="139" t="s">
         <v>367</v>
       </c>
-      <c r="G10" s="139" t="s">
+      <c r="J10" s="139" t="s">
         <v>368</v>
       </c>
-      <c r="H10" s="139" t="s">
+      <c r="K10" s="139" t="s">
         <v>369</v>
-      </c>
-      <c r="I10" s="139" t="s">
-        <v>370</v>
-      </c>
-      <c r="J10" s="139" t="s">
-        <v>371</v>
-      </c>
-      <c r="K10" s="139" t="s">
-        <v>372</v>
       </c>
       <c r="L10" s="140"/>
       <c r="M10" s="141"/>
@@ -19654,37 +19692,37 @@
         <v>10</v>
       </c>
       <c r="B11" s="138" t="s">
+        <v>370</v>
+      </c>
+      <c r="C11" s="139" t="s">
+        <v>371</v>
+      </c>
+      <c r="D11" s="139" t="s">
+        <v>372</v>
+      </c>
+      <c r="E11" s="139" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="139" t="s">
+      <c r="F11" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="D11" s="139" t="s">
+      <c r="G11" s="139" t="s">
         <v>375</v>
       </c>
-      <c r="E11" s="139" t="s">
+      <c r="H11" s="139" t="s">
         <v>376</v>
       </c>
-      <c r="F11" s="139" t="s">
+      <c r="I11" s="139" t="s">
         <v>377</v>
       </c>
-      <c r="G11" s="139" t="s">
+      <c r="J11" s="139" t="s">
         <v>378</v>
       </c>
-      <c r="H11" s="139" t="s">
+      <c r="K11" s="139" t="s">
         <v>379</v>
       </c>
-      <c r="I11" s="139" t="s">
+      <c r="L11" s="139" t="s">
         <v>380</v>
-      </c>
-      <c r="J11" s="139" t="s">
-        <v>381</v>
-      </c>
-      <c r="K11" s="139" t="s">
-        <v>382</v>
-      </c>
-      <c r="L11" s="139" t="s">
-        <v>383</v>
       </c>
       <c r="M11" s="141"/>
     </row>
@@ -19693,497 +19731,497 @@
         <v>11</v>
       </c>
       <c r="B12" s="143" t="s">
+        <v>381</v>
+      </c>
+      <c r="C12" s="144" t="s">
+        <v>382</v>
+      </c>
+      <c r="D12" s="144" t="s">
+        <v>383</v>
+      </c>
+      <c r="E12" s="144" t="s">
         <v>384</v>
       </c>
-      <c r="C12" s="144" t="s">
+      <c r="F12" s="145" t="s">
         <v>385</v>
       </c>
-      <c r="D12" s="144" t="s">
+      <c r="G12" s="144" t="s">
         <v>386</v>
       </c>
-      <c r="E12" s="144" t="s">
+      <c r="H12" s="144" t="s">
         <v>387</v>
       </c>
-      <c r="F12" s="145" t="s">
+      <c r="I12" s="144" t="s">
         <v>388</v>
       </c>
-      <c r="G12" s="144" t="s">
+      <c r="J12" s="144" t="s">
         <v>389</v>
       </c>
-      <c r="H12" s="144" t="s">
+      <c r="K12" s="144" t="s">
         <v>390</v>
       </c>
-      <c r="I12" s="144" t="s">
+      <c r="L12" s="144" t="s">
         <v>391</v>
       </c>
-      <c r="J12" s="144" t="s">
+      <c r="M12" s="146" t="s">
         <v>392</v>
-      </c>
-      <c r="K12" s="144" t="s">
-        <v>393</v>
-      </c>
-      <c r="L12" s="144" t="s">
-        <v>394</v>
-      </c>
-      <c r="M12" s="146" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="103" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14" s="147"/>
       <c r="C14" s="148" t="s">
+        <v>343</v>
+      </c>
+      <c r="D14" s="149" t="s">
+        <v>344</v>
+      </c>
+      <c r="E14" s="149" t="s">
+        <v>345</v>
+      </c>
+      <c r="F14" s="149" t="s">
         <v>346</v>
       </c>
-      <c r="D14" s="149" t="s">
+      <c r="G14" s="149" t="s">
         <v>347</v>
       </c>
-      <c r="E14" s="149" t="s">
+      <c r="H14" s="149" t="s">
         <v>348</v>
       </c>
-      <c r="F14" s="149" t="s">
+      <c r="I14" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="G14" s="149" t="s">
+      <c r="J14" s="149" t="s">
         <v>350</v>
       </c>
-      <c r="H14" s="149" t="s">
+      <c r="K14" s="148" t="s">
         <v>351</v>
       </c>
-      <c r="I14" s="149" t="s">
+      <c r="L14" s="149" t="s">
         <v>352</v>
       </c>
-      <c r="J14" s="149" t="s">
+      <c r="M14" s="149" t="s">
         <v>353</v>
       </c>
-      <c r="K14" s="148" t="s">
+      <c r="N14" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="L14" s="149" t="s">
+      <c r="O14" s="149" t="s">
         <v>355</v>
       </c>
-      <c r="M14" s="149" t="s">
+      <c r="P14" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="N14" s="149" t="s">
+      <c r="Q14" s="149" t="s">
         <v>357</v>
       </c>
-      <c r="O14" s="149" t="s">
+      <c r="R14" s="149" t="s">
         <v>358</v>
       </c>
-      <c r="P14" s="149" t="s">
+      <c r="S14" s="149" t="s">
         <v>359</v>
       </c>
-      <c r="Q14" s="149" t="s">
-        <v>360</v>
-      </c>
-      <c r="R14" s="149" t="s">
-        <v>361</v>
-      </c>
-      <c r="S14" s="149" t="s">
-        <v>362</v>
-      </c>
       <c r="T14" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="U14" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="V14" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="W14" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B15" s="148" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C15" s="149" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D15" s="148" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" s="149" t="s">
+        <v>337</v>
+      </c>
+      <c r="F15" s="149" t="s">
+        <v>338</v>
+      </c>
+      <c r="G15" s="149" t="s">
         <v>339</v>
       </c>
-      <c r="E15" s="149" t="s">
+      <c r="H15" s="149" t="s">
         <v>340</v>
       </c>
-      <c r="F15" s="149" t="s">
+      <c r="I15" s="149" t="s">
         <v>341</v>
       </c>
-      <c r="G15" s="149" t="s">
+      <c r="J15" s="149" t="s">
         <v>342</v>
       </c>
-      <c r="H15" s="149" t="s">
-        <v>343</v>
-      </c>
-      <c r="I15" s="149" t="s">
-        <v>344</v>
-      </c>
-      <c r="J15" s="149" t="s">
-        <v>345</v>
-      </c>
       <c r="K15" s="148" t="s">
+        <v>360</v>
+      </c>
+      <c r="L15" s="149" t="s">
+        <v>361</v>
+      </c>
+      <c r="M15" s="149" t="s">
+        <v>362</v>
+      </c>
+      <c r="N15" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="L15" s="149" t="s">
+      <c r="O15" s="149" t="s">
         <v>364</v>
       </c>
-      <c r="M15" s="149" t="s">
+      <c r="P15" s="149" t="s">
         <v>365</v>
       </c>
-      <c r="N15" s="149" t="s">
+      <c r="Q15" s="149" t="s">
         <v>366</v>
       </c>
-      <c r="O15" s="149" t="s">
+      <c r="R15" s="149" t="s">
         <v>367</v>
       </c>
-      <c r="P15" s="149" t="s">
+      <c r="S15" s="149" t="s">
         <v>368</v>
       </c>
-      <c r="Q15" s="149" t="s">
+      <c r="T15" s="149" t="s">
         <v>369</v>
       </c>
-      <c r="R15" s="149" t="s">
-        <v>370</v>
-      </c>
-      <c r="S15" s="149" t="s">
-        <v>371</v>
-      </c>
-      <c r="T15" s="149" t="s">
-        <v>372</v>
-      </c>
       <c r="U15" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="V15" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="W15" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="103" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B16" s="148" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C16" s="149" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D16" s="149" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E16" s="148" t="s">
+        <v>330</v>
+      </c>
+      <c r="F16" s="149" t="s">
+        <v>331</v>
+      </c>
+      <c r="G16" s="149" t="s">
+        <v>332</v>
+      </c>
+      <c r="H16" s="149" t="s">
         <v>333</v>
       </c>
-      <c r="F16" s="149" t="s">
+      <c r="I16" s="149" t="s">
         <v>334</v>
       </c>
-      <c r="G16" s="149" t="s">
+      <c r="J16" s="149" t="s">
         <v>335</v>
       </c>
-      <c r="H16" s="149" t="s">
-        <v>336</v>
-      </c>
-      <c r="I16" s="149" t="s">
-        <v>337</v>
-      </c>
-      <c r="J16" s="149" t="s">
-        <v>338</v>
-      </c>
       <c r="K16" s="148" t="s">
+        <v>370</v>
+      </c>
+      <c r="L16" s="149" t="s">
+        <v>371</v>
+      </c>
+      <c r="M16" s="149" t="s">
+        <v>372</v>
+      </c>
+      <c r="N16" s="149" t="s">
         <v>373</v>
       </c>
-      <c r="L16" s="149" t="s">
+      <c r="O16" s="149" t="s">
         <v>374</v>
       </c>
-      <c r="M16" s="149" t="s">
+      <c r="P16" s="149" t="s">
         <v>375</v>
       </c>
-      <c r="N16" s="149" t="s">
+      <c r="Q16" s="149" t="s">
         <v>376</v>
       </c>
-      <c r="O16" s="149" t="s">
+      <c r="R16" s="149" t="s">
         <v>377</v>
       </c>
-      <c r="P16" s="149" t="s">
+      <c r="S16" s="149" t="s">
         <v>378</v>
       </c>
-      <c r="Q16" s="149" t="s">
+      <c r="T16" s="149" t="s">
         <v>379</v>
       </c>
-      <c r="R16" s="149" t="s">
+      <c r="U16" s="149" t="s">
         <v>380</v>
       </c>
-      <c r="S16" s="149" t="s">
-        <v>381</v>
-      </c>
-      <c r="T16" s="149" t="s">
-        <v>382</v>
-      </c>
-      <c r="U16" s="149" t="s">
-        <v>383</v>
-      </c>
       <c r="V16" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="W16" s="103" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="103" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B17" s="148" t="s">
+        <v>321</v>
+      </c>
+      <c r="C17" s="149" t="s">
+        <v>322</v>
+      </c>
+      <c r="D17" s="149" t="s">
+        <v>323</v>
+      </c>
+      <c r="E17" s="149" t="s">
         <v>324</v>
       </c>
-      <c r="C17" s="149" t="s">
+      <c r="F17" s="148" t="s">
         <v>325</v>
       </c>
-      <c r="D17" s="149" t="s">
+      <c r="G17" s="149" t="s">
         <v>326</v>
       </c>
-      <c r="E17" s="149" t="s">
+      <c r="H17" s="149" t="s">
         <v>327</v>
       </c>
-      <c r="F17" s="148" t="s">
+      <c r="I17" s="149" t="s">
         <v>328</v>
       </c>
-      <c r="G17" s="149" t="s">
+      <c r="J17" s="149" t="s">
         <v>329</v>
       </c>
-      <c r="H17" s="149" t="s">
-        <v>330</v>
-      </c>
-      <c r="I17" s="149" t="s">
-        <v>331</v>
-      </c>
-      <c r="J17" s="149" t="s">
-        <v>332</v>
-      </c>
       <c r="K17" s="148" t="s">
+        <v>381</v>
+      </c>
+      <c r="L17" s="149" t="s">
+        <v>382</v>
+      </c>
+      <c r="M17" s="149" t="s">
+        <v>383</v>
+      </c>
+      <c r="N17" s="149" t="s">
         <v>384</v>
       </c>
-      <c r="L17" s="149" t="s">
+      <c r="O17" s="150" t="s">
         <v>385</v>
       </c>
-      <c r="M17" s="149" t="s">
+      <c r="P17" s="149" t="s">
         <v>386</v>
       </c>
-      <c r="N17" s="149" t="s">
+      <c r="Q17" s="149" t="s">
         <v>387</v>
       </c>
-      <c r="O17" s="150" t="s">
+      <c r="R17" s="149" t="s">
         <v>388</v>
       </c>
-      <c r="P17" s="149" t="s">
+      <c r="S17" s="149" t="s">
         <v>389</v>
       </c>
-      <c r="Q17" s="149" t="s">
+      <c r="T17" s="149" t="s">
         <v>390</v>
       </c>
-      <c r="R17" s="149" t="s">
+      <c r="U17" s="149" t="s">
         <v>391</v>
       </c>
-      <c r="S17" s="149" t="s">
+      <c r="V17" s="149" t="s">
         <v>392</v>
       </c>
-      <c r="T17" s="149" t="s">
+      <c r="W17" s="103" t="s">
         <v>393</v>
-      </c>
-      <c r="U17" s="149" t="s">
-        <v>394</v>
-      </c>
-      <c r="V17" s="149" t="s">
-        <v>395</v>
-      </c>
-      <c r="W17" s="103" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="103" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="148" t="s">
+        <v>351</v>
+      </c>
+      <c r="C19" s="149" t="s">
+        <v>352</v>
+      </c>
+      <c r="D19" s="149" t="s">
+        <v>353</v>
+      </c>
+      <c r="E19" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="C19" s="149" t="s">
+      <c r="F19" s="149" t="s">
         <v>355</v>
       </c>
-      <c r="D19" s="149" t="s">
+      <c r="G19" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="E19" s="149" t="s">
+      <c r="H19" s="149" t="s">
         <v>357</v>
       </c>
-      <c r="F19" s="149" t="s">
+      <c r="I19" s="149" t="s">
         <v>358</v>
       </c>
-      <c r="G19" s="149" t="s">
+      <c r="J19" s="149" t="s">
         <v>359</v>
-      </c>
-      <c r="H19" s="149" t="s">
-        <v>360</v>
-      </c>
-      <c r="I19" s="149" t="s">
-        <v>361</v>
-      </c>
-      <c r="J19" s="149" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B20" s="148" t="s">
+        <v>360</v>
+      </c>
+      <c r="C20" s="149" t="s">
+        <v>361</v>
+      </c>
+      <c r="D20" s="149" t="s">
+        <v>362</v>
+      </c>
+      <c r="E20" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="C20" s="149" t="s">
+      <c r="F20" s="149" t="s">
         <v>364</v>
       </c>
-      <c r="D20" s="149" t="s">
+      <c r="G20" s="149" t="s">
         <v>365</v>
       </c>
-      <c r="E20" s="149" t="s">
+      <c r="H20" s="149" t="s">
         <v>366</v>
       </c>
-      <c r="F20" s="149" t="s">
+      <c r="I20" s="149" t="s">
         <v>367</v>
       </c>
-      <c r="G20" s="149" t="s">
+      <c r="J20" s="149" t="s">
         <v>368</v>
       </c>
-      <c r="H20" s="149" t="s">
+      <c r="K20" s="149" t="s">
         <v>369</v>
-      </c>
-      <c r="I20" s="149" t="s">
-        <v>370</v>
-      </c>
-      <c r="J20" s="149" t="s">
-        <v>371</v>
-      </c>
-      <c r="K20" s="149" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="103" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B21" s="148" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" s="149" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" s="149" t="s">
+        <v>372</v>
+      </c>
+      <c r="E21" s="149" t="s">
         <v>373</v>
       </c>
-      <c r="C21" s="149" t="s">
+      <c r="F21" s="149" t="s">
         <v>374</v>
       </c>
-      <c r="D21" s="149" t="s">
+      <c r="G21" s="149" t="s">
         <v>375</v>
       </c>
-      <c r="E21" s="149" t="s">
+      <c r="H21" s="149" t="s">
         <v>376</v>
       </c>
-      <c r="F21" s="149" t="s">
+      <c r="I21" s="149" t="s">
         <v>377</v>
       </c>
-      <c r="G21" s="149" t="s">
+      <c r="J21" s="149" t="s">
         <v>378</v>
       </c>
-      <c r="H21" s="149" t="s">
+      <c r="K21" s="149" t="s">
         <v>379</v>
       </c>
-      <c r="I21" s="149" t="s">
+      <c r="L21" s="149" t="s">
         <v>380</v>
-      </c>
-      <c r="J21" s="149" t="s">
-        <v>381</v>
-      </c>
-      <c r="K21" s="149" t="s">
-        <v>382</v>
-      </c>
-      <c r="L21" s="149" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="103" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B22" s="148" t="s">
+        <v>381</v>
+      </c>
+      <c r="C22" s="149" t="s">
+        <v>382</v>
+      </c>
+      <c r="D22" s="149" t="s">
+        <v>383</v>
+      </c>
+      <c r="E22" s="149" t="s">
         <v>384</v>
       </c>
-      <c r="C22" s="149" t="s">
+      <c r="F22" s="150" t="s">
         <v>385</v>
       </c>
-      <c r="D22" s="149" t="s">
+      <c r="G22" s="149" t="s">
         <v>386</v>
       </c>
-      <c r="E22" s="149" t="s">
+      <c r="H22" s="149" t="s">
         <v>387</v>
       </c>
-      <c r="F22" s="150" t="s">
+      <c r="I22" s="149" t="s">
         <v>388</v>
       </c>
-      <c r="G22" s="149" t="s">
+      <c r="J22" s="149" t="s">
         <v>389</v>
       </c>
-      <c r="H22" s="149" t="s">
+      <c r="K22" s="149" t="s">
         <v>390</v>
       </c>
-      <c r="I22" s="149" t="s">
+      <c r="L22" s="149" t="s">
         <v>391</v>
       </c>
-      <c r="J22" s="149" t="s">
+      <c r="M22" s="149" t="s">
         <v>392</v>
-      </c>
-      <c r="K22" s="149" t="s">
-        <v>393</v>
-      </c>
-      <c r="L22" s="149" t="s">
-        <v>394</v>
-      </c>
-      <c r="M22" s="149" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="103" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B24" s="103" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C24" s="103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D24" s="103" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E24" s="103" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H24" s="103" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I24" s="103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J24" s="103" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K24" s="103" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -20192,13 +20230,13 @@
       </c>
       <c r="B25" s="147"/>
       <c r="C25" s="148" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D25" s="148" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="148" t="s">
         <v>321</v>
-      </c>
-      <c r="E25" s="148" t="s">
-        <v>324</v>
       </c>
       <c r="H25" s="103">
         <v>0</v>
@@ -20218,16 +20256,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="148" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C26" s="149" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D26" s="149" t="s">
+        <v>319</v>
+      </c>
+      <c r="E26" s="149" t="s">
         <v>322</v>
-      </c>
-      <c r="E26" s="149" t="s">
-        <v>325</v>
       </c>
       <c r="H26" s="103">
         <v>0</v>
@@ -20247,16 +20285,16 @@
         <v>2</v>
       </c>
       <c r="B27" s="149" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C27" s="148" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D27" s="149" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E27" s="149" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H27" s="103">
         <v>1</v>
@@ -20276,16 +20314,16 @@
         <v>3</v>
       </c>
       <c r="B28" s="149" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C28" s="149" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D28" s="148" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E28" s="149" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H28" s="103">
         <v>2</v>
@@ -20305,16 +20343,16 @@
         <v>4</v>
       </c>
       <c r="B29" s="149" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C29" s="149" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D29" s="149" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E29" s="148" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H29" s="103">
         <v>3</v>
@@ -20334,16 +20372,16 @@
         <v>5</v>
       </c>
       <c r="B30" s="149" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C30" s="149" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D30" s="149" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E30" s="149" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H30" s="103">
         <v>4</v>
@@ -20363,16 +20401,16 @@
         <v>6</v>
       </c>
       <c r="B31" s="149" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C31" s="149" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D31" s="149" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E31" s="149" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H31" s="103">
         <v>5</v>
@@ -20392,16 +20430,16 @@
         <v>7</v>
       </c>
       <c r="B32" s="149" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C32" s="149" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D32" s="149" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E32" s="149" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H32" s="103">
         <v>6</v>
@@ -20421,16 +20459,16 @@
         <v>8</v>
       </c>
       <c r="B33" s="149" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C33" s="149" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D33" s="149" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E33" s="149" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H33" s="103">
         <v>7</v>
@@ -20450,16 +20488,16 @@
         <v>9</v>
       </c>
       <c r="B34" s="148" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C34" s="148" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D34" s="148" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E34" s="148" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H34" s="103">
         <v>8</v>
@@ -20479,16 +20517,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="149" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C35" s="149" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D35" s="149" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E35" s="149" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H35" s="103">
         <v>9</v>
@@ -20508,16 +20546,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="149" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C36" s="149" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D36" s="149" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E36" s="149" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="H36" s="103">
         <v>10</v>
@@ -20537,16 +20575,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="149" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C37" s="149" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D37" s="149" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E37" s="149" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H37" s="103">
         <v>11</v>
@@ -20566,16 +20604,16 @@
         <v>13</v>
       </c>
       <c r="B38" s="149" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C38" s="149" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D38" s="149" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E38" s="149" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H38" s="103">
         <v>12</v>
@@ -20595,16 +20633,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="149" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C39" s="149" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D39" s="149" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E39" s="149" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H39" s="103">
         <v>13</v>
@@ -20624,16 +20662,16 @@
         <v>15</v>
       </c>
       <c r="B40" s="149" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C40" s="149" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D40" s="149" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E40" s="149" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H40" s="103">
         <v>14</v>
@@ -20653,16 +20691,16 @@
         <v>16</v>
       </c>
       <c r="B41" s="149" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C41" s="149" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D41" s="149" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E41" s="149" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H41" s="103">
         <v>15</v>
@@ -20682,16 +20720,16 @@
         <v>17</v>
       </c>
       <c r="B42" s="149" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C42" s="149" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D42" s="149" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E42" s="149" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H42" s="103">
         <v>16</v>
@@ -20711,16 +20749,16 @@
         <v>18</v>
       </c>
       <c r="B43" s="148" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C43" s="149" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D43" s="149" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E43" s="149" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H43" s="103">
         <v>17</v>
@@ -20740,16 +20778,16 @@
         <v>19</v>
       </c>
       <c r="B44" s="151" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C44" s="148" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D44" s="149" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E44" s="149" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H44" s="103">
         <v>18</v>
@@ -20769,16 +20807,16 @@
         <v>20</v>
       </c>
       <c r="B45" s="151" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C45" s="151" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D45" s="148" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E45" s="149" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H45" s="103">
         <v>19</v>
@@ -20798,16 +20836,16 @@
         <v>21</v>
       </c>
       <c r="B46" s="151" t="s">
+        <v>404</v>
+      </c>
+      <c r="C46" s="151" t="s">
+        <v>405</v>
+      </c>
+      <c r="D46" s="151" t="s">
+        <v>406</v>
+      </c>
+      <c r="E46" s="148" t="s">
         <v>407</v>
-      </c>
-      <c r="C46" s="151" t="s">
-        <v>408</v>
-      </c>
-      <c r="D46" s="151" t="s">
-        <v>409</v>
-      </c>
-      <c r="E46" s="148" t="s">
-        <v>410</v>
       </c>
       <c r="H46" s="103">
         <v>20</v>
@@ -20827,16 +20865,16 @@
         <v>22</v>
       </c>
       <c r="B47" s="151" t="s">
+        <v>408</v>
+      </c>
+      <c r="C47" s="151" t="s">
+        <v>409</v>
+      </c>
+      <c r="D47" s="151" t="s">
+        <v>410</v>
+      </c>
+      <c r="E47" s="151" t="s">
         <v>411</v>
-      </c>
-      <c r="C47" s="151" t="s">
-        <v>412</v>
-      </c>
-      <c r="D47" s="151" t="s">
-        <v>413</v>
-      </c>
-      <c r="E47" s="151" t="s">
-        <v>414</v>
       </c>
       <c r="H47" s="103">
         <v>21</v>
@@ -20856,16 +20894,16 @@
         <v>23</v>
       </c>
       <c r="B48" s="151" t="s">
+        <v>412</v>
+      </c>
+      <c r="C48" s="151" t="s">
+        <v>413</v>
+      </c>
+      <c r="D48" s="151" t="s">
+        <v>414</v>
+      </c>
+      <c r="E48" s="151" t="s">
         <v>415</v>
-      </c>
-      <c r="C48" s="151" t="s">
-        <v>416</v>
-      </c>
-      <c r="D48" s="151" t="s">
-        <v>417</v>
-      </c>
-      <c r="E48" s="151" t="s">
-        <v>418</v>
       </c>
       <c r="H48" s="103">
         <v>22</v>
@@ -20885,16 +20923,16 @@
         <v>24</v>
       </c>
       <c r="B49" s="151" t="s">
+        <v>416</v>
+      </c>
+      <c r="C49" s="151" t="s">
+        <v>417</v>
+      </c>
+      <c r="D49" s="151" t="s">
+        <v>418</v>
+      </c>
+      <c r="E49" s="151" t="s">
         <v>419</v>
-      </c>
-      <c r="C49" s="151" t="s">
-        <v>420</v>
-      </c>
-      <c r="D49" s="151" t="s">
-        <v>421</v>
-      </c>
-      <c r="E49" s="151" t="s">
-        <v>422</v>
       </c>
       <c r="H49" s="103">
         <v>23</v>
@@ -20914,16 +20952,16 @@
         <v>25</v>
       </c>
       <c r="B50" s="151" t="s">
+        <v>420</v>
+      </c>
+      <c r="C50" s="151" t="s">
+        <v>421</v>
+      </c>
+      <c r="D50" s="151" t="s">
+        <v>422</v>
+      </c>
+      <c r="E50" s="151" t="s">
         <v>423</v>
-      </c>
-      <c r="C50" s="151" t="s">
-        <v>424</v>
-      </c>
-      <c r="D50" s="151" t="s">
-        <v>425</v>
-      </c>
-      <c r="E50" s="151" t="s">
-        <v>426</v>
       </c>
       <c r="H50" s="103">
         <v>24</v>
@@ -20943,16 +20981,16 @@
         <v>26</v>
       </c>
       <c r="B51" s="151" t="s">
+        <v>424</v>
+      </c>
+      <c r="C51" s="151" t="s">
+        <v>425</v>
+      </c>
+      <c r="D51" s="151" t="s">
+        <v>426</v>
+      </c>
+      <c r="E51" s="151" t="s">
         <v>427</v>
-      </c>
-      <c r="C51" s="151" t="s">
-        <v>428</v>
-      </c>
-      <c r="D51" s="151" t="s">
-        <v>429</v>
-      </c>
-      <c r="E51" s="151" t="s">
-        <v>430</v>
       </c>
       <c r="H51" s="103">
         <v>25</v>
@@ -20972,16 +21010,16 @@
         <v>27</v>
       </c>
       <c r="B52" s="151" t="s">
+        <v>428</v>
+      </c>
+      <c r="C52" s="151" t="s">
+        <v>429</v>
+      </c>
+      <c r="D52" s="151" t="s">
+        <v>430</v>
+      </c>
+      <c r="E52" s="151" t="s">
         <v>431</v>
-      </c>
-      <c r="C52" s="151" t="s">
-        <v>432</v>
-      </c>
-      <c r="D52" s="151" t="s">
-        <v>433</v>
-      </c>
-      <c r="E52" s="151" t="s">
-        <v>434</v>
       </c>
       <c r="H52" s="103">
         <v>26</v>
@@ -21001,16 +21039,16 @@
         <v>28</v>
       </c>
       <c r="B53" s="151" t="s">
+        <v>432</v>
+      </c>
+      <c r="C53" s="151" t="s">
+        <v>433</v>
+      </c>
+      <c r="D53" s="151" t="s">
+        <v>434</v>
+      </c>
+      <c r="E53" s="151" t="s">
         <v>435</v>
-      </c>
-      <c r="C53" s="151" t="s">
-        <v>436</v>
-      </c>
-      <c r="D53" s="151" t="s">
-        <v>437</v>
-      </c>
-      <c r="E53" s="151" t="s">
-        <v>438</v>
       </c>
       <c r="H53" s="103">
         <v>27</v>
@@ -21030,16 +21068,16 @@
         <v>29</v>
       </c>
       <c r="B54" s="151" t="s">
+        <v>436</v>
+      </c>
+      <c r="C54" s="151" t="s">
+        <v>437</v>
+      </c>
+      <c r="D54" s="151" t="s">
+        <v>438</v>
+      </c>
+      <c r="E54" s="151" t="s">
         <v>439</v>
-      </c>
-      <c r="C54" s="151" t="s">
-        <v>440</v>
-      </c>
-      <c r="D54" s="151" t="s">
-        <v>441</v>
-      </c>
-      <c r="E54" s="151" t="s">
-        <v>442</v>
       </c>
       <c r="H54" s="103">
         <v>28</v>
@@ -21059,16 +21097,16 @@
         <v>30</v>
       </c>
       <c r="B55" s="151" t="s">
+        <v>440</v>
+      </c>
+      <c r="C55" s="151" t="s">
+        <v>441</v>
+      </c>
+      <c r="D55" s="151" t="s">
+        <v>442</v>
+      </c>
+      <c r="E55" s="151" t="s">
         <v>443</v>
-      </c>
-      <c r="C55" s="151" t="s">
-        <v>444</v>
-      </c>
-      <c r="D55" s="151" t="s">
-        <v>445</v>
-      </c>
-      <c r="E55" s="151" t="s">
-        <v>446</v>
       </c>
       <c r="H55" s="103">
         <v>29</v>
@@ -21088,16 +21126,16 @@
         <v>31</v>
       </c>
       <c r="B56" s="151" t="s">
+        <v>444</v>
+      </c>
+      <c r="C56" s="151" t="s">
+        <v>445</v>
+      </c>
+      <c r="D56" s="151" t="s">
+        <v>446</v>
+      </c>
+      <c r="E56" s="151" t="s">
         <v>447</v>
-      </c>
-      <c r="C56" s="151" t="s">
-        <v>448</v>
-      </c>
-      <c r="D56" s="151" t="s">
-        <v>449</v>
-      </c>
-      <c r="E56" s="151" t="s">
-        <v>450</v>
       </c>
       <c r="H56" s="103">
         <v>30</v>
@@ -21117,16 +21155,16 @@
         <v>32</v>
       </c>
       <c r="B57" s="151" t="s">
+        <v>448</v>
+      </c>
+      <c r="C57" s="151" t="s">
+        <v>449</v>
+      </c>
+      <c r="D57" s="151" t="s">
+        <v>450</v>
+      </c>
+      <c r="E57" s="151" t="s">
         <v>451</v>
-      </c>
-      <c r="C57" s="151" t="s">
-        <v>452</v>
-      </c>
-      <c r="D57" s="151" t="s">
-        <v>453</v>
-      </c>
-      <c r="E57" s="151" t="s">
-        <v>454</v>
       </c>
       <c r="H57" s="103">
         <v>31</v>
@@ -21146,16 +21184,16 @@
         <v>33</v>
       </c>
       <c r="B58" s="151" t="s">
+        <v>452</v>
+      </c>
+      <c r="C58" s="151" t="s">
+        <v>453</v>
+      </c>
+      <c r="D58" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="E58" s="151" t="s">
         <v>455</v>
-      </c>
-      <c r="C58" s="151" t="s">
-        <v>456</v>
-      </c>
-      <c r="D58" s="151" t="s">
-        <v>457</v>
-      </c>
-      <c r="E58" s="151" t="s">
-        <v>458</v>
       </c>
       <c r="H58" s="103">
         <v>32</v>
@@ -21180,7 +21218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -21191,31 +21229,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" thickBot="1">
       <c r="A1" s="152" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" s="152" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" s="152" t="s">
+        <v>458</v>
+      </c>
+      <c r="D1" s="152" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="E1" s="152" t="s">
         <v>460</v>
       </c>
-      <c r="C1" s="152" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="152" t="s">
-        <v>462</v>
-      </c>
-      <c r="E1" s="152" t="s">
-        <v>463</v>
-      </c>
       <c r="G1" s="152" t="s">
+        <v>457</v>
+      </c>
+      <c r="H1" s="152" t="s">
+        <v>458</v>
+      </c>
+      <c r="I1" s="152" t="s">
+        <v>459</v>
+      </c>
+      <c r="J1" s="152" t="s">
         <v>460</v>
-      </c>
-      <c r="H1" s="152" t="s">
-        <v>461</v>
-      </c>
-      <c r="I1" s="152" t="s">
-        <v>462</v>
-      </c>
-      <c r="J1" s="152" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -21223,13 +21261,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="153" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C2" s="154" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="154" t="s">
         <v>321</v>
-      </c>
-      <c r="D2" s="154" t="s">
-        <v>324</v>
       </c>
       <c r="E2" s="155"/>
       <c r="G2" s="153">
@@ -21248,13 +21286,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="156" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C3" s="157" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="157" t="s">
         <v>322</v>
-      </c>
-      <c r="D3" s="157" t="s">
-        <v>325</v>
       </c>
       <c r="E3" s="158"/>
       <c r="G3" s="156">
@@ -21273,13 +21311,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="159" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C4" s="157" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D4" s="157" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E4" s="160"/>
       <c r="G4" s="159">
@@ -21298,13 +21336,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="161" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C5" s="162" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D5" s="162" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E5" s="163"/>
       <c r="G5" s="161">
@@ -21323,16 +21361,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="153" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C6" s="154" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E6" s="164" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G6" s="153">
         <v>0</v>
@@ -21352,16 +21390,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="156" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C7" s="157" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D7" s="157" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E7" s="165" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G7" s="156">
         <v>1</v>
@@ -21381,16 +21419,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="159" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C8" s="157" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D8" s="157" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E8" s="165" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G8" s="159">
         <v>2</v>
@@ -21410,16 +21448,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="167" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C9" s="168" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D9" s="168" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E9" s="169" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G9" s="167">
         <v>3</v>
@@ -21439,16 +21477,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="156" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C10" s="157" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D10" s="157" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E10" s="165" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G10" s="153">
         <v>4</v>
@@ -21468,16 +21506,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="159" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C11" s="157" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D11" s="157" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E11" s="165" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G11" s="156">
         <v>5</v>
@@ -21497,16 +21535,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="156" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C12" s="157" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D12" s="157" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E12" s="165" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G12" s="159">
         <v>6</v>
@@ -21526,16 +21564,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="161" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C13" s="162" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D13" s="162" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E13" s="166" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G13" s="167">
         <v>7</v>

</xml_diff>

<commit_message>
220504-v2 amend base gen block
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334740E2-DB8C-4A3B-8206-DAF67BC3E9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7AB442-33B6-411F-9AAD-A8C6F68C456D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="490">
   <si>
     <t>步骤</t>
   </si>
@@ -774,10 +774,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>UPD_5转置</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>UPD_6</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -1697,6 +1693,14 @@
   <si>
     <t>G_z(奇) 3</t>
     <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_5</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_5转置(seq_cnt等待转置完成)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3215,11 +3219,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>733426</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="638175" cy="419100"/>
+    <xdr:ext cx="495300" cy="338138"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="attachment-1647339334594-2d16b7a892b9bae2" descr="attachment-1647339334594-2d16b7a892b9bae2">
@@ -3240,8 +3244,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="733425" y="13096875"/>
-          <a:ext cx="638175" cy="419100"/>
+          <a:off x="733426" y="14320837"/>
+          <a:ext cx="495300" cy="338138"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12246,9 +12250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S274"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12621,7 +12625,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="172" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="54" t="s">
@@ -12699,14 +12703,14 @@
     <row r="19" spans="1:19" ht="11.25" customHeight="1">
       <c r="A19" s="93"/>
       <c r="B19" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F19" s="93"/>
       <c r="G19" s="40"/>
@@ -12735,7 +12739,7 @@
         <v>189</v>
       </c>
       <c r="E20" s="172" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -12813,16 +12817,16 @@
     <row r="23" spans="1:19" ht="15.75" customHeight="1">
       <c r="A23" s="93"/>
       <c r="B23" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F23" s="92"/>
       <c r="G23" s="40"/>
@@ -12927,14 +12931,14 @@
     <row r="27" spans="1:19">
       <c r="A27" s="3"/>
       <c r="B27" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="7"/>
@@ -13095,7 +13099,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="172" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="66" t="s">
@@ -13173,14 +13177,14 @@
     <row r="37" spans="1:19">
       <c r="A37" s="40"/>
       <c r="B37" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F37" s="93"/>
       <c r="G37" s="40"/>
@@ -13283,14 +13287,14 @@
     <row r="41" spans="1:19">
       <c r="A41" s="40"/>
       <c r="B41" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>231</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F41" s="93"/>
       <c r="G41" s="93"/>
@@ -13391,14 +13395,14 @@
     <row r="45" spans="1:19">
       <c r="A45" s="40"/>
       <c r="B45" s="47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D45" s="42"/>
       <c r="E45" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F45" s="93"/>
       <c r="G45" s="93"/>
@@ -13499,14 +13503,14 @@
     <row r="49" spans="1:19">
       <c r="A49" s="40"/>
       <c r="B49" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F49" s="92"/>
       <c r="G49" s="40"/>
@@ -13615,16 +13619,16 @@
     <row r="53" spans="1:19">
       <c r="A53" s="40"/>
       <c r="B53" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E53" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F53" s="92"/>
       <c r="G53" s="40"/>
@@ -13860,7 +13864,7 @@
       </c>
       <c r="D63" s="41"/>
       <c r="E63" s="101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F63" s="38"/>
       <c r="G63" s="40"/>
@@ -13936,14 +13940,14 @@
         <v>218</v>
       </c>
       <c r="B66" s="173" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C66" s="75" t="s">
         <v>180</v>
       </c>
       <c r="D66" s="41"/>
       <c r="E66" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F66" s="38"/>
       <c r="G66" s="40"/>
@@ -14028,7 +14032,7 @@
       </c>
       <c r="D69" s="24"/>
       <c r="E69" s="61" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -14100,16 +14104,18 @@
       <c r="S71" s="4"/>
     </row>
     <row r="72" spans="1:19">
-      <c r="A72" s="3"/>
+      <c r="A72" s="17" t="s">
+        <v>220</v>
+      </c>
       <c r="B72" s="94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C72" s="75" t="s">
         <v>181</v>
       </c>
       <c r="D72" s="45"/>
       <c r="E72" s="62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>187</v>
@@ -14185,14 +14191,14 @@
     <row r="75" spans="1:19">
       <c r="A75" s="93"/>
       <c r="B75" s="47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D75" s="42"/>
       <c r="E75" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F75" s="93"/>
       <c r="G75" s="40"/>
@@ -14210,14 +14216,14 @@
       <c r="S75" s="40"/>
     </row>
     <row r="76" spans="1:19">
-      <c r="A76" s="17" t="s">
-        <v>220</v>
+      <c r="A76" s="152" t="s">
+        <v>488</v>
       </c>
       <c r="B76" s="60" t="s">
         <v>64</v>
       </c>
       <c r="C76" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D76" s="63" t="s">
         <v>49</v>
@@ -14305,16 +14311,16 @@
     <row r="79" spans="1:19">
       <c r="A79" s="93"/>
       <c r="B79" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F79" s="93"/>
       <c r="G79" s="40"/>
@@ -14333,7 +14339,7 @@
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="17" t="s">
-        <v>221</v>
+        <v>489</v>
       </c>
       <c r="B80" s="58" t="s">
         <v>65</v>
@@ -14410,10 +14416,10 @@
     </row>
     <row r="83" spans="1:19">
       <c r="A83" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B83" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C83" s="90" t="s">
         <v>68</v>
@@ -14496,14 +14502,14 @@
     <row r="86" spans="1:19">
       <c r="A86" s="93"/>
       <c r="B86" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F86" s="93"/>
       <c r="G86" s="40"/>
@@ -14615,7 +14621,7 @@
         <v>69</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D90" s="44" t="s">
         <v>76</v>
@@ -14700,13 +14706,13 @@
     </row>
     <row r="93" spans="1:19">
       <c r="A93" s="91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B93" s="94" t="s">
         <v>69</v>
       </c>
       <c r="C93" s="95" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D93" s="96" t="s">
         <v>76</v>
@@ -14790,10 +14796,10 @@
     <row r="96" spans="1:19">
       <c r="A96" s="40"/>
       <c r="B96" s="47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D96" s="42"/>
       <c r="E96" s="48"/>
@@ -15041,10 +15047,10 @@
     <row r="106" spans="1:19">
       <c r="A106" s="4"/>
       <c r="B106" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C106" s="18" t="s">
         <v>224</v>
-      </c>
-      <c r="C106" s="18" t="s">
-        <v>225</v>
       </c>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
@@ -15066,10 +15072,10 @@
     <row r="107" spans="1:19">
       <c r="A107" s="4"/>
       <c r="B107" s="52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C107" s="52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
@@ -15091,10 +15097,10 @@
     <row r="108" spans="1:19">
       <c r="A108" s="4"/>
       <c r="B108" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C108" s="18" t="s">
         <v>226</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>227</v>
       </c>
       <c r="D108" s="18"/>
       <c r="E108" s="18"/>
@@ -15119,7 +15125,7 @@
         <v>183</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
@@ -15141,10 +15147,10 @@
     <row r="110" spans="1:19">
       <c r="A110" s="4"/>
       <c r="B110" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
@@ -15166,10 +15172,10 @@
     <row r="111" spans="1:19">
       <c r="A111" s="4"/>
       <c r="B111" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C111" s="18" t="s">
         <v>226</v>
-      </c>
-      <c r="C111" s="18" t="s">
-        <v>227</v>
       </c>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
@@ -18514,40 +18520,40 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.25" thickBot="1">
       <c r="B1" s="103" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="103" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="D1" s="103" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="E1" s="103" t="s">
         <v>241</v>
-      </c>
-      <c r="E1" s="103" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="2:5">
       <c r="B2" s="133" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C2" s="135" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D2" s="135"/>
       <c r="E2" s="136" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="137" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="140" t="s">
         <v>245</v>
-      </c>
-      <c r="C3" s="140" t="s">
-        <v>246</v>
       </c>
       <c r="D3" s="140"/>
       <c r="E3" s="141" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="14.25" thickBot="1">
@@ -18564,26 +18570,26 @@
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="133" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C5" s="135" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D5" s="135"/>
       <c r="E5" s="136" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="137" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="140" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D6" s="140"/>
       <c r="E6" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="14.25" thickBot="1">
@@ -18600,26 +18606,26 @@
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="133" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="135" t="s">
         <v>251</v>
-      </c>
-      <c r="C8" s="135" t="s">
-        <v>252</v>
       </c>
       <c r="D8" s="135"/>
       <c r="E8" s="136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="137" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" s="140" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="140"/>
       <c r="E9" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="14.25" thickBot="1">
@@ -18636,26 +18642,26 @@
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="133" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="135" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="135"/>
       <c r="E11" s="136" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="137" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" s="140" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D12" s="140"/>
       <c r="E12" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="14.25" thickBot="1">
@@ -18672,30 +18678,30 @@
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="133" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" s="135" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" s="135" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="136" t="s">
         <v>256</v>
-      </c>
-      <c r="D14" s="135" t="s">
-        <v>255</v>
-      </c>
-      <c r="E14" s="136" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="137" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15" s="140" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="140" t="s">
         <v>249</v>
       </c>
-      <c r="D15" s="140" t="s">
-        <v>250</v>
-      </c>
       <c r="E15" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.4" customHeight="1" thickBot="1">
@@ -18714,30 +18720,30 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="133" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="135" t="s">
         <v>253</v>
       </c>
-      <c r="C17" s="135" t="s">
+      <c r="D17" s="135" t="s">
         <v>254</v>
       </c>
-      <c r="D17" s="135" t="s">
-        <v>255</v>
-      </c>
       <c r="E17" s="136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="137" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C18" s="140" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D18" s="140" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E18" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="14.25" thickBot="1">
@@ -18756,37 +18762,37 @@
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="133" t="s">
+        <v>257</v>
+      </c>
+      <c r="C20" s="135" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" s="135" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="136" t="s">
         <v>258</v>
       </c>
-      <c r="C20" s="135" t="s">
-        <v>481</v>
-      </c>
-      <c r="D20" s="135" t="s">
-        <v>255</v>
-      </c>
-      <c r="E20" s="136" t="s">
+      <c r="F20" s="104" t="s">
         <v>259</v>
-      </c>
-      <c r="F20" s="104" t="s">
-        <v>260</v>
       </c>
       <c r="G20" s="104"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="137" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C21" s="140" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D21" s="140" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E21" s="141" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F21" s="103" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="14.25" thickBot="1">
@@ -18813,7 +18819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
@@ -18962,14 +18968,14 @@
     </row>
     <row r="2" spans="1:47">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="105">
         <v>1</v>
       </c>
       <c r="C2" s="106"/>
       <c r="D2" s="107" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2" s="105">
         <v>1</v>
@@ -18977,47 +18983,47 @@
       <c r="F2" s="106"/>
       <c r="G2" s="106"/>
       <c r="H2" s="108" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I2" s="109"/>
       <c r="J2" s="110"/>
       <c r="K2" s="109" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L2" s="109"/>
       <c r="M2" s="109"/>
       <c r="N2" s="108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O2" s="109"/>
       <c r="P2" s="109"/>
       <c r="Q2" s="108" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="R2" s="109"/>
       <c r="S2" s="111">
         <v>5</v>
       </c>
       <c r="T2" s="112" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="U2" s="111">
         <v>4</v>
       </c>
       <c r="V2" s="108" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="W2" s="110"/>
       <c r="X2" s="108" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y2" s="110"/>
       <c r="Z2" s="113" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AA2" s="110"/>
       <c r="AB2" s="114" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AC2" s="115">
         <v>-3</v>
@@ -19026,57 +19032,57 @@
         <v>0</v>
       </c>
       <c r="AE2" s="114" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AF2" s="115">
         <v>3</v>
       </c>
       <c r="AG2" s="108" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AH2" s="110"/>
       <c r="AI2" s="108" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AJ2" s="109"/>
       <c r="AK2" s="109"/>
       <c r="AL2" s="109"/>
       <c r="AM2" s="109"/>
       <c r="AN2" s="114" t="s">
+        <v>270</v>
+      </c>
+      <c r="AO2" s="116" t="s">
         <v>271</v>
       </c>
-      <c r="AO2" s="116" t="s">
+      <c r="AP2" s="108" t="s">
         <v>272</v>
       </c>
-      <c r="AP2" s="108" t="s">
+      <c r="AQ2" s="110" t="s">
         <v>273</v>
       </c>
-      <c r="AQ2" s="110" t="s">
+      <c r="AR2" s="108" t="s">
         <v>274</v>
       </c>
-      <c r="AR2" s="108" t="s">
+      <c r="AS2" s="110" t="s">
         <v>275</v>
       </c>
-      <c r="AS2" s="110" t="s">
+      <c r="AT2" s="108" t="s">
         <v>276</v>
       </c>
-      <c r="AT2" s="108" t="s">
+      <c r="AU2" s="110" t="s">
         <v>277</v>
-      </c>
-      <c r="AU2" s="110" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:47" ht="14.25" thickBot="1">
       <c r="A3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B3" s="117"/>
       <c r="C3" s="118">
         <v>1</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E3" s="120"/>
       <c r="F3" s="118">
@@ -19140,33 +19146,33 @@
       <c r="AL3" s="124"/>
       <c r="AM3" s="124"/>
       <c r="AN3" s="120" t="s">
+        <v>280</v>
+      </c>
+      <c r="AO3" s="122" t="s">
         <v>281</v>
       </c>
-      <c r="AO3" s="122" t="s">
+      <c r="AP3" s="120" t="s">
         <v>282</v>
       </c>
-      <c r="AP3" s="120" t="s">
+      <c r="AQ3" s="122" t="s">
         <v>283</v>
       </c>
-      <c r="AQ3" s="122" t="s">
+      <c r="AR3" s="120" t="s">
         <v>284</v>
       </c>
-      <c r="AR3" s="120" t="s">
+      <c r="AS3" s="122" t="s">
         <v>285</v>
       </c>
-      <c r="AS3" s="122" t="s">
+      <c r="AT3" s="120" t="s">
         <v>286</v>
       </c>
-      <c r="AT3" s="120" t="s">
+      <c r="AU3" s="122" t="s">
         <v>287</v>
-      </c>
-      <c r="AU3" s="122" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:47" ht="14.25" thickBot="1">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" s="130"/>
       <c r="C4" s="131"/>
@@ -19174,10 +19180,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="107" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F4" s="119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G4" s="131">
         <v>1</v>
@@ -19214,33 +19220,33 @@
       <c r="AG4" s="132"/>
       <c r="AH4" s="132"/>
       <c r="AN4" s="120" t="s">
+        <v>289</v>
+      </c>
+      <c r="AO4" s="122" t="s">
         <v>290</v>
       </c>
-      <c r="AO4" s="122" t="s">
+      <c r="AP4" s="120" t="s">
         <v>291</v>
       </c>
-      <c r="AP4" s="120" t="s">
+      <c r="AQ4" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="AQ4" s="122" t="s">
+      <c r="AR4" s="120" t="s">
         <v>293</v>
       </c>
-      <c r="AR4" s="120" t="s">
+      <c r="AS4" s="122" t="s">
         <v>294</v>
       </c>
-      <c r="AS4" s="122" t="s">
+      <c r="AT4" s="120" t="s">
         <v>295</v>
       </c>
-      <c r="AT4" s="120" t="s">
+      <c r="AU4" s="122" t="s">
         <v>296</v>
-      </c>
-      <c r="AU4" s="122" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="14.25" thickBot="1">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E5" s="130"/>
       <c r="F5" s="131"/>
@@ -19267,45 +19273,45 @@
       <c r="AG5" s="132"/>
       <c r="AH5" s="132"/>
       <c r="AN5" s="123" t="s">
+        <v>298</v>
+      </c>
+      <c r="AO5" s="127" t="s">
         <v>299</v>
       </c>
-      <c r="AO5" s="127" t="s">
+      <c r="AP5" s="123" t="s">
         <v>300</v>
       </c>
-      <c r="AP5" s="123" t="s">
+      <c r="AQ5" s="127" t="s">
         <v>301</v>
       </c>
-      <c r="AQ5" s="127" t="s">
+      <c r="AR5" s="123" t="s">
         <v>302</v>
       </c>
-      <c r="AR5" s="123" t="s">
+      <c r="AS5" s="127" t="s">
         <v>303</v>
       </c>
-      <c r="AS5" s="127" t="s">
+      <c r="AT5" s="123" t="s">
         <v>304</v>
       </c>
-      <c r="AT5" s="123" t="s">
+      <c r="AU5" s="127" t="s">
         <v>305</v>
-      </c>
-      <c r="AU5" s="127" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
       <c r="B6" s="179" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C6" s="180"/>
       <c r="D6" s="181"/>
       <c r="E6" s="179" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F6" s="180"/>
       <c r="G6" s="181"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
       <c r="B7" s="179" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C7" s="180"/>
       <c r="D7" s="180"/>
@@ -19322,7 +19328,7 @@
       <c r="O7" s="180"/>
       <c r="P7" s="181"/>
       <c r="Q7" s="179" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R7" s="180"/>
       <c r="S7" s="180"/>
@@ -19335,7 +19341,7 @@
       <c r="Z7" s="180"/>
       <c r="AA7" s="181"/>
       <c r="AB7" s="179" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AC7" s="180"/>
       <c r="AD7" s="180"/>
@@ -19359,10 +19365,10 @@
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" t="s">
+        <v>311</v>
+      </c>
+      <c r="AM9" t="s">
         <v>312</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -19370,7 +19376,7 @@
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
       <c r="H10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -19380,7 +19386,7 @@
     </row>
     <row r="15" spans="1:47">
       <c r="AB15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -19431,10 +19437,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="138" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="139" t="s">
         <v>316</v>
-      </c>
-      <c r="C2" s="139" t="s">
-        <v>317</v>
       </c>
       <c r="D2" s="140"/>
       <c r="E2" s="140"/>
@@ -19452,13 +19458,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="138" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="139" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="139" t="s">
+      <c r="D3" s="139" t="s">
         <v>319</v>
-      </c>
-      <c r="D3" s="139" t="s">
-        <v>320</v>
       </c>
       <c r="E3" s="140"/>
       <c r="F3" s="140"/>
@@ -19475,16 +19481,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="138" t="s">
+        <v>320</v>
+      </c>
+      <c r="C4" s="139" t="s">
         <v>321</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="D4" s="139" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="E4" s="139" t="s">
         <v>323</v>
-      </c>
-      <c r="E4" s="139" t="s">
-        <v>324</v>
       </c>
       <c r="F4" s="140"/>
       <c r="G4" s="140"/>
@@ -19500,19 +19506,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="138" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" s="139" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="139" t="s">
+      <c r="D5" s="139" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="139" t="s">
+      <c r="E5" s="139" t="s">
         <v>327</v>
       </c>
-      <c r="E5" s="139" t="s">
+      <c r="F5" s="139" t="s">
         <v>328</v>
-      </c>
-      <c r="F5" s="139" t="s">
-        <v>329</v>
       </c>
       <c r="G5" s="140"/>
       <c r="H5" s="140"/>
@@ -19527,22 +19533,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="138" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="139" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="D6" s="139" t="s">
         <v>331</v>
       </c>
-      <c r="D6" s="139" t="s">
+      <c r="E6" s="139" t="s">
         <v>332</v>
       </c>
-      <c r="E6" s="139" t="s">
+      <c r="F6" s="139" t="s">
         <v>333</v>
       </c>
-      <c r="F6" s="139" t="s">
+      <c r="G6" s="139" t="s">
         <v>334</v>
-      </c>
-      <c r="G6" s="139" t="s">
-        <v>335</v>
       </c>
       <c r="H6" s="140"/>
       <c r="I6" s="140"/>
@@ -19556,25 +19562,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="138" t="s">
+        <v>335</v>
+      </c>
+      <c r="C7" s="139" t="s">
         <v>336</v>
       </c>
-      <c r="C7" s="139" t="s">
+      <c r="D7" s="139" t="s">
         <v>337</v>
       </c>
-      <c r="D7" s="139" t="s">
+      <c r="E7" s="139" t="s">
         <v>338</v>
       </c>
-      <c r="E7" s="139" t="s">
+      <c r="F7" s="139" t="s">
         <v>339</v>
       </c>
-      <c r="F7" s="139" t="s">
+      <c r="G7" s="139" t="s">
         <v>340</v>
       </c>
-      <c r="G7" s="139" t="s">
+      <c r="H7" s="139" t="s">
         <v>341</v>
-      </c>
-      <c r="H7" s="139" t="s">
-        <v>342</v>
       </c>
       <c r="I7" s="140"/>
       <c r="J7" s="140"/>
@@ -19587,28 +19593,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="138" t="s">
+        <v>342</v>
+      </c>
+      <c r="C8" s="139" t="s">
         <v>343</v>
       </c>
-      <c r="C8" s="139" t="s">
+      <c r="D8" s="139" t="s">
         <v>344</v>
       </c>
-      <c r="D8" s="139" t="s">
+      <c r="E8" s="139" t="s">
         <v>345</v>
       </c>
-      <c r="E8" s="139" t="s">
+      <c r="F8" s="139" t="s">
         <v>346</v>
       </c>
-      <c r="F8" s="139" t="s">
+      <c r="G8" s="139" t="s">
         <v>347</v>
       </c>
-      <c r="G8" s="139" t="s">
+      <c r="H8" s="139" t="s">
         <v>348</v>
       </c>
-      <c r="H8" s="139" t="s">
+      <c r="I8" s="139" t="s">
         <v>349</v>
-      </c>
-      <c r="I8" s="139" t="s">
-        <v>350</v>
       </c>
       <c r="J8" s="140"/>
       <c r="K8" s="140"/>
@@ -19620,31 +19626,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="138" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="139" t="s">
         <v>351</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="D9" s="139" t="s">
         <v>352</v>
       </c>
-      <c r="D9" s="139" t="s">
+      <c r="E9" s="139" t="s">
         <v>353</v>
       </c>
-      <c r="E9" s="139" t="s">
+      <c r="F9" s="139" t="s">
         <v>354</v>
       </c>
-      <c r="F9" s="139" t="s">
+      <c r="G9" s="139" t="s">
         <v>355</v>
       </c>
-      <c r="G9" s="139" t="s">
+      <c r="H9" s="139" t="s">
         <v>356</v>
       </c>
-      <c r="H9" s="139" t="s">
+      <c r="I9" s="139" t="s">
         <v>357</v>
       </c>
-      <c r="I9" s="139" t="s">
+      <c r="J9" s="139" t="s">
         <v>358</v>
-      </c>
-      <c r="J9" s="139" t="s">
-        <v>359</v>
       </c>
       <c r="K9" s="140"/>
       <c r="L9" s="140"/>
@@ -19655,34 +19661,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="138" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="139" t="s">
         <v>360</v>
       </c>
-      <c r="C10" s="139" t="s">
+      <c r="D10" s="139" t="s">
         <v>361</v>
       </c>
-      <c r="D10" s="139" t="s">
+      <c r="E10" s="139" t="s">
         <v>362</v>
       </c>
-      <c r="E10" s="139" t="s">
+      <c r="F10" s="139" t="s">
         <v>363</v>
       </c>
-      <c r="F10" s="139" t="s">
+      <c r="G10" s="139" t="s">
         <v>364</v>
       </c>
-      <c r="G10" s="139" t="s">
+      <c r="H10" s="139" t="s">
         <v>365</v>
       </c>
-      <c r="H10" s="139" t="s">
+      <c r="I10" s="139" t="s">
         <v>366</v>
       </c>
-      <c r="I10" s="139" t="s">
+      <c r="J10" s="139" t="s">
         <v>367</v>
       </c>
-      <c r="J10" s="139" t="s">
+      <c r="K10" s="139" t="s">
         <v>368</v>
-      </c>
-      <c r="K10" s="139" t="s">
-        <v>369</v>
       </c>
       <c r="L10" s="140"/>
       <c r="M10" s="141"/>
@@ -19692,37 +19698,37 @@
         <v>10</v>
       </c>
       <c r="B11" s="138" t="s">
+        <v>369</v>
+      </c>
+      <c r="C11" s="139" t="s">
         <v>370</v>
       </c>
-      <c r="C11" s="139" t="s">
+      <c r="D11" s="139" t="s">
         <v>371</v>
       </c>
-      <c r="D11" s="139" t="s">
+      <c r="E11" s="139" t="s">
         <v>372</v>
       </c>
-      <c r="E11" s="139" t="s">
+      <c r="F11" s="139" t="s">
         <v>373</v>
       </c>
-      <c r="F11" s="139" t="s">
+      <c r="G11" s="139" t="s">
         <v>374</v>
       </c>
-      <c r="G11" s="139" t="s">
+      <c r="H11" s="139" t="s">
         <v>375</v>
       </c>
-      <c r="H11" s="139" t="s">
+      <c r="I11" s="139" t="s">
         <v>376</v>
       </c>
-      <c r="I11" s="139" t="s">
+      <c r="J11" s="139" t="s">
         <v>377</v>
       </c>
-      <c r="J11" s="139" t="s">
+      <c r="K11" s="139" t="s">
         <v>378</v>
       </c>
-      <c r="K11" s="139" t="s">
+      <c r="L11" s="139" t="s">
         <v>379</v>
-      </c>
-      <c r="L11" s="139" t="s">
-        <v>380</v>
       </c>
       <c r="M11" s="141"/>
     </row>
@@ -19731,497 +19737,497 @@
         <v>11</v>
       </c>
       <c r="B12" s="143" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" s="144" t="s">
         <v>381</v>
       </c>
-      <c r="C12" s="144" t="s">
+      <c r="D12" s="144" t="s">
         <v>382</v>
       </c>
-      <c r="D12" s="144" t="s">
+      <c r="E12" s="144" t="s">
         <v>383</v>
       </c>
-      <c r="E12" s="144" t="s">
+      <c r="F12" s="145" t="s">
         <v>384</v>
       </c>
-      <c r="F12" s="145" t="s">
+      <c r="G12" s="144" t="s">
         <v>385</v>
       </c>
-      <c r="G12" s="144" t="s">
+      <c r="H12" s="144" t="s">
         <v>386</v>
       </c>
-      <c r="H12" s="144" t="s">
+      <c r="I12" s="144" t="s">
         <v>387</v>
       </c>
-      <c r="I12" s="144" t="s">
+      <c r="J12" s="144" t="s">
         <v>388</v>
       </c>
-      <c r="J12" s="144" t="s">
+      <c r="K12" s="144" t="s">
         <v>389</v>
       </c>
-      <c r="K12" s="144" t="s">
+      <c r="L12" s="144" t="s">
         <v>390</v>
       </c>
-      <c r="L12" s="144" t="s">
+      <c r="M12" s="146" t="s">
         <v>391</v>
-      </c>
-      <c r="M12" s="146" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B14" s="147"/>
       <c r="C14" s="148" t="s">
+        <v>342</v>
+      </c>
+      <c r="D14" s="149" t="s">
         <v>343</v>
       </c>
-      <c r="D14" s="149" t="s">
+      <c r="E14" s="149" t="s">
         <v>344</v>
       </c>
-      <c r="E14" s="149" t="s">
+      <c r="F14" s="149" t="s">
         <v>345</v>
       </c>
-      <c r="F14" s="149" t="s">
+      <c r="G14" s="149" t="s">
         <v>346</v>
       </c>
-      <c r="G14" s="149" t="s">
+      <c r="H14" s="149" t="s">
         <v>347</v>
       </c>
-      <c r="H14" s="149" t="s">
+      <c r="I14" s="149" t="s">
         <v>348</v>
       </c>
-      <c r="I14" s="149" t="s">
+      <c r="J14" s="149" t="s">
         <v>349</v>
       </c>
-      <c r="J14" s="149" t="s">
+      <c r="K14" s="148" t="s">
         <v>350</v>
       </c>
-      <c r="K14" s="148" t="s">
+      <c r="L14" s="149" t="s">
         <v>351</v>
       </c>
-      <c r="L14" s="149" t="s">
+      <c r="M14" s="149" t="s">
         <v>352</v>
       </c>
-      <c r="M14" s="149" t="s">
+      <c r="N14" s="149" t="s">
         <v>353</v>
       </c>
-      <c r="N14" s="149" t="s">
+      <c r="O14" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="O14" s="149" t="s">
+      <c r="P14" s="149" t="s">
         <v>355</v>
       </c>
-      <c r="P14" s="149" t="s">
+      <c r="Q14" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="Q14" s="149" t="s">
+      <c r="R14" s="149" t="s">
         <v>357</v>
       </c>
-      <c r="R14" s="149" t="s">
+      <c r="S14" s="149" t="s">
         <v>358</v>
       </c>
-      <c r="S14" s="149" t="s">
-        <v>359</v>
-      </c>
       <c r="T14" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="U14" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="V14" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W14" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="103" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B15" s="148" t="s">
+        <v>315</v>
+      </c>
+      <c r="C15" s="149" t="s">
         <v>316</v>
       </c>
-      <c r="C15" s="149" t="s">
-        <v>317</v>
-      </c>
       <c r="D15" s="148" t="s">
+        <v>335</v>
+      </c>
+      <c r="E15" s="149" t="s">
         <v>336</v>
       </c>
-      <c r="E15" s="149" t="s">
+      <c r="F15" s="149" t="s">
         <v>337</v>
       </c>
-      <c r="F15" s="149" t="s">
+      <c r="G15" s="149" t="s">
         <v>338</v>
       </c>
-      <c r="G15" s="149" t="s">
+      <c r="H15" s="149" t="s">
         <v>339</v>
       </c>
-      <c r="H15" s="149" t="s">
+      <c r="I15" s="149" t="s">
         <v>340</v>
       </c>
-      <c r="I15" s="149" t="s">
+      <c r="J15" s="149" t="s">
         <v>341</v>
       </c>
-      <c r="J15" s="149" t="s">
-        <v>342</v>
-      </c>
       <c r="K15" s="148" t="s">
+        <v>359</v>
+      </c>
+      <c r="L15" s="149" t="s">
         <v>360</v>
       </c>
-      <c r="L15" s="149" t="s">
+      <c r="M15" s="149" t="s">
         <v>361</v>
       </c>
-      <c r="M15" s="149" t="s">
+      <c r="N15" s="149" t="s">
         <v>362</v>
       </c>
-      <c r="N15" s="149" t="s">
+      <c r="O15" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="O15" s="149" t="s">
+      <c r="P15" s="149" t="s">
         <v>364</v>
       </c>
-      <c r="P15" s="149" t="s">
+      <c r="Q15" s="149" t="s">
         <v>365</v>
       </c>
-      <c r="Q15" s="149" t="s">
+      <c r="R15" s="149" t="s">
         <v>366</v>
       </c>
-      <c r="R15" s="149" t="s">
+      <c r="S15" s="149" t="s">
         <v>367</v>
       </c>
-      <c r="S15" s="149" t="s">
+      <c r="T15" s="149" t="s">
         <v>368</v>
       </c>
-      <c r="T15" s="149" t="s">
-        <v>369</v>
-      </c>
       <c r="U15" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="V15" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W15" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B16" s="148" t="s">
+        <v>317</v>
+      </c>
+      <c r="C16" s="149" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="149" t="s">
+      <c r="D16" s="149" t="s">
         <v>319</v>
       </c>
-      <c r="D16" s="149" t="s">
-        <v>320</v>
-      </c>
       <c r="E16" s="148" t="s">
+        <v>329</v>
+      </c>
+      <c r="F16" s="149" t="s">
         <v>330</v>
       </c>
-      <c r="F16" s="149" t="s">
+      <c r="G16" s="149" t="s">
         <v>331</v>
       </c>
-      <c r="G16" s="149" t="s">
+      <c r="H16" s="149" t="s">
         <v>332</v>
       </c>
-      <c r="H16" s="149" t="s">
+      <c r="I16" s="149" t="s">
         <v>333</v>
       </c>
-      <c r="I16" s="149" t="s">
+      <c r="J16" s="149" t="s">
         <v>334</v>
       </c>
-      <c r="J16" s="149" t="s">
-        <v>335</v>
-      </c>
       <c r="K16" s="148" t="s">
+        <v>369</v>
+      </c>
+      <c r="L16" s="149" t="s">
         <v>370</v>
       </c>
-      <c r="L16" s="149" t="s">
+      <c r="M16" s="149" t="s">
         <v>371</v>
       </c>
-      <c r="M16" s="149" t="s">
+      <c r="N16" s="149" t="s">
         <v>372</v>
       </c>
-      <c r="N16" s="149" t="s">
+      <c r="O16" s="149" t="s">
         <v>373</v>
       </c>
-      <c r="O16" s="149" t="s">
+      <c r="P16" s="149" t="s">
         <v>374</v>
       </c>
-      <c r="P16" s="149" t="s">
+      <c r="Q16" s="149" t="s">
         <v>375</v>
       </c>
-      <c r="Q16" s="149" t="s">
+      <c r="R16" s="149" t="s">
         <v>376</v>
       </c>
-      <c r="R16" s="149" t="s">
+      <c r="S16" s="149" t="s">
         <v>377</v>
       </c>
-      <c r="S16" s="149" t="s">
+      <c r="T16" s="149" t="s">
         <v>378</v>
       </c>
-      <c r="T16" s="149" t="s">
+      <c r="U16" s="149" t="s">
         <v>379</v>
       </c>
-      <c r="U16" s="149" t="s">
-        <v>380</v>
-      </c>
       <c r="V16" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W16" s="103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B17" s="148" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="149" t="s">
         <v>321</v>
       </c>
-      <c r="C17" s="149" t="s">
+      <c r="D17" s="149" t="s">
         <v>322</v>
       </c>
-      <c r="D17" s="149" t="s">
+      <c r="E17" s="149" t="s">
         <v>323</v>
       </c>
-      <c r="E17" s="149" t="s">
+      <c r="F17" s="148" t="s">
         <v>324</v>
       </c>
-      <c r="F17" s="148" t="s">
+      <c r="G17" s="149" t="s">
         <v>325</v>
       </c>
-      <c r="G17" s="149" t="s">
+      <c r="H17" s="149" t="s">
         <v>326</v>
       </c>
-      <c r="H17" s="149" t="s">
+      <c r="I17" s="149" t="s">
         <v>327</v>
       </c>
-      <c r="I17" s="149" t="s">
+      <c r="J17" s="149" t="s">
         <v>328</v>
       </c>
-      <c r="J17" s="149" t="s">
-        <v>329</v>
-      </c>
       <c r="K17" s="148" t="s">
+        <v>380</v>
+      </c>
+      <c r="L17" s="149" t="s">
         <v>381</v>
       </c>
-      <c r="L17" s="149" t="s">
+      <c r="M17" s="149" t="s">
         <v>382</v>
       </c>
-      <c r="M17" s="149" t="s">
+      <c r="N17" s="149" t="s">
         <v>383</v>
       </c>
-      <c r="N17" s="149" t="s">
+      <c r="O17" s="150" t="s">
         <v>384</v>
       </c>
-      <c r="O17" s="150" t="s">
+      <c r="P17" s="149" t="s">
         <v>385</v>
       </c>
-      <c r="P17" s="149" t="s">
+      <c r="Q17" s="149" t="s">
         <v>386</v>
       </c>
-      <c r="Q17" s="149" t="s">
+      <c r="R17" s="149" t="s">
         <v>387</v>
       </c>
-      <c r="R17" s="149" t="s">
+      <c r="S17" s="149" t="s">
         <v>388</v>
       </c>
-      <c r="S17" s="149" t="s">
+      <c r="T17" s="149" t="s">
         <v>389</v>
       </c>
-      <c r="T17" s="149" t="s">
+      <c r="U17" s="149" t="s">
         <v>390</v>
       </c>
-      <c r="U17" s="149" t="s">
+      <c r="V17" s="149" t="s">
         <v>391</v>
       </c>
-      <c r="V17" s="149" t="s">
+      <c r="W17" s="103" t="s">
         <v>392</v>
-      </c>
-      <c r="W17" s="103" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="148" t="s">
+        <v>350</v>
+      </c>
+      <c r="C19" s="149" t="s">
         <v>351</v>
       </c>
-      <c r="C19" s="149" t="s">
+      <c r="D19" s="149" t="s">
         <v>352</v>
       </c>
-      <c r="D19" s="149" t="s">
+      <c r="E19" s="149" t="s">
         <v>353</v>
       </c>
-      <c r="E19" s="149" t="s">
+      <c r="F19" s="149" t="s">
         <v>354</v>
       </c>
-      <c r="F19" s="149" t="s">
+      <c r="G19" s="149" t="s">
         <v>355</v>
       </c>
-      <c r="G19" s="149" t="s">
+      <c r="H19" s="149" t="s">
         <v>356</v>
       </c>
-      <c r="H19" s="149" t="s">
+      <c r="I19" s="149" t="s">
         <v>357</v>
       </c>
-      <c r="I19" s="149" t="s">
+      <c r="J19" s="149" t="s">
         <v>358</v>
-      </c>
-      <c r="J19" s="149" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="103" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B20" s="148" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" s="149" t="s">
         <v>360</v>
       </c>
-      <c r="C20" s="149" t="s">
+      <c r="D20" s="149" t="s">
         <v>361</v>
       </c>
-      <c r="D20" s="149" t="s">
+      <c r="E20" s="149" t="s">
         <v>362</v>
       </c>
-      <c r="E20" s="149" t="s">
+      <c r="F20" s="149" t="s">
         <v>363</v>
       </c>
-      <c r="F20" s="149" t="s">
+      <c r="G20" s="149" t="s">
         <v>364</v>
       </c>
-      <c r="G20" s="149" t="s">
+      <c r="H20" s="149" t="s">
         <v>365</v>
       </c>
-      <c r="H20" s="149" t="s">
+      <c r="I20" s="149" t="s">
         <v>366</v>
       </c>
-      <c r="I20" s="149" t="s">
+      <c r="J20" s="149" t="s">
         <v>367</v>
       </c>
-      <c r="J20" s="149" t="s">
+      <c r="K20" s="149" t="s">
         <v>368</v>
-      </c>
-      <c r="K20" s="149" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B21" s="148" t="s">
+        <v>369</v>
+      </c>
+      <c r="C21" s="149" t="s">
         <v>370</v>
       </c>
-      <c r="C21" s="149" t="s">
+      <c r="D21" s="149" t="s">
         <v>371</v>
       </c>
-      <c r="D21" s="149" t="s">
+      <c r="E21" s="149" t="s">
         <v>372</v>
       </c>
-      <c r="E21" s="149" t="s">
+      <c r="F21" s="149" t="s">
         <v>373</v>
       </c>
-      <c r="F21" s="149" t="s">
+      <c r="G21" s="149" t="s">
         <v>374</v>
       </c>
-      <c r="G21" s="149" t="s">
+      <c r="H21" s="149" t="s">
         <v>375</v>
       </c>
-      <c r="H21" s="149" t="s">
+      <c r="I21" s="149" t="s">
         <v>376</v>
       </c>
-      <c r="I21" s="149" t="s">
+      <c r="J21" s="149" t="s">
         <v>377</v>
       </c>
-      <c r="J21" s="149" t="s">
+      <c r="K21" s="149" t="s">
         <v>378</v>
       </c>
-      <c r="K21" s="149" t="s">
+      <c r="L21" s="149" t="s">
         <v>379</v>
-      </c>
-      <c r="L21" s="149" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" s="148" t="s">
+        <v>380</v>
+      </c>
+      <c r="C22" s="149" t="s">
         <v>381</v>
       </c>
-      <c r="C22" s="149" t="s">
+      <c r="D22" s="149" t="s">
         <v>382</v>
       </c>
-      <c r="D22" s="149" t="s">
+      <c r="E22" s="149" t="s">
         <v>383</v>
       </c>
-      <c r="E22" s="149" t="s">
+      <c r="F22" s="150" t="s">
         <v>384</v>
       </c>
-      <c r="F22" s="150" t="s">
+      <c r="G22" s="149" t="s">
         <v>385</v>
       </c>
-      <c r="G22" s="149" t="s">
+      <c r="H22" s="149" t="s">
         <v>386</v>
       </c>
-      <c r="H22" s="149" t="s">
+      <c r="I22" s="149" t="s">
         <v>387</v>
       </c>
-      <c r="I22" s="149" t="s">
+      <c r="J22" s="149" t="s">
         <v>388</v>
       </c>
-      <c r="J22" s="149" t="s">
+      <c r="K22" s="149" t="s">
         <v>389</v>
       </c>
-      <c r="K22" s="149" t="s">
+      <c r="L22" s="149" t="s">
         <v>390</v>
       </c>
-      <c r="L22" s="149" t="s">
+      <c r="M22" s="149" t="s">
         <v>391</v>
-      </c>
-      <c r="M22" s="149" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="103" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B24" s="103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C24" s="103" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D24" s="103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E24" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H24" s="103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I24" s="103" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J24" s="103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K24" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -20230,13 +20236,13 @@
       </c>
       <c r="B25" s="147"/>
       <c r="C25" s="148" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D25" s="148" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E25" s="148" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H25" s="103">
         <v>0</v>
@@ -20256,16 +20262,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="148" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C26" s="149" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D26" s="149" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E26" s="149" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H26" s="103">
         <v>0</v>
@@ -20285,16 +20291,16 @@
         <v>2</v>
       </c>
       <c r="B27" s="149" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C27" s="148" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D27" s="149" t="s">
+        <v>394</v>
+      </c>
+      <c r="E27" s="149" t="s">
         <v>395</v>
-      </c>
-      <c r="E27" s="149" t="s">
-        <v>396</v>
       </c>
       <c r="H27" s="103">
         <v>1</v>
@@ -20314,16 +20320,16 @@
         <v>3</v>
       </c>
       <c r="B28" s="149" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C28" s="149" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D28" s="148" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E28" s="149" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H28" s="103">
         <v>2</v>
@@ -20343,16 +20349,16 @@
         <v>4</v>
       </c>
       <c r="B29" s="149" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C29" s="149" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D29" s="149" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E29" s="148" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H29" s="103">
         <v>3</v>
@@ -20372,16 +20378,16 @@
         <v>5</v>
       </c>
       <c r="B30" s="149" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C30" s="149" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D30" s="149" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E30" s="149" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H30" s="103">
         <v>4</v>
@@ -20401,16 +20407,16 @@
         <v>6</v>
       </c>
       <c r="B31" s="149" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C31" s="149" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D31" s="149" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E31" s="149" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H31" s="103">
         <v>5</v>
@@ -20430,16 +20436,16 @@
         <v>7</v>
       </c>
       <c r="B32" s="149" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C32" s="149" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D32" s="149" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E32" s="149" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H32" s="103">
         <v>6</v>
@@ -20459,16 +20465,16 @@
         <v>8</v>
       </c>
       <c r="B33" s="149" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C33" s="149" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D33" s="149" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E33" s="149" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H33" s="103">
         <v>7</v>
@@ -20488,16 +20494,16 @@
         <v>9</v>
       </c>
       <c r="B34" s="148" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C34" s="148" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D34" s="148" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E34" s="148" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H34" s="103">
         <v>8</v>
@@ -20517,16 +20523,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="149" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C35" s="149" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D35" s="149" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E35" s="149" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H35" s="103">
         <v>9</v>
@@ -20546,16 +20552,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="149" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C36" s="149" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D36" s="149" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E36" s="149" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H36" s="103">
         <v>10</v>
@@ -20575,16 +20581,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="149" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C37" s="149" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D37" s="149" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E37" s="149" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H37" s="103">
         <v>11</v>
@@ -20604,16 +20610,16 @@
         <v>13</v>
       </c>
       <c r="B38" s="149" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C38" s="149" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D38" s="149" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E38" s="149" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H38" s="103">
         <v>12</v>
@@ -20633,16 +20639,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="149" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C39" s="149" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D39" s="149" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E39" s="149" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H39" s="103">
         <v>13</v>
@@ -20662,16 +20668,16 @@
         <v>15</v>
       </c>
       <c r="B40" s="149" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C40" s="149" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D40" s="149" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E40" s="149" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H40" s="103">
         <v>14</v>
@@ -20691,16 +20697,16 @@
         <v>16</v>
       </c>
       <c r="B41" s="149" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C41" s="149" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D41" s="149" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E41" s="149" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H41" s="103">
         <v>15</v>
@@ -20720,16 +20726,16 @@
         <v>17</v>
       </c>
       <c r="B42" s="149" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C42" s="149" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D42" s="149" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E42" s="149" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H42" s="103">
         <v>16</v>
@@ -20749,16 +20755,16 @@
         <v>18</v>
       </c>
       <c r="B43" s="148" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C43" s="149" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D43" s="149" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E43" s="149" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H43" s="103">
         <v>17</v>
@@ -20778,16 +20784,16 @@
         <v>19</v>
       </c>
       <c r="B44" s="151" t="s">
+        <v>398</v>
+      </c>
+      <c r="C44" s="148" t="s">
         <v>399</v>
       </c>
-      <c r="C44" s="148" t="s">
-        <v>400</v>
-      </c>
       <c r="D44" s="149" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E44" s="149" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H44" s="103">
         <v>18</v>
@@ -20807,16 +20813,16 @@
         <v>20</v>
       </c>
       <c r="B45" s="151" t="s">
+        <v>400</v>
+      </c>
+      <c r="C45" s="151" t="s">
         <v>401</v>
       </c>
-      <c r="C45" s="151" t="s">
+      <c r="D45" s="148" t="s">
         <v>402</v>
       </c>
-      <c r="D45" s="148" t="s">
-        <v>403</v>
-      </c>
       <c r="E45" s="149" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H45" s="103">
         <v>19</v>
@@ -20836,16 +20842,16 @@
         <v>21</v>
       </c>
       <c r="B46" s="151" t="s">
+        <v>403</v>
+      </c>
+      <c r="C46" s="151" t="s">
         <v>404</v>
       </c>
-      <c r="C46" s="151" t="s">
+      <c r="D46" s="151" t="s">
         <v>405</v>
       </c>
-      <c r="D46" s="151" t="s">
+      <c r="E46" s="148" t="s">
         <v>406</v>
-      </c>
-      <c r="E46" s="148" t="s">
-        <v>407</v>
       </c>
       <c r="H46" s="103">
         <v>20</v>
@@ -20865,16 +20871,16 @@
         <v>22</v>
       </c>
       <c r="B47" s="151" t="s">
+        <v>407</v>
+      </c>
+      <c r="C47" s="151" t="s">
         <v>408</v>
       </c>
-      <c r="C47" s="151" t="s">
+      <c r="D47" s="151" t="s">
         <v>409</v>
       </c>
-      <c r="D47" s="151" t="s">
+      <c r="E47" s="151" t="s">
         <v>410</v>
-      </c>
-      <c r="E47" s="151" t="s">
-        <v>411</v>
       </c>
       <c r="H47" s="103">
         <v>21</v>
@@ -20894,16 +20900,16 @@
         <v>23</v>
       </c>
       <c r="B48" s="151" t="s">
+        <v>411</v>
+      </c>
+      <c r="C48" s="151" t="s">
         <v>412</v>
       </c>
-      <c r="C48" s="151" t="s">
+      <c r="D48" s="151" t="s">
         <v>413</v>
       </c>
-      <c r="D48" s="151" t="s">
+      <c r="E48" s="151" t="s">
         <v>414</v>
-      </c>
-      <c r="E48" s="151" t="s">
-        <v>415</v>
       </c>
       <c r="H48" s="103">
         <v>22</v>
@@ -20923,16 +20929,16 @@
         <v>24</v>
       </c>
       <c r="B49" s="151" t="s">
+        <v>415</v>
+      </c>
+      <c r="C49" s="151" t="s">
         <v>416</v>
       </c>
-      <c r="C49" s="151" t="s">
+      <c r="D49" s="151" t="s">
         <v>417</v>
       </c>
-      <c r="D49" s="151" t="s">
+      <c r="E49" s="151" t="s">
         <v>418</v>
-      </c>
-      <c r="E49" s="151" t="s">
-        <v>419</v>
       </c>
       <c r="H49" s="103">
         <v>23</v>
@@ -20952,16 +20958,16 @@
         <v>25</v>
       </c>
       <c r="B50" s="151" t="s">
+        <v>419</v>
+      </c>
+      <c r="C50" s="151" t="s">
         <v>420</v>
       </c>
-      <c r="C50" s="151" t="s">
+      <c r="D50" s="151" t="s">
         <v>421</v>
       </c>
-      <c r="D50" s="151" t="s">
+      <c r="E50" s="151" t="s">
         <v>422</v>
-      </c>
-      <c r="E50" s="151" t="s">
-        <v>423</v>
       </c>
       <c r="H50" s="103">
         <v>24</v>
@@ -20981,16 +20987,16 @@
         <v>26</v>
       </c>
       <c r="B51" s="151" t="s">
+        <v>423</v>
+      </c>
+      <c r="C51" s="151" t="s">
         <v>424</v>
       </c>
-      <c r="C51" s="151" t="s">
+      <c r="D51" s="151" t="s">
         <v>425</v>
       </c>
-      <c r="D51" s="151" t="s">
+      <c r="E51" s="151" t="s">
         <v>426</v>
-      </c>
-      <c r="E51" s="151" t="s">
-        <v>427</v>
       </c>
       <c r="H51" s="103">
         <v>25</v>
@@ -21010,16 +21016,16 @@
         <v>27</v>
       </c>
       <c r="B52" s="151" t="s">
+        <v>427</v>
+      </c>
+      <c r="C52" s="151" t="s">
         <v>428</v>
       </c>
-      <c r="C52" s="151" t="s">
+      <c r="D52" s="151" t="s">
         <v>429</v>
       </c>
-      <c r="D52" s="151" t="s">
+      <c r="E52" s="151" t="s">
         <v>430</v>
-      </c>
-      <c r="E52" s="151" t="s">
-        <v>431</v>
       </c>
       <c r="H52" s="103">
         <v>26</v>
@@ -21039,16 +21045,16 @@
         <v>28</v>
       </c>
       <c r="B53" s="151" t="s">
+        <v>431</v>
+      </c>
+      <c r="C53" s="151" t="s">
         <v>432</v>
       </c>
-      <c r="C53" s="151" t="s">
+      <c r="D53" s="151" t="s">
         <v>433</v>
       </c>
-      <c r="D53" s="151" t="s">
+      <c r="E53" s="151" t="s">
         <v>434</v>
-      </c>
-      <c r="E53" s="151" t="s">
-        <v>435</v>
       </c>
       <c r="H53" s="103">
         <v>27</v>
@@ -21068,16 +21074,16 @@
         <v>29</v>
       </c>
       <c r="B54" s="151" t="s">
+        <v>435</v>
+      </c>
+      <c r="C54" s="151" t="s">
         <v>436</v>
       </c>
-      <c r="C54" s="151" t="s">
+      <c r="D54" s="151" t="s">
         <v>437</v>
       </c>
-      <c r="D54" s="151" t="s">
+      <c r="E54" s="151" t="s">
         <v>438</v>
-      </c>
-      <c r="E54" s="151" t="s">
-        <v>439</v>
       </c>
       <c r="H54" s="103">
         <v>28</v>
@@ -21097,16 +21103,16 @@
         <v>30</v>
       </c>
       <c r="B55" s="151" t="s">
+        <v>439</v>
+      </c>
+      <c r="C55" s="151" t="s">
         <v>440</v>
       </c>
-      <c r="C55" s="151" t="s">
+      <c r="D55" s="151" t="s">
         <v>441</v>
       </c>
-      <c r="D55" s="151" t="s">
+      <c r="E55" s="151" t="s">
         <v>442</v>
-      </c>
-      <c r="E55" s="151" t="s">
-        <v>443</v>
       </c>
       <c r="H55" s="103">
         <v>29</v>
@@ -21126,16 +21132,16 @@
         <v>31</v>
       </c>
       <c r="B56" s="151" t="s">
+        <v>443</v>
+      </c>
+      <c r="C56" s="151" t="s">
         <v>444</v>
       </c>
-      <c r="C56" s="151" t="s">
+      <c r="D56" s="151" t="s">
         <v>445</v>
       </c>
-      <c r="D56" s="151" t="s">
+      <c r="E56" s="151" t="s">
         <v>446</v>
-      </c>
-      <c r="E56" s="151" t="s">
-        <v>447</v>
       </c>
       <c r="H56" s="103">
         <v>30</v>
@@ -21155,16 +21161,16 @@
         <v>32</v>
       </c>
       <c r="B57" s="151" t="s">
+        <v>447</v>
+      </c>
+      <c r="C57" s="151" t="s">
         <v>448</v>
       </c>
-      <c r="C57" s="151" t="s">
+      <c r="D57" s="151" t="s">
         <v>449</v>
       </c>
-      <c r="D57" s="151" t="s">
+      <c r="E57" s="151" t="s">
         <v>450</v>
-      </c>
-      <c r="E57" s="151" t="s">
-        <v>451</v>
       </c>
       <c r="H57" s="103">
         <v>31</v>
@@ -21184,16 +21190,16 @@
         <v>33</v>
       </c>
       <c r="B58" s="151" t="s">
+        <v>451</v>
+      </c>
+      <c r="C58" s="151" t="s">
         <v>452</v>
       </c>
-      <c r="C58" s="151" t="s">
+      <c r="D58" s="151" t="s">
         <v>453</v>
       </c>
-      <c r="D58" s="151" t="s">
+      <c r="E58" s="151" t="s">
         <v>454</v>
-      </c>
-      <c r="E58" s="151" t="s">
-        <v>455</v>
       </c>
       <c r="H58" s="103">
         <v>32</v>
@@ -21229,31 +21235,31 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" thickBot="1">
       <c r="A1" s="152" t="s">
+        <v>455</v>
+      </c>
+      <c r="B1" s="152" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="152" t="s">
+      <c r="C1" s="152" t="s">
         <v>457</v>
       </c>
-      <c r="C1" s="152" t="s">
+      <c r="D1" s="152" t="s">
         <v>458</v>
       </c>
-      <c r="D1" s="152" t="s">
+      <c r="E1" s="152" t="s">
         <v>459</v>
       </c>
-      <c r="E1" s="152" t="s">
-        <v>460</v>
-      </c>
       <c r="G1" s="152" t="s">
+        <v>456</v>
+      </c>
+      <c r="H1" s="152" t="s">
         <v>457</v>
       </c>
-      <c r="H1" s="152" t="s">
+      <c r="I1" s="152" t="s">
         <v>458</v>
       </c>
-      <c r="I1" s="152" t="s">
+      <c r="J1" s="152" t="s">
         <v>459</v>
-      </c>
-      <c r="J1" s="152" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -21261,13 +21267,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="153" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" s="154" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D2" s="154" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E2" s="155"/>
       <c r="G2" s="153">
@@ -21286,13 +21292,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="156" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C3" s="157" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D3" s="157" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E3" s="158"/>
       <c r="G3" s="156">
@@ -21311,13 +21317,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="159" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C4" s="157" t="s">
+        <v>394</v>
+      </c>
+      <c r="D4" s="157" t="s">
         <v>395</v>
-      </c>
-      <c r="D4" s="157" t="s">
-        <v>396</v>
       </c>
       <c r="E4" s="160"/>
       <c r="G4" s="159">
@@ -21336,13 +21342,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="161" t="s">
+        <v>461</v>
+      </c>
+      <c r="C5" s="162" t="s">
         <v>462</v>
       </c>
-      <c r="C5" s="162" t="s">
-        <v>463</v>
-      </c>
       <c r="D5" s="162" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E5" s="163"/>
       <c r="G5" s="161">
@@ -21361,16 +21367,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="153" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C6" s="154" t="s">
+        <v>470</v>
+      </c>
+      <c r="D6" s="154" t="s">
         <v>471</v>
       </c>
-      <c r="D6" s="154" t="s">
-        <v>472</v>
-      </c>
       <c r="E6" s="164" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G6" s="153">
         <v>0</v>
@@ -21390,16 +21396,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="156" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C7" s="157" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D7" s="157" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E7" s="165" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G7" s="156">
         <v>1</v>
@@ -21419,16 +21425,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="159" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C8" s="157" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D8" s="157" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E8" s="165" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G8" s="159">
         <v>2</v>
@@ -21448,16 +21454,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="167" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C9" s="168" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D9" s="168" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E9" s="169" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G9" s="167">
         <v>3</v>
@@ -21477,16 +21483,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="156" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C10" s="157" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D10" s="157" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E10" s="165" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G10" s="153">
         <v>4</v>
@@ -21506,16 +21512,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="159" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C11" s="157" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D11" s="157" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E11" s="165" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G11" s="156">
         <v>5</v>
@@ -21535,16 +21541,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="156" t="s">
+        <v>474</v>
+      </c>
+      <c r="C12" s="157" t="s">
         <v>475</v>
       </c>
-      <c r="C12" s="157" t="s">
-        <v>476</v>
-      </c>
       <c r="D12" s="157" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E12" s="165" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G12" s="159">
         <v>6</v>
@@ -21564,16 +21570,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="161" t="s">
+        <v>476</v>
+      </c>
+      <c r="C13" s="162" t="s">
         <v>477</v>
       </c>
-      <c r="C13" s="162" t="s">
+      <c r="D13" s="162" t="s">
         <v>478</v>
       </c>
-      <c r="D13" s="162" t="s">
-        <v>479</v>
-      </c>
       <c r="E13" s="166" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G13" s="167">
         <v>7</v>

</xml_diff>

<commit_message>
220504-v4 sequential mode assign
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7AB442-33B6-411F-9AAD-A8C6F68C456D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82A8C4A-5DF0-4D41-ADB8-D94665AC399D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1620" windowWidth="16200" windowHeight="9397" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
220505-v1 add TB wr delay
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682D96AB-D1C3-44EF-BF40-F12CB5307B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C51C18-1213-4B07-8797-126C17F9DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="4178" windowWidth="16200" windowHeight="9405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -2901,6 +2901,18 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2923,18 +2935,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3884,10 +3884,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="174" t="s">
+      <c r="A5" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="175"/>
+      <c r="B5" s="179"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4667,12 +4667,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="180" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
+      <c r="B22" s="179"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="179"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -14247,10 +14247,10 @@
       <c r="F76" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="G76" s="182"/>
-      <c r="H76" s="183"/>
-      <c r="I76" s="182"/>
-      <c r="J76" s="184"/>
+      <c r="G76" s="174"/>
+      <c r="H76" s="175"/>
+      <c r="I76" s="174"/>
+      <c r="J76" s="176"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -14276,10 +14276,10 @@
         <v>47</v>
       </c>
       <c r="F77" s="93"/>
-      <c r="G77" s="185"/>
-      <c r="H77" s="183"/>
-      <c r="I77" s="185"/>
-      <c r="J77" s="184"/>
+      <c r="G77" s="177"/>
+      <c r="H77" s="175"/>
+      <c r="I77" s="177"/>
+      <c r="J77" s="176"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
@@ -14304,10 +14304,10 @@
       <c r="E78" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="G78" s="185"/>
-      <c r="H78" s="183"/>
-      <c r="I78" s="185"/>
-      <c r="J78" s="184"/>
+      <c r="G78" s="177"/>
+      <c r="H78" s="175"/>
+      <c r="I78" s="177"/>
+      <c r="J78" s="176"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
@@ -14332,10 +14332,10 @@
       <c r="E79" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="G79" s="185"/>
-      <c r="H79" s="183"/>
-      <c r="I79" s="185"/>
-      <c r="J79" s="184"/>
+      <c r="G79" s="177"/>
+      <c r="H79" s="175"/>
+      <c r="I79" s="177"/>
+      <c r="J79" s="176"/>
       <c r="K79" s="40"/>
       <c r="L79" s="40"/>
       <c r="M79" s="40"/>
@@ -14850,11 +14850,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="177" t="s">
+      <c r="B98" s="181" t="s">
         <v>211</v>
       </c>
-      <c r="C98" s="178"/>
-      <c r="D98" s="178"/>
+      <c r="C98" s="182"/>
+      <c r="D98" s="182"/>
       <c r="E98" s="81" t="s">
         <v>212</v>
       </c>
@@ -19307,67 +19307,67 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="183" t="s">
         <v>305</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="179" t="s">
+      <c r="C6" s="184"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="183" t="s">
         <v>306</v>
       </c>
-      <c r="F6" s="180"/>
-      <c r="G6" s="181"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="185"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="179" t="s">
+      <c r="B7" s="183" t="s">
         <v>307</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="180"/>
-      <c r="E7" s="180"/>
-      <c r="F7" s="180"/>
-      <c r="G7" s="180"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="180"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="180"/>
-      <c r="P7" s="181"/>
-      <c r="Q7" s="179" t="s">
+      <c r="C7" s="184"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="184"/>
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="184"/>
+      <c r="M7" s="184"/>
+      <c r="N7" s="184"/>
+      <c r="O7" s="184"/>
+      <c r="P7" s="185"/>
+      <c r="Q7" s="183" t="s">
         <v>308</v>
       </c>
-      <c r="R7" s="180"/>
-      <c r="S7" s="180"/>
-      <c r="T7" s="180"/>
-      <c r="U7" s="180"/>
-      <c r="V7" s="180"/>
-      <c r="W7" s="180"/>
-      <c r="X7" s="180"/>
-      <c r="Y7" s="180"/>
-      <c r="Z7" s="180"/>
-      <c r="AA7" s="181"/>
-      <c r="AB7" s="179" t="s">
+      <c r="R7" s="184"/>
+      <c r="S7" s="184"/>
+      <c r="T7" s="184"/>
+      <c r="U7" s="184"/>
+      <c r="V7" s="184"/>
+      <c r="W7" s="184"/>
+      <c r="X7" s="184"/>
+      <c r="Y7" s="184"/>
+      <c r="Z7" s="184"/>
+      <c r="AA7" s="185"/>
+      <c r="AB7" s="183" t="s">
         <v>309</v>
       </c>
-      <c r="AC7" s="180"/>
-      <c r="AD7" s="180"/>
-      <c r="AE7" s="180"/>
-      <c r="AF7" s="180"/>
-      <c r="AG7" s="180"/>
-      <c r="AH7" s="180"/>
-      <c r="AI7" s="180"/>
-      <c r="AJ7" s="180"/>
-      <c r="AK7" s="180"/>
-      <c r="AL7" s="180"/>
-      <c r="AM7" s="180"/>
-      <c r="AN7" s="180"/>
-      <c r="AO7" s="180"/>
-      <c r="AP7" s="180"/>
-      <c r="AQ7" s="180"/>
-      <c r="AR7" s="181"/>
+      <c r="AC7" s="184"/>
+      <c r="AD7" s="184"/>
+      <c r="AE7" s="184"/>
+      <c r="AF7" s="184"/>
+      <c r="AG7" s="184"/>
+      <c r="AH7" s="184"/>
+      <c r="AI7" s="184"/>
+      <c r="AJ7" s="184"/>
+      <c r="AK7" s="184"/>
+      <c r="AL7" s="184"/>
+      <c r="AM7" s="184"/>
+      <c r="AN7" s="184"/>
+      <c r="AO7" s="184"/>
+      <c r="AP7" s="184"/>
+      <c r="AQ7" s="184"/>
+      <c r="AR7" s="185"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="52"/>

</xml_diff>

<commit_message>
220505-v2 revised setting to combinational logic, add base_addr_set
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C51C18-1213-4B07-8797-126C17F9DB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E5408F-8E84-4D29-9304-F9391BA7DB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="4178" windowWidth="16200" windowHeight="9405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
220507-v2 ToDo: data flow of transfer, revise cov_vv
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F13060A-9770-404B-9287-43AF617FAE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114DE970-2620-4400-90B1-A7747B59AE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3585" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="494">
   <si>
     <t>步骤</t>
   </si>
@@ -1549,10 +1549,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>cov(1,2)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>cov(1,3)</t>
   </si>
   <si>
@@ -1656,10 +1652,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>UPD_5转置(seq_cnt等待转置完成)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>S是对称矩阵</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -1698,6 +1690,31 @@
   <si>
     <t>S, S_inv为对称 可转置</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPD_8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>state(1,1)</t>
+  </si>
+  <si>
+    <t>state(2,1)</t>
+  </si>
+  <si>
+    <t>state(3,1)</t>
+  </si>
+  <si>
+    <t>cov(1,1)</t>
+  </si>
+  <si>
+    <t>cov(2,1)</t>
+  </si>
+  <si>
+    <t>cov(3,1)</t>
+  </si>
+  <si>
+    <t>cov(1,2)</t>
   </si>
 </sst>
 </file>
@@ -1904,7 +1921,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -2361,24 +2378,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2876,12 +2882,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2904,6 +2904,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2930,16 +2942,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3889,10 +3913,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="177" t="s">
+      <c r="A5" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="178"/>
+      <c r="B5" s="180"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4672,12 +4696,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="179" t="s">
+      <c r="A22" s="181" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="178"/>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
+      <c r="B22" s="180"/>
+      <c r="C22" s="180"/>
+      <c r="D22" s="180"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -12269,8 +12293,8 @@
   <dimension ref="A1:S274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12598,7 +12622,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -12623,7 +12647,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="3" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -12644,8 +12668,8 @@
       <c r="B16" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="171" t="s">
-        <v>470</v>
+      <c r="C16" s="169" t="s">
+        <v>469</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="54" t="s">
@@ -12758,8 +12782,8 @@
       <c r="D20" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="171" t="s">
-        <v>470</v>
+      <c r="E20" s="169" t="s">
+        <v>469</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -12932,7 +12956,7 @@
         <v>188</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -13118,8 +13142,8 @@
       <c r="B34" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="171" t="s">
-        <v>470</v>
+      <c r="C34" s="169" t="s">
+        <v>469</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="66" t="s">
@@ -13317,7 +13341,7 @@
         <v>222</v>
       </c>
       <c r="F41" s="92" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="92"/>
@@ -13959,14 +13983,14 @@
       <c r="A66" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B66" s="172" t="s">
-        <v>485</v>
+      <c r="B66" s="170" t="s">
+        <v>483</v>
       </c>
       <c r="C66" s="74" t="s">
         <v>175</v>
       </c>
       <c r="D66" s="41"/>
-      <c r="E66" s="185"/>
+      <c r="E66" s="175"/>
       <c r="F66" s="38"/>
       <c r="G66" s="40"/>
       <c r="H66" s="40"/>
@@ -13985,13 +14009,13 @@
     <row r="67" spans="1:19">
       <c r="A67" s="39"/>
       <c r="B67" s="46" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>174</v>
       </c>
       <c r="D67" s="24"/>
-      <c r="E67" s="186"/>
+      <c r="E67" s="176"/>
       <c r="F67" s="38"/>
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
@@ -14016,7 +14040,7 @@
         <v>191</v>
       </c>
       <c r="D68" s="42"/>
-      <c r="E68" s="187"/>
+      <c r="E68" s="177"/>
       <c r="F68" s="38"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
@@ -14043,7 +14067,7 @@
         <v>176</v>
       </c>
       <c r="D69" s="24"/>
-      <c r="E69" s="175"/>
+      <c r="E69" s="173"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -14068,7 +14092,7 @@
         <v>177</v>
       </c>
       <c r="D70" s="17"/>
-      <c r="E70" s="175"/>
+      <c r="E70" s="173"/>
       <c r="F70" s="7"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -14093,7 +14117,7 @@
         <v>191</v>
       </c>
       <c r="D71" s="17"/>
-      <c r="E71" s="175"/>
+      <c r="E71" s="173"/>
       <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -14113,7 +14137,7 @@
       <c r="A72" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B72" s="188" t="s">
+      <c r="B72" s="178" t="s">
         <v>178</v>
       </c>
       <c r="C72" s="74" t="s">
@@ -14205,7 +14229,7 @@
         <v>220</v>
       </c>
       <c r="F75" s="92" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G75" s="40"/>
       <c r="H75" s="40"/>
@@ -14223,7 +14247,7 @@
     </row>
     <row r="76" spans="1:19">
       <c r="A76" s="151" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B76" s="60" t="s">
         <v>62</v>
@@ -14238,12 +14262,12 @@
         <v>63</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="G76" s="173"/>
-      <c r="H76" s="174"/>
-      <c r="I76" s="173"/>
-      <c r="J76" s="175"/>
+        <v>476</v>
+      </c>
+      <c r="G76" s="171"/>
+      <c r="H76" s="172"/>
+      <c r="I76" s="171"/>
+      <c r="J76" s="173"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -14269,10 +14293,10 @@
         <v>45</v>
       </c>
       <c r="F77" s="92"/>
-      <c r="G77" s="176"/>
-      <c r="H77" s="174"/>
-      <c r="I77" s="176"/>
-      <c r="J77" s="175"/>
+      <c r="G77" s="174"/>
+      <c r="H77" s="172"/>
+      <c r="I77" s="174"/>
+      <c r="J77" s="173"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
@@ -14297,10 +14321,10 @@
       <c r="E78" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="G78" s="176"/>
-      <c r="H78" s="174"/>
-      <c r="I78" s="176"/>
-      <c r="J78" s="175"/>
+      <c r="G78" s="174"/>
+      <c r="H78" s="172"/>
+      <c r="I78" s="174"/>
+      <c r="J78" s="173"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
@@ -14325,10 +14349,10 @@
       <c r="E79" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="G79" s="176"/>
-      <c r="H79" s="174"/>
-      <c r="I79" s="176"/>
-      <c r="J79" s="175"/>
+      <c r="G79" s="174"/>
+      <c r="H79" s="172"/>
+      <c r="I79" s="174"/>
+      <c r="J79" s="173"/>
       <c r="K79" s="40"/>
       <c r="L79" s="40"/>
       <c r="M79" s="40"/>
@@ -14341,7 +14365,7 @@
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="17" t="s">
-        <v>477</v>
+        <v>210</v>
       </c>
       <c r="B80" s="58" t="s">
         <v>63</v>
@@ -14418,7 +14442,7 @@
     </row>
     <row r="83" spans="1:19">
       <c r="A83" s="17" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B83" s="58" t="s">
         <v>223</v>
@@ -14485,7 +14509,7 @@
         <v>186</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -14514,7 +14538,7 @@
         <v>220</v>
       </c>
       <c r="F86" s="92" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G86" s="40"/>
       <c r="H86" s="40"/>
@@ -14708,7 +14732,7 @@
     </row>
     <row r="93" spans="1:19">
       <c r="A93" s="90" t="s">
-        <v>211</v>
+        <v>486</v>
       </c>
       <c r="B93" s="93" t="s">
         <v>66</v>
@@ -14806,7 +14830,7 @@
       <c r="D96" s="42"/>
       <c r="E96" s="48"/>
       <c r="F96" s="91" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G96" s="40"/>
       <c r="H96" s="40"/>
@@ -14845,11 +14869,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="180" t="s">
+      <c r="B98" s="182" t="s">
         <v>201</v>
       </c>
-      <c r="C98" s="181"/>
-      <c r="D98" s="181"/>
+      <c r="C98" s="183"/>
+      <c r="D98" s="183"/>
       <c r="E98" s="80" t="s">
         <v>202</v>
       </c>
@@ -18541,7 +18565,7 @@
         <v>230</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D2" s="134"/>
       <c r="E2" s="135" t="s">
@@ -18564,11 +18588,11 @@
       <c r="B4" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="167" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="169"/>
-      <c r="E4" s="170" t="s">
+      <c r="D4" s="167"/>
+      <c r="E4" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18600,11 +18624,11 @@
       <c r="B7" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="169" t="s">
+      <c r="C7" s="167" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="169"/>
-      <c r="E7" s="170" t="s">
+      <c r="D7" s="167"/>
+      <c r="E7" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18636,11 +18660,11 @@
       <c r="B10" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="169" t="s">
+      <c r="C10" s="167" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="169"/>
-      <c r="E10" s="170" t="s">
+      <c r="D10" s="167"/>
+      <c r="E10" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18672,11 +18696,11 @@
       <c r="B13" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="169" t="s">
+      <c r="C13" s="167" t="s">
         <v>186</v>
       </c>
       <c r="D13" s="123"/>
-      <c r="E13" s="170" t="s">
+      <c r="E13" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18712,13 +18736,13 @@
       <c r="B16" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="169" t="s">
+      <c r="C16" s="167" t="s">
         <v>186</v>
       </c>
       <c r="D16" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="170" t="s">
+      <c r="E16" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18754,13 +18778,13 @@
       <c r="B19" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="169" t="s">
+      <c r="C19" s="167" t="s">
         <v>186</v>
       </c>
       <c r="D19" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="170" t="s">
+      <c r="E19" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18769,7 +18793,7 @@
         <v>245</v>
       </c>
       <c r="C20" s="134" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D20" s="134" t="s">
         <v>242</v>
@@ -18787,7 +18811,7 @@
         <v>237</v>
       </c>
       <c r="C21" s="139" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D21" s="139" t="s">
         <v>237</v>
@@ -18803,13 +18827,13 @@
       <c r="B22" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="169" t="s">
+      <c r="C22" s="167" t="s">
         <v>186</v>
       </c>
       <c r="D22" s="141" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="170" t="s">
+      <c r="E22" s="168" t="s">
         <v>186</v>
       </c>
     </row>
@@ -19002,20 +19026,20 @@
       <c r="O2" s="108"/>
       <c r="P2" s="108"/>
       <c r="Q2" s="107" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="R2" s="108"/>
       <c r="S2" s="110">
         <v>5</v>
       </c>
       <c r="T2" s="111" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="U2" s="110">
         <v>4</v>
       </c>
       <c r="V2" s="107" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="W2" s="109"/>
       <c r="X2" s="107" t="s">
@@ -19027,7 +19051,7 @@
       </c>
       <c r="AA2" s="109"/>
       <c r="AB2" s="113" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AC2" s="114">
         <v>-3</v>
@@ -19036,7 +19060,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="113" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AF2" s="114">
         <v>3</v>
@@ -19302,67 +19326,67 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="184" t="s">
         <v>294</v>
       </c>
-      <c r="C6" s="183"/>
-      <c r="D6" s="184"/>
-      <c r="E6" s="182" t="s">
+      <c r="C6" s="185"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="184" t="s">
         <v>295</v>
       </c>
-      <c r="F6" s="183"/>
-      <c r="G6" s="184"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="186"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="184" t="s">
         <v>296</v>
       </c>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="183"/>
-      <c r="G7" s="183"/>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
-      <c r="K7" s="183"/>
-      <c r="L7" s="183"/>
-      <c r="M7" s="183"/>
-      <c r="N7" s="183"/>
-      <c r="O7" s="183"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="182" t="s">
+      <c r="C7" s="185"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="185"/>
+      <c r="G7" s="185"/>
+      <c r="H7" s="185"/>
+      <c r="I7" s="185"/>
+      <c r="J7" s="185"/>
+      <c r="K7" s="185"/>
+      <c r="L7" s="185"/>
+      <c r="M7" s="185"/>
+      <c r="N7" s="185"/>
+      <c r="O7" s="185"/>
+      <c r="P7" s="186"/>
+      <c r="Q7" s="184" t="s">
         <v>297</v>
       </c>
-      <c r="R7" s="183"/>
-      <c r="S7" s="183"/>
-      <c r="T7" s="183"/>
-      <c r="U7" s="183"/>
-      <c r="V7" s="183"/>
-      <c r="W7" s="183"/>
-      <c r="X7" s="183"/>
-      <c r="Y7" s="183"/>
-      <c r="Z7" s="183"/>
-      <c r="AA7" s="184"/>
-      <c r="AB7" s="182" t="s">
+      <c r="R7" s="185"/>
+      <c r="S7" s="185"/>
+      <c r="T7" s="185"/>
+      <c r="U7" s="185"/>
+      <c r="V7" s="185"/>
+      <c r="W7" s="185"/>
+      <c r="X7" s="185"/>
+      <c r="Y7" s="185"/>
+      <c r="Z7" s="185"/>
+      <c r="AA7" s="186"/>
+      <c r="AB7" s="184" t="s">
         <v>298</v>
       </c>
-      <c r="AC7" s="183"/>
-      <c r="AD7" s="183"/>
-      <c r="AE7" s="183"/>
-      <c r="AF7" s="183"/>
-      <c r="AG7" s="183"/>
-      <c r="AH7" s="183"/>
-      <c r="AI7" s="183"/>
-      <c r="AJ7" s="183"/>
-      <c r="AK7" s="183"/>
-      <c r="AL7" s="183"/>
-      <c r="AM7" s="183"/>
-      <c r="AN7" s="183"/>
-      <c r="AO7" s="183"/>
-      <c r="AP7" s="183"/>
-      <c r="AQ7" s="183"/>
-      <c r="AR7" s="184"/>
+      <c r="AC7" s="185"/>
+      <c r="AD7" s="185"/>
+      <c r="AE7" s="185"/>
+      <c r="AF7" s="185"/>
+      <c r="AG7" s="185"/>
+      <c r="AH7" s="185"/>
+      <c r="AI7" s="185"/>
+      <c r="AJ7" s="185"/>
+      <c r="AK7" s="185"/>
+      <c r="AL7" s="185"/>
+      <c r="AM7" s="185"/>
+      <c r="AN7" s="185"/>
+      <c r="AO7" s="185"/>
+      <c r="AP7" s="185"/>
+      <c r="AQ7" s="185"/>
+      <c r="AR7" s="186"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="52"/>
@@ -21229,7 +21253,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:J25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -21271,13 +21295,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="152" t="s">
-        <v>303</v>
+        <v>490</v>
       </c>
       <c r="C2" s="153" t="s">
-        <v>305</v>
+        <v>491</v>
       </c>
       <c r="D2" s="153" t="s">
-        <v>308</v>
+        <v>492</v>
       </c>
       <c r="E2" s="154"/>
       <c r="G2" s="152">
@@ -21296,13 +21320,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="155" t="s">
-        <v>304</v>
+        <v>493</v>
       </c>
       <c r="C3" s="156" t="s">
-        <v>306</v>
+        <v>382</v>
       </c>
       <c r="D3" s="156" t="s">
-        <v>309</v>
+        <v>383</v>
       </c>
       <c r="E3" s="157"/>
       <c r="G3" s="155">
@@ -21324,10 +21348,10 @@
         <v>448</v>
       </c>
       <c r="C4" s="156" t="s">
-        <v>382</v>
+        <v>449</v>
       </c>
       <c r="D4" s="156" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E4" s="159"/>
       <c r="G4" s="158">
@@ -21345,14 +21369,14 @@
       <c r="A5" s="151">
         <v>3</v>
       </c>
-      <c r="B5" s="160" t="s">
-        <v>449</v>
-      </c>
-      <c r="C5" s="161" t="s">
-        <v>450</v>
-      </c>
-      <c r="D5" s="161" t="s">
-        <v>384</v>
+      <c r="B5" s="187" t="s">
+        <v>487</v>
+      </c>
+      <c r="C5" s="188" t="s">
+        <v>488</v>
+      </c>
+      <c r="D5" s="188" t="s">
+        <v>489</v>
       </c>
       <c r="E5" s="162"/>
       <c r="G5" s="160">
@@ -21370,17 +21394,17 @@
       <c r="A6" s="151">
         <v>4</v>
       </c>
-      <c r="B6" s="152" t="s">
-        <v>451</v>
-      </c>
-      <c r="C6" s="153" t="s">
-        <v>458</v>
-      </c>
-      <c r="D6" s="153" t="s">
+      <c r="B6" s="189" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" s="190" t="s">
+        <v>318</v>
+      </c>
+      <c r="D6" s="190" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6" s="191" t="s">
         <v>459</v>
-      </c>
-      <c r="E6" s="163" t="s">
-        <v>330</v>
       </c>
       <c r="G6" s="152">
         <v>0</v>
@@ -21399,17 +21423,17 @@
       <c r="A7" s="151">
         <v>5</v>
       </c>
-      <c r="B7" s="155" t="s">
-        <v>313</v>
+      <c r="B7" s="158" t="s">
+        <v>451</v>
       </c>
       <c r="C7" s="156" t="s">
-        <v>318</v>
+        <v>453</v>
       </c>
       <c r="D7" s="156" t="s">
-        <v>324</v>
+        <v>455</v>
       </c>
       <c r="E7" s="164" t="s">
-        <v>460</v>
+        <v>332</v>
       </c>
       <c r="G7" s="155">
         <v>1</v>
@@ -21428,7 +21452,7 @@
       <c r="A8" s="151">
         <v>6</v>
       </c>
-      <c r="B8" s="158" t="s">
+      <c r="B8" s="155" t="s">
         <v>452</v>
       </c>
       <c r="C8" s="156" t="s">
@@ -21438,7 +21462,7 @@
         <v>456</v>
       </c>
       <c r="E8" s="164" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G8" s="158">
         <v>2</v>
@@ -21457,17 +21481,17 @@
       <c r="A9" s="151">
         <v>7</v>
       </c>
-      <c r="B9" s="166" t="s">
-        <v>453</v>
-      </c>
-      <c r="C9" s="167" t="s">
-        <v>455</v>
-      </c>
-      <c r="D9" s="167" t="s">
+      <c r="B9" s="192" t="s">
+        <v>450</v>
+      </c>
+      <c r="C9" s="193" t="s">
         <v>457</v>
       </c>
-      <c r="E9" s="168" t="s">
-        <v>333</v>
+      <c r="D9" s="193" t="s">
+        <v>458</v>
+      </c>
+      <c r="E9" s="194" t="s">
+        <v>330</v>
       </c>
       <c r="G9" s="166">
         <v>3</v>
@@ -21516,7 +21540,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="158" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C11" s="156" t="s">
         <v>322</v>
@@ -21545,10 +21569,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="155" t="s">
+        <v>461</v>
+      </c>
+      <c r="C12" s="156" t="s">
         <v>462</v>
-      </c>
-      <c r="C12" s="156" t="s">
-        <v>463</v>
       </c>
       <c r="D12" s="156" t="s">
         <v>329</v>
@@ -21574,13 +21598,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="C13" s="161" t="s">
         <v>464</v>
       </c>
-      <c r="C13" s="161" t="s">
+      <c r="D13" s="161" t="s">
         <v>465</v>
-      </c>
-      <c r="D13" s="161" t="s">
-        <v>466</v>
       </c>
       <c r="E13" s="165" t="s">
         <v>337</v>
@@ -21615,7 +21639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="14.25" thickBot="1">
       <c r="A15" s="151">
         <v>13</v>
       </c>
@@ -21635,6 +21659,18 @@
     <row r="16" spans="1:10">
       <c r="A16" s="151">
         <v>14</v>
+      </c>
+      <c r="B16" s="152" t="s">
+        <v>450</v>
+      </c>
+      <c r="C16" s="153" t="s">
+        <v>457</v>
+      </c>
+      <c r="D16" s="153" t="s">
+        <v>458</v>
+      </c>
+      <c r="E16" s="163" t="s">
+        <v>330</v>
       </c>
       <c r="G16" s="158">
         <v>10</v>

</xml_diff>

<commit_message>
220507-v3 finished code, not simed
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114DE970-2620-4400-90B1-A7747B59AE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54029D-2C91-420C-82E7-B38184FFD5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3585" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="494">
   <si>
     <t>步骤</t>
   </si>
@@ -1024,13 +1024,6 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>cov_vl_H_T(3,1)</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(3,2)</t>
-  </si>
-  <si>
     <t>cov_l/K(3,1)</t>
   </si>
   <si>
@@ -1715,6 +1708,14 @@
   </si>
   <si>
     <t>cov(1,2)</t>
+  </si>
+  <si>
+    <t>vt(0,1)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>vt(0,2)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1822,7 +1823,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1917,6 +1918,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2384,7 +2391,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2726,9 +2733,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="37" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="38" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2918,6 +2922,30 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2942,29 +2970,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="31" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="41" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3913,10 +3929,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="179" t="s">
+      <c r="A5" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="180"/>
+      <c r="B5" s="187"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4696,12 +4712,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="181" t="s">
+      <c r="A22" s="188" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="180"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="180"/>
+      <c r="B22" s="187"/>
+      <c r="C22" s="187"/>
+      <c r="D22" s="187"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -12293,8 +12309,8 @@
   <dimension ref="A1:S274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12622,7 +12638,7 @@
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -12647,7 +12663,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="3" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -12668,8 +12684,8 @@
       <c r="B16" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="169" t="s">
-        <v>469</v>
+      <c r="C16" s="168" t="s">
+        <v>467</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="54" t="s">
@@ -12782,8 +12798,8 @@
       <c r="D20" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="169" t="s">
-        <v>469</v>
+      <c r="E20" s="168" t="s">
+        <v>467</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -12956,7 +12972,7 @@
         <v>188</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -13142,8 +13158,8 @@
       <c r="B34" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="169" t="s">
-        <v>469</v>
+      <c r="C34" s="168" t="s">
+        <v>467</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="66" t="s">
@@ -13341,7 +13357,7 @@
         <v>222</v>
       </c>
       <c r="F41" s="92" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G41" s="92"/>
       <c r="H41" s="92"/>
@@ -13983,14 +13999,14 @@
       <c r="A66" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B66" s="170" t="s">
-        <v>483</v>
+      <c r="B66" s="169" t="s">
+        <v>481</v>
       </c>
       <c r="C66" s="74" t="s">
         <v>175</v>
       </c>
       <c r="D66" s="41"/>
-      <c r="E66" s="175"/>
+      <c r="E66" s="174"/>
       <c r="F66" s="38"/>
       <c r="G66" s="40"/>
       <c r="H66" s="40"/>
@@ -14009,13 +14025,13 @@
     <row r="67" spans="1:19">
       <c r="A67" s="39"/>
       <c r="B67" s="46" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>174</v>
       </c>
       <c r="D67" s="24"/>
-      <c r="E67" s="176"/>
+      <c r="E67" s="175"/>
       <c r="F67" s="38"/>
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
@@ -14040,7 +14056,7 @@
         <v>191</v>
       </c>
       <c r="D68" s="42"/>
-      <c r="E68" s="177"/>
+      <c r="E68" s="176"/>
       <c r="F68" s="38"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
@@ -14067,7 +14083,7 @@
         <v>176</v>
       </c>
       <c r="D69" s="24"/>
-      <c r="E69" s="173"/>
+      <c r="E69" s="172"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -14092,7 +14108,7 @@
         <v>177</v>
       </c>
       <c r="D70" s="17"/>
-      <c r="E70" s="173"/>
+      <c r="E70" s="172"/>
       <c r="F70" s="7"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -14117,7 +14133,7 @@
         <v>191</v>
       </c>
       <c r="D71" s="17"/>
-      <c r="E71" s="173"/>
+      <c r="E71" s="172"/>
       <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -14137,7 +14153,7 @@
       <c r="A72" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B72" s="178" t="s">
+      <c r="B72" s="177" t="s">
         <v>178</v>
       </c>
       <c r="C72" s="74" t="s">
@@ -14229,7 +14245,7 @@
         <v>220</v>
       </c>
       <c r="F75" s="92" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G75" s="40"/>
       <c r="H75" s="40"/>
@@ -14246,8 +14262,8 @@
       <c r="S75" s="40"/>
     </row>
     <row r="76" spans="1:19">
-      <c r="A76" s="151" t="s">
-        <v>475</v>
+      <c r="A76" s="150" t="s">
+        <v>473</v>
       </c>
       <c r="B76" s="60" t="s">
         <v>62</v>
@@ -14262,12 +14278,12 @@
         <v>63</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="G76" s="171"/>
-      <c r="H76" s="172"/>
-      <c r="I76" s="171"/>
-      <c r="J76" s="173"/>
+        <v>474</v>
+      </c>
+      <c r="G76" s="170"/>
+      <c r="H76" s="171"/>
+      <c r="I76" s="170"/>
+      <c r="J76" s="172"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -14293,10 +14309,10 @@
         <v>45</v>
       </c>
       <c r="F77" s="92"/>
-      <c r="G77" s="174"/>
-      <c r="H77" s="172"/>
-      <c r="I77" s="174"/>
-      <c r="J77" s="173"/>
+      <c r="G77" s="173"/>
+      <c r="H77" s="171"/>
+      <c r="I77" s="173"/>
+      <c r="J77" s="172"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
@@ -14321,10 +14337,10 @@
       <c r="E78" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="G78" s="174"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="174"/>
-      <c r="J78" s="173"/>
+      <c r="G78" s="173"/>
+      <c r="H78" s="171"/>
+      <c r="I78" s="173"/>
+      <c r="J78" s="172"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
@@ -14349,10 +14365,10 @@
       <c r="E79" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="G79" s="174"/>
-      <c r="H79" s="172"/>
-      <c r="I79" s="174"/>
-      <c r="J79" s="173"/>
+      <c r="G79" s="173"/>
+      <c r="H79" s="171"/>
+      <c r="I79" s="173"/>
+      <c r="J79" s="172"/>
       <c r="K79" s="40"/>
       <c r="L79" s="40"/>
       <c r="M79" s="40"/>
@@ -14509,7 +14525,7 @@
         <v>186</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -14538,7 +14554,7 @@
         <v>220</v>
       </c>
       <c r="F86" s="92" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G86" s="40"/>
       <c r="H86" s="40"/>
@@ -14732,7 +14748,7 @@
     </row>
     <row r="93" spans="1:19">
       <c r="A93" s="90" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B93" s="93" t="s">
         <v>66</v>
@@ -14830,7 +14846,7 @@
       <c r="D96" s="42"/>
       <c r="E96" s="48"/>
       <c r="F96" s="91" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G96" s="40"/>
       <c r="H96" s="40"/>
@@ -14869,11 +14885,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="182" t="s">
+      <c r="B98" s="189" t="s">
         <v>201</v>
       </c>
-      <c r="C98" s="183"/>
-      <c r="D98" s="183"/>
+      <c r="C98" s="190"/>
+      <c r="D98" s="190"/>
       <c r="E98" s="80" t="s">
         <v>202</v>
       </c>
@@ -18561,244 +18577,244 @@
       </c>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="131" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="134" t="s">
-        <v>466</v>
-      </c>
-      <c r="D2" s="134"/>
-      <c r="E2" s="135" t="s">
+      <c r="C2" s="133" t="s">
+        <v>464</v>
+      </c>
+      <c r="D2" s="133"/>
+      <c r="E2" s="134" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="135" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="139" t="s">
+      <c r="C3" s="138" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140" t="s">
+      <c r="D3" s="138"/>
+      <c r="E3" s="139" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="14.25" thickBot="1">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="167" t="s">
+      <c r="C4" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="168" t="s">
+      <c r="D4" s="166"/>
+      <c r="E4" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="132" t="s">
+      <c r="B5" s="131" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="134" t="s">
+      <c r="C5" s="133" t="s">
         <v>234</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="135" t="s">
+      <c r="D5" s="133"/>
+      <c r="E5" s="134" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="135" t="s">
         <v>232</v>
       </c>
-      <c r="C6" s="139" t="s">
+      <c r="C6" s="138" t="s">
         <v>236</v>
       </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="140" t="s">
+      <c r="D6" s="138"/>
+      <c r="E6" s="139" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="14.25" thickBot="1">
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="167" t="s">
+      <c r="C7" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="167"/>
-      <c r="E7" s="168" t="s">
+      <c r="D7" s="166"/>
+      <c r="E7" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="131" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="133" t="s">
         <v>239</v>
       </c>
-      <c r="D8" s="134"/>
-      <c r="E8" s="135" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="134" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="135" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="D9" s="139"/>
-      <c r="E9" s="140" t="s">
+      <c r="D9" s="138"/>
+      <c r="E9" s="139" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="14.25" thickBot="1">
-      <c r="B10" s="141" t="s">
+      <c r="B10" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="167" t="s">
+      <c r="C10" s="166" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="167"/>
-      <c r="E10" s="168" t="s">
+      <c r="D10" s="166"/>
+      <c r="E10" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="131" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="133" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="134"/>
-      <c r="E11" s="135" t="s">
+      <c r="D11" s="133"/>
+      <c r="E11" s="134" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="135" t="s">
         <v>237</v>
       </c>
-      <c r="C12" s="139" t="s">
+      <c r="C12" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="D12" s="139"/>
-      <c r="E12" s="140" t="s">
+      <c r="D12" s="138"/>
+      <c r="E12" s="139" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="14.25" thickBot="1">
-      <c r="B13" s="141" t="s">
+      <c r="B13" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="167" t="s">
+      <c r="C13" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="D13" s="123"/>
-      <c r="E13" s="168" t="s">
+      <c r="D13" s="122"/>
+      <c r="E13" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="131" t="s">
         <v>231</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="133" t="s">
         <v>243</v>
       </c>
-      <c r="D14" s="134" t="s">
+      <c r="D14" s="133" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="135" t="s">
+      <c r="E14" s="134" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="135" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="138" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="139" t="s">
+      <c r="D15" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="E15" s="140" t="s">
+      <c r="E15" s="139" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.4" customHeight="1" thickBot="1">
-      <c r="B16" s="141" t="s">
+      <c r="B16" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="167" t="s">
+      <c r="C16" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="D16" s="141" t="s">
+      <c r="D16" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="168" t="s">
+      <c r="E16" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="132" t="s">
+      <c r="B17" s="131" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="134" t="s">
+      <c r="C17" s="133" t="s">
         <v>241</v>
       </c>
-      <c r="D17" s="134" t="s">
+      <c r="D17" s="133" t="s">
         <v>242</v>
       </c>
-      <c r="E17" s="135" t="s">
+      <c r="E17" s="134" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="135" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="139" t="s">
+      <c r="C18" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="D18" s="139" t="s">
+      <c r="D18" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="E18" s="140" t="s">
+      <c r="E18" s="139" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="14.25" thickBot="1">
-      <c r="B19" s="141" t="s">
+      <c r="B19" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="167" t="s">
+      <c r="C19" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="D19" s="141" t="s">
+      <c r="D19" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="168" t="s">
+      <c r="E19" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="132" t="s">
+      <c r="B20" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="134" t="s">
-        <v>467</v>
-      </c>
-      <c r="D20" s="134" t="s">
+      <c r="C20" s="133" t="s">
+        <v>465</v>
+      </c>
+      <c r="D20" s="133" t="s">
         <v>242</v>
       </c>
-      <c r="E20" s="135" t="s">
+      <c r="E20" s="134" t="s">
         <v>246</v>
       </c>
       <c r="F20" s="103" t="s">
@@ -18807,16 +18823,16 @@
       <c r="G20" s="103"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="135" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="139" t="s">
-        <v>468</v>
-      </c>
-      <c r="D21" s="139" t="s">
+      <c r="C21" s="138" t="s">
+        <v>466</v>
+      </c>
+      <c r="D21" s="138" t="s">
         <v>237</v>
       </c>
-      <c r="E21" s="140" t="s">
+      <c r="E21" s="139" t="s">
         <v>237</v>
       </c>
       <c r="F21" s="102" t="s">
@@ -18824,16 +18840,16 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="14.25" thickBot="1">
-      <c r="B22" s="141" t="s">
+      <c r="B22" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="167" t="s">
+      <c r="C22" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="D22" s="141" t="s">
+      <c r="D22" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="168" t="s">
+      <c r="E22" s="167" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18848,7 +18864,7 @@
   <dimension ref="A1:AU15"/>
   <sheetViews>
     <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="AK32" sqref="AK32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -19026,20 +19042,20 @@
       <c r="O2" s="108"/>
       <c r="P2" s="108"/>
       <c r="Q2" s="107" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="R2" s="108"/>
       <c r="S2" s="110">
         <v>5</v>
       </c>
       <c r="T2" s="111" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="U2" s="110">
         <v>4</v>
       </c>
       <c r="V2" s="107" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="W2" s="109"/>
       <c r="X2" s="107" t="s">
@@ -19051,7 +19067,7 @@
       </c>
       <c r="AA2" s="109"/>
       <c r="AB2" s="113" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="AC2" s="114">
         <v>-3</v>
@@ -19060,7 +19076,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="113" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="AF2" s="114">
         <v>3</v>
@@ -19076,10 +19092,10 @@
       <c r="AK2" s="108"/>
       <c r="AL2" s="108"/>
       <c r="AM2" s="108"/>
-      <c r="AN2" s="113" t="s">
+      <c r="AN2" s="194" t="s">
         <v>258</v>
       </c>
-      <c r="AO2" s="115" t="s">
+      <c r="AO2" s="195" t="s">
         <v>259</v>
       </c>
       <c r="AP2" s="107" t="s">
@@ -19105,96 +19121,96 @@
       <c r="A3" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="117">
+      <c r="B3" s="115"/>
+      <c r="C3" s="116">
         <v>1</v>
       </c>
-      <c r="D3" s="118" t="s">
+      <c r="D3" s="117" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="119"/>
-      <c r="F3" s="117">
+      <c r="E3" s="118"/>
+      <c r="F3" s="116">
         <v>1</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="120">
+      <c r="G3" s="116"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="119">
         <v>1</v>
       </c>
-      <c r="J3" s="121"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="120">
+      <c r="J3" s="120"/>
+      <c r="K3" s="119"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="119">
         <v>1</v>
       </c>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="122"/>
-      <c r="R3" s="123">
+      <c r="P3" s="120"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" s="122">
         <v>1</v>
       </c>
-      <c r="S3" s="124">
+      <c r="S3" s="123">
         <v>6</v>
       </c>
-      <c r="T3" s="125">
+      <c r="T3" s="124">
         <v>5</v>
       </c>
-      <c r="U3" s="124">
+      <c r="U3" s="123">
         <v>6</v>
       </c>
-      <c r="V3" s="122"/>
-      <c r="W3" s="126">
+      <c r="V3" s="121"/>
+      <c r="W3" s="125">
         <v>1</v>
       </c>
-      <c r="X3" s="122"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="122"/>
-      <c r="AA3" s="126"/>
-      <c r="AB3" s="127">
+      <c r="X3" s="121"/>
+      <c r="Y3" s="125"/>
+      <c r="Z3" s="121"/>
+      <c r="AA3" s="125"/>
+      <c r="AB3" s="126">
         <v>4</v>
       </c>
-      <c r="AC3" s="128">
+      <c r="AC3" s="127">
         <v>-5</v>
       </c>
-      <c r="AD3" s="123">
+      <c r="AD3" s="122">
         <v>-1</v>
       </c>
-      <c r="AE3" s="127">
+      <c r="AE3" s="126">
         <v>-4</v>
       </c>
-      <c r="AF3" s="128">
+      <c r="AF3" s="127">
         <v>5</v>
       </c>
-      <c r="AG3" s="122"/>
-      <c r="AH3" s="126"/>
-      <c r="AI3" s="122"/>
-      <c r="AJ3" s="123"/>
-      <c r="AK3" s="123"/>
-      <c r="AL3" s="123"/>
-      <c r="AM3" s="123"/>
-      <c r="AN3" s="119" t="s">
+      <c r="AG3" s="121"/>
+      <c r="AH3" s="125"/>
+      <c r="AI3" s="121"/>
+      <c r="AJ3" s="122"/>
+      <c r="AK3" s="122"/>
+      <c r="AL3" s="122"/>
+      <c r="AM3" s="122"/>
+      <c r="AN3" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="AO3" s="121" t="s">
+      <c r="AO3" s="120" t="s">
         <v>269</v>
       </c>
-      <c r="AP3" s="119" t="s">
+      <c r="AP3" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="AQ3" s="121" t="s">
+      <c r="AQ3" s="120" t="s">
         <v>271</v>
       </c>
-      <c r="AR3" s="119" t="s">
+      <c r="AR3" s="118" t="s">
         <v>272</v>
       </c>
-      <c r="AS3" s="121" t="s">
+      <c r="AS3" s="120" t="s">
         <v>273</v>
       </c>
-      <c r="AT3" s="119" t="s">
+      <c r="AT3" s="118" t="s">
         <v>274</v>
       </c>
-      <c r="AU3" s="121" t="s">
+      <c r="AU3" s="120" t="s">
         <v>275</v>
       </c>
     </row>
@@ -19202,73 +19218,73 @@
       <c r="A4" t="s">
         <v>276</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130">
+      <c r="B4" s="128"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129">
         <v>1</v>
       </c>
       <c r="E4" s="106" t="s">
         <v>250</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="117" t="s">
         <v>267</v>
       </c>
-      <c r="G4" s="130">
+      <c r="G4" s="129">
         <v>1</v>
       </c>
-      <c r="H4" s="122"/>
-      <c r="I4" s="123"/>
-      <c r="J4" s="126">
+      <c r="H4" s="121"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="125">
         <v>1</v>
       </c>
-      <c r="K4" s="123"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="122"/>
-      <c r="O4" s="123"/>
-      <c r="P4" s="123">
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="122"/>
+      <c r="P4" s="122">
         <v>2</v>
       </c>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="131"/>
-      <c r="T4" s="131"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="131"/>
-      <c r="Z4" s="131"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
-      <c r="AE4" s="131"/>
-      <c r="AF4" s="131"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AN4" s="119" t="s">
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
+      <c r="W4" s="130"/>
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="130"/>
+      <c r="AC4" s="130"/>
+      <c r="AD4" s="130"/>
+      <c r="AE4" s="130"/>
+      <c r="AF4" s="130"/>
+      <c r="AG4" s="130"/>
+      <c r="AH4" s="130"/>
+      <c r="AN4" s="118" t="s">
         <v>277</v>
       </c>
-      <c r="AO4" s="121" t="s">
+      <c r="AO4" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="AP4" s="119" t="s">
+      <c r="AP4" s="118" t="s">
         <v>279</v>
       </c>
-      <c r="AQ4" s="121" t="s">
+      <c r="AQ4" s="120" t="s">
         <v>280</v>
       </c>
-      <c r="AR4" s="119" t="s">
+      <c r="AR4" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="AS4" s="121" t="s">
+      <c r="AS4" s="120" t="s">
         <v>282</v>
       </c>
-      <c r="AT4" s="119" t="s">
+      <c r="AT4" s="118" t="s">
         <v>283</v>
       </c>
-      <c r="AU4" s="121" t="s">
+      <c r="AU4" s="120" t="s">
         <v>284</v>
       </c>
     </row>
@@ -19276,127 +19292,127 @@
       <c r="A5" t="s">
         <v>285</v>
       </c>
-      <c r="E5" s="129"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="131"/>
-      <c r="S5" s="131"/>
-      <c r="T5" s="131"/>
-      <c r="U5" s="131"/>
-      <c r="V5" s="131"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="131"/>
-      <c r="Y5" s="131"/>
-      <c r="Z5" s="131"/>
-      <c r="AA5" s="131"/>
-      <c r="AB5" s="131"/>
-      <c r="AC5" s="131"/>
-      <c r="AD5" s="131"/>
-      <c r="AE5" s="131"/>
-      <c r="AF5" s="131"/>
-      <c r="AG5" s="131"/>
-      <c r="AH5" s="131"/>
-      <c r="AN5" s="122" t="s">
+      <c r="E5" s="128"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+      <c r="Q5" s="130"/>
+      <c r="R5" s="130"/>
+      <c r="S5" s="130"/>
+      <c r="T5" s="130"/>
+      <c r="U5" s="130"/>
+      <c r="V5" s="130"/>
+      <c r="W5" s="130"/>
+      <c r="X5" s="130"/>
+      <c r="Y5" s="130"/>
+      <c r="Z5" s="130"/>
+      <c r="AA5" s="130"/>
+      <c r="AB5" s="130"/>
+      <c r="AC5" s="130"/>
+      <c r="AD5" s="130"/>
+      <c r="AE5" s="130"/>
+      <c r="AF5" s="130"/>
+      <c r="AG5" s="130"/>
+      <c r="AH5" s="130"/>
+      <c r="AN5" s="196" t="s">
+        <v>492</v>
+      </c>
+      <c r="AO5" s="197" t="s">
+        <v>493</v>
+      </c>
+      <c r="AP5" s="121" t="s">
         <v>286</v>
       </c>
-      <c r="AO5" s="126" t="s">
+      <c r="AQ5" s="125" t="s">
         <v>287</v>
       </c>
-      <c r="AP5" s="122" t="s">
+      <c r="AR5" s="121" t="s">
         <v>288</v>
       </c>
-      <c r="AQ5" s="126" t="s">
+      <c r="AS5" s="125" t="s">
         <v>289</v>
       </c>
-      <c r="AR5" s="122" t="s">
+      <c r="AT5" s="121" t="s">
         <v>290</v>
       </c>
-      <c r="AS5" s="126" t="s">
+      <c r="AU5" s="125" t="s">
         <v>291</v>
       </c>
-      <c r="AT5" s="122" t="s">
+    </row>
+    <row r="6" spans="1:47" ht="14.25" thickBot="1">
+      <c r="B6" s="191" t="s">
         <v>292</v>
       </c>
-      <c r="AU5" s="126" t="s">
+      <c r="C6" s="192"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="191" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="184" t="s">
+      <c r="F6" s="192"/>
+      <c r="G6" s="193"/>
+    </row>
+    <row r="7" spans="1:47" ht="14.25" thickBot="1">
+      <c r="B7" s="191" t="s">
         <v>294</v>
       </c>
-      <c r="C6" s="185"/>
-      <c r="D6" s="186"/>
-      <c r="E6" s="184" t="s">
+      <c r="C7" s="192"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="192"/>
+      <c r="J7" s="192"/>
+      <c r="K7" s="192"/>
+      <c r="L7" s="192"/>
+      <c r="M7" s="192"/>
+      <c r="N7" s="192"/>
+      <c r="O7" s="192"/>
+      <c r="P7" s="193"/>
+      <c r="Q7" s="191" t="s">
         <v>295</v>
       </c>
-      <c r="F6" s="185"/>
-      <c r="G6" s="186"/>
-    </row>
-    <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="184" t="s">
+      <c r="R7" s="192"/>
+      <c r="S7" s="192"/>
+      <c r="T7" s="192"/>
+      <c r="U7" s="192"/>
+      <c r="V7" s="192"/>
+      <c r="W7" s="192"/>
+      <c r="X7" s="192"/>
+      <c r="Y7" s="192"/>
+      <c r="Z7" s="192"/>
+      <c r="AA7" s="193"/>
+      <c r="AB7" s="191" t="s">
         <v>296</v>
       </c>
-      <c r="C7" s="185"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="185"/>
-      <c r="H7" s="185"/>
-      <c r="I7" s="185"/>
-      <c r="J7" s="185"/>
-      <c r="K7" s="185"/>
-      <c r="L7" s="185"/>
-      <c r="M7" s="185"/>
-      <c r="N7" s="185"/>
-      <c r="O7" s="185"/>
-      <c r="P7" s="186"/>
-      <c r="Q7" s="184" t="s">
-        <v>297</v>
-      </c>
-      <c r="R7" s="185"/>
-      <c r="S7" s="185"/>
-      <c r="T7" s="185"/>
-      <c r="U7" s="185"/>
-      <c r="V7" s="185"/>
-      <c r="W7" s="185"/>
-      <c r="X7" s="185"/>
-      <c r="Y7" s="185"/>
-      <c r="Z7" s="185"/>
-      <c r="AA7" s="186"/>
-      <c r="AB7" s="184" t="s">
-        <v>298</v>
-      </c>
-      <c r="AC7" s="185"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="185"/>
-      <c r="AF7" s="185"/>
-      <c r="AG7" s="185"/>
-      <c r="AH7" s="185"/>
-      <c r="AI7" s="185"/>
-      <c r="AJ7" s="185"/>
-      <c r="AK7" s="185"/>
-      <c r="AL7" s="185"/>
-      <c r="AM7" s="185"/>
-      <c r="AN7" s="185"/>
-      <c r="AO7" s="185"/>
-      <c r="AP7" s="185"/>
-      <c r="AQ7" s="185"/>
-      <c r="AR7" s="186"/>
+      <c r="AC7" s="192"/>
+      <c r="AD7" s="192"/>
+      <c r="AE7" s="192"/>
+      <c r="AF7" s="192"/>
+      <c r="AG7" s="192"/>
+      <c r="AH7" s="192"/>
+      <c r="AI7" s="192"/>
+      <c r="AJ7" s="192"/>
+      <c r="AK7" s="192"/>
+      <c r="AL7" s="192"/>
+      <c r="AM7" s="192"/>
+      <c r="AN7" s="192"/>
+      <c r="AO7" s="192"/>
+      <c r="AP7" s="192"/>
+      <c r="AQ7" s="192"/>
+      <c r="AR7" s="193"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AM9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -19404,7 +19420,7 @@
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
       <c r="H10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -19414,7 +19430,7 @@
     </row>
     <row r="15" spans="1:47">
       <c r="AB15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -19444,794 +19460,794 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="132">
+      <c r="A1" s="131">
         <v>0</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="135"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="134"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="136">
+      <c r="A2" s="135">
         <v>1</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="136" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="137" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="139"/>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" s="135">
+        <v>2</v>
+      </c>
+      <c r="B3" s="136" t="s">
         <v>303</v>
       </c>
-      <c r="C2" s="138" t="s">
+      <c r="C3" s="137" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="140"/>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="136">
-        <v>2</v>
-      </c>
-      <c r="B3" s="137" t="s">
+      <c r="D3" s="137" t="s">
         <v>305</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="139"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" s="135">
+        <v>3</v>
+      </c>
+      <c r="B4" s="136" t="s">
         <v>306</v>
       </c>
-      <c r="D3" s="138" t="s">
+      <c r="C4" s="137" t="s">
         <v>307</v>
       </c>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="140"/>
-    </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="136">
-        <v>3</v>
-      </c>
-      <c r="B4" s="137" t="s">
+      <c r="D4" s="137" t="s">
         <v>308</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="E4" s="137" t="s">
         <v>309</v>
       </c>
-      <c r="D4" s="138" t="s">
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="139"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" s="135">
+        <v>4</v>
+      </c>
+      <c r="B5" s="136" t="s">
         <v>310</v>
       </c>
-      <c r="E4" s="138" t="s">
+      <c r="C5" s="137" t="s">
         <v>311</v>
       </c>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="140"/>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="136">
-        <v>4</v>
-      </c>
-      <c r="B5" s="137" t="s">
+      <c r="D5" s="137" t="s">
         <v>312</v>
       </c>
-      <c r="C5" s="138" t="s">
+      <c r="E5" s="137" t="s">
         <v>313</v>
       </c>
-      <c r="D5" s="138" t="s">
+      <c r="F5" s="137" t="s">
         <v>314</v>
       </c>
-      <c r="E5" s="138" t="s">
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="138"/>
+      <c r="J5" s="138"/>
+      <c r="K5" s="138"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="139"/>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" s="135">
+        <v>5</v>
+      </c>
+      <c r="B6" s="136" t="s">
         <v>315</v>
       </c>
-      <c r="F5" s="138" t="s">
+      <c r="C6" s="137" t="s">
         <v>316</v>
       </c>
-      <c r="G5" s="139"/>
-      <c r="H5" s="139"/>
-      <c r="I5" s="139"/>
-      <c r="J5" s="139"/>
-      <c r="K5" s="139"/>
-      <c r="L5" s="139"/>
-      <c r="M5" s="140"/>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="136">
-        <v>5</v>
-      </c>
-      <c r="B6" s="137" t="s">
+      <c r="D6" s="137" t="s">
         <v>317</v>
       </c>
-      <c r="C6" s="138" t="s">
+      <c r="E6" s="137" t="s">
         <v>318</v>
       </c>
-      <c r="D6" s="138" t="s">
+      <c r="F6" s="137" t="s">
         <v>319</v>
       </c>
-      <c r="E6" s="138" t="s">
+      <c r="G6" s="137" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="138" t="s">
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="138"/>
+      <c r="K6" s="138"/>
+      <c r="L6" s="138"/>
+      <c r="M6" s="139"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" s="135">
+        <v>6</v>
+      </c>
+      <c r="B7" s="136" t="s">
         <v>321</v>
       </c>
-      <c r="G6" s="138" t="s">
+      <c r="C7" s="137" t="s">
         <v>322</v>
       </c>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="139"/>
-      <c r="M6" s="140"/>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="136">
-        <v>6</v>
-      </c>
-      <c r="B7" s="137" t="s">
+      <c r="D7" s="137" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="138" t="s">
+      <c r="E7" s="137" t="s">
         <v>324</v>
       </c>
-      <c r="D7" s="138" t="s">
+      <c r="F7" s="137" t="s">
         <v>325</v>
       </c>
-      <c r="E7" s="138" t="s">
+      <c r="G7" s="137" t="s">
         <v>326</v>
       </c>
-      <c r="F7" s="138" t="s">
+      <c r="H7" s="137" t="s">
         <v>327</v>
       </c>
-      <c r="G7" s="138" t="s">
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="139"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" s="135">
+        <v>7</v>
+      </c>
+      <c r="B8" s="136" t="s">
         <v>328</v>
       </c>
-      <c r="H7" s="138" t="s">
+      <c r="C8" s="137" t="s">
         <v>329</v>
       </c>
-      <c r="I7" s="139"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="139"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="140"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="136">
-        <v>7</v>
-      </c>
-      <c r="B8" s="137" t="s">
+      <c r="D8" s="137" t="s">
         <v>330</v>
       </c>
-      <c r="C8" s="138" t="s">
+      <c r="E8" s="137" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="138" t="s">
+      <c r="F8" s="137" t="s">
         <v>332</v>
       </c>
-      <c r="E8" s="138" t="s">
+      <c r="G8" s="137" t="s">
         <v>333</v>
       </c>
-      <c r="F8" s="138" t="s">
+      <c r="H8" s="137" t="s">
         <v>334</v>
       </c>
-      <c r="G8" s="138" t="s">
+      <c r="I8" s="137" t="s">
         <v>335</v>
       </c>
-      <c r="H8" s="138" t="s">
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="139"/>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" s="135">
+        <v>8</v>
+      </c>
+      <c r="B9" s="136" t="s">
         <v>336</v>
       </c>
-      <c r="I8" s="138" t="s">
+      <c r="C9" s="137" t="s">
         <v>337</v>
       </c>
-      <c r="J8" s="139"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="140"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="136">
-        <v>8</v>
-      </c>
-      <c r="B9" s="137" t="s">
+      <c r="D9" s="137" t="s">
         <v>338</v>
       </c>
-      <c r="C9" s="138" t="s">
+      <c r="E9" s="137" t="s">
         <v>339</v>
       </c>
-      <c r="D9" s="138" t="s">
+      <c r="F9" s="137" t="s">
         <v>340</v>
       </c>
-      <c r="E9" s="138" t="s">
+      <c r="G9" s="137" t="s">
         <v>341</v>
       </c>
-      <c r="F9" s="138" t="s">
+      <c r="H9" s="137" t="s">
         <v>342</v>
       </c>
-      <c r="G9" s="138" t="s">
+      <c r="I9" s="137" t="s">
         <v>343</v>
       </c>
-      <c r="H9" s="138" t="s">
+      <c r="J9" s="137" t="s">
         <v>344</v>
       </c>
-      <c r="I9" s="138" t="s">
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="139"/>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" s="135">
+        <v>9</v>
+      </c>
+      <c r="B10" s="136" t="s">
         <v>345</v>
       </c>
-      <c r="J9" s="138" t="s">
+      <c r="C10" s="137" t="s">
         <v>346</v>
       </c>
-      <c r="K9" s="139"/>
-      <c r="L9" s="139"/>
-      <c r="M9" s="140"/>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="136">
-        <v>9</v>
-      </c>
-      <c r="B10" s="137" t="s">
+      <c r="D10" s="137" t="s">
         <v>347</v>
       </c>
-      <c r="C10" s="138" t="s">
+      <c r="E10" s="137" t="s">
         <v>348</v>
       </c>
-      <c r="D10" s="138" t="s">
+      <c r="F10" s="137" t="s">
         <v>349</v>
       </c>
-      <c r="E10" s="138" t="s">
+      <c r="G10" s="137" t="s">
         <v>350</v>
       </c>
-      <c r="F10" s="138" t="s">
+      <c r="H10" s="137" t="s">
         <v>351</v>
       </c>
-      <c r="G10" s="138" t="s">
+      <c r="I10" s="137" t="s">
         <v>352</v>
       </c>
-      <c r="H10" s="138" t="s">
+      <c r="J10" s="137" t="s">
         <v>353</v>
       </c>
-      <c r="I10" s="138" t="s">
+      <c r="K10" s="137" t="s">
         <v>354</v>
       </c>
-      <c r="J10" s="138" t="s">
+      <c r="L10" s="138"/>
+      <c r="M10" s="139"/>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="135">
+        <v>10</v>
+      </c>
+      <c r="B11" s="136" t="s">
         <v>355</v>
       </c>
-      <c r="K10" s="138" t="s">
+      <c r="C11" s="137" t="s">
         <v>356</v>
       </c>
-      <c r="L10" s="139"/>
-      <c r="M10" s="140"/>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="136">
-        <v>10</v>
-      </c>
-      <c r="B11" s="137" t="s">
+      <c r="D11" s="137" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="138" t="s">
+      <c r="E11" s="137" t="s">
         <v>358</v>
       </c>
-      <c r="D11" s="138" t="s">
+      <c r="F11" s="137" t="s">
         <v>359</v>
       </c>
-      <c r="E11" s="138" t="s">
+      <c r="G11" s="137" t="s">
         <v>360</v>
       </c>
-      <c r="F11" s="138" t="s">
+      <c r="H11" s="137" t="s">
         <v>361</v>
       </c>
-      <c r="G11" s="138" t="s">
+      <c r="I11" s="137" t="s">
         <v>362</v>
       </c>
-      <c r="H11" s="138" t="s">
+      <c r="J11" s="137" t="s">
         <v>363</v>
       </c>
-      <c r="I11" s="138" t="s">
+      <c r="K11" s="137" t="s">
         <v>364</v>
       </c>
-      <c r="J11" s="138" t="s">
+      <c r="L11" s="137" t="s">
         <v>365</v>
       </c>
-      <c r="K11" s="138" t="s">
+      <c r="M11" s="139"/>
+    </row>
+    <row r="12" spans="1:23" ht="14.25" thickBot="1">
+      <c r="A12" s="140">
+        <v>11</v>
+      </c>
+      <c r="B12" s="141" t="s">
         <v>366</v>
       </c>
-      <c r="L11" s="138" t="s">
+      <c r="C12" s="142" t="s">
         <v>367</v>
       </c>
-      <c r="M11" s="140"/>
-    </row>
-    <row r="12" spans="1:23" ht="14.25" thickBot="1">
-      <c r="A12" s="141">
-        <v>11</v>
-      </c>
-      <c r="B12" s="142" t="s">
+      <c r="D12" s="142" t="s">
         <v>368</v>
       </c>
-      <c r="C12" s="143" t="s">
+      <c r="E12" s="142" t="s">
         <v>369</v>
       </c>
-      <c r="D12" s="143" t="s">
+      <c r="F12" s="143" t="s">
         <v>370</v>
       </c>
-      <c r="E12" s="143" t="s">
+      <c r="G12" s="142" t="s">
         <v>371</v>
       </c>
-      <c r="F12" s="144" t="s">
+      <c r="H12" s="142" t="s">
         <v>372</v>
       </c>
-      <c r="G12" s="143" t="s">
+      <c r="I12" s="142" t="s">
         <v>373</v>
       </c>
-      <c r="H12" s="143" t="s">
+      <c r="J12" s="142" t="s">
         <v>374</v>
       </c>
-      <c r="I12" s="143" t="s">
+      <c r="K12" s="142" t="s">
         <v>375</v>
       </c>
-      <c r="J12" s="143" t="s">
+      <c r="L12" s="142" t="s">
         <v>376</v>
       </c>
-      <c r="K12" s="143" t="s">
+      <c r="M12" s="144" t="s">
         <v>377</v>
-      </c>
-      <c r="L12" s="143" t="s">
-        <v>378</v>
-      </c>
-      <c r="M12" s="145" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="102" t="s">
         <v>249</v>
       </c>
-      <c r="B14" s="146"/>
-      <c r="C14" s="147" t="s">
+      <c r="B14" s="145"/>
+      <c r="C14" s="146" t="s">
+        <v>328</v>
+      </c>
+      <c r="D14" s="147" t="s">
+        <v>329</v>
+      </c>
+      <c r="E14" s="147" t="s">
         <v>330</v>
       </c>
-      <c r="D14" s="148" t="s">
+      <c r="F14" s="147" t="s">
         <v>331</v>
       </c>
-      <c r="E14" s="148" t="s">
+      <c r="G14" s="147" t="s">
         <v>332</v>
       </c>
-      <c r="F14" s="148" t="s">
+      <c r="H14" s="147" t="s">
         <v>333</v>
       </c>
-      <c r="G14" s="148" t="s">
+      <c r="I14" s="147" t="s">
         <v>334</v>
       </c>
-      <c r="H14" s="148" t="s">
+      <c r="J14" s="147" t="s">
         <v>335</v>
       </c>
-      <c r="I14" s="148" t="s">
+      <c r="K14" s="146" t="s">
         <v>336</v>
       </c>
-      <c r="J14" s="148" t="s">
+      <c r="L14" s="147" t="s">
         <v>337</v>
       </c>
-      <c r="K14" s="147" t="s">
+      <c r="M14" s="147" t="s">
         <v>338</v>
       </c>
-      <c r="L14" s="148" t="s">
+      <c r="N14" s="147" t="s">
         <v>339</v>
       </c>
-      <c r="M14" s="148" t="s">
+      <c r="O14" s="147" t="s">
         <v>340</v>
       </c>
-      <c r="N14" s="148" t="s">
+      <c r="P14" s="147" t="s">
         <v>341</v>
       </c>
-      <c r="O14" s="148" t="s">
+      <c r="Q14" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="P14" s="148" t="s">
+      <c r="R14" s="147" t="s">
         <v>343</v>
       </c>
-      <c r="Q14" s="148" t="s">
+      <c r="S14" s="147" t="s">
         <v>344</v>
       </c>
-      <c r="R14" s="148" t="s">
-        <v>345</v>
-      </c>
-      <c r="S14" s="148" t="s">
-        <v>346</v>
-      </c>
       <c r="T14" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="U14" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="V14" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W14" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="B15" s="147" t="s">
-        <v>303</v>
-      </c>
-      <c r="C15" s="148" t="s">
-        <v>304</v>
-      </c>
-      <c r="D15" s="147" t="s">
+      <c r="B15" s="146" t="s">
+        <v>301</v>
+      </c>
+      <c r="C15" s="147" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="146" t="s">
+        <v>321</v>
+      </c>
+      <c r="E15" s="147" t="s">
+        <v>322</v>
+      </c>
+      <c r="F15" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="E15" s="148" t="s">
+      <c r="G15" s="147" t="s">
         <v>324</v>
       </c>
-      <c r="F15" s="148" t="s">
+      <c r="H15" s="147" t="s">
         <v>325</v>
       </c>
-      <c r="G15" s="148" t="s">
+      <c r="I15" s="147" t="s">
         <v>326</v>
       </c>
-      <c r="H15" s="148" t="s">
+      <c r="J15" s="147" t="s">
         <v>327</v>
       </c>
-      <c r="I15" s="148" t="s">
-        <v>328</v>
-      </c>
-      <c r="J15" s="148" t="s">
-        <v>329</v>
-      </c>
-      <c r="K15" s="147" t="s">
+      <c r="K15" s="146" t="s">
+        <v>345</v>
+      </c>
+      <c r="L15" s="147" t="s">
+        <v>346</v>
+      </c>
+      <c r="M15" s="147" t="s">
         <v>347</v>
       </c>
-      <c r="L15" s="148" t="s">
+      <c r="N15" s="147" t="s">
         <v>348</v>
       </c>
-      <c r="M15" s="148" t="s">
+      <c r="O15" s="147" t="s">
         <v>349</v>
       </c>
-      <c r="N15" s="148" t="s">
+      <c r="P15" s="147" t="s">
         <v>350</v>
       </c>
-      <c r="O15" s="148" t="s">
+      <c r="Q15" s="147" t="s">
         <v>351</v>
       </c>
-      <c r="P15" s="148" t="s">
+      <c r="R15" s="147" t="s">
         <v>352</v>
       </c>
-      <c r="Q15" s="148" t="s">
+      <c r="S15" s="147" t="s">
         <v>353</v>
       </c>
-      <c r="R15" s="148" t="s">
+      <c r="T15" s="147" t="s">
         <v>354</v>
       </c>
-      <c r="S15" s="148" t="s">
-        <v>355</v>
-      </c>
-      <c r="T15" s="148" t="s">
-        <v>356</v>
-      </c>
       <c r="U15" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="V15" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W15" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="146" t="s">
+        <v>303</v>
+      </c>
+      <c r="C16" s="147" t="s">
+        <v>304</v>
+      </c>
+      <c r="D16" s="147" t="s">
         <v>305</v>
       </c>
-      <c r="C16" s="148" t="s">
-        <v>306</v>
-      </c>
-      <c r="D16" s="148" t="s">
-        <v>307</v>
-      </c>
-      <c r="E16" s="147" t="s">
+      <c r="E16" s="146" t="s">
+        <v>315</v>
+      </c>
+      <c r="F16" s="147" t="s">
+        <v>316</v>
+      </c>
+      <c r="G16" s="147" t="s">
         <v>317</v>
       </c>
-      <c r="F16" s="148" t="s">
+      <c r="H16" s="147" t="s">
         <v>318</v>
       </c>
-      <c r="G16" s="148" t="s">
+      <c r="I16" s="147" t="s">
         <v>319</v>
       </c>
-      <c r="H16" s="148" t="s">
+      <c r="J16" s="147" t="s">
         <v>320</v>
       </c>
-      <c r="I16" s="148" t="s">
-        <v>321</v>
-      </c>
-      <c r="J16" s="148" t="s">
-        <v>322</v>
-      </c>
-      <c r="K16" s="147" t="s">
+      <c r="K16" s="146" t="s">
+        <v>355</v>
+      </c>
+      <c r="L16" s="147" t="s">
+        <v>356</v>
+      </c>
+      <c r="M16" s="147" t="s">
         <v>357</v>
       </c>
-      <c r="L16" s="148" t="s">
+      <c r="N16" s="147" t="s">
         <v>358</v>
       </c>
-      <c r="M16" s="148" t="s">
+      <c r="O16" s="147" t="s">
         <v>359</v>
       </c>
-      <c r="N16" s="148" t="s">
+      <c r="P16" s="147" t="s">
         <v>360</v>
       </c>
-      <c r="O16" s="148" t="s">
+      <c r="Q16" s="147" t="s">
         <v>361</v>
       </c>
-      <c r="P16" s="148" t="s">
+      <c r="R16" s="147" t="s">
         <v>362</v>
       </c>
-      <c r="Q16" s="148" t="s">
+      <c r="S16" s="147" t="s">
         <v>363</v>
       </c>
-      <c r="R16" s="148" t="s">
+      <c r="T16" s="147" t="s">
         <v>364</v>
       </c>
-      <c r="S16" s="148" t="s">
+      <c r="U16" s="147" t="s">
         <v>365</v>
       </c>
-      <c r="T16" s="148" t="s">
-        <v>366</v>
-      </c>
-      <c r="U16" s="148" t="s">
-        <v>367</v>
-      </c>
       <c r="V16" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="W16" s="102" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="B17" s="147" t="s">
+      <c r="B17" s="146" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="147" t="s">
+        <v>307</v>
+      </c>
+      <c r="D17" s="147" t="s">
         <v>308</v>
       </c>
-      <c r="C17" s="148" t="s">
+      <c r="E17" s="147" t="s">
         <v>309</v>
       </c>
-      <c r="D17" s="148" t="s">
+      <c r="F17" s="146" t="s">
         <v>310</v>
       </c>
-      <c r="E17" s="148" t="s">
+      <c r="G17" s="147" t="s">
         <v>311</v>
       </c>
-      <c r="F17" s="147" t="s">
+      <c r="H17" s="147" t="s">
         <v>312</v>
       </c>
-      <c r="G17" s="148" t="s">
+      <c r="I17" s="147" t="s">
         <v>313</v>
       </c>
-      <c r="H17" s="148" t="s">
+      <c r="J17" s="147" t="s">
         <v>314</v>
       </c>
-      <c r="I17" s="148" t="s">
-        <v>315</v>
-      </c>
-      <c r="J17" s="148" t="s">
-        <v>316</v>
-      </c>
-      <c r="K17" s="147" t="s">
+      <c r="K17" s="146" t="s">
+        <v>366</v>
+      </c>
+      <c r="L17" s="147" t="s">
+        <v>367</v>
+      </c>
+      <c r="M17" s="147" t="s">
         <v>368</v>
       </c>
-      <c r="L17" s="148" t="s">
+      <c r="N17" s="147" t="s">
         <v>369</v>
       </c>
-      <c r="M17" s="148" t="s">
+      <c r="O17" s="148" t="s">
         <v>370</v>
       </c>
-      <c r="N17" s="148" t="s">
+      <c r="P17" s="147" t="s">
         <v>371</v>
       </c>
-      <c r="O17" s="149" t="s">
+      <c r="Q17" s="147" t="s">
         <v>372</v>
       </c>
-      <c r="P17" s="148" t="s">
+      <c r="R17" s="147" t="s">
         <v>373</v>
       </c>
-      <c r="Q17" s="148" t="s">
+      <c r="S17" s="147" t="s">
         <v>374</v>
       </c>
-      <c r="R17" s="148" t="s">
+      <c r="T17" s="147" t="s">
         <v>375</v>
       </c>
-      <c r="S17" s="148" t="s">
+      <c r="U17" s="147" t="s">
         <v>376</v>
       </c>
-      <c r="T17" s="148" t="s">
+      <c r="V17" s="147" t="s">
         <v>377</v>
       </c>
-      <c r="U17" s="148" t="s">
+      <c r="W17" s="102" t="s">
         <v>378</v>
-      </c>
-      <c r="V17" s="148" t="s">
-        <v>379</v>
-      </c>
-      <c r="W17" s="102" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="102" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="147" t="s">
+      <c r="B19" s="146" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="147" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" s="147" t="s">
         <v>338</v>
       </c>
-      <c r="C19" s="148" t="s">
+      <c r="E19" s="147" t="s">
         <v>339</v>
       </c>
-      <c r="D19" s="148" t="s">
+      <c r="F19" s="147" t="s">
         <v>340</v>
       </c>
-      <c r="E19" s="148" t="s">
+      <c r="G19" s="147" t="s">
         <v>341</v>
       </c>
-      <c r="F19" s="148" t="s">
+      <c r="H19" s="147" t="s">
         <v>342</v>
       </c>
-      <c r="G19" s="148" t="s">
+      <c r="I19" s="147" t="s">
         <v>343</v>
       </c>
-      <c r="H19" s="148" t="s">
+      <c r="J19" s="147" t="s">
         <v>344</v>
-      </c>
-      <c r="I19" s="148" t="s">
-        <v>345</v>
-      </c>
-      <c r="J19" s="148" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="B20" s="147" t="s">
+      <c r="B20" s="146" t="s">
+        <v>345</v>
+      </c>
+      <c r="C20" s="147" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" s="147" t="s">
         <v>347</v>
       </c>
-      <c r="C20" s="148" t="s">
+      <c r="E20" s="147" t="s">
         <v>348</v>
       </c>
-      <c r="D20" s="148" t="s">
+      <c r="F20" s="147" t="s">
         <v>349</v>
       </c>
-      <c r="E20" s="148" t="s">
+      <c r="G20" s="147" t="s">
         <v>350</v>
       </c>
-      <c r="F20" s="148" t="s">
+      <c r="H20" s="147" t="s">
         <v>351</v>
       </c>
-      <c r="G20" s="148" t="s">
+      <c r="I20" s="147" t="s">
         <v>352</v>
       </c>
-      <c r="H20" s="148" t="s">
+      <c r="J20" s="147" t="s">
         <v>353</v>
       </c>
-      <c r="I20" s="148" t="s">
+      <c r="K20" s="147" t="s">
         <v>354</v>
-      </c>
-      <c r="J20" s="148" t="s">
-        <v>355</v>
-      </c>
-      <c r="K20" s="148" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="102" t="s">
         <v>276</v>
       </c>
-      <c r="B21" s="147" t="s">
+      <c r="B21" s="146" t="s">
+        <v>355</v>
+      </c>
+      <c r="C21" s="147" t="s">
+        <v>356</v>
+      </c>
+      <c r="D21" s="147" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="148" t="s">
+      <c r="E21" s="147" t="s">
         <v>358</v>
       </c>
-      <c r="D21" s="148" t="s">
+      <c r="F21" s="147" t="s">
         <v>359</v>
       </c>
-      <c r="E21" s="148" t="s">
+      <c r="G21" s="147" t="s">
         <v>360</v>
       </c>
-      <c r="F21" s="148" t="s">
+      <c r="H21" s="147" t="s">
         <v>361</v>
       </c>
-      <c r="G21" s="148" t="s">
+      <c r="I21" s="147" t="s">
         <v>362</v>
       </c>
-      <c r="H21" s="148" t="s">
+      <c r="J21" s="147" t="s">
         <v>363</v>
       </c>
-      <c r="I21" s="148" t="s">
+      <c r="K21" s="147" t="s">
         <v>364</v>
       </c>
-      <c r="J21" s="148" t="s">
+      <c r="L21" s="147" t="s">
         <v>365</v>
-      </c>
-      <c r="K21" s="148" t="s">
-        <v>366</v>
-      </c>
-      <c r="L21" s="148" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="147" t="s">
+      <c r="B22" s="146" t="s">
+        <v>366</v>
+      </c>
+      <c r="C22" s="147" t="s">
+        <v>367</v>
+      </c>
+      <c r="D22" s="147" t="s">
         <v>368</v>
       </c>
-      <c r="C22" s="148" t="s">
+      <c r="E22" s="147" t="s">
         <v>369</v>
       </c>
-      <c r="D22" s="148" t="s">
+      <c r="F22" s="148" t="s">
         <v>370</v>
       </c>
-      <c r="E22" s="148" t="s">
+      <c r="G22" s="147" t="s">
         <v>371</v>
       </c>
-      <c r="F22" s="149" t="s">
+      <c r="H22" s="147" t="s">
         <v>372</v>
       </c>
-      <c r="G22" s="148" t="s">
+      <c r="I22" s="147" t="s">
         <v>373</v>
       </c>
-      <c r="H22" s="148" t="s">
+      <c r="J22" s="147" t="s">
         <v>374</v>
       </c>
-      <c r="I22" s="148" t="s">
+      <c r="K22" s="147" t="s">
         <v>375</v>
       </c>
-      <c r="J22" s="148" t="s">
+      <c r="L22" s="147" t="s">
         <v>376</v>
       </c>
-      <c r="K22" s="148" t="s">
+      <c r="M22" s="147" t="s">
         <v>377</v>
-      </c>
-      <c r="L22" s="148" t="s">
-        <v>378</v>
-      </c>
-      <c r="M22" s="148" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="102" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B24" s="102" t="s">
         <v>249</v>
@@ -20262,15 +20278,15 @@
       <c r="A25" s="102">
         <v>0</v>
       </c>
-      <c r="B25" s="146"/>
-      <c r="C25" s="147" t="s">
+      <c r="B25" s="145"/>
+      <c r="C25" s="146" t="s">
+        <v>301</v>
+      </c>
+      <c r="D25" s="146" t="s">
         <v>303</v>
       </c>
-      <c r="D25" s="147" t="s">
-        <v>305</v>
-      </c>
-      <c r="E25" s="147" t="s">
-        <v>308</v>
+      <c r="E25" s="146" t="s">
+        <v>306</v>
       </c>
       <c r="H25" s="102">
         <v>0</v>
@@ -20289,17 +20305,17 @@
       <c r="A26" s="102">
         <v>1</v>
       </c>
-      <c r="B26" s="147" t="s">
-        <v>330</v>
-      </c>
-      <c r="C26" s="148" t="s">
+      <c r="B26" s="146" t="s">
+        <v>328</v>
+      </c>
+      <c r="C26" s="147" t="s">
+        <v>302</v>
+      </c>
+      <c r="D26" s="147" t="s">
         <v>304</v>
       </c>
-      <c r="D26" s="148" t="s">
-        <v>306</v>
-      </c>
-      <c r="E26" s="148" t="s">
-        <v>309</v>
+      <c r="E26" s="147" t="s">
+        <v>307</v>
       </c>
       <c r="H26" s="102">
         <v>0</v>
@@ -20318,17 +20334,17 @@
       <c r="A27" s="102">
         <v>2</v>
       </c>
-      <c r="B27" s="148" t="s">
-        <v>331</v>
-      </c>
-      <c r="C27" s="147" t="s">
-        <v>323</v>
-      </c>
-      <c r="D27" s="148" t="s">
-        <v>382</v>
-      </c>
-      <c r="E27" s="148" t="s">
-        <v>383</v>
+      <c r="B27" s="147" t="s">
+        <v>329</v>
+      </c>
+      <c r="C27" s="146" t="s">
+        <v>321</v>
+      </c>
+      <c r="D27" s="147" t="s">
+        <v>380</v>
+      </c>
+      <c r="E27" s="147" t="s">
+        <v>381</v>
       </c>
       <c r="H27" s="102">
         <v>1</v>
@@ -20347,17 +20363,17 @@
       <c r="A28" s="102">
         <v>3</v>
       </c>
-      <c r="B28" s="148" t="s">
-        <v>332</v>
-      </c>
-      <c r="C28" s="148" t="s">
-        <v>324</v>
-      </c>
-      <c r="D28" s="147" t="s">
-        <v>317</v>
-      </c>
-      <c r="E28" s="148" t="s">
-        <v>384</v>
+      <c r="B28" s="147" t="s">
+        <v>330</v>
+      </c>
+      <c r="C28" s="147" t="s">
+        <v>322</v>
+      </c>
+      <c r="D28" s="146" t="s">
+        <v>315</v>
+      </c>
+      <c r="E28" s="147" t="s">
+        <v>382</v>
       </c>
       <c r="H28" s="102">
         <v>2</v>
@@ -20376,17 +20392,17 @@
       <c r="A29" s="102">
         <v>4</v>
       </c>
-      <c r="B29" s="148" t="s">
-        <v>333</v>
-      </c>
-      <c r="C29" s="148" t="s">
-        <v>325</v>
-      </c>
-      <c r="D29" s="148" t="s">
-        <v>318</v>
-      </c>
-      <c r="E29" s="147" t="s">
-        <v>312</v>
+      <c r="B29" s="147" t="s">
+        <v>331</v>
+      </c>
+      <c r="C29" s="147" t="s">
+        <v>323</v>
+      </c>
+      <c r="D29" s="147" t="s">
+        <v>316</v>
+      </c>
+      <c r="E29" s="146" t="s">
+        <v>310</v>
       </c>
       <c r="H29" s="102">
         <v>3</v>
@@ -20405,17 +20421,17 @@
       <c r="A30" s="102">
         <v>5</v>
       </c>
-      <c r="B30" s="148" t="s">
-        <v>334</v>
-      </c>
-      <c r="C30" s="148" t="s">
-        <v>326</v>
-      </c>
-      <c r="D30" s="148" t="s">
-        <v>319</v>
-      </c>
-      <c r="E30" s="148" t="s">
-        <v>313</v>
+      <c r="B30" s="147" t="s">
+        <v>332</v>
+      </c>
+      <c r="C30" s="147" t="s">
+        <v>324</v>
+      </c>
+      <c r="D30" s="147" t="s">
+        <v>317</v>
+      </c>
+      <c r="E30" s="147" t="s">
+        <v>311</v>
       </c>
       <c r="H30" s="102">
         <v>4</v>
@@ -20434,17 +20450,17 @@
       <c r="A31" s="102">
         <v>6</v>
       </c>
-      <c r="B31" s="148" t="s">
-        <v>335</v>
-      </c>
-      <c r="C31" s="148" t="s">
-        <v>327</v>
-      </c>
-      <c r="D31" s="148" t="s">
-        <v>320</v>
-      </c>
-      <c r="E31" s="148" t="s">
-        <v>314</v>
+      <c r="B31" s="147" t="s">
+        <v>333</v>
+      </c>
+      <c r="C31" s="147" t="s">
+        <v>325</v>
+      </c>
+      <c r="D31" s="147" t="s">
+        <v>318</v>
+      </c>
+      <c r="E31" s="147" t="s">
+        <v>312</v>
       </c>
       <c r="H31" s="102">
         <v>5</v>
@@ -20463,17 +20479,17 @@
       <c r="A32" s="102">
         <v>7</v>
       </c>
-      <c r="B32" s="148" t="s">
-        <v>336</v>
-      </c>
-      <c r="C32" s="148" t="s">
-        <v>328</v>
-      </c>
-      <c r="D32" s="148" t="s">
-        <v>321</v>
-      </c>
-      <c r="E32" s="148" t="s">
-        <v>315</v>
+      <c r="B32" s="147" t="s">
+        <v>334</v>
+      </c>
+      <c r="C32" s="147" t="s">
+        <v>326</v>
+      </c>
+      <c r="D32" s="147" t="s">
+        <v>319</v>
+      </c>
+      <c r="E32" s="147" t="s">
+        <v>313</v>
       </c>
       <c r="H32" s="102">
         <v>6</v>
@@ -20492,17 +20508,17 @@
       <c r="A33" s="102">
         <v>8</v>
       </c>
-      <c r="B33" s="148" t="s">
-        <v>337</v>
-      </c>
-      <c r="C33" s="148" t="s">
-        <v>329</v>
-      </c>
-      <c r="D33" s="148" t="s">
-        <v>322</v>
-      </c>
-      <c r="E33" s="148" t="s">
-        <v>316</v>
+      <c r="B33" s="147" t="s">
+        <v>335</v>
+      </c>
+      <c r="C33" s="147" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" s="147" t="s">
+        <v>320</v>
+      </c>
+      <c r="E33" s="147" t="s">
+        <v>314</v>
       </c>
       <c r="H33" s="102">
         <v>7</v>
@@ -20521,17 +20537,17 @@
       <c r="A34" s="102">
         <v>9</v>
       </c>
-      <c r="B34" s="147" t="s">
-        <v>338</v>
-      </c>
-      <c r="C34" s="147" t="s">
-        <v>347</v>
-      </c>
-      <c r="D34" s="147" t="s">
-        <v>357</v>
-      </c>
-      <c r="E34" s="147" t="s">
-        <v>368</v>
+      <c r="B34" s="146" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" s="146" t="s">
+        <v>345</v>
+      </c>
+      <c r="D34" s="146" t="s">
+        <v>355</v>
+      </c>
+      <c r="E34" s="146" t="s">
+        <v>366</v>
       </c>
       <c r="H34" s="102">
         <v>8</v>
@@ -20550,17 +20566,17 @@
       <c r="A35" s="102">
         <v>10</v>
       </c>
-      <c r="B35" s="148" t="s">
-        <v>339</v>
-      </c>
-      <c r="C35" s="148" t="s">
-        <v>348</v>
-      </c>
-      <c r="D35" s="148" t="s">
-        <v>358</v>
-      </c>
-      <c r="E35" s="148" t="s">
-        <v>369</v>
+      <c r="B35" s="147" t="s">
+        <v>337</v>
+      </c>
+      <c r="C35" s="147" t="s">
+        <v>346</v>
+      </c>
+      <c r="D35" s="147" t="s">
+        <v>356</v>
+      </c>
+      <c r="E35" s="147" t="s">
+        <v>367</v>
       </c>
       <c r="H35" s="102">
         <v>9</v>
@@ -20579,17 +20595,17 @@
       <c r="A36" s="102">
         <v>11</v>
       </c>
-      <c r="B36" s="148" t="s">
-        <v>340</v>
-      </c>
-      <c r="C36" s="148" t="s">
-        <v>349</v>
-      </c>
-      <c r="D36" s="148" t="s">
-        <v>359</v>
-      </c>
-      <c r="E36" s="148" t="s">
-        <v>370</v>
+      <c r="B36" s="147" t="s">
+        <v>338</v>
+      </c>
+      <c r="C36" s="147" t="s">
+        <v>347</v>
+      </c>
+      <c r="D36" s="147" t="s">
+        <v>357</v>
+      </c>
+      <c r="E36" s="147" t="s">
+        <v>368</v>
       </c>
       <c r="H36" s="102">
         <v>10</v>
@@ -20608,17 +20624,17 @@
       <c r="A37" s="102">
         <v>12</v>
       </c>
-      <c r="B37" s="148" t="s">
-        <v>341</v>
-      </c>
-      <c r="C37" s="148" t="s">
-        <v>350</v>
-      </c>
-      <c r="D37" s="148" t="s">
-        <v>360</v>
-      </c>
-      <c r="E37" s="148" t="s">
-        <v>371</v>
+      <c r="B37" s="147" t="s">
+        <v>339</v>
+      </c>
+      <c r="C37" s="147" t="s">
+        <v>348</v>
+      </c>
+      <c r="D37" s="147" t="s">
+        <v>358</v>
+      </c>
+      <c r="E37" s="147" t="s">
+        <v>369</v>
       </c>
       <c r="H37" s="102">
         <v>11</v>
@@ -20637,17 +20653,17 @@
       <c r="A38" s="102">
         <v>13</v>
       </c>
-      <c r="B38" s="148" t="s">
-        <v>342</v>
-      </c>
-      <c r="C38" s="148" t="s">
-        <v>351</v>
-      </c>
-      <c r="D38" s="148" t="s">
-        <v>361</v>
-      </c>
-      <c r="E38" s="148" t="s">
-        <v>372</v>
+      <c r="B38" s="147" t="s">
+        <v>340</v>
+      </c>
+      <c r="C38" s="147" t="s">
+        <v>349</v>
+      </c>
+      <c r="D38" s="147" t="s">
+        <v>359</v>
+      </c>
+      <c r="E38" s="147" t="s">
+        <v>370</v>
       </c>
       <c r="H38" s="102">
         <v>12</v>
@@ -20666,17 +20682,17 @@
       <c r="A39" s="102">
         <v>14</v>
       </c>
-      <c r="B39" s="148" t="s">
-        <v>343</v>
-      </c>
-      <c r="C39" s="148" t="s">
-        <v>352</v>
-      </c>
-      <c r="D39" s="148" t="s">
-        <v>362</v>
-      </c>
-      <c r="E39" s="148" t="s">
-        <v>373</v>
+      <c r="B39" s="147" t="s">
+        <v>341</v>
+      </c>
+      <c r="C39" s="147" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" s="147" t="s">
+        <v>360</v>
+      </c>
+      <c r="E39" s="147" t="s">
+        <v>371</v>
       </c>
       <c r="H39" s="102">
         <v>13</v>
@@ -20695,17 +20711,17 @@
       <c r="A40" s="102">
         <v>15</v>
       </c>
-      <c r="B40" s="148" t="s">
-        <v>344</v>
-      </c>
-      <c r="C40" s="148" t="s">
-        <v>353</v>
-      </c>
-      <c r="D40" s="148" t="s">
-        <v>363</v>
-      </c>
-      <c r="E40" s="148" t="s">
-        <v>374</v>
+      <c r="B40" s="147" t="s">
+        <v>342</v>
+      </c>
+      <c r="C40" s="147" t="s">
+        <v>351</v>
+      </c>
+      <c r="D40" s="147" t="s">
+        <v>361</v>
+      </c>
+      <c r="E40" s="147" t="s">
+        <v>372</v>
       </c>
       <c r="H40" s="102">
         <v>14</v>
@@ -20724,17 +20740,17 @@
       <c r="A41" s="102">
         <v>16</v>
       </c>
-      <c r="B41" s="148" t="s">
-        <v>345</v>
-      </c>
-      <c r="C41" s="148" t="s">
-        <v>354</v>
-      </c>
-      <c r="D41" s="148" t="s">
-        <v>364</v>
-      </c>
-      <c r="E41" s="148" t="s">
-        <v>375</v>
+      <c r="B41" s="147" t="s">
+        <v>343</v>
+      </c>
+      <c r="C41" s="147" t="s">
+        <v>352</v>
+      </c>
+      <c r="D41" s="147" t="s">
+        <v>362</v>
+      </c>
+      <c r="E41" s="147" t="s">
+        <v>373</v>
       </c>
       <c r="H41" s="102">
         <v>15</v>
@@ -20753,17 +20769,17 @@
       <c r="A42" s="102">
         <v>17</v>
       </c>
-      <c r="B42" s="148" t="s">
-        <v>346</v>
-      </c>
-      <c r="C42" s="148" t="s">
-        <v>355</v>
-      </c>
-      <c r="D42" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E42" s="148" t="s">
-        <v>376</v>
+      <c r="B42" s="147" t="s">
+        <v>344</v>
+      </c>
+      <c r="C42" s="147" t="s">
+        <v>353</v>
+      </c>
+      <c r="D42" s="147" t="s">
+        <v>363</v>
+      </c>
+      <c r="E42" s="147" t="s">
+        <v>374</v>
       </c>
       <c r="H42" s="102">
         <v>16</v>
@@ -20782,17 +20798,17 @@
       <c r="A43" s="102">
         <v>18</v>
       </c>
-      <c r="B43" s="147" t="s">
-        <v>385</v>
-      </c>
-      <c r="C43" s="148" t="s">
-        <v>356</v>
-      </c>
-      <c r="D43" s="148" t="s">
-        <v>366</v>
-      </c>
-      <c r="E43" s="148" t="s">
-        <v>377</v>
+      <c r="B43" s="146" t="s">
+        <v>383</v>
+      </c>
+      <c r="C43" s="147" t="s">
+        <v>354</v>
+      </c>
+      <c r="D43" s="147" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" s="147" t="s">
+        <v>375</v>
       </c>
       <c r="H43" s="102">
         <v>17</v>
@@ -20811,17 +20827,17 @@
       <c r="A44" s="102">
         <v>19</v>
       </c>
-      <c r="B44" s="150" t="s">
-        <v>386</v>
-      </c>
-      <c r="C44" s="147" t="s">
-        <v>387</v>
-      </c>
-      <c r="D44" s="148" t="s">
-        <v>367</v>
-      </c>
-      <c r="E44" s="148" t="s">
-        <v>378</v>
+      <c r="B44" s="149" t="s">
+        <v>384</v>
+      </c>
+      <c r="C44" s="146" t="s">
+        <v>385</v>
+      </c>
+      <c r="D44" s="147" t="s">
+        <v>365</v>
+      </c>
+      <c r="E44" s="147" t="s">
+        <v>376</v>
       </c>
       <c r="H44" s="102">
         <v>18</v>
@@ -20840,17 +20856,17 @@
       <c r="A45" s="102">
         <v>20</v>
       </c>
-      <c r="B45" s="150" t="s">
+      <c r="B45" s="149" t="s">
+        <v>386</v>
+      </c>
+      <c r="C45" s="149" t="s">
+        <v>387</v>
+      </c>
+      <c r="D45" s="146" t="s">
         <v>388</v>
       </c>
-      <c r="C45" s="150" t="s">
-        <v>389</v>
-      </c>
-      <c r="D45" s="147" t="s">
-        <v>390</v>
-      </c>
-      <c r="E45" s="148" t="s">
-        <v>379</v>
+      <c r="E45" s="147" t="s">
+        <v>377</v>
       </c>
       <c r="H45" s="102">
         <v>19</v>
@@ -20869,17 +20885,17 @@
       <c r="A46" s="102">
         <v>21</v>
       </c>
-      <c r="B46" s="150" t="s">
+      <c r="B46" s="149" t="s">
+        <v>389</v>
+      </c>
+      <c r="C46" s="149" t="s">
+        <v>390</v>
+      </c>
+      <c r="D46" s="149" t="s">
         <v>391</v>
       </c>
-      <c r="C46" s="150" t="s">
+      <c r="E46" s="146" t="s">
         <v>392</v>
-      </c>
-      <c r="D46" s="150" t="s">
-        <v>393</v>
-      </c>
-      <c r="E46" s="147" t="s">
-        <v>394</v>
       </c>
       <c r="H46" s="102">
         <v>20</v>
@@ -20898,17 +20914,17 @@
       <c r="A47" s="102">
         <v>22</v>
       </c>
-      <c r="B47" s="150" t="s">
+      <c r="B47" s="149" t="s">
+        <v>393</v>
+      </c>
+      <c r="C47" s="149" t="s">
+        <v>394</v>
+      </c>
+      <c r="D47" s="149" t="s">
         <v>395</v>
       </c>
-      <c r="C47" s="150" t="s">
+      <c r="E47" s="149" t="s">
         <v>396</v>
-      </c>
-      <c r="D47" s="150" t="s">
-        <v>397</v>
-      </c>
-      <c r="E47" s="150" t="s">
-        <v>398</v>
       </c>
       <c r="H47" s="102">
         <v>21</v>
@@ -20927,17 +20943,17 @@
       <c r="A48" s="102">
         <v>23</v>
       </c>
-      <c r="B48" s="150" t="s">
+      <c r="B48" s="149" t="s">
+        <v>397</v>
+      </c>
+      <c r="C48" s="149" t="s">
+        <v>398</v>
+      </c>
+      <c r="D48" s="149" t="s">
         <v>399</v>
       </c>
-      <c r="C48" s="150" t="s">
+      <c r="E48" s="149" t="s">
         <v>400</v>
-      </c>
-      <c r="D48" s="150" t="s">
-        <v>401</v>
-      </c>
-      <c r="E48" s="150" t="s">
-        <v>402</v>
       </c>
       <c r="H48" s="102">
         <v>22</v>
@@ -20956,17 +20972,17 @@
       <c r="A49" s="102">
         <v>24</v>
       </c>
-      <c r="B49" s="150" t="s">
+      <c r="B49" s="149" t="s">
+        <v>401</v>
+      </c>
+      <c r="C49" s="149" t="s">
+        <v>402</v>
+      </c>
+      <c r="D49" s="149" t="s">
         <v>403</v>
       </c>
-      <c r="C49" s="150" t="s">
+      <c r="E49" s="149" t="s">
         <v>404</v>
-      </c>
-      <c r="D49" s="150" t="s">
-        <v>405</v>
-      </c>
-      <c r="E49" s="150" t="s">
-        <v>406</v>
       </c>
       <c r="H49" s="102">
         <v>23</v>
@@ -20985,17 +21001,17 @@
       <c r="A50" s="102">
         <v>25</v>
       </c>
-      <c r="B50" s="150" t="s">
+      <c r="B50" s="149" t="s">
+        <v>405</v>
+      </c>
+      <c r="C50" s="149" t="s">
+        <v>406</v>
+      </c>
+      <c r="D50" s="149" t="s">
         <v>407</v>
       </c>
-      <c r="C50" s="150" t="s">
+      <c r="E50" s="149" t="s">
         <v>408</v>
-      </c>
-      <c r="D50" s="150" t="s">
-        <v>409</v>
-      </c>
-      <c r="E50" s="150" t="s">
-        <v>410</v>
       </c>
       <c r="H50" s="102">
         <v>24</v>
@@ -21014,17 +21030,17 @@
       <c r="A51" s="102">
         <v>26</v>
       </c>
-      <c r="B51" s="150" t="s">
+      <c r="B51" s="149" t="s">
+        <v>409</v>
+      </c>
+      <c r="C51" s="149" t="s">
+        <v>410</v>
+      </c>
+      <c r="D51" s="149" t="s">
         <v>411</v>
       </c>
-      <c r="C51" s="150" t="s">
+      <c r="E51" s="149" t="s">
         <v>412</v>
-      </c>
-      <c r="D51" s="150" t="s">
-        <v>413</v>
-      </c>
-      <c r="E51" s="150" t="s">
-        <v>414</v>
       </c>
       <c r="H51" s="102">
         <v>25</v>
@@ -21043,17 +21059,17 @@
       <c r="A52" s="102">
         <v>27</v>
       </c>
-      <c r="B52" s="150" t="s">
+      <c r="B52" s="149" t="s">
+        <v>413</v>
+      </c>
+      <c r="C52" s="149" t="s">
+        <v>414</v>
+      </c>
+      <c r="D52" s="149" t="s">
         <v>415</v>
       </c>
-      <c r="C52" s="150" t="s">
+      <c r="E52" s="149" t="s">
         <v>416</v>
-      </c>
-      <c r="D52" s="150" t="s">
-        <v>417</v>
-      </c>
-      <c r="E52" s="150" t="s">
-        <v>418</v>
       </c>
       <c r="H52" s="102">
         <v>26</v>
@@ -21072,17 +21088,17 @@
       <c r="A53" s="102">
         <v>28</v>
       </c>
-      <c r="B53" s="150" t="s">
+      <c r="B53" s="149" t="s">
+        <v>417</v>
+      </c>
+      <c r="C53" s="149" t="s">
+        <v>418</v>
+      </c>
+      <c r="D53" s="149" t="s">
         <v>419</v>
       </c>
-      <c r="C53" s="150" t="s">
+      <c r="E53" s="149" t="s">
         <v>420</v>
-      </c>
-      <c r="D53" s="150" t="s">
-        <v>421</v>
-      </c>
-      <c r="E53" s="150" t="s">
-        <v>422</v>
       </c>
       <c r="H53" s="102">
         <v>27</v>
@@ -21101,17 +21117,17 @@
       <c r="A54" s="102">
         <v>29</v>
       </c>
-      <c r="B54" s="150" t="s">
+      <c r="B54" s="149" t="s">
+        <v>421</v>
+      </c>
+      <c r="C54" s="149" t="s">
+        <v>422</v>
+      </c>
+      <c r="D54" s="149" t="s">
         <v>423</v>
       </c>
-      <c r="C54" s="150" t="s">
+      <c r="E54" s="149" t="s">
         <v>424</v>
-      </c>
-      <c r="D54" s="150" t="s">
-        <v>425</v>
-      </c>
-      <c r="E54" s="150" t="s">
-        <v>426</v>
       </c>
       <c r="H54" s="102">
         <v>28</v>
@@ -21130,17 +21146,17 @@
       <c r="A55" s="102">
         <v>30</v>
       </c>
-      <c r="B55" s="150" t="s">
+      <c r="B55" s="149" t="s">
+        <v>425</v>
+      </c>
+      <c r="C55" s="149" t="s">
+        <v>426</v>
+      </c>
+      <c r="D55" s="149" t="s">
         <v>427</v>
       </c>
-      <c r="C55" s="150" t="s">
+      <c r="E55" s="149" t="s">
         <v>428</v>
-      </c>
-      <c r="D55" s="150" t="s">
-        <v>429</v>
-      </c>
-      <c r="E55" s="150" t="s">
-        <v>430</v>
       </c>
       <c r="H55" s="102">
         <v>29</v>
@@ -21159,17 +21175,17 @@
       <c r="A56" s="102">
         <v>31</v>
       </c>
-      <c r="B56" s="150" t="s">
+      <c r="B56" s="149" t="s">
+        <v>429</v>
+      </c>
+      <c r="C56" s="149" t="s">
+        <v>430</v>
+      </c>
+      <c r="D56" s="149" t="s">
         <v>431</v>
       </c>
-      <c r="C56" s="150" t="s">
+      <c r="E56" s="149" t="s">
         <v>432</v>
-      </c>
-      <c r="D56" s="150" t="s">
-        <v>433</v>
-      </c>
-      <c r="E56" s="150" t="s">
-        <v>434</v>
       </c>
       <c r="H56" s="102">
         <v>30</v>
@@ -21188,17 +21204,17 @@
       <c r="A57" s="102">
         <v>32</v>
       </c>
-      <c r="B57" s="150" t="s">
+      <c r="B57" s="149" t="s">
+        <v>433</v>
+      </c>
+      <c r="C57" s="149" t="s">
+        <v>434</v>
+      </c>
+      <c r="D57" s="149" t="s">
         <v>435</v>
       </c>
-      <c r="C57" s="150" t="s">
+      <c r="E57" s="149" t="s">
         <v>436</v>
-      </c>
-      <c r="D57" s="150" t="s">
-        <v>437</v>
-      </c>
-      <c r="E57" s="150" t="s">
-        <v>438</v>
       </c>
       <c r="H57" s="102">
         <v>31</v>
@@ -21217,17 +21233,17 @@
       <c r="A58" s="102">
         <v>33</v>
       </c>
-      <c r="B58" s="150" t="s">
+      <c r="B58" s="149" t="s">
+        <v>437</v>
+      </c>
+      <c r="C58" s="149" t="s">
+        <v>438</v>
+      </c>
+      <c r="D58" s="149" t="s">
         <v>439</v>
       </c>
-      <c r="C58" s="150" t="s">
+      <c r="E58" s="149" t="s">
         <v>440</v>
-      </c>
-      <c r="D58" s="150" t="s">
-        <v>441</v>
-      </c>
-      <c r="E58" s="150" t="s">
-        <v>442</v>
       </c>
       <c r="H58" s="102">
         <v>32</v>
@@ -21253,638 +21269,630 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="16384" width="9.06640625" style="151"/>
+    <col min="1" max="16384" width="9.06640625" style="150"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="150" t="s">
+        <v>441</v>
+      </c>
+      <c r="B1" s="150" t="s">
+        <v>442</v>
+      </c>
+      <c r="C1" s="150" t="s">
         <v>443</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="D1" s="150" t="s">
         <v>444</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="E1" s="150" t="s">
         <v>445</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="G1" s="150" t="s">
+        <v>442</v>
+      </c>
+      <c r="H1" s="150" t="s">
+        <v>443</v>
+      </c>
+      <c r="I1" s="150" t="s">
+        <v>444</v>
+      </c>
+      <c r="J1" s="150" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="150">
+        <v>0</v>
+      </c>
+      <c r="B2" s="151" t="s">
+        <v>488</v>
+      </c>
+      <c r="C2" s="152" t="s">
+        <v>489</v>
+      </c>
+      <c r="D2" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="E2" s="153"/>
+      <c r="G2" s="151">
+        <v>1</v>
+      </c>
+      <c r="H2" s="152">
+        <v>0</v>
+      </c>
+      <c r="I2" s="152">
+        <v>0</v>
+      </c>
+      <c r="J2" s="153"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="150">
+        <v>1</v>
+      </c>
+      <c r="B3" s="154" t="s">
+        <v>491</v>
+      </c>
+      <c r="C3" s="155" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="155" t="s">
+        <v>381</v>
+      </c>
+      <c r="E3" s="156"/>
+      <c r="G3" s="154">
+        <v>0</v>
+      </c>
+      <c r="H3" s="155">
+        <v>1</v>
+      </c>
+      <c r="I3" s="155">
+        <v>0</v>
+      </c>
+      <c r="J3" s="156"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="150">
+        <v>2</v>
+      </c>
+      <c r="B4" s="157" t="s">
         <v>446</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="C4" s="155" t="s">
         <v>447</v>
       </c>
-      <c r="G1" s="151" t="s">
-        <v>444</v>
-      </c>
-      <c r="H1" s="151" t="s">
-        <v>445</v>
-      </c>
-      <c r="I1" s="151" t="s">
-        <v>446</v>
-      </c>
-      <c r="J1" s="151" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="151">
+      <c r="D4" s="155" t="s">
+        <v>382</v>
+      </c>
+      <c r="E4" s="158"/>
+      <c r="G4" s="157">
         <v>0</v>
       </c>
-      <c r="B2" s="152" t="s">
-        <v>490</v>
-      </c>
-      <c r="C2" s="153" t="s">
-        <v>491</v>
-      </c>
-      <c r="D2" s="153" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2" s="154"/>
-      <c r="G2" s="152">
+      <c r="H4" s="155">
         <v>0</v>
       </c>
-      <c r="H2" s="153">
+      <c r="I4" s="155">
+        <v>1</v>
+      </c>
+      <c r="J4" s="158"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A5" s="150">
+        <v>3</v>
+      </c>
+      <c r="B5" s="178" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" s="179" t="s">
+        <v>486</v>
+      </c>
+      <c r="D5" s="179" t="s">
+        <v>487</v>
+      </c>
+      <c r="E5" s="161"/>
+      <c r="G5" s="159">
         <v>0</v>
       </c>
-      <c r="I2" s="153">
+      <c r="H5" s="160">
         <v>0</v>
       </c>
-      <c r="J2" s="154"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="151">
+      <c r="I5" s="160">
+        <v>0</v>
+      </c>
+      <c r="J5" s="161"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="150">
+        <v>4</v>
+      </c>
+      <c r="B6" s="180" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="181" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="181" t="s">
+        <v>322</v>
+      </c>
+      <c r="E6" s="182" t="s">
+        <v>457</v>
+      </c>
+      <c r="G6" s="151">
+        <v>0</v>
+      </c>
+      <c r="H6" s="151">
+        <v>0</v>
+      </c>
+      <c r="I6" s="151">
+        <v>0</v>
+      </c>
+      <c r="J6" s="151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="150">
+        <v>5</v>
+      </c>
+      <c r="B7" s="157" t="s">
+        <v>449</v>
+      </c>
+      <c r="C7" s="155" t="s">
+        <v>451</v>
+      </c>
+      <c r="D7" s="155" t="s">
+        <v>453</v>
+      </c>
+      <c r="E7" s="163" t="s">
+        <v>330</v>
+      </c>
+      <c r="G7" s="154">
         <v>1</v>
       </c>
-      <c r="B3" s="155" t="s">
-        <v>493</v>
-      </c>
-      <c r="C3" s="156" t="s">
-        <v>382</v>
-      </c>
-      <c r="D3" s="156" t="s">
-        <v>383</v>
-      </c>
-      <c r="E3" s="157"/>
-      <c r="G3" s="155">
+      <c r="H7" s="154">
         <v>1</v>
       </c>
-      <c r="H3" s="156">
-        <v>0</v>
-      </c>
-      <c r="I3" s="156">
-        <v>0</v>
-      </c>
-      <c r="J3" s="157"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="151">
+      <c r="I7" s="154">
+        <v>1</v>
+      </c>
+      <c r="J7" s="154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="150">
+        <v>6</v>
+      </c>
+      <c r="B8" s="154" t="s">
+        <v>450</v>
+      </c>
+      <c r="C8" s="155" t="s">
+        <v>452</v>
+      </c>
+      <c r="D8" s="155" t="s">
+        <v>454</v>
+      </c>
+      <c r="E8" s="163" t="s">
+        <v>331</v>
+      </c>
+      <c r="G8" s="157">
         <v>2</v>
       </c>
-      <c r="B4" s="158" t="s">
+      <c r="H8" s="157">
+        <v>2</v>
+      </c>
+      <c r="I8" s="157">
+        <v>2</v>
+      </c>
+      <c r="J8" s="157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A9" s="150">
+        <v>7</v>
+      </c>
+      <c r="B9" s="183" t="s">
         <v>448</v>
       </c>
-      <c r="C4" s="156" t="s">
-        <v>449</v>
-      </c>
-      <c r="D4" s="156" t="s">
-        <v>384</v>
-      </c>
-      <c r="E4" s="159"/>
-      <c r="G4" s="158">
-        <v>0</v>
-      </c>
-      <c r="H4" s="156">
-        <v>1</v>
-      </c>
-      <c r="I4" s="156">
-        <v>0</v>
-      </c>
-      <c r="J4" s="159"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A5" s="151">
+      <c r="C9" s="184" t="s">
+        <v>455</v>
+      </c>
+      <c r="D9" s="184" t="s">
+        <v>456</v>
+      </c>
+      <c r="E9" s="185" t="s">
+        <v>328</v>
+      </c>
+      <c r="G9" s="165">
         <v>3</v>
       </c>
-      <c r="B5" s="187" t="s">
-        <v>487</v>
-      </c>
-      <c r="C5" s="188" t="s">
-        <v>488</v>
-      </c>
-      <c r="D5" s="188" t="s">
-        <v>489</v>
-      </c>
-      <c r="E5" s="162"/>
-      <c r="G5" s="160">
-        <v>0</v>
-      </c>
-      <c r="H5" s="161">
-        <v>0</v>
-      </c>
-      <c r="I5" s="161">
-        <v>1</v>
-      </c>
-      <c r="J5" s="162"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="151">
+      <c r="H9" s="165">
+        <v>3</v>
+      </c>
+      <c r="I9" s="165">
+        <v>3</v>
+      </c>
+      <c r="J9" s="165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="150">
+        <v>8</v>
+      </c>
+      <c r="B10" s="154" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="155" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" s="155" t="s">
+        <v>325</v>
+      </c>
+      <c r="E10" s="163" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" s="151">
         <v>4</v>
       </c>
-      <c r="B6" s="189" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6" s="190" t="s">
-        <v>318</v>
-      </c>
-      <c r="D6" s="190" t="s">
-        <v>324</v>
-      </c>
-      <c r="E6" s="191" t="s">
+      <c r="H10" s="151">
+        <v>4</v>
+      </c>
+      <c r="I10" s="151">
+        <v>4</v>
+      </c>
+      <c r="J10" s="151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="150">
+        <v>9</v>
+      </c>
+      <c r="B11" s="157" t="s">
+        <v>458</v>
+      </c>
+      <c r="C11" s="155" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="155" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="163" t="s">
+        <v>333</v>
+      </c>
+      <c r="G11" s="154">
+        <v>5</v>
+      </c>
+      <c r="H11" s="154">
+        <v>5</v>
+      </c>
+      <c r="I11" s="154">
+        <v>5</v>
+      </c>
+      <c r="J11" s="154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="150">
+        <v>10</v>
+      </c>
+      <c r="B12" s="154" t="s">
         <v>459</v>
       </c>
-      <c r="G6" s="152">
-        <v>0</v>
-      </c>
-      <c r="H6" s="152">
-        <v>0</v>
-      </c>
-      <c r="I6" s="152">
-        <v>0</v>
-      </c>
-      <c r="J6" s="152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="151">
-        <v>5</v>
-      </c>
-      <c r="B7" s="158" t="s">
-        <v>451</v>
-      </c>
-      <c r="C7" s="156" t="s">
-        <v>453</v>
-      </c>
-      <c r="D7" s="156" t="s">
-        <v>455</v>
-      </c>
-      <c r="E7" s="164" t="s">
-        <v>332</v>
-      </c>
-      <c r="G7" s="155">
-        <v>1</v>
-      </c>
-      <c r="H7" s="155">
-        <v>1</v>
-      </c>
-      <c r="I7" s="155">
-        <v>1</v>
-      </c>
-      <c r="J7" s="155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="151">
+      <c r="C12" s="155" t="s">
+        <v>460</v>
+      </c>
+      <c r="D12" s="155" t="s">
+        <v>327</v>
+      </c>
+      <c r="E12" s="163" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" s="157">
         <v>6</v>
       </c>
-      <c r="B8" s="155" t="s">
-        <v>452</v>
-      </c>
-      <c r="C8" s="156" t="s">
-        <v>454</v>
-      </c>
-      <c r="D8" s="156" t="s">
-        <v>456</v>
-      </c>
-      <c r="E8" s="164" t="s">
-        <v>333</v>
-      </c>
-      <c r="G8" s="158">
-        <v>2</v>
-      </c>
-      <c r="H8" s="158">
-        <v>2</v>
-      </c>
-      <c r="I8" s="158">
-        <v>2</v>
-      </c>
-      <c r="J8" s="158">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A9" s="151">
+      <c r="H12" s="157">
+        <v>6</v>
+      </c>
+      <c r="I12" s="157">
+        <v>6</v>
+      </c>
+      <c r="J12" s="157">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A13" s="150">
+        <v>11</v>
+      </c>
+      <c r="B13" s="159" t="s">
+        <v>461</v>
+      </c>
+      <c r="C13" s="160" t="s">
+        <v>462</v>
+      </c>
+      <c r="D13" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="E13" s="164" t="s">
+        <v>335</v>
+      </c>
+      <c r="G13" s="165">
         <v>7</v>
       </c>
-      <c r="B9" s="192" t="s">
-        <v>450</v>
-      </c>
-      <c r="C9" s="193" t="s">
-        <v>457</v>
-      </c>
-      <c r="D9" s="193" t="s">
-        <v>458</v>
-      </c>
-      <c r="E9" s="194" t="s">
-        <v>330</v>
-      </c>
-      <c r="G9" s="166">
-        <v>3</v>
-      </c>
-      <c r="H9" s="166">
-        <v>3</v>
-      </c>
-      <c r="I9" s="166">
-        <v>3</v>
-      </c>
-      <c r="J9" s="166">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="151">
+      <c r="H13" s="165">
+        <v>7</v>
+      </c>
+      <c r="I13" s="165">
+        <v>7</v>
+      </c>
+      <c r="J13" s="165">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="150">
+        <v>12</v>
+      </c>
+      <c r="G14" s="151">
         <v>8</v>
       </c>
-      <c r="B10" s="155" t="s">
-        <v>316</v>
-      </c>
-      <c r="C10" s="156" t="s">
-        <v>321</v>
-      </c>
-      <c r="D10" s="156" t="s">
-        <v>327</v>
-      </c>
-      <c r="E10" s="164" t="s">
-        <v>334</v>
-      </c>
-      <c r="G10" s="152">
-        <v>4</v>
-      </c>
-      <c r="H10" s="152">
-        <v>4</v>
-      </c>
-      <c r="I10" s="152">
-        <v>4</v>
-      </c>
-      <c r="J10" s="152">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="151">
+      <c r="H14" s="151">
+        <v>8</v>
+      </c>
+      <c r="I14" s="151">
+        <v>8</v>
+      </c>
+      <c r="J14" s="151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A15" s="150">
+        <v>13</v>
+      </c>
+      <c r="G15" s="154">
         <v>9</v>
       </c>
-      <c r="B11" s="158" t="s">
-        <v>460</v>
-      </c>
-      <c r="C11" s="156" t="s">
-        <v>322</v>
-      </c>
-      <c r="D11" s="156" t="s">
-        <v>328</v>
-      </c>
-      <c r="E11" s="164" t="s">
-        <v>335</v>
-      </c>
-      <c r="G11" s="155">
-        <v>5</v>
-      </c>
-      <c r="H11" s="155">
-        <v>5</v>
-      </c>
-      <c r="I11" s="155">
-        <v>5</v>
-      </c>
-      <c r="J11" s="155">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="151">
+      <c r="H15" s="154">
+        <v>9</v>
+      </c>
+      <c r="I15" s="154">
+        <v>9</v>
+      </c>
+      <c r="J15" s="154">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="150">
+        <v>14</v>
+      </c>
+      <c r="B16" s="151"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="162"/>
+      <c r="G16" s="157">
         <v>10</v>
       </c>
-      <c r="B12" s="155" t="s">
-        <v>461</v>
-      </c>
-      <c r="C12" s="156" t="s">
-        <v>462</v>
-      </c>
-      <c r="D12" s="156" t="s">
-        <v>329</v>
-      </c>
-      <c r="E12" s="164" t="s">
-        <v>336</v>
-      </c>
-      <c r="G12" s="158">
-        <v>6</v>
-      </c>
-      <c r="H12" s="158">
-        <v>6</v>
-      </c>
-      <c r="I12" s="158">
-        <v>6</v>
-      </c>
-      <c r="J12" s="158">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A13" s="151">
+      <c r="H16" s="157">
+        <v>10</v>
+      </c>
+      <c r="I16" s="157">
+        <v>10</v>
+      </c>
+      <c r="J16" s="157">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A17" s="150">
+        <v>15</v>
+      </c>
+      <c r="G17" s="165">
         <v>11</v>
       </c>
-      <c r="B13" s="160" t="s">
-        <v>463</v>
-      </c>
-      <c r="C13" s="161" t="s">
-        <v>464</v>
-      </c>
-      <c r="D13" s="161" t="s">
-        <v>465</v>
-      </c>
-      <c r="E13" s="165" t="s">
-        <v>337</v>
-      </c>
-      <c r="G13" s="166">
-        <v>7</v>
-      </c>
-      <c r="H13" s="166">
-        <v>7</v>
-      </c>
-      <c r="I13" s="166">
-        <v>7</v>
-      </c>
-      <c r="J13" s="166">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="151">
+      <c r="H17" s="165">
+        <v>11</v>
+      </c>
+      <c r="I17" s="165">
+        <v>11</v>
+      </c>
+      <c r="J17" s="165">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="150">
+        <v>16</v>
+      </c>
+      <c r="G18" s="151">
         <v>12</v>
       </c>
-      <c r="G14" s="152">
-        <v>8</v>
-      </c>
-      <c r="H14" s="152">
-        <v>8</v>
-      </c>
-      <c r="I14" s="152">
-        <v>8</v>
-      </c>
-      <c r="J14" s="152">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A15" s="151">
+      <c r="H18" s="151">
+        <v>12</v>
+      </c>
+      <c r="I18" s="151">
+        <v>12</v>
+      </c>
+      <c r="J18" s="151">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="150">
+        <v>17</v>
+      </c>
+      <c r="G19" s="154">
         <v>13</v>
       </c>
-      <c r="G15" s="155">
-        <v>9</v>
-      </c>
-      <c r="H15" s="155">
-        <v>9</v>
-      </c>
-      <c r="I15" s="155">
-        <v>9</v>
-      </c>
-      <c r="J15" s="155">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="151">
+      <c r="H19" s="154">
+        <v>13</v>
+      </c>
+      <c r="I19" s="154">
+        <v>13</v>
+      </c>
+      <c r="J19" s="154">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="150">
+        <v>18</v>
+      </c>
+      <c r="G20" s="157">
         <v>14</v>
       </c>
-      <c r="B16" s="152" t="s">
-        <v>450</v>
-      </c>
-      <c r="C16" s="153" t="s">
-        <v>457</v>
-      </c>
-      <c r="D16" s="153" t="s">
-        <v>458</v>
-      </c>
-      <c r="E16" s="163" t="s">
-        <v>330</v>
-      </c>
-      <c r="G16" s="158">
-        <v>10</v>
-      </c>
-      <c r="H16" s="158">
-        <v>10</v>
-      </c>
-      <c r="I16" s="158">
-        <v>10</v>
-      </c>
-      <c r="J16" s="158">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A17" s="151">
+      <c r="H20" s="157">
+        <v>14</v>
+      </c>
+      <c r="I20" s="157">
+        <v>14</v>
+      </c>
+      <c r="J20" s="157">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A21" s="150">
+        <v>19</v>
+      </c>
+      <c r="G21" s="165">
         <v>15</v>
       </c>
-      <c r="G17" s="166">
-        <v>11</v>
-      </c>
-      <c r="H17" s="166">
-        <v>11</v>
-      </c>
-      <c r="I17" s="166">
-        <v>11</v>
-      </c>
-      <c r="J17" s="166">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="151">
+      <c r="H21" s="165">
+        <v>15</v>
+      </c>
+      <c r="I21" s="165">
+        <v>15</v>
+      </c>
+      <c r="J21" s="165">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="150">
+        <v>20</v>
+      </c>
+      <c r="G22" s="151">
         <v>16</v>
       </c>
-      <c r="G18" s="152">
-        <v>12</v>
-      </c>
-      <c r="H18" s="152">
-        <v>12</v>
-      </c>
-      <c r="I18" s="152">
-        <v>12</v>
-      </c>
-      <c r="J18" s="152">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="151">
+      <c r="H22" s="151">
+        <v>16</v>
+      </c>
+      <c r="I22" s="151">
+        <v>16</v>
+      </c>
+      <c r="J22" s="151">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="150">
+        <v>21</v>
+      </c>
+      <c r="G23" s="154">
         <v>17</v>
       </c>
-      <c r="G19" s="155">
-        <v>13</v>
-      </c>
-      <c r="H19" s="155">
-        <v>13</v>
-      </c>
-      <c r="I19" s="155">
-        <v>13</v>
-      </c>
-      <c r="J19" s="155">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="151">
+      <c r="H23" s="154">
+        <v>17</v>
+      </c>
+      <c r="I23" s="154">
+        <v>17</v>
+      </c>
+      <c r="J23" s="154">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="150">
+        <v>22</v>
+      </c>
+      <c r="G24" s="157">
         <v>18</v>
       </c>
-      <c r="G20" s="158">
-        <v>14</v>
-      </c>
-      <c r="H20" s="158">
-        <v>14</v>
-      </c>
-      <c r="I20" s="158">
-        <v>14</v>
-      </c>
-      <c r="J20" s="158">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="14.25" thickBot="1">
-      <c r="A21" s="151">
+      <c r="H24" s="157">
+        <v>18</v>
+      </c>
+      <c r="I24" s="157">
+        <v>18</v>
+      </c>
+      <c r="J24" s="157">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="150">
+        <v>23</v>
+      </c>
+      <c r="G25" s="165">
         <v>19</v>
       </c>
-      <c r="G21" s="166">
-        <v>15</v>
-      </c>
-      <c r="H21" s="166">
-        <v>15</v>
-      </c>
-      <c r="I21" s="166">
-        <v>15</v>
-      </c>
-      <c r="J21" s="166">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="151">
-        <v>20</v>
-      </c>
-      <c r="G22" s="152">
-        <v>16</v>
-      </c>
-      <c r="H22" s="152">
-        <v>16</v>
-      </c>
-      <c r="I22" s="152">
-        <v>16</v>
-      </c>
-      <c r="J22" s="152">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="151">
-        <v>21</v>
-      </c>
-      <c r="G23" s="155">
-        <v>17</v>
-      </c>
-      <c r="H23" s="155">
-        <v>17</v>
-      </c>
-      <c r="I23" s="155">
-        <v>17</v>
-      </c>
-      <c r="J23" s="155">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="151">
-        <v>22</v>
-      </c>
-      <c r="G24" s="158">
-        <v>18</v>
-      </c>
-      <c r="H24" s="158">
-        <v>18</v>
-      </c>
-      <c r="I24" s="158">
-        <v>18</v>
-      </c>
-      <c r="J24" s="158">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="151">
-        <v>23</v>
-      </c>
-      <c r="G25" s="166">
+      <c r="H25" s="165">
         <v>19</v>
       </c>
-      <c r="H25" s="166">
+      <c r="I25" s="165">
         <v>19</v>
       </c>
-      <c r="I25" s="166">
+      <c r="J25" s="165">
         <v>19</v>
       </c>
-      <c r="J25" s="166">
-        <v>19</v>
-      </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="151">
+      <c r="A26" s="150">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="151">
+      <c r="A27" s="150">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="151">
+      <c r="A28" s="150">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="151">
+      <c r="A29" s="150">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="151">
+      <c r="A30" s="150">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="151">
+      <c r="A31" s="150">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="151">
+      <c r="A32" s="150">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="151">
+      <c r="A33" s="150">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="151">
+      <c r="A34" s="150">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="151">
+      <c r="A35" s="150">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
220507-v4 OK to sim with some bugs, revise TB_base_addr
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54029D-2C91-420C-82E7-B38184FFD5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06395DC-59B7-43A9-A531-7BAF3A087E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3585" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3585" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="513">
   <si>
     <t>步骤</t>
   </si>
@@ -1716,6 +1716,63 @@
   <si>
     <t>vt(0,2)</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>cov(8,1)</t>
+  </si>
+  <si>
+    <t>cov(9,1)</t>
+  </si>
+  <si>
+    <t>cov(10,1)</t>
+  </si>
+  <si>
+    <t>cov(11,1)</t>
+  </si>
+  <si>
+    <t>cov(8,9)</t>
+  </si>
+  <si>
+    <t>cov(8,10)</t>
+  </si>
+  <si>
+    <t>cov(9,10)</t>
+  </si>
+  <si>
+    <t>cov(8,11)</t>
+  </si>
+  <si>
+    <t>cov(9,11)</t>
+  </si>
+  <si>
+    <t>cov(10,11)</t>
+  </si>
+  <si>
+    <t>cov(12,1)</t>
+  </si>
+  <si>
+    <t>cov(12,2)</t>
+  </si>
+  <si>
+    <t>state(12,1)</t>
+  </si>
+  <si>
+    <t>cov(12,13)</t>
+  </si>
+  <si>
+    <t>cov(12,14)</t>
+  </si>
+  <si>
+    <t>cov(13,14)</t>
+  </si>
+  <si>
+    <t>cov(12,15)</t>
+  </si>
+  <si>
+    <t>cov(13,15)</t>
+  </si>
+  <si>
+    <t>cov(14,15)</t>
   </si>
 </sst>
 </file>
@@ -2391,7 +2448,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2874,9 +2931,6 @@
     <xf numFmtId="0" fontId="13" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2946,6 +3000,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="31" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="41" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2969,18 +3035,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="31" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="41" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3929,10 +3983,10 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A5" s="186" t="s">
+      <c r="A5" s="189" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="187"/>
+      <c r="B5" s="190"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4712,12 +4766,12 @@
       <c r="AE21" s="4"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="188" t="s">
+      <c r="A22" s="191" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="187"/>
-      <c r="C22" s="187"/>
-      <c r="D22" s="187"/>
+      <c r="B22" s="190"/>
+      <c r="C22" s="190"/>
+      <c r="D22" s="190"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
@@ -12308,7 +12362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S274"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
@@ -12684,7 +12738,7 @@
       <c r="B16" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="168" t="s">
+      <c r="C16" s="167" t="s">
         <v>467</v>
       </c>
       <c r="D16" s="19"/>
@@ -12798,7 +12852,7 @@
       <c r="D20" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="168" t="s">
+      <c r="E20" s="167" t="s">
         <v>467</v>
       </c>
       <c r="F20" s="3"/>
@@ -13158,7 +13212,7 @@
       <c r="B34" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="168" t="s">
+      <c r="C34" s="167" t="s">
         <v>467</v>
       </c>
       <c r="D34" s="25"/>
@@ -13999,14 +14053,14 @@
       <c r="A66" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B66" s="169" t="s">
+      <c r="B66" s="168" t="s">
         <v>481</v>
       </c>
       <c r="C66" s="74" t="s">
         <v>175</v>
       </c>
       <c r="D66" s="41"/>
-      <c r="E66" s="174"/>
+      <c r="E66" s="173"/>
       <c r="F66" s="38"/>
       <c r="G66" s="40"/>
       <c r="H66" s="40"/>
@@ -14031,7 +14085,7 @@
         <v>174</v>
       </c>
       <c r="D67" s="24"/>
-      <c r="E67" s="175"/>
+      <c r="E67" s="174"/>
       <c r="F67" s="38"/>
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
@@ -14056,7 +14110,7 @@
         <v>191</v>
       </c>
       <c r="D68" s="42"/>
-      <c r="E68" s="176"/>
+      <c r="E68" s="175"/>
       <c r="F68" s="38"/>
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
@@ -14083,7 +14137,7 @@
         <v>176</v>
       </c>
       <c r="D69" s="24"/>
-      <c r="E69" s="172"/>
+      <c r="E69" s="171"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -14108,7 +14162,7 @@
         <v>177</v>
       </c>
       <c r="D70" s="17"/>
-      <c r="E70" s="172"/>
+      <c r="E70" s="171"/>
       <c r="F70" s="7"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -14133,7 +14187,7 @@
         <v>191</v>
       </c>
       <c r="D71" s="17"/>
-      <c r="E71" s="172"/>
+      <c r="E71" s="171"/>
       <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -14153,7 +14207,7 @@
       <c r="A72" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B72" s="177" t="s">
+      <c r="B72" s="176" t="s">
         <v>178</v>
       </c>
       <c r="C72" s="74" t="s">
@@ -14280,10 +14334,10 @@
       <c r="F76" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="G76" s="170"/>
-      <c r="H76" s="171"/>
-      <c r="I76" s="170"/>
-      <c r="J76" s="172"/>
+      <c r="G76" s="169"/>
+      <c r="H76" s="170"/>
+      <c r="I76" s="169"/>
+      <c r="J76" s="171"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -14309,10 +14363,10 @@
         <v>45</v>
       </c>
       <c r="F77" s="92"/>
-      <c r="G77" s="173"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="173"/>
-      <c r="J77" s="172"/>
+      <c r="G77" s="172"/>
+      <c r="H77" s="170"/>
+      <c r="I77" s="172"/>
+      <c r="J77" s="171"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
@@ -14337,10 +14391,10 @@
       <c r="E78" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="G78" s="173"/>
-      <c r="H78" s="171"/>
-      <c r="I78" s="173"/>
-      <c r="J78" s="172"/>
+      <c r="G78" s="172"/>
+      <c r="H78" s="170"/>
+      <c r="I78" s="172"/>
+      <c r="J78" s="171"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
@@ -14365,10 +14419,10 @@
       <c r="E79" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="G79" s="173"/>
-      <c r="H79" s="171"/>
-      <c r="I79" s="173"/>
-      <c r="J79" s="172"/>
+      <c r="G79" s="172"/>
+      <c r="H79" s="170"/>
+      <c r="I79" s="172"/>
+      <c r="J79" s="171"/>
       <c r="K79" s="40"/>
       <c r="L79" s="40"/>
       <c r="M79" s="40"/>
@@ -14885,11 +14939,11 @@
     </row>
     <row r="98" spans="1:19" ht="14.25" thickBot="1">
       <c r="A98" s="7"/>
-      <c r="B98" s="189" t="s">
+      <c r="B98" s="192" t="s">
         <v>201</v>
       </c>
-      <c r="C98" s="190"/>
-      <c r="D98" s="190"/>
+      <c r="C98" s="193"/>
+      <c r="D98" s="193"/>
       <c r="E98" s="80" t="s">
         <v>202</v>
       </c>
@@ -18604,11 +18658,11 @@
       <c r="B4" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="166" t="s">
+      <c r="C4" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="166"/>
-      <c r="E4" s="167" t="s">
+      <c r="D4" s="165"/>
+      <c r="E4" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18640,11 +18694,11 @@
       <c r="B7" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="166" t="s">
+      <c r="C7" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="166"/>
-      <c r="E7" s="167" t="s">
+      <c r="D7" s="165"/>
+      <c r="E7" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18676,11 +18730,11 @@
       <c r="B10" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="166" t="s">
+      <c r="C10" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="166"/>
-      <c r="E10" s="167" t="s">
+      <c r="D10" s="165"/>
+      <c r="E10" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18712,11 +18766,11 @@
       <c r="B13" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="166" t="s">
+      <c r="C13" s="165" t="s">
         <v>186</v>
       </c>
       <c r="D13" s="122"/>
-      <c r="E13" s="167" t="s">
+      <c r="E13" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18752,13 +18806,13 @@
       <c r="B16" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="166" t="s">
+      <c r="C16" s="165" t="s">
         <v>186</v>
       </c>
       <c r="D16" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="167" t="s">
+      <c r="E16" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18794,13 +18848,13 @@
       <c r="B19" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="166" t="s">
+      <c r="C19" s="165" t="s">
         <v>186</v>
       </c>
       <c r="D19" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="167" t="s">
+      <c r="E19" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -18843,13 +18897,13 @@
       <c r="B22" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="166" t="s">
+      <c r="C22" s="165" t="s">
         <v>186</v>
       </c>
       <c r="D22" s="140" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="167" t="s">
+      <c r="E22" s="166" t="s">
         <v>186</v>
       </c>
     </row>
@@ -19092,10 +19146,10 @@
       <c r="AK2" s="108"/>
       <c r="AL2" s="108"/>
       <c r="AM2" s="108"/>
-      <c r="AN2" s="194" t="s">
+      <c r="AN2" s="185" t="s">
         <v>258</v>
       </c>
-      <c r="AO2" s="195" t="s">
+      <c r="AO2" s="186" t="s">
         <v>259</v>
       </c>
       <c r="AP2" s="107" t="s">
@@ -19316,10 +19370,10 @@
       <c r="AF5" s="130"/>
       <c r="AG5" s="130"/>
       <c r="AH5" s="130"/>
-      <c r="AN5" s="196" t="s">
+      <c r="AN5" s="187" t="s">
         <v>492</v>
       </c>
-      <c r="AO5" s="197" t="s">
+      <c r="AO5" s="188" t="s">
         <v>493</v>
       </c>
       <c r="AP5" s="121" t="s">
@@ -19342,67 +19396,67 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="191" t="s">
+      <c r="B6" s="194" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="192"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="191" t="s">
+      <c r="C6" s="195"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="194" t="s">
         <v>293</v>
       </c>
-      <c r="F6" s="192"/>
-      <c r="G6" s="193"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="196"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="191" t="s">
+      <c r="B7" s="194" t="s">
         <v>294</v>
       </c>
-      <c r="C7" s="192"/>
-      <c r="D7" s="192"/>
-      <c r="E7" s="192"/>
-      <c r="F7" s="192"/>
-      <c r="G7" s="192"/>
-      <c r="H7" s="192"/>
-      <c r="I7" s="192"/>
-      <c r="J7" s="192"/>
-      <c r="K7" s="192"/>
-      <c r="L7" s="192"/>
-      <c r="M7" s="192"/>
-      <c r="N7" s="192"/>
-      <c r="O7" s="192"/>
-      <c r="P7" s="193"/>
-      <c r="Q7" s="191" t="s">
+      <c r="C7" s="195"/>
+      <c r="D7" s="195"/>
+      <c r="E7" s="195"/>
+      <c r="F7" s="195"/>
+      <c r="G7" s="195"/>
+      <c r="H7" s="195"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="195"/>
+      <c r="K7" s="195"/>
+      <c r="L7" s="195"/>
+      <c r="M7" s="195"/>
+      <c r="N7" s="195"/>
+      <c r="O7" s="195"/>
+      <c r="P7" s="196"/>
+      <c r="Q7" s="194" t="s">
         <v>295</v>
       </c>
-      <c r="R7" s="192"/>
-      <c r="S7" s="192"/>
-      <c r="T7" s="192"/>
-      <c r="U7" s="192"/>
-      <c r="V7" s="192"/>
-      <c r="W7" s="192"/>
-      <c r="X7" s="192"/>
-      <c r="Y7" s="192"/>
-      <c r="Z7" s="192"/>
-      <c r="AA7" s="193"/>
-      <c r="AB7" s="191" t="s">
+      <c r="R7" s="195"/>
+      <c r="S7" s="195"/>
+      <c r="T7" s="195"/>
+      <c r="U7" s="195"/>
+      <c r="V7" s="195"/>
+      <c r="W7" s="195"/>
+      <c r="X7" s="195"/>
+      <c r="Y7" s="195"/>
+      <c r="Z7" s="195"/>
+      <c r="AA7" s="196"/>
+      <c r="AB7" s="194" t="s">
         <v>296</v>
       </c>
-      <c r="AC7" s="192"/>
-      <c r="AD7" s="192"/>
-      <c r="AE7" s="192"/>
-      <c r="AF7" s="192"/>
-      <c r="AG7" s="192"/>
-      <c r="AH7" s="192"/>
-      <c r="AI7" s="192"/>
-      <c r="AJ7" s="192"/>
-      <c r="AK7" s="192"/>
-      <c r="AL7" s="192"/>
-      <c r="AM7" s="192"/>
-      <c r="AN7" s="192"/>
-      <c r="AO7" s="192"/>
-      <c r="AP7" s="192"/>
-      <c r="AQ7" s="192"/>
-      <c r="AR7" s="193"/>
+      <c r="AC7" s="195"/>
+      <c r="AD7" s="195"/>
+      <c r="AE7" s="195"/>
+      <c r="AF7" s="195"/>
+      <c r="AG7" s="195"/>
+      <c r="AH7" s="195"/>
+      <c r="AI7" s="195"/>
+      <c r="AJ7" s="195"/>
+      <c r="AK7" s="195"/>
+      <c r="AL7" s="195"/>
+      <c r="AM7" s="195"/>
+      <c r="AN7" s="195"/>
+      <c r="AO7" s="195"/>
+      <c r="AP7" s="195"/>
+      <c r="AQ7" s="195"/>
+      <c r="AR7" s="196"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="52"/>
@@ -21266,10 +21320,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -21385,13 +21439,13 @@
       <c r="A5" s="150">
         <v>3</v>
       </c>
-      <c r="B5" s="178" t="s">
+      <c r="B5" s="177" t="s">
         <v>485</v>
       </c>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="178" t="s">
         <v>486</v>
       </c>
-      <c r="D5" s="179" t="s">
+      <c r="D5" s="178" t="s">
         <v>487</v>
       </c>
       <c r="E5" s="161"/>
@@ -21410,29 +21464,29 @@
       <c r="A6" s="150">
         <v>4</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="179" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="180" t="s">
         <v>316</v>
       </c>
-      <c r="D6" s="181" t="s">
+      <c r="D6" s="180" t="s">
         <v>322</v>
       </c>
-      <c r="E6" s="182" t="s">
+      <c r="E6" s="181" t="s">
         <v>457</v>
       </c>
       <c r="G6" s="151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -21448,20 +21502,20 @@
       <c r="D7" s="155" t="s">
         <v>453</v>
       </c>
-      <c r="E7" s="163" t="s">
+      <c r="E7" s="162" t="s">
         <v>330</v>
       </c>
       <c r="G7" s="154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="154">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -21477,49 +21531,49 @@
       <c r="D8" s="155" t="s">
         <v>454</v>
       </c>
-      <c r="E8" s="163" t="s">
+      <c r="E8" s="162" t="s">
         <v>331</v>
       </c>
       <c r="G8" s="157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8" s="157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8" s="157">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" thickBot="1">
       <c r="A9" s="150">
         <v>7</v>
       </c>
-      <c r="B9" s="183" t="s">
+      <c r="B9" s="182" t="s">
         <v>448</v>
       </c>
-      <c r="C9" s="184" t="s">
+      <c r="C9" s="183" t="s">
         <v>455</v>
       </c>
-      <c r="D9" s="184" t="s">
+      <c r="D9" s="183" t="s">
         <v>456</v>
       </c>
-      <c r="E9" s="185" t="s">
+      <c r="E9" s="184" t="s">
         <v>328</v>
       </c>
-      <c r="G9" s="165">
-        <v>3</v>
-      </c>
-      <c r="H9" s="165">
-        <v>3</v>
-      </c>
-      <c r="I9" s="165">
-        <v>3</v>
-      </c>
-      <c r="J9" s="165">
-        <v>3</v>
+      <c r="G9" s="164">
+        <v>0</v>
+      </c>
+      <c r="H9" s="164">
+        <v>0</v>
+      </c>
+      <c r="I9" s="164">
+        <v>0</v>
+      </c>
+      <c r="J9" s="164">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21535,7 +21589,7 @@
       <c r="D10" s="155" t="s">
         <v>325</v>
       </c>
-      <c r="E10" s="163" t="s">
+      <c r="E10" s="162" t="s">
         <v>332</v>
       </c>
       <c r="G10" s="151">
@@ -21564,7 +21618,7 @@
       <c r="D11" s="155" t="s">
         <v>326</v>
       </c>
-      <c r="E11" s="163" t="s">
+      <c r="E11" s="162" t="s">
         <v>333</v>
       </c>
       <c r="G11" s="154">
@@ -21593,7 +21647,7 @@
       <c r="D12" s="155" t="s">
         <v>327</v>
       </c>
-      <c r="E12" s="163" t="s">
+      <c r="E12" s="162" t="s">
         <v>334</v>
       </c>
       <c r="G12" s="157">
@@ -21622,19 +21676,19 @@
       <c r="D13" s="160" t="s">
         <v>463</v>
       </c>
-      <c r="E13" s="164" t="s">
+      <c r="E13" s="163" t="s">
         <v>335</v>
       </c>
-      <c r="G13" s="165">
+      <c r="G13" s="164">
         <v>7</v>
       </c>
-      <c r="H13" s="165">
+      <c r="H13" s="164">
         <v>7</v>
       </c>
-      <c r="I13" s="165">
+      <c r="I13" s="164">
         <v>7</v>
       </c>
-      <c r="J13" s="165">
+      <c r="J13" s="164">
         <v>7</v>
       </c>
     </row>
@@ -21642,6 +21696,18 @@
       <c r="A14" s="150">
         <v>12</v>
       </c>
+      <c r="B14" s="179" t="s">
+        <v>494</v>
+      </c>
+      <c r="C14" s="180" t="s">
+        <v>495</v>
+      </c>
+      <c r="D14" s="180" t="s">
+        <v>496</v>
+      </c>
+      <c r="E14" s="181" t="s">
+        <v>497</v>
+      </c>
       <c r="G14" s="151">
         <v>8</v>
       </c>
@@ -21655,9 +21721,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.25" thickBot="1">
+    <row r="15" spans="1:10">
       <c r="A15" s="150">
         <v>13</v>
+      </c>
+      <c r="B15" s="157" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" s="155" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="155" t="s">
+        <v>357</v>
+      </c>
+      <c r="E15" s="162" t="s">
+        <v>368</v>
       </c>
       <c r="G15" s="154">
         <v>9</v>
@@ -21676,10 +21754,18 @@
       <c r="A16" s="150">
         <v>14</v>
       </c>
-      <c r="B16" s="151"/>
-      <c r="C16" s="152"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="162"/>
+      <c r="B16" s="154" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" s="155" t="s">
+        <v>348</v>
+      </c>
+      <c r="D16" s="155" t="s">
+        <v>358</v>
+      </c>
+      <c r="E16" s="162" t="s">
+        <v>369</v>
+      </c>
       <c r="G16" s="157">
         <v>10</v>
       </c>
@@ -21697,16 +21783,28 @@
       <c r="A17" s="150">
         <v>15</v>
       </c>
-      <c r="G17" s="165">
+      <c r="B17" s="182" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" s="183" t="s">
+        <v>345</v>
+      </c>
+      <c r="D17" s="183" t="s">
+        <v>355</v>
+      </c>
+      <c r="E17" s="184" t="s">
+        <v>366</v>
+      </c>
+      <c r="G17" s="164">
         <v>11</v>
       </c>
-      <c r="H17" s="165">
+      <c r="H17" s="164">
         <v>11</v>
       </c>
-      <c r="I17" s="165">
+      <c r="I17" s="164">
         <v>11</v>
       </c>
-      <c r="J17" s="165">
+      <c r="J17" s="164">
         <v>11</v>
       </c>
     </row>
@@ -21714,6 +21812,18 @@
       <c r="A18" s="150">
         <v>16</v>
       </c>
+      <c r="B18" s="154" t="s">
+        <v>340</v>
+      </c>
+      <c r="C18" s="155" t="s">
+        <v>349</v>
+      </c>
+      <c r="D18" s="155" t="s">
+        <v>359</v>
+      </c>
+      <c r="E18" s="162" t="s">
+        <v>370</v>
+      </c>
       <c r="G18" s="151">
         <v>12</v>
       </c>
@@ -21731,6 +21841,18 @@
       <c r="A19" s="150">
         <v>17</v>
       </c>
+      <c r="B19" s="157" t="s">
+        <v>341</v>
+      </c>
+      <c r="C19" s="155" t="s">
+        <v>350</v>
+      </c>
+      <c r="D19" s="155" t="s">
+        <v>360</v>
+      </c>
+      <c r="E19" s="162" t="s">
+        <v>371</v>
+      </c>
       <c r="G19" s="154">
         <v>13</v>
       </c>
@@ -21748,6 +21870,18 @@
       <c r="A20" s="150">
         <v>18</v>
       </c>
+      <c r="B20" s="154" t="s">
+        <v>342</v>
+      </c>
+      <c r="C20" s="155" t="s">
+        <v>351</v>
+      </c>
+      <c r="D20" s="155" t="s">
+        <v>361</v>
+      </c>
+      <c r="E20" s="162" t="s">
+        <v>372</v>
+      </c>
       <c r="G20" s="157">
         <v>14</v>
       </c>
@@ -21765,16 +21899,28 @@
       <c r="A21" s="150">
         <v>19</v>
       </c>
-      <c r="G21" s="165">
+      <c r="B21" s="159" t="s">
+        <v>343</v>
+      </c>
+      <c r="C21" s="160" t="s">
+        <v>352</v>
+      </c>
+      <c r="D21" s="160" t="s">
+        <v>362</v>
+      </c>
+      <c r="E21" s="163" t="s">
+        <v>373</v>
+      </c>
+      <c r="G21" s="164">
         <v>15</v>
       </c>
-      <c r="H21" s="165">
+      <c r="H21" s="164">
         <v>15</v>
       </c>
-      <c r="I21" s="165">
+      <c r="I21" s="164">
         <v>15</v>
       </c>
-      <c r="J21" s="165">
+      <c r="J21" s="164">
         <v>15</v>
       </c>
     </row>
@@ -21782,6 +21928,18 @@
       <c r="A22" s="150">
         <v>20</v>
       </c>
+      <c r="B22" s="154" t="s">
+        <v>344</v>
+      </c>
+      <c r="C22" s="155" t="s">
+        <v>353</v>
+      </c>
+      <c r="D22" s="155" t="s">
+        <v>363</v>
+      </c>
+      <c r="E22" s="162" t="s">
+        <v>374</v>
+      </c>
       <c r="G22" s="151">
         <v>16</v>
       </c>
@@ -21799,6 +21957,18 @@
       <c r="A23" s="150">
         <v>21</v>
       </c>
+      <c r="B23" s="157" t="s">
+        <v>498</v>
+      </c>
+      <c r="C23" s="155" t="s">
+        <v>354</v>
+      </c>
+      <c r="D23" s="155" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="162" t="s">
+        <v>375</v>
+      </c>
       <c r="G23" s="154">
         <v>17</v>
       </c>
@@ -21816,6 +21986,18 @@
       <c r="A24" s="150">
         <v>22</v>
       </c>
+      <c r="B24" s="154" t="s">
+        <v>499</v>
+      </c>
+      <c r="C24" s="155" t="s">
+        <v>500</v>
+      </c>
+      <c r="D24" s="155" t="s">
+        <v>365</v>
+      </c>
+      <c r="E24" s="162" t="s">
+        <v>376</v>
+      </c>
       <c r="G24" s="157">
         <v>18</v>
       </c>
@@ -21829,20 +22011,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="14.25" thickBot="1">
       <c r="A25" s="150">
         <v>23</v>
       </c>
-      <c r="G25" s="165">
+      <c r="B25" s="159" t="s">
+        <v>501</v>
+      </c>
+      <c r="C25" s="160" t="s">
+        <v>502</v>
+      </c>
+      <c r="D25" s="160" t="s">
+        <v>503</v>
+      </c>
+      <c r="E25" s="163" t="s">
+        <v>377</v>
+      </c>
+      <c r="G25" s="164">
         <v>19</v>
       </c>
-      <c r="H25" s="165">
+      <c r="H25" s="164">
         <v>19</v>
       </c>
-      <c r="I25" s="165">
+      <c r="I25" s="164">
         <v>19</v>
       </c>
-      <c r="J25" s="165">
+      <c r="J25" s="164">
         <v>19</v>
       </c>
     </row>
@@ -21850,50 +22044,494 @@
       <c r="A26" s="150">
         <v>24</v>
       </c>
+      <c r="B26" s="179" t="s">
+        <v>504</v>
+      </c>
+      <c r="C26" s="180" t="s">
+        <v>391</v>
+      </c>
+      <c r="D26" s="180" t="s">
+        <v>387</v>
+      </c>
+      <c r="E26" s="181" t="s">
+        <v>384</v>
+      </c>
+      <c r="G26" s="151">
+        <v>20</v>
+      </c>
+      <c r="H26" s="151">
+        <v>20</v>
+      </c>
+      <c r="I26" s="151">
+        <v>20</v>
+      </c>
+      <c r="J26" s="151">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="150">
         <v>25</v>
       </c>
+      <c r="B27" s="157" t="s">
+        <v>505</v>
+      </c>
+      <c r="C27" s="155" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" s="155" t="s">
+        <v>390</v>
+      </c>
+      <c r="E27" s="162" t="s">
+        <v>386</v>
+      </c>
+      <c r="G27" s="154">
+        <v>21</v>
+      </c>
+      <c r="H27" s="154">
+        <v>21</v>
+      </c>
+      <c r="I27" s="154">
+        <v>21</v>
+      </c>
+      <c r="J27" s="154">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="150">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="B28" s="154" t="s">
+        <v>404</v>
+      </c>
+      <c r="C28" s="155" t="s">
+        <v>399</v>
+      </c>
+      <c r="D28" s="155" t="s">
+        <v>394</v>
+      </c>
+      <c r="E28" s="162" t="s">
+        <v>389</v>
+      </c>
+      <c r="G28" s="157">
+        <v>22</v>
+      </c>
+      <c r="H28" s="157">
+        <v>22</v>
+      </c>
+      <c r="I28" s="157">
+        <v>22</v>
+      </c>
+      <c r="J28" s="157">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" thickBot="1">
       <c r="A29" s="150">
         <v>27</v>
+      </c>
+      <c r="B29" s="182" t="s">
+        <v>506</v>
+      </c>
+      <c r="C29" s="183" t="s">
+        <v>388</v>
+      </c>
+      <c r="D29" s="183" t="s">
+        <v>385</v>
+      </c>
+      <c r="E29" s="184" t="s">
+        <v>383</v>
+      </c>
+      <c r="G29" s="164">
+        <v>23</v>
+      </c>
+      <c r="H29" s="164">
+        <v>23</v>
+      </c>
+      <c r="I29" s="164">
+        <v>23</v>
+      </c>
+      <c r="J29" s="164">
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="150">
         <v>28</v>
       </c>
+      <c r="B30" s="154" t="s">
+        <v>408</v>
+      </c>
+      <c r="C30" s="155" t="s">
+        <v>403</v>
+      </c>
+      <c r="D30" s="155" t="s">
+        <v>398</v>
+      </c>
+      <c r="E30" s="162" t="s">
+        <v>393</v>
+      </c>
+      <c r="G30" s="151">
+        <v>24</v>
+      </c>
+      <c r="H30" s="151">
+        <v>24</v>
+      </c>
+      <c r="I30" s="151">
+        <v>24</v>
+      </c>
+      <c r="J30" s="151">
+        <v>24</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="150">
         <v>29</v>
       </c>
+      <c r="B31" s="157" t="s">
+        <v>412</v>
+      </c>
+      <c r="C31" s="155" t="s">
+        <v>407</v>
+      </c>
+      <c r="D31" s="155" t="s">
+        <v>402</v>
+      </c>
+      <c r="E31" s="162" t="s">
+        <v>397</v>
+      </c>
+      <c r="G31" s="154">
+        <v>25</v>
+      </c>
+      <c r="H31" s="154">
+        <v>25</v>
+      </c>
+      <c r="I31" s="154">
+        <v>25</v>
+      </c>
+      <c r="J31" s="154">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="150">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="154" t="s">
+        <v>416</v>
+      </c>
+      <c r="C32" s="155" t="s">
+        <v>411</v>
+      </c>
+      <c r="D32" s="155" t="s">
+        <v>406</v>
+      </c>
+      <c r="E32" s="162" t="s">
+        <v>401</v>
+      </c>
+      <c r="G32" s="157">
+        <v>26</v>
+      </c>
+      <c r="H32" s="157">
+        <v>26</v>
+      </c>
+      <c r="I32" s="157">
+        <v>26</v>
+      </c>
+      <c r="J32" s="157">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.25" thickBot="1">
       <c r="A33" s="150">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="159" t="s">
+        <v>420</v>
+      </c>
+      <c r="C33" s="160" t="s">
+        <v>415</v>
+      </c>
+      <c r="D33" s="160" t="s">
+        <v>410</v>
+      </c>
+      <c r="E33" s="163" t="s">
+        <v>405</v>
+      </c>
+      <c r="G33" s="164">
+        <v>27</v>
+      </c>
+      <c r="H33" s="164">
+        <v>27</v>
+      </c>
+      <c r="I33" s="164">
+        <v>27</v>
+      </c>
+      <c r="J33" s="164">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="150">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="154" t="s">
+        <v>424</v>
+      </c>
+      <c r="C34" s="155" t="s">
+        <v>419</v>
+      </c>
+      <c r="D34" s="155" t="s">
+        <v>414</v>
+      </c>
+      <c r="E34" s="162" t="s">
+        <v>409</v>
+      </c>
+      <c r="G34" s="151">
+        <v>28</v>
+      </c>
+      <c r="H34" s="151">
+        <v>28</v>
+      </c>
+      <c r="I34" s="151">
+        <v>28</v>
+      </c>
+      <c r="J34" s="151">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="150">
         <v>33</v>
+      </c>
+      <c r="B35" s="157" t="s">
+        <v>428</v>
+      </c>
+      <c r="C35" s="155" t="s">
+        <v>423</v>
+      </c>
+      <c r="D35" s="155" t="s">
+        <v>418</v>
+      </c>
+      <c r="E35" s="162" t="s">
+        <v>413</v>
+      </c>
+      <c r="G35" s="154">
+        <v>29</v>
+      </c>
+      <c r="H35" s="154">
+        <v>29</v>
+      </c>
+      <c r="I35" s="154">
+        <v>29</v>
+      </c>
+      <c r="J35" s="154">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="150">
+        <v>34</v>
+      </c>
+      <c r="B36" s="154" t="s">
+        <v>432</v>
+      </c>
+      <c r="C36" s="155" t="s">
+        <v>427</v>
+      </c>
+      <c r="D36" s="155" t="s">
+        <v>422</v>
+      </c>
+      <c r="E36" s="162" t="s">
+        <v>417</v>
+      </c>
+      <c r="G36" s="157">
+        <v>30</v>
+      </c>
+      <c r="H36" s="157">
+        <v>30</v>
+      </c>
+      <c r="I36" s="157">
+        <v>30</v>
+      </c>
+      <c r="J36" s="157">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A37" s="150">
+        <v>35</v>
+      </c>
+      <c r="B37" s="159" t="s">
+        <v>436</v>
+      </c>
+      <c r="C37" s="160" t="s">
+        <v>431</v>
+      </c>
+      <c r="D37" s="160" t="s">
+        <v>426</v>
+      </c>
+      <c r="E37" s="163" t="s">
+        <v>421</v>
+      </c>
+      <c r="G37" s="164">
+        <v>31</v>
+      </c>
+      <c r="H37" s="164">
+        <v>31</v>
+      </c>
+      <c r="I37" s="164">
+        <v>31</v>
+      </c>
+      <c r="J37" s="164">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="150">
+        <v>36</v>
+      </c>
+      <c r="B38" s="154" t="s">
+        <v>440</v>
+      </c>
+      <c r="C38" s="155" t="s">
+        <v>435</v>
+      </c>
+      <c r="D38" s="155" t="s">
+        <v>430</v>
+      </c>
+      <c r="E38" s="162" t="s">
+        <v>425</v>
+      </c>
+      <c r="G38" s="151">
+        <v>32</v>
+      </c>
+      <c r="H38" s="151">
+        <v>32</v>
+      </c>
+      <c r="I38" s="151">
+        <v>32</v>
+      </c>
+      <c r="J38" s="151">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="150">
+        <v>37</v>
+      </c>
+      <c r="B39" s="157" t="s">
+        <v>507</v>
+      </c>
+      <c r="C39" s="155" t="s">
+        <v>439</v>
+      </c>
+      <c r="D39" s="155" t="s">
+        <v>434</v>
+      </c>
+      <c r="E39" s="162" t="s">
+        <v>429</v>
+      </c>
+      <c r="G39" s="154">
+        <v>33</v>
+      </c>
+      <c r="H39" s="154">
+        <v>33</v>
+      </c>
+      <c r="I39" s="154">
+        <v>33</v>
+      </c>
+      <c r="J39" s="154">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="150">
+        <v>38</v>
+      </c>
+      <c r="B40" s="154" t="s">
+        <v>508</v>
+      </c>
+      <c r="C40" s="155" t="s">
+        <v>509</v>
+      </c>
+      <c r="D40" s="155" t="s">
+        <v>438</v>
+      </c>
+      <c r="E40" s="162" t="s">
+        <v>433</v>
+      </c>
+      <c r="G40" s="157">
+        <v>34</v>
+      </c>
+      <c r="H40" s="157">
+        <v>34</v>
+      </c>
+      <c r="I40" s="157">
+        <v>34</v>
+      </c>
+      <c r="J40" s="157">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="14.25" thickBot="1">
+      <c r="A41" s="150">
+        <v>39</v>
+      </c>
+      <c r="B41" s="159" t="s">
+        <v>510</v>
+      </c>
+      <c r="C41" s="160" t="s">
+        <v>511</v>
+      </c>
+      <c r="D41" s="160" t="s">
+        <v>512</v>
+      </c>
+      <c r="E41" s="163" t="s">
+        <v>437</v>
+      </c>
+      <c r="G41" s="164">
+        <v>35</v>
+      </c>
+      <c r="H41" s="164">
+        <v>35</v>
+      </c>
+      <c r="I41" s="164">
+        <v>35</v>
+      </c>
+      <c r="J41" s="164">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="150">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="150">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="150">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="150">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="150">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="150">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
220507-v5 UPD stage transfer OK
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06395DC-59B7-43A9-A531-7BAF3A087E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3481FD2F-11B3-447E-B307-2A2EB3A02CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3585" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
220508-v7 add output bram ports
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138D502F-22D3-4CA5-9A23-9D4A0E18C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D12116-8271-4F7F-A05B-1429B42A10B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="16200" windowHeight="9397" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -18917,8 +18917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AK32" sqref="AK32"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -21322,8 +21322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:J41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>

<commit_message>
220519-v1 input data flow OK, PE array cannot compute
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D12116-8271-4F7F-A05B-1429B42A10B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5855A-91FB-4E46-AE80-7D92E70601AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="353" yWindow="338" windowWidth="9584" windowHeight="5400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="非线性运算" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="514">
   <si>
     <t>步骤</t>
   </si>
@@ -1773,6 +1773,10 @@
   </si>
   <si>
     <t>cov(14,15)</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -18608,15 +18612,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696DFE49-C43E-4BC5-A72A-A7713F047E7F}">
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.25" thickBot="1">
+    <row r="1" spans="2:9" ht="14.25" thickBot="1">
       <c r="B1" s="102" t="s">
         <v>226</v>
       </c>
@@ -18629,8 +18633,17 @@
       <c r="E1" s="102" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="2:5">
+      <c r="G1" s="102" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="102" t="s">
+        <v>513</v>
+      </c>
+      <c r="I1" s="102" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
       <c r="B2" s="131" t="s">
         <v>230</v>
       </c>
@@ -18642,7 +18655,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:9">
       <c r="B3" s="135" t="s">
         <v>232</v>
       </c>
@@ -18653,8 +18666,17 @@
       <c r="E3" s="139" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="14.25" thickBot="1">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="14.25" thickBot="1">
       <c r="B4" s="140" t="s">
         <v>185</v>
       </c>
@@ -18666,7 +18688,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:9">
       <c r="B5" s="131" t="s">
         <v>230</v>
       </c>
@@ -18678,7 +18700,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:9">
       <c r="B6" s="135" t="s">
         <v>232</v>
       </c>
@@ -18689,8 +18711,17 @@
       <c r="E6" s="139" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="14.25" thickBot="1">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="14.25" thickBot="1">
       <c r="B7" s="140" t="s">
         <v>185</v>
       </c>
@@ -18702,7 +18733,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:9">
       <c r="B8" s="131" t="s">
         <v>238</v>
       </c>
@@ -18714,7 +18745,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:9">
       <c r="B9" s="135" t="s">
         <v>237</v>
       </c>
@@ -18725,8 +18756,17 @@
       <c r="E9" s="139" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="14.25" thickBot="1">
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="14.25" thickBot="1">
       <c r="B10" s="140" t="s">
         <v>185</v>
       </c>
@@ -18738,7 +18778,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:9">
       <c r="B11" s="131" t="s">
         <v>235</v>
       </c>
@@ -18750,7 +18790,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:9">
       <c r="B12" s="135" t="s">
         <v>237</v>
       </c>
@@ -18761,8 +18801,17 @@
       <c r="E12" s="139" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" ht="14.25" thickBot="1">
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="14.25" thickBot="1">
       <c r="B13" s="140" t="s">
         <v>185</v>
       </c>
@@ -18774,7 +18823,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:9">
       <c r="B14" s="131" t="s">
         <v>231</v>
       </c>
@@ -18788,7 +18837,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:9">
       <c r="B15" s="135" t="s">
         <v>232</v>
       </c>
@@ -18801,8 +18850,17 @@
       <c r="E15" s="139" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.4" customHeight="1" thickBot="1">
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.4" customHeight="1" thickBot="1">
       <c r="B16" s="140" t="s">
         <v>185</v>
       </c>
@@ -18816,7 +18874,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:9">
       <c r="B17" s="131" t="s">
         <v>240</v>
       </c>
@@ -18830,7 +18888,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:9">
       <c r="B18" s="135" t="s">
         <v>237</v>
       </c>
@@ -18843,8 +18901,17 @@
       <c r="E18" s="139" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="14.25" thickBot="1">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="14.25" thickBot="1">
       <c r="B19" s="140" t="s">
         <v>185</v>
       </c>
@@ -18858,7 +18925,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:9">
       <c r="B20" s="131" t="s">
         <v>245</v>
       </c>
@@ -18874,9 +18941,8 @@
       <c r="F20" s="103" t="s">
         <v>247</v>
       </c>
-      <c r="G20" s="103"/>
-    </row>
-    <row r="21" spans="2:7">
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" s="135" t="s">
         <v>237</v>
       </c>
@@ -18892,8 +18958,17 @@
       <c r="F21" s="102" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="14.25" thickBot="1">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="14.25" thickBot="1">
       <c r="B22" s="140" t="s">
         <v>185</v>
       </c>
@@ -18917,7 +18992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
220704-v1 revised partly nonlinear RD and WR
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C039B8F-708B-4784-B504-9E2570968E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8E8555-91BD-47AB-B52C-10FC312885D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7635" yWindow="2123" windowWidth="9585" windowHeight="6000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
@@ -10158,8 +10158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10745,7 +10745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -13964,5 +13964,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
220707-v1 finished PRD code, to be sim
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8E8555-91BD-47AB-B52C-10FC312885D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3015675-123C-4D42-A3A7-C450E3CA8071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="2123" windowWidth="9585" windowHeight="6000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
@@ -10158,7 +10158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -10745,8 +10745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528C72A8-6F35-4983-A50F-4303D71F9B39}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10927,13 +10927,13 @@
       </c>
       <c r="E5" s="143"/>
       <c r="G5" s="141">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="142">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" s="142">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5" s="143"/>
       <c r="M5" s="132">

</xml_diff>

<commit_message>
220709-v2 not cplt for NEW
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04473B4E-A490-44C0-81F1-5C40A7B0003F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F8CAD3-8829-4A38-87B0-08E309938A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="421">
   <si>
     <t>步骤</t>
   </si>
@@ -585,18 +585,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>t_cov_vl_H_T</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(0,1) = vt(1,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(0,2) = vt(2,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>cov_l/K(0,1) = 0</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -604,14 +592,6 @@
     <t>cov_l/K(0,2) = 0</t>
   </si>
   <si>
-    <t>cov_vl_H_T(7,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(7,2)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>cov_l/K(7,1)</t>
   </si>
   <si>
@@ -626,25 +606,10 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>cov_vl_H_T(1,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(1,2)</t>
-  </si>
-  <si>
     <t>cov_l/K(1,1)</t>
   </si>
   <si>
     <t>cov_l/K(1,2)</t>
-  </si>
-  <si>
-    <t>cov_vl_H_T(6,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(6,2)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>cov_l/K(6,1)</t>
@@ -657,25 +622,10 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>cov_vl_H_T(2,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(2,2)</t>
-  </si>
-  <si>
     <t>cov_l/K(2,1)</t>
   </si>
   <si>
     <t>cov_l/K(2,2)</t>
-  </si>
-  <si>
-    <t>cov_vl_H_T(5,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(5,2)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>cov_l/K(5,1)</t>
@@ -694,14 +644,6 @@
     <t>cov_l/K(3,2)</t>
   </si>
   <si>
-    <t>cov_vl_H_T(4,1)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vl_H_T(4,2)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>cov_l/K(4,1)</t>
   </si>
   <si>
@@ -1337,10 +1279,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>(3+2n * 3)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>S, S_inv为对称 可转置</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1439,14 +1377,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>cov_mm</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>cov_vm</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>(3 * 3)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -1488,6 +1418,61 @@
   </si>
   <si>
     <t>F_cov</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cov_mv</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2n * 3)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_cov_HT</t>
+  </si>
+  <si>
+    <t>cov_HT(7,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(7,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(1,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(1,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(6,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(6,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(2,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(2,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(5,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(5,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(4,1)</t>
+  </si>
+  <si>
+    <t>cov_HT(4,2)</t>
+  </si>
+  <si>
+    <t>cov_HT(0,1)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>cov_HT(0,2)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -3486,9 +3471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -3816,7 +3801,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="3" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -3841,7 +3826,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="1" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -3860,14 +3845,14 @@
     <row r="16" spans="1:19" ht="36" customHeight="1">
       <c r="A16" s="8"/>
       <c r="B16" s="40" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="C16" s="149" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="41" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3968,7 +3953,7 @@
     <row r="20" spans="1:19" ht="38.25" customHeight="1">
       <c r="A20" s="8"/>
       <c r="B20" s="42" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>19</v>
@@ -3977,7 +3962,7 @@
         <v>81</v>
       </c>
       <c r="E20" s="149" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -4150,7 +4135,7 @@
         <v>86</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -4337,7 +4322,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="149" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="51" t="s">
@@ -4535,7 +4520,7 @@
         <v>119</v>
       </c>
       <c r="F41" s="74" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="G41" s="74"/>
       <c r="H41" s="74"/>
@@ -5163,7 +5148,7 @@
         <v>84</v>
       </c>
       <c r="F65" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
@@ -5184,7 +5169,7 @@
         <v>105</v>
       </c>
       <c r="B66" s="150" t="s">
-        <v>409</v>
+        <v>348</v>
       </c>
       <c r="C66" s="58" t="s">
         <v>73</v>
@@ -5209,7 +5194,7 @@
     <row r="67" spans="1:19">
       <c r="A67" s="8"/>
       <c r="B67" s="34" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>72</v>
@@ -5237,7 +5222,7 @@
         <v>85</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="31"/>
@@ -5261,7 +5246,7 @@
         <v>106</v>
       </c>
       <c r="B69" s="150" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C69" s="58" t="s">
         <v>73</v>
@@ -5286,7 +5271,7 @@
     <row r="70" spans="1:19">
       <c r="A70" s="8"/>
       <c r="B70" s="34" t="s">
-        <v>377</v>
+        <v>405</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>72</v>
@@ -5314,7 +5299,7 @@
         <v>85</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="157"/>
@@ -5391,7 +5376,7 @@
         <v>83</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="153"/>
@@ -5412,7 +5397,7 @@
     </row>
     <row r="75" spans="1:19">
       <c r="A75" s="8" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="B75" s="158" t="s">
         <v>76</v>
@@ -5422,7 +5407,7 @@
       </c>
       <c r="D75" s="33"/>
       <c r="E75" s="49" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="28"/>
@@ -5472,7 +5457,7 @@
         <v>83</v>
       </c>
       <c r="C77" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D77" s="15"/>
       <c r="E77" s="31" t="s">
@@ -5498,7 +5483,7 @@
         <v>108</v>
       </c>
       <c r="B78" s="49" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="D78" s="33"/>
       <c r="E78" s="59" t="s">
@@ -5522,7 +5507,7 @@
     <row r="79" spans="1:19">
       <c r="A79" s="8"/>
       <c r="B79" s="31" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="D79" s="15"/>
       <c r="E79" s="8" t="s">
@@ -5550,7 +5535,7 @@
       </c>
       <c r="D80" s="15"/>
       <c r="E80" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="F80" s="172"/>
       <c r="G80" s="28"/>
@@ -5584,7 +5569,7 @@
         <v>58</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="G81" s="28"/>
       <c r="H81" s="28"/>
@@ -5603,7 +5588,7 @@
     <row r="82" spans="1:19">
       <c r="A82" s="8"/>
       <c r="B82" s="17" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>55</v>
@@ -5635,7 +5620,7 @@
         <v>83</v>
       </c>
       <c r="C83" s="30" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>83</v>
@@ -5659,7 +5644,7 @@
     </row>
     <row r="84" spans="1:19">
       <c r="A84" s="8" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B84" s="45" t="s">
         <v>58</v>
@@ -5736,7 +5721,7 @@
     </row>
     <row r="87" spans="1:19">
       <c r="A87" s="8" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="B87" s="45" t="s">
         <v>120</v>
@@ -5776,7 +5761,7 @@
         <v>56</v>
       </c>
       <c r="F88" s="74" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -5805,7 +5790,7 @@
         <v>84</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -5999,7 +5984,7 @@
     </row>
     <row r="96" spans="1:19">
       <c r="A96" s="72" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="B96" s="75" t="s">
         <v>60</v>
@@ -6034,7 +6019,7 @@
         <v>69</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>70</v>
@@ -6072,7 +6057,7 @@
         <v>86</v>
       </c>
       <c r="F98" s="73" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
@@ -9820,7 +9805,7 @@
         <v>81</v>
       </c>
       <c r="H1" s="84" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="I1" s="84" t="s">
         <v>80</v>
@@ -9831,7 +9816,7 @@
         <v>127</v>
       </c>
       <c r="C2" s="115" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="D2" s="115"/>
       <c r="E2" s="116" t="s">
@@ -10113,7 +10098,7 @@
         <v>142</v>
       </c>
       <c r="C20" s="115" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="D20" s="115" t="s">
         <v>139</v>
@@ -10130,7 +10115,7 @@
         <v>134</v>
       </c>
       <c r="C21" s="120" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="D21" s="120" t="s">
         <v>134</v>
@@ -10175,8 +10160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AV5" sqref="AV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10187,14 +10172,16 @@
     <col min="37" max="37" width="9.1328125" customWidth="1"/>
     <col min="38" max="38" width="8.796875" customWidth="1"/>
     <col min="39" max="39" width="7" customWidth="1"/>
-    <col min="40" max="40" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="14.25" thickBot="1">
       <c r="A1" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -10343,7 +10330,7 @@
       <c r="F2" s="87"/>
       <c r="G2" s="87"/>
       <c r="H2" s="89" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="I2" s="90"/>
       <c r="J2" s="91"/>
@@ -10355,20 +10342,20 @@
       <c r="O2" s="90"/>
       <c r="P2" s="90"/>
       <c r="Q2" s="89" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="R2" s="90"/>
       <c r="S2" s="92">
         <v>5</v>
       </c>
       <c r="T2" s="93" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="U2" s="92">
         <v>4</v>
       </c>
       <c r="V2" s="89" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="W2" s="91"/>
       <c r="X2" s="89" t="s">
@@ -10380,7 +10367,7 @@
       </c>
       <c r="AA2" s="91"/>
       <c r="AB2" s="95" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="AC2" s="96">
         <v>-3</v>
@@ -10389,7 +10376,7 @@
         <v>0</v>
       </c>
       <c r="AE2" s="95" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="AF2" s="96">
         <v>3</v>
@@ -10399,47 +10386,47 @@
       </c>
       <c r="AH2" s="91"/>
       <c r="AI2" s="89" t="s">
-        <v>153</v>
+        <v>406</v>
       </c>
       <c r="AJ2" s="90"/>
       <c r="AK2" s="90"/>
       <c r="AL2" s="90"/>
       <c r="AM2" s="90"/>
       <c r="AN2" s="167" t="s">
+        <v>419</v>
+      </c>
+      <c r="AO2" s="168" t="s">
+        <v>420</v>
+      </c>
+      <c r="AP2" s="89" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="91" t="s">
         <v>154</v>
       </c>
-      <c r="AO2" s="168" t="s">
+      <c r="AR2" s="89" t="s">
+        <v>407</v>
+      </c>
+      <c r="AS2" s="91" t="s">
+        <v>408</v>
+      </c>
+      <c r="AT2" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="AP2" s="89" t="s">
+      <c r="AU2" s="91" t="s">
         <v>156</v>
-      </c>
-      <c r="AQ2" s="91" t="s">
-        <v>157</v>
-      </c>
-      <c r="AR2" s="89" t="s">
-        <v>158</v>
-      </c>
-      <c r="AS2" s="91" t="s">
-        <v>159</v>
-      </c>
-      <c r="AT2" s="89" t="s">
-        <v>160</v>
-      </c>
-      <c r="AU2" s="91" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:47" ht="14.25" thickBot="1">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B3" s="97"/>
       <c r="C3" s="98">
         <v>1</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E3" s="100"/>
       <c r="F3" s="98">
@@ -10503,33 +10490,33 @@
       <c r="AL3" s="104"/>
       <c r="AM3" s="104"/>
       <c r="AN3" s="100" t="s">
-        <v>164</v>
+        <v>409</v>
       </c>
       <c r="AO3" s="102" t="s">
-        <v>165</v>
+        <v>410</v>
       </c>
       <c r="AP3" s="100" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="AQ3" s="102" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="AR3" s="100" t="s">
-        <v>168</v>
+        <v>411</v>
       </c>
       <c r="AS3" s="102" t="s">
-        <v>169</v>
+        <v>412</v>
       </c>
       <c r="AT3" s="100" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="AU3" s="102" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:47" ht="14.25" thickBot="1">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B4" s="110"/>
       <c r="C4" s="111"/>
@@ -10540,7 +10527,7 @@
         <v>147</v>
       </c>
       <c r="F4" s="99" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G4" s="111">
         <v>1</v>
@@ -10577,33 +10564,33 @@
       <c r="AG4" s="112"/>
       <c r="AH4" s="112"/>
       <c r="AN4" s="100" t="s">
-        <v>173</v>
+        <v>413</v>
       </c>
       <c r="AO4" s="102" t="s">
-        <v>174</v>
+        <v>414</v>
       </c>
       <c r="AP4" s="100" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="AQ4" s="102" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="AR4" s="100" t="s">
-        <v>177</v>
+        <v>415</v>
       </c>
       <c r="AS4" s="102" t="s">
-        <v>178</v>
+        <v>416</v>
       </c>
       <c r="AT4" s="100" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="AU4" s="102" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="14.25" thickBot="1">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="E5" s="110"/>
       <c r="F5" s="111"/>
@@ -10630,38 +10617,38 @@
       <c r="AG5" s="112"/>
       <c r="AH5" s="112"/>
       <c r="AN5" s="169" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="AO5" s="170" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="AP5" s="103" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="AQ5" s="107" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="AR5" s="103" t="s">
-        <v>184</v>
+        <v>417</v>
       </c>
       <c r="AS5" s="107" t="s">
-        <v>185</v>
+        <v>418</v>
       </c>
       <c r="AT5" s="103" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="AU5" s="107" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
       <c r="B6" s="186" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C6" s="187"/>
       <c r="D6" s="188"/>
       <c r="E6" s="186" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F6" s="187"/>
       <c r="G6" s="188"/>
@@ -10676,7 +10663,7 @@
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
       <c r="B7" s="186" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C7" s="187"/>
       <c r="D7" s="187"/>
@@ -10693,7 +10680,7 @@
       <c r="O7" s="187"/>
       <c r="P7" s="188"/>
       <c r="Q7" s="186" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="R7" s="187"/>
       <c r="S7" s="187"/>
@@ -10706,7 +10693,7 @@
       <c r="Z7" s="187"/>
       <c r="AA7" s="188"/>
       <c r="AB7" s="186" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="AC7" s="187"/>
       <c r="AD7" s="187"/>
@@ -10730,10 +10717,10 @@
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
       <c r="H9" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="AM9" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -10741,7 +10728,7 @@
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
       <c r="H10" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -10751,7 +10738,7 @@
     </row>
     <row r="15" spans="1:47">
       <c r="AB15" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -10774,7 +10761,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10784,31 +10771,31 @@
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" thickBot="1">
       <c r="A1" s="132" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="B1" s="132" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C1" s="132" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="D1" s="132" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="E1" s="132" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="G1" s="132" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="H1" s="132" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="I1" s="132" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="J1" s="132" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="M1" s="191"/>
       <c r="N1" s="191"/>
@@ -10822,13 +10809,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="133" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="C2" s="134" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="D2" s="134" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="E2" s="135"/>
       <c r="G2" s="133">
@@ -10853,13 +10840,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="136" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="D3" s="137" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="E3" s="138"/>
       <c r="G3" s="136">
@@ -10884,13 +10871,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="139" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="D4" s="137" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="E4" s="140"/>
       <c r="G4" s="139">
@@ -10915,13 +10902,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="159" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C5" s="160" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="D5" s="160" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="E5" s="143"/>
       <c r="G5" s="141">
@@ -10946,16 +10933,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="161" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C6" s="162" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="D6" s="162" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="E6" s="163" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="G6" s="133">
         <v>1</v>
@@ -10976,16 +10963,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="139" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="D7" s="137" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="E7" s="144" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="G7" s="136">
         <v>2</v>
@@ -11006,16 +10993,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="136" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="D8" s="137" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="E8" s="144" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="G8" s="139">
         <v>3</v>
@@ -11035,16 +11022,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="164" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C9" s="165" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="D9" s="165" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="E9" s="166" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="G9" s="146">
         <v>0</v>
@@ -11064,16 +11051,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="136" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D10" s="137" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E10" s="144" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="G10" s="133">
         <v>4</v>
@@ -11093,16 +11080,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="139" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="E11" s="144" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G11" s="136">
         <v>5</v>
@@ -11122,16 +11109,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="E12" s="144" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="G12" s="139">
         <v>6</v>
@@ -11151,16 +11138,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="141" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C13" s="142" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="D13" s="142" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="E13" s="145" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G13" s="146">
         <v>7</v>
@@ -11180,16 +11167,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="161" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C14" s="162" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="D14" s="162" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="E14" s="163" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="G14" s="133">
         <v>8</v>
@@ -11209,16 +11196,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="139" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C15" s="137" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E15" s="144" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="G15" s="136">
         <v>9</v>
@@ -11238,16 +11225,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="136" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D16" s="137" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E16" s="144" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="G16" s="139">
         <v>10</v>
@@ -11267,16 +11254,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="164" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C17" s="165" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D17" s="165" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E17" s="166" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="G17" s="146">
         <v>11</v>
@@ -11296,16 +11283,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="136" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D18" s="137" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E18" s="144" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="G18" s="133">
         <v>12</v>
@@ -11325,16 +11312,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="139" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="C19" s="137" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D19" s="137" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E19" s="144" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="G19" s="136">
         <v>13</v>
@@ -11354,16 +11341,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="136" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C20" s="137" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D20" s="137" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E20" s="144" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="G20" s="139">
         <v>14</v>
@@ -11383,16 +11370,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="141" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C21" s="142" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D21" s="142" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E21" s="145" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="G21" s="146">
         <v>15</v>
@@ -11412,16 +11399,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="136" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C22" s="137" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D22" s="137" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E22" s="144" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="G22" s="133">
         <v>16</v>
@@ -11441,16 +11428,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="139" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="C23" s="137" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D23" s="137" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E23" s="144" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="G23" s="136">
         <v>17</v>
@@ -11470,16 +11457,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="136" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="C24" s="137" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="D24" s="137" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E24" s="144" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="G24" s="139">
         <v>18</v>
@@ -11499,16 +11486,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="141" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C25" s="142" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D25" s="142" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="E25" s="145" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="G25" s="146">
         <v>19</v>
@@ -11528,16 +11515,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="161" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="C26" s="162" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D26" s="162" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E26" s="163" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="G26" s="133">
         <v>20</v>
@@ -11557,16 +11544,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="139" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="C27" s="137" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D27" s="137" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="E27" s="144" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="G27" s="136">
         <v>21</v>
@@ -11586,16 +11573,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="136" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="D28" s="137" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E28" s="144" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="G28" s="139">
         <v>22</v>
@@ -11615,16 +11602,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="164" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="C29" s="165" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="D29" s="165" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="E29" s="166" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="G29" s="146">
         <v>23</v>
@@ -11644,16 +11631,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="136" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C30" s="137" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="D30" s="137" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E30" s="144" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="G30" s="133">
         <v>24</v>
@@ -11673,16 +11660,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="139" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C31" s="137" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="D31" s="137" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="E31" s="144" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="G31" s="136">
         <v>25</v>
@@ -11702,16 +11689,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="136" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C32" s="137" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="D32" s="137" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="E32" s="144" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="G32" s="139">
         <v>26</v>
@@ -11731,16 +11718,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="141" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C33" s="142" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="D33" s="142" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="E33" s="145" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="G33" s="146">
         <v>27</v>
@@ -11760,16 +11747,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="136" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C34" s="137" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="D34" s="137" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="E34" s="144" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="G34" s="133">
         <v>28</v>
@@ -11789,16 +11776,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="139" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="C35" s="137" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="D35" s="137" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="E35" s="144" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="G35" s="136">
         <v>29</v>
@@ -11818,16 +11805,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="136" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="C36" s="137" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="D36" s="137" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="E36" s="144" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="G36" s="139">
         <v>30</v>
@@ -11847,16 +11834,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="141" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C37" s="142" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="D37" s="142" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="E37" s="145" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="G37" s="146">
         <v>31</v>
@@ -11876,16 +11863,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="136" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C38" s="137" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="D38" s="137" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="E38" s="144" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="G38" s="133">
         <v>32</v>
@@ -11905,16 +11892,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="139" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="C39" s="137" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="D39" s="137" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="E39" s="144" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="G39" s="136">
         <v>33</v>
@@ -11934,16 +11921,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="136" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="C40" s="137" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D40" s="137" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E40" s="144" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="G40" s="139">
         <v>34</v>
@@ -11963,16 +11950,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="141" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="C41" s="142" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="D41" s="142" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="E41" s="145" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="G41" s="146">
         <v>35</v>
@@ -12059,10 +12046,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C2" s="119" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D2" s="120"/>
       <c r="E2" s="120"/>
@@ -12080,13 +12067,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="118" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C3" s="119" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D3" s="119" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E3" s="120"/>
       <c r="F3" s="120"/>
@@ -12103,16 +12090,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="118" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C4" s="119" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D4" s="119" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E4" s="119" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F4" s="120"/>
       <c r="G4" s="120"/>
@@ -12128,19 +12115,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="118" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C5" s="119" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D5" s="119" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E5" s="119" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="F5" s="119" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="G5" s="120"/>
       <c r="H5" s="120"/>
@@ -12155,22 +12142,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="118" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C6" s="119" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="D6" s="119" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="E6" s="119" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F6" s="119" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G6" s="119" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H6" s="120"/>
       <c r="I6" s="120"/>
@@ -12184,25 +12171,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="118" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="C7" s="119" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D7" s="119" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="E7" s="119" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="G7" s="119" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H7" s="119" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I7" s="120"/>
       <c r="J7" s="120"/>
@@ -12215,28 +12202,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="118" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C8" s="119" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="D8" s="119" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="E8" s="119" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="G8" s="119" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="H8" s="119" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="I8" s="119" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="J8" s="120"/>
       <c r="K8" s="120"/>
@@ -12248,31 +12235,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="118" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C9" s="119" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D9" s="119" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E9" s="119" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F9" s="119" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="G9" s="119" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="H9" s="119" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="I9" s="119" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="J9" s="119" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="K9" s="120"/>
       <c r="L9" s="120"/>
@@ -12283,34 +12270,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="118" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="C10" s="119" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D10" s="119" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="E10" s="119" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F10" s="119" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G10" s="119" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="H10" s="119" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="I10" s="119" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="J10" s="119" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="K10" s="119" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="L10" s="120"/>
       <c r="M10" s="121"/>
@@ -12320,37 +12307,37 @@
         <v>10</v>
       </c>
       <c r="B11" s="118" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D11" s="119" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E11" s="119" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F11" s="119" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G11" s="119" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="H11" s="119" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="I11" s="119" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="J11" s="119" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="K11" s="119" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="L11" s="119" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="M11" s="121"/>
     </row>
@@ -12359,40 +12346,40 @@
         <v>11</v>
       </c>
       <c r="B12" s="123" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D12" s="124" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E12" s="124" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F12" s="125" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="G12" s="124" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="H12" s="124" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="I12" s="124" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="J12" s="124" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="K12" s="124" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="L12" s="124" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="M12" s="126" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -12401,280 +12388,280 @@
       </c>
       <c r="B14" s="127"/>
       <c r="C14" s="128" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="129" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="129" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" s="129" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" s="129" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="129" t="s">
+        <v>214</v>
+      </c>
+      <c r="I14" s="129" t="s">
+        <v>215</v>
+      </c>
+      <c r="J14" s="129" t="s">
+        <v>216</v>
+      </c>
+      <c r="K14" s="128" t="s">
+        <v>217</v>
+      </c>
+      <c r="L14" s="129" t="s">
+        <v>218</v>
+      </c>
+      <c r="M14" s="129" t="s">
+        <v>219</v>
+      </c>
+      <c r="N14" s="129" t="s">
+        <v>220</v>
+      </c>
+      <c r="O14" s="129" t="s">
+        <v>221</v>
+      </c>
+      <c r="P14" s="129" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q14" s="129" t="s">
+        <v>223</v>
+      </c>
+      <c r="R14" s="129" t="s">
         <v>224</v>
       </c>
-      <c r="D14" s="129" t="s">
+      <c r="S14" s="129" t="s">
         <v>225</v>
       </c>
-      <c r="E14" s="129" t="s">
-        <v>226</v>
-      </c>
-      <c r="F14" s="129" t="s">
-        <v>227</v>
-      </c>
-      <c r="G14" s="129" t="s">
-        <v>228</v>
-      </c>
-      <c r="H14" s="129" t="s">
-        <v>229</v>
-      </c>
-      <c r="I14" s="129" t="s">
-        <v>230</v>
-      </c>
-      <c r="J14" s="129" t="s">
-        <v>231</v>
-      </c>
-      <c r="K14" s="128" t="s">
-        <v>232</v>
-      </c>
-      <c r="L14" s="129" t="s">
-        <v>233</v>
-      </c>
-      <c r="M14" s="129" t="s">
-        <v>234</v>
-      </c>
-      <c r="N14" s="129" t="s">
-        <v>235</v>
-      </c>
-      <c r="O14" s="129" t="s">
-        <v>236</v>
-      </c>
-      <c r="P14" s="129" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q14" s="129" t="s">
-        <v>238</v>
-      </c>
-      <c r="R14" s="129" t="s">
-        <v>239</v>
-      </c>
-      <c r="S14" s="129" t="s">
-        <v>240</v>
-      </c>
       <c r="T14" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="U14" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="V14" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="W14" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="84" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B15" s="128" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C15" s="129" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D15" s="128" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E15" s="129" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F15" s="129" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="G15" s="129" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="H15" s="129" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I15" s="129" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="J15" s="129" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K15" s="128" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="L15" s="129" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="M15" s="129" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="N15" s="129" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="O15" s="129" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="P15" s="129" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="Q15" s="129" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="R15" s="129" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="S15" s="129" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="T15" s="129" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="U15" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="V15" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="W15" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B16" s="128" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="129" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="129" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" s="128" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" s="129" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" s="129" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="129" t="s">
         <v>199</v>
       </c>
-      <c r="C16" s="129" t="s">
+      <c r="I16" s="129" t="s">
         <v>200</v>
       </c>
-      <c r="D16" s="129" t="s">
+      <c r="J16" s="129" t="s">
         <v>201</v>
       </c>
-      <c r="E16" s="128" t="s">
-        <v>211</v>
-      </c>
-      <c r="F16" s="129" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="129" t="s">
-        <v>213</v>
-      </c>
-      <c r="H16" s="129" t="s">
-        <v>214</v>
-      </c>
-      <c r="I16" s="129" t="s">
-        <v>215</v>
-      </c>
-      <c r="J16" s="129" t="s">
-        <v>216</v>
-      </c>
       <c r="K16" s="128" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="L16" s="129" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="M16" s="129" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="N16" s="129" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="O16" s="129" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="P16" s="129" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="Q16" s="129" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="R16" s="129" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="S16" s="129" t="s">
+        <v>244</v>
+      </c>
+      <c r="T16" s="129" t="s">
+        <v>245</v>
+      </c>
+      <c r="U16" s="129" t="s">
+        <v>246</v>
+      </c>
+      <c r="V16" s="84" t="s">
         <v>259</v>
       </c>
-      <c r="T16" s="129" t="s">
-        <v>260</v>
-      </c>
-      <c r="U16" s="129" t="s">
-        <v>261</v>
-      </c>
-      <c r="V16" s="84" t="s">
-        <v>274</v>
-      </c>
       <c r="W16" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="84" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B17" s="128" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="C17" s="129" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="D17" s="129" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E17" s="129" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F17" s="128" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G17" s="129" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="H17" s="129" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="I17" s="129" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="J17" s="129" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="K17" s="128" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="L17" s="129" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="M17" s="129" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="N17" s="129" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="O17" s="130" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="P17" s="129" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="Q17" s="129" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="R17" s="129" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="S17" s="129" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="T17" s="129" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="U17" s="129" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="V17" s="129" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="W17" s="84" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -12682,202 +12669,202 @@
         <v>146</v>
       </c>
       <c r="B19" s="128" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C19" s="129" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E19" s="129" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F19" s="129" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="G19" s="129" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="H19" s="129" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="I19" s="129" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="J19" s="129" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="84" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B20" s="128" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="C20" s="129" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="E20" s="129" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="F20" s="129" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G20" s="129" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="H20" s="129" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="I20" s="129" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="J20" s="129" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="K20" s="129" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B21" s="128" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="C21" s="129" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D21" s="129" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E21" s="129" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F21" s="129" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="G21" s="129" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="H21" s="129" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="I21" s="129" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="J21" s="129" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="K21" s="129" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="L21" s="129" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="84" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B22" s="128" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C22" s="129" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D22" s="129" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E22" s="129" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F22" s="130" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="G22" s="129" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="H22" s="129" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="I22" s="129" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="J22" s="129" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="K22" s="129" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="L22" s="129" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="M22" s="129" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="84" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="B24" s="84" t="s">
         <v>146</v>
       </c>
       <c r="C24" s="84" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E24" s="84" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H24" s="84" t="s">
         <v>146</v>
       </c>
       <c r="I24" s="84" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J24" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="K24" s="84" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="Q24" s="84" t="s">
         <v>146</v>
       </c>
       <c r="R24" s="128"/>
       <c r="S24" s="131" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="T24" s="129" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="U24" s="129" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="V24" s="129" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="W24" s="129" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="X24" s="129" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="Y24" s="129" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="Z24" s="129" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -12886,13 +12873,13 @@
       </c>
       <c r="B25" s="127"/>
       <c r="C25" s="128" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D25" s="128" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E25" s="128" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="H25" s="84">
         <v>0</v>
@@ -12907,34 +12894,34 @@
         <v>0</v>
       </c>
       <c r="Q25" s="84" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="R25" s="128" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="S25" s="173" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="T25" s="131" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="U25" s="129" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="V25" s="129" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="W25" s="129" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="X25" s="129" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="Y25" s="129" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="Z25" s="129" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -12942,16 +12929,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="128" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C26" s="129" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D26" s="129" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="E26" s="129" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="H26" s="84">
         <v>0</v>
@@ -12966,34 +12953,34 @@
         <v>0</v>
       </c>
       <c r="Q26" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="R26" s="128" t="s">
+        <v>184</v>
+      </c>
+      <c r="S26" s="173" t="s">
+        <v>185</v>
+      </c>
+      <c r="T26" s="173" t="s">
+        <v>186</v>
+      </c>
+      <c r="U26" s="131" t="s">
+        <v>196</v>
+      </c>
+      <c r="V26" s="129" t="s">
+        <v>197</v>
+      </c>
+      <c r="W26" s="129" t="s">
+        <v>198</v>
+      </c>
+      <c r="X26" s="129" t="s">
         <v>199</v>
       </c>
-      <c r="S26" s="173" t="s">
+      <c r="Y26" s="129" t="s">
         <v>200</v>
       </c>
-      <c r="T26" s="173" t="s">
+      <c r="Z26" s="129" t="s">
         <v>201</v>
-      </c>
-      <c r="U26" s="131" t="s">
-        <v>211</v>
-      </c>
-      <c r="V26" s="129" t="s">
-        <v>212</v>
-      </c>
-      <c r="W26" s="129" t="s">
-        <v>213</v>
-      </c>
-      <c r="X26" s="129" t="s">
-        <v>214</v>
-      </c>
-      <c r="Y26" s="129" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z26" s="129" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -13001,16 +12988,16 @@
         <v>2</v>
       </c>
       <c r="B27" s="129" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C27" s="128" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="D27" s="129" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="E27" s="129" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="H27" s="84">
         <v>1</v>
@@ -13025,34 +13012,34 @@
         <v>0</v>
       </c>
       <c r="Q27" s="84" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="R27" s="128" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="S27" s="173" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="T27" s="173" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="U27" s="173" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="V27" s="131" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="W27" s="129" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="X27" s="129" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="Y27" s="129" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="Z27" s="129" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -13060,16 +13047,16 @@
         <v>3</v>
       </c>
       <c r="B28" s="129" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C28" s="129" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D28" s="128" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="E28" s="129" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H28" s="84">
         <v>2</v>
@@ -13089,16 +13076,16 @@
         <v>4</v>
       </c>
       <c r="B29" s="129" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C29" s="129" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D29" s="129" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="E29" s="128" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H29" s="84">
         <v>3</v>
@@ -13118,16 +13105,16 @@
         <v>5</v>
       </c>
       <c r="B30" s="129" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C30" s="129" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="D30" s="129" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="E30" s="129" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="H30" s="84">
         <v>4</v>
@@ -13147,16 +13134,16 @@
         <v>6</v>
       </c>
       <c r="B31" s="129" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="C31" s="129" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D31" s="129" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="E31" s="129" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H31" s="84">
         <v>5</v>
@@ -13176,16 +13163,16 @@
         <v>7</v>
       </c>
       <c r="B32" s="129" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="C32" s="129" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D32" s="129" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="E32" s="129" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="H32" s="84">
         <v>6</v>
@@ -13205,16 +13192,16 @@
         <v>8</v>
       </c>
       <c r="B33" s="129" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C33" s="129" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="D33" s="129" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="E33" s="129" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="H33" s="84">
         <v>7</v>
@@ -13234,16 +13221,16 @@
         <v>9</v>
       </c>
       <c r="B34" s="128" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C34" s="128" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D34" s="128" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E34" s="128" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="H34" s="84">
         <v>8</v>
@@ -13263,16 +13250,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="129" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C35" s="129" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D35" s="129" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="E35" s="129" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="H35" s="84">
         <v>9</v>
@@ -13292,16 +13279,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="129" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C36" s="129" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D36" s="129" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E36" s="129" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="H36" s="84">
         <v>10</v>
@@ -13321,16 +13308,16 @@
         <v>12</v>
       </c>
       <c r="B37" s="129" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C37" s="129" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D37" s="129" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E37" s="129" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="H37" s="84">
         <v>11</v>
@@ -13350,16 +13337,16 @@
         <v>13</v>
       </c>
       <c r="B38" s="129" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C38" s="129" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D38" s="129" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E38" s="129" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="H38" s="84">
         <v>12</v>
@@ -13379,16 +13366,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="129" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="C39" s="129" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D39" s="129" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="E39" s="129" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="H39" s="84">
         <v>13</v>
@@ -13408,16 +13395,16 @@
         <v>15</v>
       </c>
       <c r="B40" s="129" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C40" s="129" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D40" s="129" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E40" s="129" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="H40" s="84">
         <v>14</v>
@@ -13437,16 +13424,16 @@
         <v>16</v>
       </c>
       <c r="B41" s="129" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C41" s="129" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D41" s="129" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E41" s="129" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="H41" s="84">
         <v>15</v>
@@ -13466,16 +13453,16 @@
         <v>17</v>
       </c>
       <c r="B42" s="129" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C42" s="129" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D42" s="129" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="E42" s="129" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="H42" s="84">
         <v>16</v>
@@ -13495,16 +13482,16 @@
         <v>18</v>
       </c>
       <c r="B43" s="128" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C43" s="129" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D43" s="129" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E43" s="129" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="H43" s="84">
         <v>17</v>
@@ -13524,16 +13511,16 @@
         <v>19</v>
       </c>
       <c r="B44" s="131" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C44" s="128" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D44" s="129" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E44" s="129" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="H44" s="84">
         <v>18</v>
@@ -13553,16 +13540,16 @@
         <v>20</v>
       </c>
       <c r="B45" s="131" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C45" s="131" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="D45" s="128" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="E45" s="129" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="H45" s="84">
         <v>19</v>
@@ -13582,16 +13569,16 @@
         <v>21</v>
       </c>
       <c r="B46" s="131" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C46" s="131" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="D46" s="131" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="E46" s="128" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="H46" s="84">
         <v>20</v>
@@ -13611,16 +13598,16 @@
         <v>22</v>
       </c>
       <c r="B47" s="131" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C47" s="131" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D47" s="131" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E47" s="131" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="H47" s="84">
         <v>21</v>
@@ -13640,16 +13627,16 @@
         <v>23</v>
       </c>
       <c r="B48" s="131" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C48" s="131" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="D48" s="131" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="E48" s="131" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="H48" s="84">
         <v>22</v>
@@ -13669,16 +13656,16 @@
         <v>24</v>
       </c>
       <c r="B49" s="131" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="C49" s="131" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="D49" s="131" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="E49" s="131" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="H49" s="84">
         <v>23</v>
@@ -13698,16 +13685,16 @@
         <v>25</v>
       </c>
       <c r="B50" s="131" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C50" s="131" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="D50" s="131" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="E50" s="131" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="H50" s="84">
         <v>24</v>
@@ -13727,16 +13714,16 @@
         <v>26</v>
       </c>
       <c r="B51" s="131" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="C51" s="131" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="D51" s="131" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="E51" s="131" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="H51" s="84">
         <v>25</v>
@@ -13756,16 +13743,16 @@
         <v>27</v>
       </c>
       <c r="B52" s="131" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="C52" s="131" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="D52" s="131" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="E52" s="131" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="H52" s="84">
         <v>26</v>
@@ -13785,16 +13772,16 @@
         <v>28</v>
       </c>
       <c r="B53" s="131" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C53" s="131" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="D53" s="131" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="E53" s="131" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="H53" s="84">
         <v>27</v>
@@ -13814,16 +13801,16 @@
         <v>29</v>
       </c>
       <c r="B54" s="131" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C54" s="131" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="D54" s="131" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="E54" s="131" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="H54" s="84">
         <v>28</v>
@@ -13843,16 +13830,16 @@
         <v>30</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C55" s="131" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="D55" s="131" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="E55" s="131" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="H55" s="84">
         <v>29</v>
@@ -13872,16 +13859,16 @@
         <v>31</v>
       </c>
       <c r="B56" s="131" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C56" s="131" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="D56" s="131" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="E56" s="131" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="H56" s="84">
         <v>30</v>
@@ -13901,16 +13888,16 @@
         <v>32</v>
       </c>
       <c r="B57" s="131" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C57" s="131" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="D57" s="131" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="E57" s="131" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="H57" s="84">
         <v>31</v>
@@ -13930,16 +13917,16 @@
         <v>33</v>
       </c>
       <c r="B58" s="131" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C58" s="131" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="D58" s="131" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="E58" s="131" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="H58" s="84">
         <v>32</v>

</xml_diff>

<commit_message>
220710-v2 problems with ABCM_en
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F8CAD3-8829-4A38-87B0-08E309938A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CF5FE-C7F0-47CA-90F3-CBE3FB833E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
@@ -3471,9 +3471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S277"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F65" s="30" t="s">
         <v>394</v>
@@ -5454,7 +5454,7 @@
     <row r="77" spans="1:19">
       <c r="A77" s="8"/>
       <c r="B77" s="34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C77" s="30" t="s">
         <v>394</v>
@@ -10160,8 +10160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AV5" sqref="AV5"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1:AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10311,6 +10311,15 @@
       </c>
       <c r="AR1">
         <v>42</v>
+      </c>
+      <c r="AS1">
+        <v>43</v>
+      </c>
+      <c r="AT1">
+        <v>44</v>
+      </c>
+      <c r="AU1">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -10761,7 +10770,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B14" sqref="B14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -12016,7 +12025,7 @@
   <dimension ref="A1:Z58"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U41" sqref="U41"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>

<commit_message>
220710-v3 problems with UPD6 addr shift
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CF5FE-C7F0-47CA-90F3-CBE3FB833E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD520B-F3EE-4515-832A-047C4E7D2802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3472,8 +3472,8 @@
   <dimension ref="A1:S277"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -5482,7 +5482,7 @@
       <c r="A78" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B78" s="49" t="s">
+      <c r="C78" s="49" t="s">
         <v>395</v>
       </c>
       <c r="D78" s="33"/>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="79" spans="1:19">
       <c r="A79" s="8"/>
-      <c r="B79" s="31" t="s">
+      <c r="C79" s="31" t="s">
         <v>396</v>
       </c>
       <c r="D79" s="15"/>
@@ -5530,8 +5530,8 @@
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="8"/>
-      <c r="B80" s="31" t="s">
-        <v>83</v>
+      <c r="C80" s="31" t="s">
+        <v>84</v>
       </c>
       <c r="D80" s="15"/>
       <c r="E80" s="30" t="s">
@@ -5646,10 +5646,9 @@
       <c r="A84" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="B84" s="45" t="s">
+      <c r="C84" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C84" s="16"/>
       <c r="D84" s="16"/>
       <c r="E84" s="46" t="s">
         <v>59</v>
@@ -5671,10 +5670,9 @@
     </row>
     <row r="85" spans="1:19">
       <c r="A85" s="8"/>
-      <c r="B85" s="17" t="s">
+      <c r="C85" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="18" t="s">
         <v>41</v>
@@ -5696,10 +5694,9 @@
     </row>
     <row r="86" spans="1:19">
       <c r="A86" s="8"/>
-      <c r="B86" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C86" s="8"/>
+      <c r="C86" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="D86" s="8"/>
       <c r="E86" s="18" t="s">
         <v>84</v>
@@ -10770,7 +10767,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E16"/>
+      <selection activeCell="B20" sqref="B20:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>

<commit_message>
220710-v4 TB-B conflict on UPD6
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD520B-F3EE-4515-832A-047C4E7D2802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E85CC7-547B-4BEF-AA16-7F0AABC209FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2142,7 +2142,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2719,6 +2719,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3472,8 +3475,8 @@
   <dimension ref="A1:S277"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -5141,11 +5144,11 @@
         <v>86</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F65" s="30" t="s">
         <v>394</v>
@@ -5482,7 +5485,7 @@
       <c r="A78" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="B78" s="49" t="s">
         <v>395</v>
       </c>
       <c r="D78" s="33"/>
@@ -5506,7 +5509,7 @@
     </row>
     <row r="79" spans="1:19">
       <c r="A79" s="8"/>
-      <c r="C79" s="31" t="s">
+      <c r="B79" s="31" t="s">
         <v>396</v>
       </c>
       <c r="D79" s="15"/>
@@ -5530,8 +5533,8 @@
     </row>
     <row r="80" spans="1:19">
       <c r="A80" s="8"/>
-      <c r="C80" s="31" t="s">
-        <v>84</v>
+      <c r="B80" s="31" t="s">
+        <v>83</v>
       </c>
       <c r="D80" s="15"/>
       <c r="E80" s="30" t="s">
@@ -5646,11 +5649,11 @@
       <c r="A84" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C84" s="45" t="s">
+      <c r="B84" s="45" t="s">
         <v>58</v>
       </c>
       <c r="D84" s="16"/>
-      <c r="E84" s="46" t="s">
+      <c r="E84" s="194" t="s">
         <v>59</v>
       </c>
       <c r="F84" s="3"/>
@@ -5670,7 +5673,7 @@
     </row>
     <row r="85" spans="1:19">
       <c r="A85" s="8"/>
-      <c r="C85" s="17" t="s">
+      <c r="B85" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D85" s="8"/>
@@ -5694,12 +5697,12 @@
     </row>
     <row r="86" spans="1:19">
       <c r="A86" s="8"/>
-      <c r="C86" s="17" t="s">
-        <v>84</v>
+      <c r="B86" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="D86" s="8"/>
-      <c r="E86" s="18" t="s">
-        <v>84</v>
+      <c r="E86" s="30" t="s">
+        <v>394</v>
       </c>
       <c r="F86" s="27"/>
       <c r="G86" s="2"/>

</xml_diff>

<commit_message>
220711-v1 temp with xlsx
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E85CC7-547B-4BEF-AA16-7F0AABC209FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D105DBC-F832-4B41-81AC-D8D7077A63BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
@@ -3474,9 +3474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10160,7 +10160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="AQ1" sqref="AQ1:AU1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
220711 OK for impl
</commit_message>
<xml_diff>
--- a/EKF-SLAMv5.0运算统计.xlsx
+++ b/EKF-SLAMv5.0运算统计.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DigitalLAB\A_EKF_SLAM\EKF_SLAM_RTL\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D105DBC-F832-4B41-81AC-D8D7077A63BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46CBAA9-E274-4144-BD69-3907387F3C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="矩阵运算" sheetId="2" r:id="rId1"/>
     <sheet name="数据关联" sheetId="3" r:id="rId2"/>
     <sheet name="TEMP_BANK" sheetId="4" r:id="rId3"/>
     <sheet name="COV_BANK" sheetId="6" r:id="rId4"/>
-    <sheet name="(old)COV_BANK" sheetId="5" r:id="rId5"/>
+    <sheet name="COV_example" sheetId="7" r:id="rId5"/>
+    <sheet name="(old)COV_BANK" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="425">
   <si>
     <t>步骤</t>
   </si>
@@ -1475,12 +1476,29 @@
     <t>cov_HT(0,2)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>hat_state</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>hat_sigma</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>BANK2</t>
+  </si>
+  <si>
+    <t>BANK3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0000000_ "/>
+  </numFmts>
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1568,6 +1586,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1679,7 +1713,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -2136,13 +2170,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2691,6 +2736,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2712,17 +2769,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5653,7 +5737,7 @@
         <v>58</v>
       </c>
       <c r="D84" s="16"/>
-      <c r="E84" s="194" t="s">
+      <c r="E84" s="187" t="s">
         <v>59</v>
       </c>
       <c r="F84" s="3"/>
@@ -6096,11 +6180,11 @@
     </row>
     <row r="100" spans="1:19" ht="14.25" thickBot="1">
       <c r="A100" s="9"/>
-      <c r="B100" s="184" t="s">
+      <c r="B100" s="188" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="185"/>
-      <c r="D100" s="185"/>
+      <c r="C100" s="189"/>
+      <c r="D100" s="189"/>
       <c r="E100" s="64" t="s">
         <v>100</v>
       </c>
@@ -10160,7 +10244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE525808-D087-4D79-9C47-22478BDACE0A}">
   <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+    <sheetView topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="AQ1" sqref="AQ1:AU1"/>
     </sheetView>
   </sheetViews>
@@ -10651,75 +10735,75 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="190" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="188"/>
-      <c r="E6" s="186" t="s">
+      <c r="C6" s="191"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="190" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="187"/>
-      <c r="G6" s="188"/>
-      <c r="H6" s="189"/>
-      <c r="I6" s="190"/>
-      <c r="J6" s="190"/>
-      <c r="K6" s="190" t="s">
+      <c r="F6" s="191"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="194"/>
+      <c r="K6" s="194" t="s">
         <v>148</v>
       </c>
-      <c r="L6" s="190"/>
-      <c r="M6" s="190"/>
+      <c r="L6" s="194"/>
+      <c r="M6" s="194"/>
     </row>
     <row r="7" spans="1:47" ht="14.25" thickBot="1">
-      <c r="B7" s="186" t="s">
+      <c r="B7" s="190" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="187"/>
-      <c r="D7" s="187"/>
-      <c r="E7" s="187"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="187"/>
-      <c r="H7" s="187"/>
-      <c r="I7" s="187"/>
-      <c r="J7" s="187"/>
-      <c r="K7" s="187"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="188"/>
-      <c r="Q7" s="186" t="s">
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
+      <c r="O7" s="191"/>
+      <c r="P7" s="192"/>
+      <c r="Q7" s="190" t="s">
         <v>176</v>
       </c>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="187"/>
-      <c r="X7" s="187"/>
-      <c r="Y7" s="187"/>
-      <c r="Z7" s="187"/>
-      <c r="AA7" s="188"/>
-      <c r="AB7" s="186" t="s">
+      <c r="R7" s="191"/>
+      <c r="S7" s="191"/>
+      <c r="T7" s="191"/>
+      <c r="U7" s="191"/>
+      <c r="V7" s="191"/>
+      <c r="W7" s="191"/>
+      <c r="X7" s="191"/>
+      <c r="Y7" s="191"/>
+      <c r="Z7" s="191"/>
+      <c r="AA7" s="192"/>
+      <c r="AB7" s="190" t="s">
         <v>177</v>
       </c>
-      <c r="AC7" s="187"/>
-      <c r="AD7" s="187"/>
-      <c r="AE7" s="187"/>
-      <c r="AF7" s="187"/>
-      <c r="AG7" s="187"/>
-      <c r="AH7" s="187"/>
-      <c r="AI7" s="187"/>
-      <c r="AJ7" s="187"/>
-      <c r="AK7" s="187"/>
-      <c r="AL7" s="187"/>
-      <c r="AM7" s="187"/>
-      <c r="AN7" s="187"/>
-      <c r="AO7" s="187"/>
-      <c r="AP7" s="187"/>
-      <c r="AQ7" s="187"/>
-      <c r="AR7" s="188"/>
+      <c r="AC7" s="191"/>
+      <c r="AD7" s="191"/>
+      <c r="AE7" s="191"/>
+      <c r="AF7" s="191"/>
+      <c r="AG7" s="191"/>
+      <c r="AH7" s="191"/>
+      <c r="AI7" s="191"/>
+      <c r="AJ7" s="191"/>
+      <c r="AK7" s="191"/>
+      <c r="AL7" s="191"/>
+      <c r="AM7" s="191"/>
+      <c r="AN7" s="191"/>
+      <c r="AO7" s="191"/>
+      <c r="AP7" s="191"/>
+      <c r="AQ7" s="191"/>
+      <c r="AR7" s="192"/>
     </row>
     <row r="9" spans="1:47">
       <c r="E9" s="39"/>
@@ -10770,7 +10854,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:C21"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>
@@ -10806,12 +10890,12 @@
       <c r="J1" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="M1" s="191"/>
-      <c r="N1" s="191"/>
-      <c r="O1" s="191"/>
-      <c r="P1" s="191"/>
-      <c r="Q1" s="191"/>
-      <c r="R1" s="191"/>
+      <c r="M1" s="184"/>
+      <c r="N1" s="184"/>
+      <c r="O1" s="184"/>
+      <c r="P1" s="184"/>
+      <c r="Q1" s="184"/>
+      <c r="R1" s="184"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="132">
@@ -10837,12 +10921,12 @@
         <v>0</v>
       </c>
       <c r="J2" s="135"/>
-      <c r="M2" s="191"/>
-      <c r="N2" s="191"/>
-      <c r="O2" s="191"/>
-      <c r="P2" s="191"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="191"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="184"/>
+      <c r="O2" s="184"/>
+      <c r="P2" s="184"/>
+      <c r="Q2" s="185"/>
+      <c r="R2" s="184"/>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="132">
@@ -10868,12 +10952,12 @@
         <v>0</v>
       </c>
       <c r="J3" s="138"/>
-      <c r="M3" s="191"/>
-      <c r="N3" s="192"/>
-      <c r="O3" s="192"/>
-      <c r="P3" s="192"/>
-      <c r="Q3" s="192"/>
-      <c r="R3" s="191"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="185"/>
+      <c r="O3" s="185"/>
+      <c r="P3" s="185"/>
+      <c r="Q3" s="185"/>
+      <c r="R3" s="184"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="132">
@@ -10899,12 +10983,12 @@
         <v>1</v>
       </c>
       <c r="J4" s="140"/>
-      <c r="M4" s="191"/>
+      <c r="M4" s="184"/>
       <c r="N4" s="137"/>
       <c r="O4" s="137"/>
       <c r="P4" s="137"/>
       <c r="Q4" s="137"/>
-      <c r="R4" s="191"/>
+      <c r="R4" s="184"/>
     </row>
     <row r="5" spans="1:18" ht="14.25" thickBot="1">
       <c r="A5" s="132">
@@ -10930,12 +11014,12 @@
         <v>4</v>
       </c>
       <c r="J5" s="143"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="192"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="185"/>
       <c r="O5" s="137"/>
       <c r="P5" s="137"/>
       <c r="Q5" s="137"/>
-      <c r="R5" s="191"/>
+      <c r="R5" s="184"/>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="132">
@@ -10965,7 +11049,7 @@
       <c r="J6" s="133">
         <v>1</v>
       </c>
-      <c r="Q6" s="193"/>
+      <c r="Q6" s="186"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="132">
@@ -10995,7 +11079,7 @@
       <c r="J7" s="136">
         <v>2</v>
       </c>
-      <c r="Q7" s="193"/>
+      <c r="Q7" s="186"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="132">
@@ -12021,6 +12105,1500 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC085BC2-4F5E-4FDE-A992-D60BF52E4672}">
+  <dimension ref="A1:Y32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9"/>
+  <cols>
+    <col min="1" max="25" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="11.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="15">
+      <c r="B1" s="205" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+    </row>
+    <row r="2" spans="1:25" ht="14.25" thickBot="1">
+      <c r="B2" s="100">
+        <v>0</v>
+      </c>
+      <c r="C2" s="101">
+        <v>1</v>
+      </c>
+      <c r="D2" s="101">
+        <v>2</v>
+      </c>
+      <c r="E2" s="112">
+        <v>3</v>
+      </c>
+      <c r="F2" s="100">
+        <v>4</v>
+      </c>
+      <c r="G2" s="101">
+        <v>5</v>
+      </c>
+      <c r="H2" s="101">
+        <v>6</v>
+      </c>
+      <c r="I2" s="112">
+        <v>7</v>
+      </c>
+      <c r="J2" s="101">
+        <v>8</v>
+      </c>
+      <c r="K2" s="101">
+        <v>9</v>
+      </c>
+      <c r="L2" s="101">
+        <v>10</v>
+      </c>
+      <c r="M2" s="112">
+        <v>11</v>
+      </c>
+      <c r="N2" s="100">
+        <v>12</v>
+      </c>
+      <c r="O2" s="101">
+        <v>13</v>
+      </c>
+      <c r="P2" s="101">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="112">
+        <v>15</v>
+      </c>
+      <c r="R2" s="101">
+        <v>16</v>
+      </c>
+      <c r="S2" s="101">
+        <v>17</v>
+      </c>
+      <c r="T2" s="101">
+        <v>18</v>
+      </c>
+      <c r="U2" s="101">
+        <v>19</v>
+      </c>
+      <c r="V2" s="101">
+        <v>20</v>
+      </c>
+      <c r="W2" s="101">
+        <v>21</v>
+      </c>
+      <c r="X2" s="101">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="207">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="195">
+        <v>2.57066E-2</v>
+      </c>
+      <c r="C3" s="196">
+        <v>-1.43443E-3</v>
+      </c>
+      <c r="D3" s="196">
+        <v>1.14122E-4</v>
+      </c>
+      <c r="E3" s="197">
+        <v>1.52742E-16</v>
+      </c>
+      <c r="F3" s="195">
+        <v>1.66695E-2</v>
+      </c>
+      <c r="G3" s="196">
+        <v>-8.4224400000000002E-4</v>
+      </c>
+      <c r="H3" s="196">
+        <v>6.2616699999999996E-4</v>
+      </c>
+      <c r="I3" s="197">
+        <v>20.434100000000001</v>
+      </c>
+      <c r="J3" s="195">
+        <v>0.14232700000000001</v>
+      </c>
+      <c r="K3" s="196">
+        <v>9.18929E-2</v>
+      </c>
+      <c r="L3" s="196">
+        <v>1.10495E-2</v>
+      </c>
+      <c r="M3" s="197">
+        <v>1.2732800000000001E-2</v>
+      </c>
+      <c r="N3" s="195">
+        <v>1.60701E-2</v>
+      </c>
+      <c r="O3" s="196">
+        <v>2.8933600000000001E-4</v>
+      </c>
+      <c r="P3" s="196">
+        <v>-4.5249000000000001E-3</v>
+      </c>
+      <c r="Q3" s="197">
+        <v>27.1313</v>
+      </c>
+      <c r="R3" s="196">
+        <v>7.9215699999999993E-3</v>
+      </c>
+      <c r="S3" s="196">
+        <v>-6.7892999999999995E-2</v>
+      </c>
+      <c r="T3" s="196">
+        <v>1.95199E-2</v>
+      </c>
+      <c r="U3" s="197">
+        <v>-9.8136500000000002E-2</v>
+      </c>
+      <c r="V3" s="195">
+        <v>0.48695500000000003</v>
+      </c>
+      <c r="W3" s="196">
+        <v>-1.0168200000000001</v>
+      </c>
+      <c r="X3" s="196">
+        <v>2.8707E-2</v>
+      </c>
+      <c r="Y3" s="197">
+        <v>-3.8772599999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="199">
+        <v>-1.43443E-3</v>
+      </c>
+      <c r="C4" s="200">
+        <v>2.8123499999999999E-2</v>
+      </c>
+      <c r="D4" s="200">
+        <v>-2.1550399999999999E-4</v>
+      </c>
+      <c r="E4" s="204">
+        <v>-8.6733400000000004E-18</v>
+      </c>
+      <c r="F4" s="199">
+        <v>4.4881700000000001E-4</v>
+      </c>
+      <c r="G4" s="200">
+        <v>1.5610000000000001E-2</v>
+      </c>
+      <c r="H4" s="200">
+        <v>9.9144799999999998E-3</v>
+      </c>
+      <c r="I4" s="204">
+        <v>-1.1603399999999999</v>
+      </c>
+      <c r="J4" s="199">
+        <v>9.18929E-2</v>
+      </c>
+      <c r="K4" s="200">
+        <v>1.75088</v>
+      </c>
+      <c r="L4" s="200">
+        <v>-1.6714099999999999E-2</v>
+      </c>
+      <c r="M4" s="204">
+        <v>0.22678000000000001</v>
+      </c>
+      <c r="N4" s="199">
+        <v>8.3126599999999999E-4</v>
+      </c>
+      <c r="O4" s="200">
+        <v>1.48886E-2</v>
+      </c>
+      <c r="P4" s="200">
+        <v>1.3199199999999999E-2</v>
+      </c>
+      <c r="Q4" s="204">
+        <v>9.3420699999999997</v>
+      </c>
+      <c r="R4" s="200">
+        <v>1.16696E-2</v>
+      </c>
+      <c r="S4" s="200">
+        <v>0.20938100000000001</v>
+      </c>
+      <c r="T4" s="200">
+        <v>-2.2115300000000001E-2</v>
+      </c>
+      <c r="U4" s="204">
+        <v>0.29747800000000002</v>
+      </c>
+      <c r="V4" s="199">
+        <v>-1.0168200000000001</v>
+      </c>
+      <c r="W4" s="200">
+        <v>3.0904400000000001</v>
+      </c>
+      <c r="X4" s="200">
+        <v>-4.8876299999999998E-2</v>
+      </c>
+      <c r="Y4" s="204">
+        <v>0.124556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B5" s="199">
+        <v>1.14122E-4</v>
+      </c>
+      <c r="C5" s="200">
+        <v>-2.1550399999999999E-4</v>
+      </c>
+      <c r="D5" s="200">
+        <v>7.5246600000000003E-4</v>
+      </c>
+      <c r="E5" s="204">
+        <v>0.62831899999999996</v>
+      </c>
+      <c r="F5" s="199">
+        <v>1.6470700000000001E-2</v>
+      </c>
+      <c r="G5" s="200">
+        <v>-4.6690499999999999E-4</v>
+      </c>
+      <c r="H5" s="200">
+        <v>-1.0823199999999999E-3</v>
+      </c>
+      <c r="I5" s="204">
+        <v>29.517399999999999</v>
+      </c>
+      <c r="J5" s="199">
+        <v>1.10495E-2</v>
+      </c>
+      <c r="K5" s="200">
+        <v>-1.6714099999999999E-2</v>
+      </c>
+      <c r="L5" s="200">
+        <v>0.158638</v>
+      </c>
+      <c r="M5" s="204">
+        <v>-0.27535999999999999</v>
+      </c>
+      <c r="N5" s="199">
+        <v>1.63132E-2</v>
+      </c>
+      <c r="O5" s="200">
+        <v>-1.6958399999999999E-4</v>
+      </c>
+      <c r="P5" s="200">
+        <v>-2.4356099999999999E-3</v>
+      </c>
+      <c r="Q5" s="204">
+        <v>11.6883</v>
+      </c>
+      <c r="R5" s="200">
+        <v>9.8198899999999995E-3</v>
+      </c>
+      <c r="S5" s="200">
+        <v>-3.6832700000000003E-2</v>
+      </c>
+      <c r="T5" s="200">
+        <v>1.6084299999999999E-2</v>
+      </c>
+      <c r="U5" s="204">
+        <v>-5.3167600000000002E-2</v>
+      </c>
+      <c r="V5" s="199">
+        <v>2.8707E-2</v>
+      </c>
+      <c r="W5" s="200">
+        <v>-4.8876299999999998E-2</v>
+      </c>
+      <c r="X5" s="200">
+        <v>0.224522</v>
+      </c>
+      <c r="Y5" s="204">
+        <v>-0.20158300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="14.25" thickBot="1">
+      <c r="A6" t="s">
+        <v>424</v>
+      </c>
+      <c r="B6" s="201">
+        <v>0</v>
+      </c>
+      <c r="C6" s="202">
+        <v>0</v>
+      </c>
+      <c r="D6" s="202">
+        <v>0</v>
+      </c>
+      <c r="E6" s="203">
+        <v>0</v>
+      </c>
+      <c r="F6" s="201">
+        <v>9.6713300000000001E-4</v>
+      </c>
+      <c r="G6" s="202">
+        <v>1.46312E-2</v>
+      </c>
+      <c r="H6" s="202">
+        <v>1.43695E-2</v>
+      </c>
+      <c r="I6" s="203">
+        <v>2.3230599999999999</v>
+      </c>
+      <c r="J6" s="201">
+        <v>1.2732800000000001E-2</v>
+      </c>
+      <c r="K6" s="202">
+        <v>0.22678000000000001</v>
+      </c>
+      <c r="L6" s="202">
+        <v>-0.27535999999999999</v>
+      </c>
+      <c r="M6" s="203">
+        <v>3.641</v>
+      </c>
+      <c r="N6" s="201">
+        <v>-5.01223E-5</v>
+      </c>
+      <c r="O6" s="202">
+        <v>1.6552399999999998E-2</v>
+      </c>
+      <c r="P6" s="202">
+        <v>5.6249200000000003E-3</v>
+      </c>
+      <c r="Q6" s="203">
+        <v>5.0822099999999999</v>
+      </c>
+      <c r="R6" s="202">
+        <v>4.7876000000000004E-3</v>
+      </c>
+      <c r="S6" s="202">
+        <v>9.6779500000000004E-2</v>
+      </c>
+      <c r="T6" s="202">
+        <v>-9.6602500000000004E-3</v>
+      </c>
+      <c r="U6" s="203">
+        <v>0.13445299999999999</v>
+      </c>
+      <c r="V6" s="201">
+        <v>-3.8772599999999997E-2</v>
+      </c>
+      <c r="W6" s="202">
+        <v>0.124556</v>
+      </c>
+      <c r="X6" s="202">
+        <v>-0.20158300000000001</v>
+      </c>
+      <c r="Y6" s="203">
+        <v>0.60057300000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="14.25" thickBot="1"/>
+    <row r="13" spans="1:25">
+      <c r="A13" t="s">
+        <v>421</v>
+      </c>
+      <c r="D13" s="195" t="s">
+        <v>422</v>
+      </c>
+      <c r="E13" s="196"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="197"/>
+      <c r="H13" s="198"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="198"/>
+      <c r="L13" s="198"/>
+      <c r="M13" s="198"/>
+      <c r="N13" s="198"/>
+      <c r="O13" s="198"/>
+      <c r="P13" s="198"/>
+      <c r="Q13" s="198"/>
+      <c r="R13" s="198"/>
+      <c r="S13" s="198"/>
+      <c r="T13" s="198"/>
+      <c r="U13" s="198"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="D14" s="100">
+        <v>0</v>
+      </c>
+      <c r="E14" s="101">
+        <v>1</v>
+      </c>
+      <c r="F14" s="101">
+        <v>2</v>
+      </c>
+      <c r="G14" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="198">
+        <v>1.52742E-16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="199">
+        <v>2.57066E-2</v>
+      </c>
+      <c r="E15" s="200">
+        <v>-1.43443E-3</v>
+      </c>
+      <c r="F15" s="200">
+        <v>1.14122E-4</v>
+      </c>
+      <c r="G15" s="198">
+        <v>1.52742E-16</v>
+      </c>
+      <c r="H15" s="198">
+        <v>1.66695E-2</v>
+      </c>
+      <c r="I15" s="198">
+        <v>4.4881700000000001E-4</v>
+      </c>
+      <c r="J15" s="198">
+        <v>1.6470700000000001E-2</v>
+      </c>
+      <c r="K15" s="198">
+        <v>9.6713300000000001E-4</v>
+      </c>
+      <c r="L15" s="198">
+        <v>1.60701E-2</v>
+      </c>
+      <c r="M15" s="198">
+        <v>8.3126599999999999E-4</v>
+      </c>
+      <c r="N15" s="198">
+        <v>1.63132E-2</v>
+      </c>
+      <c r="O15" s="198">
+        <v>-5.01223E-5</v>
+      </c>
+      <c r="P15" s="198">
+        <v>1.5893600000000001E-2</v>
+      </c>
+      <c r="Q15" s="198">
+        <v>4.52232E-4</v>
+      </c>
+      <c r="R15" s="198">
+        <v>1.5532199999999999E-2</v>
+      </c>
+      <c r="S15" s="198">
+        <v>1.89476E-4</v>
+      </c>
+      <c r="T15" s="198">
+        <v>1.6008399999999999E-2</v>
+      </c>
+      <c r="U15" s="198">
+        <v>-3.0460099999999999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="198">
+        <v>-8.6733400000000004E-18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="199">
+        <v>-1.43443E-3</v>
+      </c>
+      <c r="E16" s="200">
+        <v>2.8123499999999999E-2</v>
+      </c>
+      <c r="F16" s="200">
+        <v>-2.1550399999999999E-4</v>
+      </c>
+      <c r="G16" s="198">
+        <v>-8.6733400000000004E-18</v>
+      </c>
+      <c r="H16" s="198">
+        <v>-8.4224400000000002E-4</v>
+      </c>
+      <c r="I16" s="198">
+        <v>1.5610000000000001E-2</v>
+      </c>
+      <c r="J16" s="198">
+        <v>-4.6690499999999999E-4</v>
+      </c>
+      <c r="K16" s="198">
+        <v>1.46312E-2</v>
+      </c>
+      <c r="L16" s="198">
+        <v>2.8933600000000001E-4</v>
+      </c>
+      <c r="M16" s="198">
+        <v>1.48886E-2</v>
+      </c>
+      <c r="N16" s="198">
+        <v>-1.6958399999999999E-4</v>
+      </c>
+      <c r="O16" s="198">
+        <v>1.6552399999999998E-2</v>
+      </c>
+      <c r="P16" s="198">
+        <v>6.2245499999999995E-4</v>
+      </c>
+      <c r="Q16" s="198">
+        <v>1.5604099999999999E-2</v>
+      </c>
+      <c r="R16" s="198">
+        <v>1.3045999999999999E-3</v>
+      </c>
+      <c r="S16" s="198">
+        <v>1.6100199999999999E-2</v>
+      </c>
+      <c r="T16" s="198">
+        <v>4.05652E-4</v>
+      </c>
+      <c r="U16" s="198">
+        <v>1.7032800000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="198">
+        <v>0.62831899999999996</v>
+      </c>
+      <c r="C17" t="s">
+        <v>423</v>
+      </c>
+      <c r="D17" s="199">
+        <v>1.14122E-4</v>
+      </c>
+      <c r="E17" s="200">
+        <v>-2.1550399999999999E-4</v>
+      </c>
+      <c r="F17" s="200">
+        <v>7.5246600000000003E-4</v>
+      </c>
+      <c r="G17" s="198">
+        <v>0.62831899999999996</v>
+      </c>
+      <c r="H17" s="198">
+        <v>6.2616699999999996E-4</v>
+      </c>
+      <c r="I17" s="198">
+        <v>9.9144799999999998E-3</v>
+      </c>
+      <c r="J17" s="198">
+        <v>-1.0823199999999999E-3</v>
+      </c>
+      <c r="K17" s="198">
+        <v>1.43695E-2</v>
+      </c>
+      <c r="L17" s="198">
+        <v>-4.5249000000000001E-3</v>
+      </c>
+      <c r="M17" s="198">
+        <v>1.3199199999999999E-2</v>
+      </c>
+      <c r="N17" s="198">
+        <v>-2.4356099999999999E-3</v>
+      </c>
+      <c r="O17" s="198">
+        <v>5.6249200000000003E-3</v>
+      </c>
+      <c r="P17" s="198">
+        <v>-6.0412199999999999E-3</v>
+      </c>
+      <c r="Q17" s="198">
+        <v>9.9418400000000004E-3</v>
+      </c>
+      <c r="R17" s="198">
+        <v>-9.1472800000000007E-3</v>
+      </c>
+      <c r="S17" s="198">
+        <v>7.6842500000000001E-3</v>
+      </c>
+      <c r="T17" s="198">
+        <v>-5.0545E-3</v>
+      </c>
+      <c r="U17" s="198">
+        <v>3.4382100000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="14.25" thickBot="1">
+      <c r="A18" s="198"/>
+      <c r="C18" t="s">
+        <v>424</v>
+      </c>
+      <c r="D18" s="201">
+        <v>0</v>
+      </c>
+      <c r="E18" s="202">
+        <v>0</v>
+      </c>
+      <c r="F18" s="202">
+        <v>0</v>
+      </c>
+      <c r="G18" s="203">
+        <v>0</v>
+      </c>
+      <c r="H18" s="198"/>
+      <c r="I18" s="198"/>
+      <c r="J18" s="198"/>
+      <c r="K18" s="198"/>
+      <c r="L18" s="198"/>
+      <c r="M18" s="198"/>
+      <c r="N18" s="198"/>
+      <c r="O18" s="198"/>
+      <c r="P18" s="198"/>
+      <c r="Q18" s="198"/>
+      <c r="R18" s="198"/>
+      <c r="S18" s="198"/>
+      <c r="T18" s="198"/>
+      <c r="U18" s="198"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="198">
+        <v>20.434100000000001</v>
+      </c>
+      <c r="D19" s="195">
+        <v>1.66695E-2</v>
+      </c>
+      <c r="E19" s="196">
+        <v>-8.4224400000000002E-4</v>
+      </c>
+      <c r="F19" s="196">
+        <v>6.2616699999999996E-4</v>
+      </c>
+      <c r="G19" s="198">
+        <v>20.434100000000001</v>
+      </c>
+      <c r="H19" s="195">
+        <v>0.14232700000000001</v>
+      </c>
+      <c r="I19" s="196">
+        <v>9.18929E-2</v>
+      </c>
+      <c r="J19" s="196">
+        <v>1.10495E-2</v>
+      </c>
+      <c r="K19" s="197">
+        <v>1.2732800000000001E-2</v>
+      </c>
+      <c r="L19" s="198">
+        <v>7.9215699999999993E-3</v>
+      </c>
+      <c r="M19" s="198">
+        <v>1.16696E-2</v>
+      </c>
+      <c r="N19" s="198">
+        <v>9.8198899999999995E-3</v>
+      </c>
+      <c r="O19" s="198">
+        <v>4.7876000000000004E-3</v>
+      </c>
+      <c r="P19" s="198">
+        <v>6.5438299999999996E-3</v>
+      </c>
+      <c r="Q19" s="198">
+        <v>8.7099699999999992E-3</v>
+      </c>
+      <c r="R19" s="198">
+        <v>3.7216699999999998E-3</v>
+      </c>
+      <c r="S19" s="198">
+        <v>6.6586900000000001E-3</v>
+      </c>
+      <c r="T19" s="198">
+        <v>7.4403500000000001E-3</v>
+      </c>
+      <c r="U19" s="198">
+        <v>2.8007399999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="198">
+        <v>-1.1603399999999999</v>
+      </c>
+      <c r="D20" s="199">
+        <v>4.4881700000000001E-4</v>
+      </c>
+      <c r="E20" s="200">
+        <v>1.5610000000000001E-2</v>
+      </c>
+      <c r="F20" s="200">
+        <v>9.9144799999999998E-3</v>
+      </c>
+      <c r="G20" s="198">
+        <v>-1.1603399999999999</v>
+      </c>
+      <c r="H20" s="199">
+        <v>9.18929E-2</v>
+      </c>
+      <c r="I20" s="200">
+        <v>1.75088</v>
+      </c>
+      <c r="J20" s="200">
+        <v>-1.6714099999999999E-2</v>
+      </c>
+      <c r="K20" s="204">
+        <v>0.22678000000000001</v>
+      </c>
+      <c r="L20" s="198">
+        <v>-6.7892999999999995E-2</v>
+      </c>
+      <c r="M20" s="198">
+        <v>0.20938100000000001</v>
+      </c>
+      <c r="N20" s="198">
+        <v>-3.6832700000000003E-2</v>
+      </c>
+      <c r="O20" s="198">
+        <v>9.6779500000000004E-2</v>
+      </c>
+      <c r="P20" s="198">
+        <v>-9.0435299999999996E-2</v>
+      </c>
+      <c r="Q20" s="198">
+        <v>0.16095699999999999</v>
+      </c>
+      <c r="R20" s="198">
+        <v>-0.13661100000000001</v>
+      </c>
+      <c r="S20" s="198">
+        <v>0.12739400000000001</v>
+      </c>
+      <c r="T20" s="198">
+        <v>-7.5766299999999995E-2</v>
+      </c>
+      <c r="U20" s="198">
+        <v>6.4270900000000006E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="198">
+        <v>29.517399999999999</v>
+      </c>
+      <c r="D21" s="199">
+        <v>1.6470700000000001E-2</v>
+      </c>
+      <c r="E21" s="200">
+        <v>-4.6690499999999999E-4</v>
+      </c>
+      <c r="F21" s="200">
+        <v>-1.0823199999999999E-3</v>
+      </c>
+      <c r="G21" s="198">
+        <v>29.517399999999999</v>
+      </c>
+      <c r="H21" s="199">
+        <v>1.10495E-2</v>
+      </c>
+      <c r="I21" s="200">
+        <v>-1.6714099999999999E-2</v>
+      </c>
+      <c r="J21" s="200">
+        <v>0.158638</v>
+      </c>
+      <c r="K21" s="204">
+        <v>-0.27535999999999999</v>
+      </c>
+      <c r="L21" s="198">
+        <v>1.95199E-2</v>
+      </c>
+      <c r="M21" s="198">
+        <v>-2.2115300000000001E-2</v>
+      </c>
+      <c r="N21" s="198">
+        <v>1.6084299999999999E-2</v>
+      </c>
+      <c r="O21" s="198">
+        <v>-9.6602500000000004E-3</v>
+      </c>
+      <c r="P21" s="198">
+        <v>2.20133E-2</v>
+      </c>
+      <c r="Q21" s="198">
+        <v>-1.6759E-2</v>
+      </c>
+      <c r="R21" s="198">
+        <v>2.7120999999999999E-2</v>
+      </c>
+      <c r="S21" s="198">
+        <v>-1.30466E-2</v>
+      </c>
+      <c r="T21" s="198">
+        <v>2.0390800000000001E-2</v>
+      </c>
+      <c r="U21" s="198">
+        <v>-6.0644399999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="14.25" thickBot="1">
+      <c r="A22" s="198">
+        <v>2.3230599999999999</v>
+      </c>
+      <c r="D22" s="201">
+        <v>9.6713300000000001E-4</v>
+      </c>
+      <c r="E22" s="202">
+        <v>1.46312E-2</v>
+      </c>
+      <c r="F22" s="202">
+        <v>1.43695E-2</v>
+      </c>
+      <c r="G22" s="198">
+        <v>2.3230599999999999</v>
+      </c>
+      <c r="H22" s="201">
+        <v>1.2732800000000001E-2</v>
+      </c>
+      <c r="I22" s="202">
+        <v>0.22678000000000001</v>
+      </c>
+      <c r="J22" s="202">
+        <v>-0.27535999999999999</v>
+      </c>
+      <c r="K22" s="203">
+        <v>3.641</v>
+      </c>
+      <c r="L22" s="198">
+        <v>-9.8136500000000002E-2</v>
+      </c>
+      <c r="M22" s="198">
+        <v>0.29747800000000002</v>
+      </c>
+      <c r="N22" s="198">
+        <v>-5.3167600000000002E-2</v>
+      </c>
+      <c r="O22" s="198">
+        <v>0.13445299999999999</v>
+      </c>
+      <c r="P22" s="198">
+        <v>-0.130773</v>
+      </c>
+      <c r="Q22" s="198">
+        <v>0.22736899999999999</v>
+      </c>
+      <c r="R22" s="198">
+        <v>-0.197627</v>
+      </c>
+      <c r="S22" s="198">
+        <v>0.17877699999999999</v>
+      </c>
+      <c r="T22" s="198">
+        <v>-0.10953499999999999</v>
+      </c>
+      <c r="U22" s="198">
+        <v>8.7387500000000007E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="198">
+        <v>27.1313</v>
+      </c>
+      <c r="D23" s="195">
+        <v>1.60701E-2</v>
+      </c>
+      <c r="E23" s="196">
+        <v>2.8933600000000001E-4</v>
+      </c>
+      <c r="F23" s="196">
+        <v>-4.5249000000000001E-3</v>
+      </c>
+      <c r="G23" s="198">
+        <v>27.1313</v>
+      </c>
+      <c r="H23" s="195">
+        <v>7.9215699999999993E-3</v>
+      </c>
+      <c r="I23" s="196">
+        <v>-6.7892999999999995E-2</v>
+      </c>
+      <c r="J23" s="196">
+        <v>1.95199E-2</v>
+      </c>
+      <c r="K23" s="197">
+        <v>-9.8136500000000002E-2</v>
+      </c>
+      <c r="L23" s="195">
+        <v>0.48695500000000003</v>
+      </c>
+      <c r="M23" s="196">
+        <v>-1.0168200000000001</v>
+      </c>
+      <c r="N23" s="196">
+        <v>2.8707E-2</v>
+      </c>
+      <c r="O23" s="197">
+        <v>-3.8772599999999997E-2</v>
+      </c>
+      <c r="P23" s="198">
+        <v>5.3184200000000001E-2</v>
+      </c>
+      <c r="Q23" s="198">
+        <v>-6.8078700000000006E-2</v>
+      </c>
+      <c r="R23" s="198">
+        <v>7.4270199999999995E-2</v>
+      </c>
+      <c r="S23" s="198">
+        <v>-5.2752599999999997E-2</v>
+      </c>
+      <c r="T23" s="198">
+        <v>4.6485699999999998E-2</v>
+      </c>
+      <c r="U23" s="198">
+        <v>-2.39277E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="198">
+        <v>9.3420699999999997</v>
+      </c>
+      <c r="D24" s="199">
+        <v>8.3126599999999999E-4</v>
+      </c>
+      <c r="E24" s="200">
+        <v>1.48886E-2</v>
+      </c>
+      <c r="F24" s="200">
+        <v>1.3199199999999999E-2</v>
+      </c>
+      <c r="G24" s="198">
+        <v>9.3420699999999997</v>
+      </c>
+      <c r="H24" s="199">
+        <v>1.16696E-2</v>
+      </c>
+      <c r="I24" s="200">
+        <v>0.20938100000000001</v>
+      </c>
+      <c r="J24" s="200">
+        <v>-2.2115300000000001E-2</v>
+      </c>
+      <c r="K24" s="204">
+        <v>0.29747800000000002</v>
+      </c>
+      <c r="L24" s="199">
+        <v>-1.0168200000000001</v>
+      </c>
+      <c r="M24" s="200">
+        <v>3.0904400000000001</v>
+      </c>
+      <c r="N24" s="200">
+        <v>-4.8876299999999998E-2</v>
+      </c>
+      <c r="O24" s="204">
+        <v>0.124556</v>
+      </c>
+      <c r="P24" s="198">
+        <v>-0.12017600000000001</v>
+      </c>
+      <c r="Q24" s="198">
+        <v>0.209923</v>
+      </c>
+      <c r="R24" s="198">
+        <v>-0.18159800000000001</v>
+      </c>
+      <c r="S24" s="198">
+        <v>0.16527900000000001</v>
+      </c>
+      <c r="T24" s="198">
+        <v>-0.100664</v>
+      </c>
+      <c r="U24" s="198">
+        <v>8.1314899999999996E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="198">
+        <v>11.6883</v>
+      </c>
+      <c r="D25" s="199">
+        <v>1.63132E-2</v>
+      </c>
+      <c r="E25" s="200">
+        <v>-1.6958399999999999E-4</v>
+      </c>
+      <c r="F25" s="200">
+        <v>-2.4356099999999999E-3</v>
+      </c>
+      <c r="G25" s="198">
+        <v>11.6883</v>
+      </c>
+      <c r="H25" s="199">
+        <v>9.8198899999999995E-3</v>
+      </c>
+      <c r="I25" s="200">
+        <v>-3.6832700000000003E-2</v>
+      </c>
+      <c r="J25" s="200">
+        <v>1.6084299999999999E-2</v>
+      </c>
+      <c r="K25" s="204">
+        <v>-5.3167600000000002E-2</v>
+      </c>
+      <c r="L25" s="199">
+        <v>2.8707E-2</v>
+      </c>
+      <c r="M25" s="200">
+        <v>-4.8876299999999998E-2</v>
+      </c>
+      <c r="N25" s="200">
+        <v>0.224522</v>
+      </c>
+      <c r="O25" s="204">
+        <v>-0.20158300000000001</v>
+      </c>
+      <c r="P25" s="198">
+        <v>3.4266699999999997E-2</v>
+      </c>
+      <c r="Q25" s="198">
+        <v>-3.6933000000000001E-2</v>
+      </c>
+      <c r="R25" s="198">
+        <v>4.5655500000000002E-2</v>
+      </c>
+      <c r="S25" s="198">
+        <v>-2.8655199999999999E-2</v>
+      </c>
+      <c r="T25" s="198">
+        <v>3.06488E-2</v>
+      </c>
+      <c r="U25" s="198">
+        <v>-1.30866E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="14.25" thickBot="1">
+      <c r="A26" s="198">
+        <v>5.0822099999999999</v>
+      </c>
+      <c r="D26" s="201">
+        <v>-5.01223E-5</v>
+      </c>
+      <c r="E26" s="202">
+        <v>1.6552399999999998E-2</v>
+      </c>
+      <c r="F26" s="202">
+        <v>5.6249200000000003E-3</v>
+      </c>
+      <c r="G26" s="198">
+        <v>5.0822099999999999</v>
+      </c>
+      <c r="H26" s="201">
+        <v>4.7876000000000004E-3</v>
+      </c>
+      <c r="I26" s="202">
+        <v>9.6779500000000004E-2</v>
+      </c>
+      <c r="J26" s="202">
+        <v>-9.6602500000000004E-3</v>
+      </c>
+      <c r="K26" s="203">
+        <v>0.13445299999999999</v>
+      </c>
+      <c r="L26" s="201">
+        <v>-3.8772599999999997E-2</v>
+      </c>
+      <c r="M26" s="202">
+        <v>0.124556</v>
+      </c>
+      <c r="N26" s="202">
+        <v>-0.20158300000000001</v>
+      </c>
+      <c r="O26" s="203">
+        <v>0.60057300000000002</v>
+      </c>
+      <c r="P26" s="198">
+        <v>-5.15954E-2</v>
+      </c>
+      <c r="Q26" s="198">
+        <v>9.7011E-2</v>
+      </c>
+      <c r="R26" s="198">
+        <v>-7.7862000000000001E-2</v>
+      </c>
+      <c r="S26" s="198">
+        <v>7.7919600000000006E-2</v>
+      </c>
+      <c r="T26" s="198">
+        <v>-4.3251199999999997E-2</v>
+      </c>
+      <c r="U26" s="198">
+        <v>4.2012800000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="198">
+        <v>20.49</v>
+      </c>
+      <c r="D27" s="198">
+        <v>1.5893600000000001E-2</v>
+      </c>
+      <c r="E27" s="198">
+        <v>6.2245499999999995E-4</v>
+      </c>
+      <c r="F27" s="198">
+        <v>-6.0412199999999999E-3</v>
+      </c>
+      <c r="G27" s="198">
+        <v>20.49</v>
+      </c>
+      <c r="H27" s="198">
+        <v>6.5438299999999996E-3</v>
+      </c>
+      <c r="I27" s="198">
+        <v>-9.0435299999999996E-2</v>
+      </c>
+      <c r="J27" s="198">
+        <v>2.20133E-2</v>
+      </c>
+      <c r="K27" s="198">
+        <v>-0.130773</v>
+      </c>
+      <c r="L27" s="198">
+        <v>5.3184200000000001E-2</v>
+      </c>
+      <c r="M27" s="198">
+        <v>-0.12017600000000001</v>
+      </c>
+      <c r="N27" s="198">
+        <v>3.4266699999999997E-2</v>
+      </c>
+      <c r="O27" s="198">
+        <v>-5.15954E-2</v>
+      </c>
+      <c r="P27" s="198">
+        <v>0.74693200000000004</v>
+      </c>
+      <c r="Q27" s="198">
+        <v>-1.00532</v>
+      </c>
+      <c r="R27" s="198">
+        <v>9.50376E-2</v>
+      </c>
+      <c r="S27" s="198">
+        <v>-7.0241499999999998E-2</v>
+      </c>
+      <c r="T27" s="198">
+        <v>5.7979500000000003E-2</v>
+      </c>
+      <c r="U27" s="198">
+        <v>-3.1795799999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="198">
+        <v>12.4336</v>
+      </c>
+      <c r="D28" s="198">
+        <v>4.52232E-4</v>
+      </c>
+      <c r="E28" s="198">
+        <v>1.5604099999999999E-2</v>
+      </c>
+      <c r="F28" s="198">
+        <v>9.9418400000000004E-3</v>
+      </c>
+      <c r="G28" s="198">
+        <v>12.4336</v>
+      </c>
+      <c r="H28" s="198">
+        <v>8.7099699999999992E-3</v>
+      </c>
+      <c r="I28" s="198">
+        <v>0.16095699999999999</v>
+      </c>
+      <c r="J28" s="198">
+        <v>-1.6759E-2</v>
+      </c>
+      <c r="K28" s="198">
+        <v>0.22736899999999999</v>
+      </c>
+      <c r="L28" s="198">
+        <v>-6.8078700000000006E-2</v>
+      </c>
+      <c r="M28" s="198">
+        <v>0.209923</v>
+      </c>
+      <c r="N28" s="198">
+        <v>-3.6933000000000001E-2</v>
+      </c>
+      <c r="O28" s="198">
+        <v>9.7011E-2</v>
+      </c>
+      <c r="P28" s="198">
+        <v>-1.00532</v>
+      </c>
+      <c r="Q28" s="198">
+        <v>1.7936300000000001</v>
+      </c>
+      <c r="R28" s="198">
+        <v>-0.136986</v>
+      </c>
+      <c r="S28" s="198">
+        <v>0.12770999999999999</v>
+      </c>
+      <c r="T28" s="198">
+        <v>-7.5973700000000005E-2</v>
+      </c>
+      <c r="U28" s="198">
+        <v>6.4412999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="198">
+        <v>15.887</v>
+      </c>
+      <c r="D29" s="198">
+        <v>1.5532199999999999E-2</v>
+      </c>
+      <c r="E29" s="198">
+        <v>1.3045999999999999E-3</v>
+      </c>
+      <c r="F29" s="198">
+        <v>-9.1472800000000007E-3</v>
+      </c>
+      <c r="G29" s="198">
+        <v>15.887</v>
+      </c>
+      <c r="H29" s="198">
+        <v>3.7216699999999998E-3</v>
+      </c>
+      <c r="I29" s="198">
+        <v>-0.13661100000000001</v>
+      </c>
+      <c r="J29" s="198">
+        <v>2.7120999999999999E-2</v>
+      </c>
+      <c r="K29" s="198">
+        <v>-0.197627</v>
+      </c>
+      <c r="L29" s="198">
+        <v>7.4270199999999995E-2</v>
+      </c>
+      <c r="M29" s="198">
+        <v>-0.18159800000000001</v>
+      </c>
+      <c r="N29" s="198">
+        <v>4.5655500000000002E-2</v>
+      </c>
+      <c r="O29" s="198">
+        <v>-7.7862000000000001E-2</v>
+      </c>
+      <c r="P29" s="198">
+        <v>9.50376E-2</v>
+      </c>
+      <c r="Q29" s="198">
+        <v>-0.136986</v>
+      </c>
+      <c r="R29" s="198">
+        <v>1.53078</v>
+      </c>
+      <c r="S29" s="198">
+        <v>-1.17967</v>
+      </c>
+      <c r="T29" s="198">
+        <v>8.1523600000000002E-2</v>
+      </c>
+      <c r="U29" s="198">
+        <v>-4.7912999999999997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="198">
+        <v>18.766500000000001</v>
+      </c>
+      <c r="D30" s="198">
+        <v>1.89476E-4</v>
+      </c>
+      <c r="E30" s="198">
+        <v>1.6100199999999999E-2</v>
+      </c>
+      <c r="F30" s="198">
+        <v>7.6842500000000001E-3</v>
+      </c>
+      <c r="G30" s="198">
+        <v>18.766500000000001</v>
+      </c>
+      <c r="H30" s="198">
+        <v>6.6586900000000001E-3</v>
+      </c>
+      <c r="I30" s="198">
+        <v>0.12739400000000001</v>
+      </c>
+      <c r="J30" s="198">
+        <v>-1.30466E-2</v>
+      </c>
+      <c r="K30" s="198">
+        <v>0.17877699999999999</v>
+      </c>
+      <c r="L30" s="198">
+        <v>-5.2752599999999997E-2</v>
+      </c>
+      <c r="M30" s="198">
+        <v>0.16527900000000001</v>
+      </c>
+      <c r="N30" s="198">
+        <v>-2.8655199999999999E-2</v>
+      </c>
+      <c r="O30" s="198">
+        <v>7.7919600000000006E-2</v>
+      </c>
+      <c r="P30" s="198">
+        <v>-7.0241499999999998E-2</v>
+      </c>
+      <c r="Q30" s="198">
+        <v>0.12770999999999999</v>
+      </c>
+      <c r="R30" s="198">
+        <v>-1.17967</v>
+      </c>
+      <c r="S30" s="198">
+        <v>1.13554</v>
+      </c>
+      <c r="T30" s="198">
+        <v>-5.8860999999999997E-2</v>
+      </c>
+      <c r="U30" s="198">
+        <v>5.2698599999999998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="198">
+        <v>7.2298600000000004</v>
+      </c>
+      <c r="D31" s="198">
+        <v>1.6008399999999999E-2</v>
+      </c>
+      <c r="E31" s="198">
+        <v>4.05652E-4</v>
+      </c>
+      <c r="F31" s="198">
+        <v>-5.0545E-3</v>
+      </c>
+      <c r="G31" s="198">
+        <v>7.2298600000000004</v>
+      </c>
+      <c r="H31" s="198">
+        <v>7.4403500000000001E-3</v>
+      </c>
+      <c r="I31" s="198">
+        <v>-7.5766299999999995E-2</v>
+      </c>
+      <c r="J31" s="198">
+        <v>2.0390800000000001E-2</v>
+      </c>
+      <c r="K31" s="198">
+        <v>-0.10953499999999999</v>
+      </c>
+      <c r="L31" s="198">
+        <v>4.6485699999999998E-2</v>
+      </c>
+      <c r="M31" s="198">
+        <v>-0.100664</v>
+      </c>
+      <c r="N31" s="198">
+        <v>3.06488E-2</v>
+      </c>
+      <c r="O31" s="198">
+        <v>-4.3251199999999997E-2</v>
+      </c>
+      <c r="P31" s="198">
+        <v>5.7979500000000003E-2</v>
+      </c>
+      <c r="Q31" s="198">
+        <v>-7.5973700000000005E-2</v>
+      </c>
+      <c r="R31" s="198">
+        <v>8.1523600000000002E-2</v>
+      </c>
+      <c r="S31" s="198">
+        <v>-5.8860999999999997E-2</v>
+      </c>
+      <c r="T31" s="198">
+        <v>0.50468900000000005</v>
+      </c>
+      <c r="U31" s="198">
+        <v>-0.25503900000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="198">
+        <v>10.421799999999999</v>
+      </c>
+      <c r="D32" s="198">
+        <v>-3.0460099999999999E-4</v>
+      </c>
+      <c r="E32" s="198">
+        <v>1.7032800000000001E-2</v>
+      </c>
+      <c r="F32" s="198">
+        <v>3.4382100000000001E-3</v>
+      </c>
+      <c r="G32" s="198">
+        <v>10.421799999999999</v>
+      </c>
+      <c r="H32" s="198">
+        <v>2.8007399999999999E-3</v>
+      </c>
+      <c r="I32" s="198">
+        <v>6.4270900000000006E-2</v>
+      </c>
+      <c r="J32" s="198">
+        <v>-6.0644399999999999E-3</v>
+      </c>
+      <c r="K32" s="198">
+        <v>8.7387500000000007E-2</v>
+      </c>
+      <c r="L32" s="198">
+        <v>-2.39277E-2</v>
+      </c>
+      <c r="M32" s="198">
+        <v>8.1314899999999996E-2</v>
+      </c>
+      <c r="N32" s="198">
+        <v>-1.30866E-2</v>
+      </c>
+      <c r="O32" s="198">
+        <v>4.2012800000000003E-2</v>
+      </c>
+      <c r="P32" s="198">
+        <v>-3.1795799999999999E-2</v>
+      </c>
+      <c r="Q32" s="198">
+        <v>6.4412999999999998E-2</v>
+      </c>
+      <c r="R32" s="198">
+        <v>-4.7912999999999997E-2</v>
+      </c>
+      <c r="S32" s="198">
+        <v>5.2698599999999998E-2</v>
+      </c>
+      <c r="T32" s="198">
+        <v>-0.25503900000000002</v>
+      </c>
+      <c r="U32" s="198">
+        <v>0.31408599999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF31A2A6-BB98-4ABD-94E7-4BC4F8C140C1}">
   <dimension ref="A1:Z58"/>
   <sheetViews>

</xml_diff>